<commit_message>
add real wages and hours to graph
</commit_message>
<xml_diff>
--- a/Data/main_file.xlsx
+++ b/Data/main_file.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\th3\Documents\Noise_Over_Cycles\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitocormun/Desktop/Literature/Beliefs/Noise_Over_Cycles/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -167,12 +170,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,16 +253,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,17 +607,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO327"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="V223" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="AA56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="22" style="4" customWidth="1"/>
     <col min="4" max="4" width="22" style="3"/>
     <col min="5" max="5" width="22" style="4"/>
@@ -651,7 +654,7 @@
     <col min="41" max="16384" width="22" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="3" customFormat="1">
+    <row r="1" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -776,7 +779,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="3" customFormat="1">
+    <row r="2" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -862,7 +865,7 @@
         <v>5</v>
       </c>
       <c r="AC2" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AD2" s="2">
         <v>5</v>
@@ -901,7 +904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="3" customFormat="1">
+    <row r="3" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="3" customFormat="1">
+    <row r="4" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="3" customFormat="1">
+    <row r="5" spans="1:41" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>1950</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>1.2816901408450703</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>1950.25</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>1.3066922736002364</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <v>1950.5</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>1.4061596298438404</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <v>1950.75</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>1.4485450674237048</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <v>1951</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>1.4661551109893121</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <v>1951.25</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>1.4266267356384428</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <v>1951.5</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>1.5822052921569962</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <v>1951.75</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>1.5986280180240768</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <v>1952</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>1.6396420641862344</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <v>1952.25</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>1.6771939255476416</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <v>1952.5</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>1.6307814992025518</v>
       </c>
     </row>
-    <row r="17" spans="2:39">
+    <row r="17" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>1952.75</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>1.7606520442647937</v>
       </c>
     </row>
-    <row r="18" spans="2:39">
+    <row r="18" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <v>1953</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>1.6752782193958664</v>
       </c>
     </row>
-    <row r="19" spans="2:39">
+    <row r="19" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>1953.25</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>1.5960330578512396</v>
       </c>
     </row>
-    <row r="20" spans="2:39">
+    <row r="20" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>1953.5</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>1.537397945746642</v>
       </c>
     </row>
-    <row r="21" spans="2:39">
+    <row r="21" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <v>1953.75</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>1.6301990932387147</v>
       </c>
     </row>
-    <row r="22" spans="2:39">
+    <row r="22" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <v>1954</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>1.7647058823529413</v>
       </c>
     </row>
-    <row r="23" spans="2:39">
+    <row r="23" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <v>1954.25</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>1.9115241149139455</v>
       </c>
     </row>
-    <row r="24" spans="2:39">
+    <row r="24" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <v>1954.5</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>2.111764705882353</v>
       </c>
     </row>
-    <row r="25" spans="2:39">
+    <row r="25" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <v>1954.75</v>
       </c>
@@ -2486,7 +2489,7 @@
         <v>2.3450433422407611</v>
       </c>
     </row>
-    <row r="26" spans="2:39">
+    <row r="26" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <v>1955</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>2.3727054550171887</v>
       </c>
     </row>
-    <row r="27" spans="2:39">
+    <row r="27" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B27" s="3">
         <v>1955.25</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>2.6503455849105357</v>
       </c>
     </row>
-    <row r="28" spans="2:39">
+    <row r="28" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B28" s="3">
         <v>1955.5</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>2.8011545862732521</v>
       </c>
     </row>
-    <row r="29" spans="2:39">
+    <row r="29" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B29" s="3">
         <v>1955.75</v>
       </c>
@@ -2746,7 +2749,7 @@
         <v>2.8889030045099409</v>
       </c>
     </row>
-    <row r="30" spans="2:39">
+    <row r="30" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B30" s="3">
         <v>1956</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>3.0486731228776254</v>
       </c>
     </row>
-    <row r="31" spans="2:39">
+    <row r="31" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B31" s="3">
         <v>1956.25</v>
       </c>
@@ -2876,7 +2879,7 @@
         <v>2.9361755329124208</v>
       </c>
     </row>
-    <row r="32" spans="2:39">
+    <row r="32" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B32" s="3">
         <v>1956.5</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>2.7999012162746189</v>
       </c>
     </row>
-    <row r="33" spans="2:40">
+    <row r="33" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B33" s="3">
         <v>1956.75</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>2.8695277914412203</v>
       </c>
     </row>
-    <row r="34" spans="2:40">
+    <row r="34" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B34" s="3">
         <v>1957</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>2.6757658477403701</v>
       </c>
     </row>
-    <row r="35" spans="2:40">
+    <row r="35" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B35" s="3">
         <v>1957.25</v>
       </c>
@@ -3136,7 +3139,7 @@
         <v>2.8534425637009817</v>
       </c>
     </row>
-    <row r="36" spans="2:40">
+    <row r="36" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B36" s="3">
         <v>1957.5</v>
       </c>
@@ -3201,7 +3204,7 @@
         <v>2.5399676666067901</v>
       </c>
     </row>
-    <row r="37" spans="2:40">
+    <row r="37" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B37" s="3">
         <v>1957.75</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>2.3930345281551078</v>
       </c>
     </row>
-    <row r="38" spans="2:40">
+    <row r="38" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B38" s="3">
         <v>1958</v>
       </c>
@@ -3331,7 +3334,7 @@
         <v>2.4923040492540851</v>
       </c>
     </row>
-    <row r="39" spans="2:40">
+    <row r="39" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B39" s="3">
         <v>1958.25</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>2.6706021251475796</v>
       </c>
     </row>
-    <row r="40" spans="2:40">
+    <row r="40" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B40" s="3">
         <v>1958.5</v>
       </c>
@@ -3461,7 +3464,7 @@
         <v>2.9372763011206948</v>
       </c>
     </row>
-    <row r="41" spans="2:40">
+    <row r="41" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B41" s="3">
         <v>1958.75</v>
       </c>
@@ -3526,7 +3529,7 @@
         <v>3.2243181685452313</v>
       </c>
     </row>
-    <row r="42" spans="2:40">
+    <row r="42" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B42" s="3">
         <v>1959</v>
       </c>
@@ -3591,7 +3594,7 @@
         <v>3.2290756596190806</v>
       </c>
     </row>
-    <row r="43" spans="2:40">
+    <row r="43" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B43" s="3">
         <v>1959.25</v>
       </c>
@@ -3656,7 +3659,7 @@
         <v>3.4006048621612193</v>
       </c>
     </row>
-    <row r="44" spans="2:40">
+    <row r="44" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B44" s="3">
         <v>1959.5</v>
       </c>
@@ -3721,7 +3724,7 @@
         <v>3.2958627882721059</v>
       </c>
     </row>
-    <row r="45" spans="2:40">
+    <row r="45" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B45" s="3">
         <v>1959.75</v>
       </c>
@@ -3786,7 +3789,7 @@
         <v>3.4566547385432296</v>
       </c>
     </row>
-    <row r="46" spans="2:40">
+    <row r="46" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B46" s="3">
         <v>1960</v>
       </c>
@@ -3854,7 +3857,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:40">
+    <row r="47" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B47" s="3">
         <v>1960.25</v>
       </c>
@@ -3922,7 +3925,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="2:40">
+    <row r="48" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B48" s="3">
         <v>1960.5</v>
       </c>
@@ -3990,7 +3993,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="2:40">
+    <row r="49" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B49" s="3">
         <v>1960.75</v>
       </c>
@@ -4058,7 +4061,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="2:40">
+    <row r="50" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B50" s="3">
         <v>1961</v>
       </c>
@@ -4126,7 +4129,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="2:40">
+    <row r="51" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B51" s="3">
         <v>1961.25</v>
       </c>
@@ -4194,7 +4197,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="2:40">
+    <row r="52" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B52" s="3">
         <v>1961.5</v>
       </c>
@@ -4262,7 +4265,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="2:40">
+    <row r="53" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B53" s="3">
         <v>1961.75</v>
       </c>
@@ -4330,7 +4333,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="2:40">
+    <row r="54" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B54" s="3">
         <v>1962</v>
       </c>
@@ -4398,7 +4401,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="2:40">
+    <row r="55" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B55" s="3">
         <v>1962.25</v>
       </c>
@@ -4466,7 +4469,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="2:40">
+    <row r="56" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B56" s="3">
         <v>1962.5</v>
       </c>
@@ -4534,7 +4537,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="2:40">
+    <row r="57" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B57" s="3">
         <v>1962.75</v>
       </c>
@@ -4602,7 +4605,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="2:40">
+    <row r="58" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B58" s="3">
         <v>1963</v>
       </c>
@@ -4670,7 +4673,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="2:40">
+    <row r="59" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B59" s="3">
         <v>1963.25</v>
       </c>
@@ -4738,7 +4741,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="2:40">
+    <row r="60" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B60" s="3">
         <v>1963.5</v>
       </c>
@@ -4806,7 +4809,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="2:40">
+    <row r="61" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B61" s="3">
         <v>1963.75</v>
       </c>
@@ -4874,7 +4877,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="2:40">
+    <row r="62" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B62" s="3">
         <v>1964</v>
       </c>
@@ -4942,7 +4945,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="2:40">
+    <row r="63" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B63" s="3">
         <v>1964.25</v>
       </c>
@@ -5010,7 +5013,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="2:40">
+    <row r="64" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B64" s="3">
         <v>1964.5</v>
       </c>
@@ -5078,7 +5081,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="2:40">
+    <row r="65" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B65" s="3">
         <v>1964.75</v>
       </c>
@@ -5146,7 +5149,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="2:40">
+    <row r="66" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B66" s="3">
         <v>1965</v>
       </c>
@@ -5214,7 +5217,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="2:40">
+    <row r="67" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B67" s="3">
         <v>1965.25</v>
       </c>
@@ -5282,7 +5285,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="2:40">
+    <row r="68" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B68" s="3">
         <v>1965.5</v>
       </c>
@@ -5350,7 +5353,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="2:40">
+    <row r="69" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B69" s="3">
         <v>1965.75</v>
       </c>
@@ -5418,7 +5421,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="2:40">
+    <row r="70" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B70" s="3">
         <v>1966</v>
       </c>
@@ -5486,7 +5489,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="2:40">
+    <row r="71" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B71" s="3">
         <v>1966.25</v>
       </c>
@@ -5554,7 +5557,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="72" spans="2:40">
+    <row r="72" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B72" s="3">
         <v>1966.5</v>
       </c>
@@ -5622,7 +5625,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="2:40">
+    <row r="73" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B73" s="3">
         <v>1966.75</v>
       </c>
@@ -5690,7 +5693,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="2:40">
+    <row r="74" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B74" s="3">
         <v>1967</v>
       </c>
@@ -5758,7 +5761,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="2:40">
+    <row r="75" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B75" s="3">
         <v>1967.25</v>
       </c>
@@ -5826,7 +5829,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="2:40">
+    <row r="76" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B76" s="3">
         <v>1967.5</v>
       </c>
@@ -5894,7 +5897,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="2:40">
+    <row r="77" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B77" s="3">
         <v>1967.75</v>
       </c>
@@ -5962,7 +5965,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="2:40">
+    <row r="78" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B78" s="3">
         <v>1968</v>
       </c>
@@ -6030,7 +6033,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="2:40">
+    <row r="79" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B79" s="3">
         <v>1968.25</v>
       </c>
@@ -6098,7 +6101,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="2:40">
+    <row r="80" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B80" s="3">
         <v>1968.5</v>
       </c>
@@ -6166,7 +6169,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="2:40">
+    <row r="81" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B81" s="3">
         <v>1968.75</v>
       </c>
@@ -6266,7 +6269,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="2:40">
+    <row r="82" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B82" s="3">
         <v>1969</v>
       </c>
@@ -6370,7 +6373,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="2:40">
+    <row r="83" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B83" s="3">
         <v>1969.25</v>
       </c>
@@ -6474,7 +6477,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="2:40">
+    <row r="84" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B84" s="3">
         <v>1969.5</v>
       </c>
@@ -6578,7 +6581,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="85" spans="2:40">
+    <row r="85" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B85" s="3">
         <v>1969.75</v>
       </c>
@@ -6681,7 +6684,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="2:40">
+    <row r="86" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B86" s="3">
         <v>1970</v>
       </c>
@@ -6785,7 +6788,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="2:40">
+    <row r="87" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B87" s="3">
         <v>1970.25</v>
       </c>
@@ -6888,7 +6891,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="2:40">
+    <row r="88" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B88" s="3">
         <v>1970.5</v>
       </c>
@@ -6991,7 +6994,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="2:40">
+    <row r="89" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B89" s="3">
         <v>1970.75</v>
       </c>
@@ -7094,7 +7097,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="2:40">
+    <row r="90" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B90" s="3">
         <v>1971</v>
       </c>
@@ -7197,7 +7200,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="91" spans="2:40">
+    <row r="91" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B91" s="3">
         <v>1971.25</v>
       </c>
@@ -7300,7 +7303,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="2:40">
+    <row r="92" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B92" s="3">
         <v>1971.5</v>
       </c>
@@ -7403,7 +7406,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="93" spans="2:40">
+    <row r="93" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B93" s="3">
         <v>1971.75</v>
       </c>
@@ -7506,7 +7509,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="2:40">
+    <row r="94" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B94" s="3">
         <v>1972</v>
       </c>
@@ -7609,7 +7612,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="2:40">
+    <row r="95" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B95" s="3">
         <v>1972.25</v>
       </c>
@@ -7712,7 +7715,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="2:40">
+    <row r="96" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B96" s="3">
         <v>1972.5</v>
       </c>
@@ -7815,7 +7818,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="97" spans="2:40">
+    <row r="97" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B97" s="3">
         <v>1972.75</v>
       </c>
@@ -7918,7 +7921,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="98" spans="2:40">
+    <row r="98" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B98" s="3">
         <v>1973</v>
       </c>
@@ -8021,7 +8024,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="2:40">
+    <row r="99" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B99" s="3">
         <v>1973.25</v>
       </c>
@@ -8124,7 +8127,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="2:40">
+    <row r="100" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B100" s="3">
         <v>1973.5</v>
       </c>
@@ -8227,7 +8230,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="101" spans="2:40">
+    <row r="101" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B101" s="3">
         <v>1973.75</v>
       </c>
@@ -8330,7 +8333,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="2:40">
+    <row r="102" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B102" s="3">
         <v>1974</v>
       </c>
@@ -8433,7 +8436,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="2:40">
+    <row r="103" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B103" s="3">
         <v>1974.25</v>
       </c>
@@ -8536,7 +8539,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="104" spans="2:40">
+    <row r="104" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B104" s="3">
         <v>1974.5</v>
       </c>
@@ -8640,7 +8643,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="2:40">
+    <row r="105" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B105" s="3">
         <v>1974.75</v>
       </c>
@@ -8743,7 +8746,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="106" spans="2:40">
+    <row r="106" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B106" s="3">
         <v>1975</v>
       </c>
@@ -8846,7 +8849,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="2:40">
+    <row r="107" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B107" s="3">
         <v>1975.25</v>
       </c>
@@ -8949,7 +8952,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="2:40">
+    <row r="108" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B108" s="3">
         <v>1975.5</v>
       </c>
@@ -9052,7 +9055,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="2:40">
+    <row r="109" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B109" s="3">
         <v>1975.75</v>
       </c>
@@ -9155,7 +9158,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="110" spans="2:40">
+    <row r="110" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B110" s="3">
         <v>1976</v>
       </c>
@@ -9258,7 +9261,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="111" spans="2:40">
+    <row r="111" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B111" s="3">
         <v>1976.25</v>
       </c>
@@ -9361,7 +9364,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="2:40">
+    <row r="112" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B112" s="3">
         <v>1976.5</v>
       </c>
@@ -9464,7 +9467,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="113" spans="2:41">
+    <row r="113" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B113" s="3">
         <v>1976.75</v>
       </c>
@@ -9567,7 +9570,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="114" spans="2:41">
+    <row r="114" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B114" s="3">
         <v>1977</v>
       </c>
@@ -9670,7 +9673,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="115" spans="2:41">
+    <row r="115" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B115" s="3">
         <v>1977.25</v>
       </c>
@@ -9773,7 +9776,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="116" spans="2:41">
+    <row r="116" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B116" s="3">
         <v>1977.5</v>
       </c>
@@ -9876,7 +9879,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="117" spans="2:41">
+    <row r="117" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B117" s="3">
         <v>1977.75</v>
       </c>
@@ -9979,7 +9982,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="118" spans="2:41">
+    <row r="118" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B118" s="3">
         <v>1978</v>
       </c>
@@ -10082,7 +10085,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="2:41">
+    <row r="119" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B119" s="3">
         <v>1978.25</v>
       </c>
@@ -10188,7 +10191,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="2:41">
+    <row r="120" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B120" s="3">
         <v>1978.5</v>
       </c>
@@ -10294,7 +10297,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="2:41">
+    <row r="121" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B121" s="3">
         <v>1978.75</v>
       </c>
@@ -10400,7 +10403,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" spans="2:41">
+    <row r="122" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B122" s="3">
         <v>1979</v>
       </c>
@@ -10506,7 +10509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="123" spans="2:41">
+    <row r="123" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B123" s="3">
         <v>1979.25</v>
       </c>
@@ -10612,7 +10615,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="124" spans="2:41">
+    <row r="124" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B124" s="3">
         <v>1979.5</v>
       </c>
@@ -10718,7 +10721,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="2:41">
+    <row r="125" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B125" s="3">
         <v>1979.75</v>
       </c>
@@ -10824,7 +10827,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="2:41">
+    <row r="126" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B126" s="3">
         <v>1980</v>
       </c>
@@ -10930,7 +10933,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="127" spans="2:41">
+    <row r="127" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B127" s="3">
         <v>1980.25</v>
       </c>
@@ -11036,7 +11039,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="2:41">
+    <row r="128" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B128" s="3">
         <v>1980.5</v>
       </c>
@@ -11142,7 +11145,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="129" spans="2:41">
+    <row r="129" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B129" s="3">
         <v>1980.75</v>
       </c>
@@ -11248,7 +11251,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="130" spans="2:41">
+    <row r="130" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B130" s="3">
         <v>1981</v>
       </c>
@@ -11354,7 +11357,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="131" spans="2:41">
+    <row r="131" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B131" s="3">
         <v>1981.25</v>
       </c>
@@ -11460,7 +11463,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="132" spans="2:41">
+    <row r="132" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B132" s="3">
         <v>1981.5</v>
       </c>
@@ -11582,7 +11585,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="2:41">
+    <row r="133" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B133" s="3">
         <v>1981.75</v>
       </c>
@@ -11704,7 +11707,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="134" spans="2:41">
+    <row r="134" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B134" s="3">
         <v>1982</v>
       </c>
@@ -11826,7 +11829,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="135" spans="2:41">
+    <row r="135" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B135" s="3">
         <v>1982.25</v>
       </c>
@@ -11948,7 +11951,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="2:41">
+    <row r="136" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B136" s="3">
         <v>1982.5</v>
       </c>
@@ -12070,7 +12073,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="137" spans="2:41">
+    <row r="137" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B137" s="3">
         <v>1982.75</v>
       </c>
@@ -12192,7 +12195,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="138" spans="2:41">
+    <row r="138" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B138" s="3">
         <v>1983</v>
       </c>
@@ -12314,7 +12317,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="139" spans="2:41">
+    <row r="139" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B139" s="3">
         <v>1983.25</v>
       </c>
@@ -12436,7 +12439,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="140" spans="2:41">
+    <row r="140" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B140" s="3">
         <v>1983.5</v>
       </c>
@@ -12558,7 +12561,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="141" spans="2:41">
+    <row r="141" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B141" s="3">
         <v>1983.75</v>
       </c>
@@ -12680,7 +12683,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="142" spans="2:41">
+    <row r="142" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B142" s="3">
         <v>1984</v>
       </c>
@@ -12802,7 +12805,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="143" spans="2:41">
+    <row r="143" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B143" s="3">
         <v>1984.25</v>
       </c>
@@ -12924,7 +12927,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="144" spans="2:41">
+    <row r="144" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B144" s="3">
         <v>1984.5</v>
       </c>
@@ -13046,7 +13049,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="145" spans="2:41">
+    <row r="145" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B145" s="3">
         <v>1984.75</v>
       </c>
@@ -13168,7 +13171,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="2:41">
+    <row r="146" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B146" s="3">
         <v>1985</v>
       </c>
@@ -13290,7 +13293,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="147" spans="2:41">
+    <row r="147" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B147" s="3">
         <v>1985.25</v>
       </c>
@@ -13412,7 +13415,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="148" spans="2:41">
+    <row r="148" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B148" s="3">
         <v>1985.5</v>
       </c>
@@ -13534,7 +13537,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="149" spans="2:41">
+    <row r="149" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B149" s="3">
         <v>1985.75</v>
       </c>
@@ -13656,7 +13659,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="150" spans="2:41">
+    <row r="150" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B150" s="3">
         <v>1986</v>
       </c>
@@ -13778,7 +13781,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="151" spans="2:41">
+    <row r="151" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B151" s="3">
         <v>1986.25</v>
       </c>
@@ -13900,7 +13903,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="152" spans="2:41">
+    <row r="152" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B152" s="3">
         <v>1986.5</v>
       </c>
@@ -14022,7 +14025,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="153" spans="2:41">
+    <row r="153" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B153" s="3">
         <v>1986.75</v>
       </c>
@@ -14144,7 +14147,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="154" spans="2:41">
+    <row r="154" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B154" s="3">
         <v>1987</v>
       </c>
@@ -14266,7 +14269,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="155" spans="2:41">
+    <row r="155" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B155" s="3">
         <v>1987.25</v>
       </c>
@@ -14388,7 +14391,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="156" spans="2:41">
+    <row r="156" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B156" s="3">
         <v>1987.5</v>
       </c>
@@ -14510,7 +14513,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="157" spans="2:41">
+    <row r="157" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B157" s="3">
         <v>1987.75</v>
       </c>
@@ -14632,7 +14635,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158" spans="2:41">
+    <row r="158" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B158" s="3">
         <v>1988</v>
       </c>
@@ -14754,7 +14757,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="159" spans="2:41">
+    <row r="159" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B159" s="3">
         <v>1988.25</v>
       </c>
@@ -14876,7 +14879,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="160" spans="2:41">
+    <row r="160" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B160" s="3">
         <v>1988.5</v>
       </c>
@@ -14998,7 +15001,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="161" spans="2:41">
+    <row r="161" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B161" s="3">
         <v>1988.75</v>
       </c>
@@ -15120,7 +15123,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="162" spans="2:41">
+    <row r="162" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B162" s="3">
         <v>1989</v>
       </c>
@@ -15242,7 +15245,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="2:41">
+    <row r="163" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B163" s="3">
         <v>1989.25</v>
       </c>
@@ -15364,7 +15367,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="164" spans="2:41">
+    <row r="164" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B164" s="3">
         <v>1989.5</v>
       </c>
@@ -15486,7 +15489,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="165" spans="2:41">
+    <row r="165" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B165" s="3">
         <v>1989.75</v>
       </c>
@@ -15608,7 +15611,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="166" spans="2:41">
+    <row r="166" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B166" s="3">
         <v>1990</v>
       </c>
@@ -15730,7 +15733,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="167" spans="2:41">
+    <row r="167" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B167" s="3">
         <v>1990.25</v>
       </c>
@@ -15852,7 +15855,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="168" spans="2:41">
+    <row r="168" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B168" s="3">
         <v>1990.5</v>
       </c>
@@ -15974,7 +15977,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="2:41">
+    <row r="169" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B169" s="3">
         <v>1990.75</v>
       </c>
@@ -16096,7 +16099,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="170" spans="2:41">
+    <row r="170" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B170" s="3">
         <v>1991</v>
       </c>
@@ -16218,7 +16221,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="171" spans="2:41">
+    <row r="171" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B171" s="3">
         <v>1991.25</v>
       </c>
@@ -16340,7 +16343,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="172" spans="2:41">
+    <row r="172" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B172" s="3">
         <v>1991.5</v>
       </c>
@@ -16462,7 +16465,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="173" spans="2:41">
+    <row r="173" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B173" s="3">
         <v>1991.75</v>
       </c>
@@ -16584,7 +16587,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="174" spans="2:41">
+    <row r="174" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B174" s="3">
         <v>1992</v>
       </c>
@@ -16706,7 +16709,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="175" spans="2:41">
+    <row r="175" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B175" s="3">
         <v>1992.25</v>
       </c>
@@ -16828,7 +16831,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="176" spans="2:41">
+    <row r="176" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B176" s="3">
         <v>1992.5</v>
       </c>
@@ -16950,7 +16953,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="177" spans="2:41">
+    <row r="177" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B177" s="3">
         <v>1992.75</v>
       </c>
@@ -17072,7 +17075,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="178" spans="2:41">
+    <row r="178" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B178" s="3">
         <v>1993</v>
       </c>
@@ -17194,7 +17197,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="179" spans="2:41">
+    <row r="179" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B179" s="3">
         <v>1993.25</v>
       </c>
@@ -17316,7 +17319,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="180" spans="2:41">
+    <row r="180" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B180" s="3">
         <v>1993.5</v>
       </c>
@@ -17438,7 +17441,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="181" spans="2:41">
+    <row r="181" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B181" s="3">
         <v>1993.75</v>
       </c>
@@ -17560,7 +17563,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="182" spans="2:41">
+    <row r="182" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B182" s="3">
         <v>1994</v>
       </c>
@@ -17682,7 +17685,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="183" spans="2:41">
+    <row r="183" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B183" s="3">
         <v>1994.25</v>
       </c>
@@ -17804,7 +17807,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="184" spans="2:41">
+    <row r="184" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B184" s="3">
         <v>1994.5</v>
       </c>
@@ -17926,7 +17929,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="185" spans="2:41">
+    <row r="185" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B185" s="3">
         <v>1994.75</v>
       </c>
@@ -18048,7 +18051,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="186" spans="2:41">
+    <row r="186" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B186" s="3">
         <v>1995</v>
       </c>
@@ -18170,7 +18173,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="187" spans="2:41">
+    <row r="187" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B187" s="3">
         <v>1995.25</v>
       </c>
@@ -18292,7 +18295,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="188" spans="2:41">
+    <row r="188" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B188" s="3">
         <v>1995.5</v>
       </c>
@@ -18414,7 +18417,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="189" spans="2:41">
+    <row r="189" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B189" s="3">
         <v>1995.75</v>
       </c>
@@ -18536,7 +18539,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="190" spans="2:41">
+    <row r="190" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B190" s="3">
         <v>1996</v>
       </c>
@@ -18658,7 +18661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="191" spans="2:41">
+    <row r="191" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B191" s="3">
         <v>1996.25</v>
       </c>
@@ -18780,7 +18783,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="192" spans="2:41">
+    <row r="192" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B192" s="3">
         <v>1996.5</v>
       </c>
@@ -18902,7 +18905,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="193" spans="2:41">
+    <row r="193" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B193" s="3">
         <v>1996.75</v>
       </c>
@@ -19024,7 +19027,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="194" spans="2:41">
+    <row r="194" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B194" s="3">
         <v>1997</v>
       </c>
@@ -19146,7 +19149,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="195" spans="2:41">
+    <row r="195" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B195" s="3">
         <v>1997.25</v>
       </c>
@@ -19268,7 +19271,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="196" spans="2:41">
+    <row r="196" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B196" s="3">
         <v>1997.5</v>
       </c>
@@ -19390,7 +19393,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="197" spans="2:41">
+    <row r="197" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B197" s="3">
         <v>1997.75</v>
       </c>
@@ -19512,7 +19515,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="198" spans="2:41">
+    <row r="198" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B198" s="3">
         <v>1998</v>
       </c>
@@ -19634,7 +19637,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="199" spans="2:41">
+    <row r="199" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B199" s="3">
         <v>1998.25</v>
       </c>
@@ -19756,7 +19759,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="200" spans="2:41">
+    <row r="200" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B200" s="3">
         <v>1998.5</v>
       </c>
@@ -19878,7 +19881,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="201" spans="2:41">
+    <row r="201" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B201" s="3">
         <v>1998.75</v>
       </c>
@@ -20000,7 +20003,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="202" spans="2:41">
+    <row r="202" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B202" s="3">
         <v>1999</v>
       </c>
@@ -20122,7 +20125,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="203" spans="2:41">
+    <row r="203" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B203" s="3">
         <v>1999.25</v>
       </c>
@@ -20244,7 +20247,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="204" spans="2:41">
+    <row r="204" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B204" s="3">
         <v>1999.5</v>
       </c>
@@ -20366,7 +20369,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="205" spans="2:41">
+    <row r="205" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B205" s="3">
         <v>1999.75</v>
       </c>
@@ -20488,7 +20491,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="206" spans="2:41">
+    <row r="206" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B206" s="3">
         <v>2000</v>
       </c>
@@ -20610,7 +20613,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="207" spans="2:41">
+    <row r="207" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B207" s="3">
         <v>2000.25</v>
       </c>
@@ -20732,7 +20735,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="208" spans="2:41">
+    <row r="208" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B208" s="3">
         <v>2000.5</v>
       </c>
@@ -20854,7 +20857,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="209" spans="2:41">
+    <row r="209" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B209" s="3">
         <v>2000.75</v>
       </c>
@@ -20976,7 +20979,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="210" spans="2:41">
+    <row r="210" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B210" s="3">
         <v>2001</v>
       </c>
@@ -21098,7 +21101,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="211" spans="2:41">
+    <row r="211" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B211" s="3">
         <v>2001.25</v>
       </c>
@@ -21220,7 +21223,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="212" spans="2:41">
+    <row r="212" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B212" s="3">
         <v>2001.5</v>
       </c>
@@ -21342,7 +21345,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="213" spans="2:41">
+    <row r="213" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B213" s="3">
         <v>2001.75</v>
       </c>
@@ -21464,7 +21467,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="214" spans="2:41">
+    <row r="214" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B214" s="3">
         <v>2002</v>
       </c>
@@ -21586,7 +21589,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="215" spans="2:41">
+    <row r="215" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B215" s="3">
         <v>2002.25</v>
       </c>
@@ -21708,7 +21711,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="216" spans="2:41">
+    <row r="216" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B216" s="3">
         <v>2002.5</v>
       </c>
@@ -21830,7 +21833,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="217" spans="2:41">
+    <row r="217" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B217" s="3">
         <v>2002.75</v>
       </c>
@@ -21952,7 +21955,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="218" spans="2:41">
+    <row r="218" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B218" s="3">
         <v>2003</v>
       </c>
@@ -22074,7 +22077,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="219" spans="2:41">
+    <row r="219" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B219" s="3">
         <v>2003.25</v>
       </c>
@@ -22196,7 +22199,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="220" spans="2:41">
+    <row r="220" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B220" s="3">
         <v>2003.5</v>
       </c>
@@ -22318,7 +22321,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="221" spans="2:41">
+    <row r="221" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B221" s="3">
         <v>2003.75</v>
       </c>
@@ -22440,7 +22443,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="222" spans="2:41">
+    <row r="222" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B222" s="3">
         <v>2004</v>
       </c>
@@ -22562,7 +22565,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="223" spans="2:41">
+    <row r="223" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B223" s="3">
         <v>2004.25</v>
       </c>
@@ -22684,7 +22687,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="224" spans="2:41">
+    <row r="224" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B224" s="3">
         <v>2004.5</v>
       </c>
@@ -22806,7 +22809,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="225" spans="2:41">
+    <row r="225" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B225" s="3">
         <v>2004.75</v>
       </c>
@@ -22928,7 +22931,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="226" spans="2:41">
+    <row r="226" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B226" s="3">
         <v>2005</v>
       </c>
@@ -23050,7 +23053,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="227" spans="2:41">
+    <row r="227" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B227" s="3">
         <v>2005.25</v>
       </c>
@@ -23172,7 +23175,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="228" spans="2:41">
+    <row r="228" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B228" s="3">
         <v>2005.5</v>
       </c>
@@ -23294,7 +23297,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="229" spans="2:41">
+    <row r="229" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B229" s="3">
         <v>2005.75</v>
       </c>
@@ -23416,7 +23419,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="230" spans="2:41">
+    <row r="230" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B230" s="3">
         <v>2006</v>
       </c>
@@ -23538,7 +23541,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="231" spans="2:41">
+    <row r="231" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B231" s="3">
         <v>2006.25</v>
       </c>
@@ -23658,7 +23661,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="232" spans="2:41">
+    <row r="232" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B232" s="3">
         <v>2006.5</v>
       </c>
@@ -23778,7 +23781,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="233" spans="2:41">
+    <row r="233" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B233" s="3">
         <v>2006.75</v>
       </c>
@@ -23898,7 +23901,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="234" spans="2:41">
+    <row r="234" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B234" s="3">
         <v>2007</v>
       </c>
@@ -24003,7 +24006,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="235" spans="2:41">
+    <row r="235" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B235" s="3">
         <v>2007.25</v>
       </c>
@@ -24108,7 +24111,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="236" spans="2:41">
+    <row r="236" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B236" s="3">
         <v>2007.5</v>
       </c>
@@ -24213,7 +24216,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="237" spans="2:41">
+    <row r="237" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B237" s="3">
         <v>2007.75</v>
       </c>
@@ -24318,7 +24321,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="238" spans="2:41">
+    <row r="238" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B238" s="3">
         <v>2008</v>
       </c>
@@ -24423,7 +24426,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="239" spans="2:41">
+    <row r="239" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B239" s="3">
         <v>2008.25</v>
       </c>
@@ -24528,7 +24531,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="240" spans="2:41">
+    <row r="240" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B240" s="3">
         <v>2008.5</v>
       </c>
@@ -24633,7 +24636,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="241" spans="2:41">
+    <row r="241" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B241" s="3">
         <v>2008.75</v>
       </c>
@@ -24738,7 +24741,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="242" spans="2:41">
+    <row r="242" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B242" s="3">
         <v>2009</v>
       </c>
@@ -24843,7 +24846,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="243" spans="2:41">
+    <row r="243" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B243" s="3">
         <v>2009.25</v>
       </c>
@@ -24948,7 +24951,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="244" spans="2:41">
+    <row r="244" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B244" s="3">
         <v>2009.5</v>
       </c>
@@ -25053,7 +25056,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="245" spans="2:41">
+    <row r="245" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B245" s="3">
         <v>2009.75</v>
       </c>
@@ -25158,7 +25161,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="246" spans="2:41">
+    <row r="246" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B246" s="3">
         <v>2010</v>
       </c>
@@ -25261,7 +25264,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="247" spans="2:41">
+    <row r="247" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B247" s="3">
         <v>2010.25</v>
       </c>
@@ -25364,7 +25367,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="248" spans="2:41">
+    <row r="248" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B248" s="3">
         <v>2010.5</v>
       </c>
@@ -25467,7 +25470,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="249" spans="2:41">
+    <row r="249" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B249" s="3">
         <v>2010.75</v>
       </c>
@@ -25570,7 +25573,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="250" spans="2:41">
+    <row r="250" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B250" s="3">
         <v>2011</v>
       </c>
@@ -25673,7 +25676,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="251" spans="2:41">
+    <row r="251" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B251" s="3">
         <v>2011.25</v>
       </c>
@@ -25776,7 +25779,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="252" spans="2:41">
+    <row r="252" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B252" s="3">
         <v>2011.5</v>
       </c>
@@ -25879,7 +25882,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="253" spans="2:41">
+    <row r="253" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B253" s="3">
         <v>2011.75</v>
       </c>
@@ -25982,7 +25985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="254" spans="2:41">
+    <row r="254" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B254" s="3">
         <v>2012</v>
       </c>
@@ -26085,7 +26088,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="255" spans="2:41">
+    <row r="255" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B255" s="3">
         <v>2012.25</v>
       </c>
@@ -26188,7 +26191,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="256" spans="2:41">
+    <row r="256" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B256" s="3">
         <v>2012.5</v>
       </c>
@@ -26291,7 +26294,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="257" spans="2:41">
+    <row r="257" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B257" s="3">
         <v>2012.75</v>
       </c>
@@ -26394,7 +26397,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="258" spans="2:41">
+    <row r="258" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B258" s="3">
         <v>2013</v>
       </c>
@@ -26497,7 +26500,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="259" spans="2:41">
+    <row r="259" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B259" s="3">
         <v>2013.25</v>
       </c>
@@ -26600,7 +26603,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="260" spans="2:41">
+    <row r="260" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B260" s="3">
         <v>2013.5</v>
       </c>
@@ -26703,7 +26706,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="261" spans="2:41">
+    <row r="261" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B261" s="3">
         <v>2013.75</v>
       </c>
@@ -26806,7 +26809,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="262" spans="2:41">
+    <row r="262" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B262" s="3">
         <v>2014</v>
       </c>
@@ -26909,7 +26912,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="263" spans="2:41">
+    <row r="263" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B263" s="3">
         <v>2014.25</v>
       </c>
@@ -27012,7 +27015,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="264" spans="2:41">
+    <row r="264" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B264" s="3">
         <v>2014.5</v>
       </c>
@@ -27115,7 +27118,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="265" spans="2:41">
+    <row r="265" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B265" s="3">
         <v>2014.75</v>
       </c>
@@ -27218,7 +27221,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="266" spans="2:41">
+    <row r="266" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B266" s="3">
         <v>2015</v>
       </c>
@@ -27321,7 +27324,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="267" spans="2:41">
+    <row r="267" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B267" s="3">
         <v>2015.25</v>
       </c>
@@ -27424,7 +27427,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="268" spans="2:41">
+    <row r="268" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B268" s="3">
         <v>2015.5</v>
       </c>
@@ -27527,7 +27530,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="269" spans="2:41">
+    <row r="269" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B269" s="3">
         <v>2015.75</v>
       </c>
@@ -27630,7 +27633,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="270" spans="2:41">
+    <row r="270" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B270" s="3">
         <v>2016</v>
       </c>
@@ -27733,7 +27736,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="271" spans="2:41">
+    <row r="271" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B271" s="3">
         <v>2016.25</v>
       </c>
@@ -27836,7 +27839,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="272" spans="2:41">
+    <row r="272" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B272" s="3">
         <v>2016.5</v>
       </c>
@@ -27939,7 +27942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="273" spans="2:41">
+    <row r="273" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B273" s="3">
         <v>2016.75</v>
       </c>
@@ -28042,7 +28045,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="274" spans="2:41">
+    <row r="274" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B274" s="3">
         <v>2017</v>
       </c>
@@ -28145,7 +28148,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="275" spans="2:41">
+    <row r="275" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B275" s="3">
         <v>2017.25</v>
       </c>
@@ -28248,7 +28251,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="276" spans="2:41">
+    <row r="276" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B276" s="3">
         <v>2017.5</v>
       </c>
@@ -28336,7 +28339,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="277" spans="2:41">
+    <row r="277" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B277" s="3">
         <v>2017.75</v>
       </c>
@@ -28391,7 +28394,7 @@
       <c r="Y277" s="5"/>
       <c r="Z277" s="3"/>
     </row>
-    <row r="278" spans="2:41">
+    <row r="278" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B278" s="3">
         <v>2018</v>
       </c>
@@ -28446,7 +28449,7 @@
       <c r="Y278" s="5"/>
       <c r="Z278" s="3"/>
     </row>
-    <row r="279" spans="2:41">
+    <row r="279" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B279" s="3">
         <v>2018.25</v>
       </c>
@@ -28501,7 +28504,7 @@
       <c r="Y279" s="5"/>
       <c r="Z279" s="3"/>
     </row>
-    <row r="280" spans="2:41">
+    <row r="280" spans="2:41" x14ac:dyDescent="0.2">
       <c r="M280" s="5"/>
       <c r="N280" s="12"/>
       <c r="O280" s="5"/>
@@ -28517,7 +28520,7 @@
       <c r="Y280" s="5"/>
       <c r="Z280" s="3"/>
     </row>
-    <row r="281" spans="2:41">
+    <row r="281" spans="2:41" x14ac:dyDescent="0.2">
       <c r="M281" s="5"/>
       <c r="N281" s="12"/>
       <c r="O281" s="5"/>
@@ -28533,7 +28536,7 @@
       <c r="Y281" s="5"/>
       <c r="Z281" s="3"/>
     </row>
-    <row r="282" spans="2:41">
+    <row r="282" spans="2:41" x14ac:dyDescent="0.2">
       <c r="M282" s="5"/>
       <c r="N282" s="12"/>
       <c r="O282" s="5"/>
@@ -28549,139 +28552,139 @@
       <c r="Y282" s="5"/>
       <c r="Z282" s="3"/>
     </row>
-    <row r="283" spans="2:41">
+    <row r="283" spans="2:41" x14ac:dyDescent="0.2">
       <c r="Z283" s="3"/>
     </row>
-    <row r="284" spans="2:41">
+    <row r="284" spans="2:41" x14ac:dyDescent="0.2">
       <c r="Z284" s="3"/>
     </row>
-    <row r="285" spans="2:41">
+    <row r="285" spans="2:41" x14ac:dyDescent="0.2">
       <c r="Z285" s="3"/>
     </row>
-    <row r="286" spans="2:41">
+    <row r="286" spans="2:41" x14ac:dyDescent="0.2">
       <c r="Z286" s="3"/>
     </row>
-    <row r="287" spans="2:41">
+    <row r="287" spans="2:41" x14ac:dyDescent="0.2">
       <c r="Z287" s="3"/>
     </row>
-    <row r="288" spans="2:41">
+    <row r="288" spans="2:41" x14ac:dyDescent="0.2">
       <c r="Z288" s="3"/>
     </row>
-    <row r="289" spans="26:26">
+    <row r="289" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z289" s="3"/>
     </row>
-    <row r="290" spans="26:26">
+    <row r="290" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z290" s="3"/>
     </row>
-    <row r="291" spans="26:26">
+    <row r="291" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z291" s="3"/>
     </row>
-    <row r="292" spans="26:26">
+    <row r="292" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z292" s="3"/>
     </row>
-    <row r="293" spans="26:26">
+    <row r="293" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z293" s="3"/>
     </row>
-    <row r="294" spans="26:26">
+    <row r="294" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z294" s="3"/>
     </row>
-    <row r="295" spans="26:26">
+    <row r="295" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z295" s="3"/>
     </row>
-    <row r="296" spans="26:26">
+    <row r="296" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z296" s="3"/>
     </row>
-    <row r="297" spans="26:26">
+    <row r="297" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z297" s="3"/>
     </row>
-    <row r="298" spans="26:26">
+    <row r="298" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z298" s="3"/>
     </row>
-    <row r="299" spans="26:26">
+    <row r="299" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z299" s="3"/>
     </row>
-    <row r="300" spans="26:26">
+    <row r="300" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z300" s="3"/>
     </row>
-    <row r="301" spans="26:26">
+    <row r="301" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z301" s="3"/>
     </row>
-    <row r="302" spans="26:26">
+    <row r="302" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z302" s="3"/>
     </row>
-    <row r="303" spans="26:26">
+    <row r="303" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z303" s="3"/>
     </row>
-    <row r="304" spans="26:26">
+    <row r="304" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z304" s="3"/>
     </row>
-    <row r="305" spans="26:26">
+    <row r="305" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z305" s="3"/>
     </row>
-    <row r="306" spans="26:26">
+    <row r="306" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z306" s="3"/>
     </row>
-    <row r="307" spans="26:26">
+    <row r="307" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z307" s="3"/>
     </row>
-    <row r="308" spans="26:26">
+    <row r="308" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z308" s="3"/>
     </row>
-    <row r="309" spans="26:26">
+    <row r="309" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z309" s="3"/>
     </row>
-    <row r="310" spans="26:26">
+    <row r="310" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z310" s="3"/>
     </row>
-    <row r="311" spans="26:26">
+    <row r="311" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z311" s="3"/>
     </row>
-    <row r="312" spans="26:26">
+    <row r="312" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z312" s="3"/>
     </row>
-    <row r="313" spans="26:26">
+    <row r="313" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z313" s="3"/>
     </row>
-    <row r="314" spans="26:26">
+    <row r="314" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z314" s="3"/>
     </row>
-    <row r="315" spans="26:26">
+    <row r="315" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z315" s="3"/>
     </row>
-    <row r="316" spans="26:26">
+    <row r="316" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z316" s="3"/>
     </row>
-    <row r="317" spans="26:26">
+    <row r="317" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z317" s="3"/>
     </row>
-    <row r="318" spans="26:26">
+    <row r="318" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z318" s="3"/>
     </row>
-    <row r="319" spans="26:26">
+    <row r="319" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z319" s="3"/>
     </row>
-    <row r="320" spans="26:26">
+    <row r="320" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z320" s="3"/>
     </row>
-    <row r="321" spans="26:26">
+    <row r="321" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z321" s="3"/>
     </row>
-    <row r="322" spans="26:26">
+    <row r="322" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z322" s="3"/>
     </row>
-    <row r="323" spans="26:26">
+    <row r="323" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z323" s="3"/>
     </row>
-    <row r="324" spans="26:26">
+    <row r="324" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z324" s="3"/>
     </row>
-    <row r="325" spans="26:26">
+    <row r="325" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z325" s="3"/>
     </row>
-    <row r="326" spans="26:26">
+    <row r="326" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z326" s="3"/>
     </row>
-    <row r="327" spans="26:26">
+    <row r="327" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z327" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Y = MichIndex1Year - interesting results
</commit_message>
<xml_diff>
--- a/Data/main_file.xlsx
+++ b/Data/main_file.xlsx
@@ -640,7 +640,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="AG6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AO14" sqref="AO14"/>
+      <selection pane="bottomRight" activeCell="AO15" sqref="AO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="15.75"/>
@@ -935,7 +935,7 @@
         <v>5</v>
       </c>
       <c r="AN2" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AO2" s="17">
         <v>2</v>

</xml_diff>

<commit_message>
Adding Gilchrist Spread and FFR
</commit_message>
<xml_diff>
--- a/Data/main_file.xlsx
+++ b/Data/main_file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>MUNI1Y</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Vix</t>
+  </si>
+  <si>
+    <t>GZ_Spread</t>
   </si>
 </sst>
 </file>
@@ -645,13 +648,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS327"/>
+  <dimension ref="A1:AU327"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AD6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AM6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AE7" sqref="AE7"/>
+      <selection pane="bottomRight" activeCell="AT319" sqref="AT319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="15.75"/>
@@ -690,7 +693,7 @@
     <col min="45" max="16384" width="22" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="16" customFormat="1">
+    <row r="1" spans="1:47" s="16" customFormat="1">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -826,8 +829,14 @@
       <c r="AS1" s="16" t="s">
         <v>50</v>
       </c>
+      <c r="AT1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:45" s="16" customFormat="1">
+    <row r="2" spans="1:47" s="16" customFormat="1">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -963,8 +972,14 @@
       <c r="AS2" s="1">
         <v>3</v>
       </c>
+      <c r="AT2" s="16">
+        <v>3</v>
+      </c>
+      <c r="AU2" s="16">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" s="16" customFormat="1">
+    <row r="3" spans="1:47" s="16" customFormat="1">
       <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
@@ -1100,8 +1115,14 @@
       <c r="AS3" s="16">
         <v>1</v>
       </c>
+      <c r="AT3" s="16">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" s="16" customFormat="1">
+    <row r="4" spans="1:47" s="16" customFormat="1">
       <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
@@ -1237,8 +1258,14 @@
       <c r="AS4" s="16">
         <v>44</v>
       </c>
+      <c r="AT4" s="16">
+        <v>45</v>
+      </c>
+      <c r="AU4" s="16">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" s="16" customFormat="1">
+    <row r="5" spans="1:47" s="16" customFormat="1">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -1374,8 +1401,14 @@
       <c r="AS5" s="16">
         <v>44</v>
       </c>
+      <c r="AT5" s="16">
+        <v>45</v>
+      </c>
+      <c r="AU5" s="16">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:47">
       <c r="B6" s="2">
         <v>1950</v>
       </c>
@@ -1438,8 +1471,9 @@
         <v>13.49</v>
       </c>
       <c r="AS6" s="10"/>
+      <c r="AU6" s="10"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:47">
       <c r="B7" s="2">
         <v>1950.25</v>
       </c>
@@ -1502,8 +1536,9 @@
         <v>13.538</v>
       </c>
       <c r="AS7" s="10"/>
+      <c r="AU7" s="10"/>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:47">
       <c r="B8" s="2">
         <v>1950.5</v>
       </c>
@@ -1566,8 +1601,9 @@
         <v>13.832000000000001</v>
       </c>
       <c r="AS8" s="10"/>
+      <c r="AU8" s="10"/>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:47">
       <c r="B9" s="2">
         <v>1950.75</v>
       </c>
@@ -1630,8 +1666,9 @@
         <v>14.09</v>
       </c>
       <c r="AS9" s="10"/>
+      <c r="AU9" s="10"/>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:47">
       <c r="B10" s="2">
         <v>1951</v>
       </c>
@@ -1694,8 +1731,9 @@
         <v>14.596</v>
       </c>
       <c r="AS10" s="10"/>
+      <c r="AU10" s="10"/>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:47">
       <c r="B11" s="2">
         <v>1951.25</v>
       </c>
@@ -1758,8 +1796,9 @@
         <v>14.692</v>
       </c>
       <c r="AS11" s="10"/>
+      <c r="AU11" s="10"/>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:47">
       <c r="B12" s="2">
         <v>1951.5</v>
       </c>
@@ -1822,8 +1861,9 @@
         <v>14.701000000000001</v>
       </c>
       <c r="AS12" s="10"/>
+      <c r="AU12" s="10"/>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:47">
       <c r="B13" s="2">
         <v>1951.75</v>
       </c>
@@ -1886,8 +1926,9 @@
         <v>14.869</v>
       </c>
       <c r="AS13" s="10"/>
+      <c r="AU13" s="10"/>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:47">
       <c r="B14" s="2">
         <v>1952</v>
       </c>
@@ -1950,8 +1991,9 @@
         <v>14.863</v>
       </c>
       <c r="AS14" s="10"/>
+      <c r="AU14" s="10"/>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:47">
       <c r="B15" s="2">
         <v>1952.25</v>
       </c>
@@ -2014,8 +2056,9 @@
         <v>14.882</v>
       </c>
       <c r="AS15" s="10"/>
+      <c r="AU15" s="10"/>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:47">
       <c r="B16" s="2">
         <v>1952.5</v>
       </c>
@@ -2078,8 +2121,9 @@
         <v>15.048</v>
       </c>
       <c r="AS16" s="10"/>
+      <c r="AU16" s="10"/>
     </row>
-    <row r="17" spans="2:45">
+    <row r="17" spans="2:47">
       <c r="B17" s="2">
         <v>1952.75</v>
       </c>
@@ -2142,8 +2186,9 @@
         <v>15.090999999999999</v>
       </c>
       <c r="AS17" s="10"/>
+      <c r="AU17" s="10"/>
     </row>
-    <row r="18" spans="2:45">
+    <row r="18" spans="2:47">
       <c r="B18" s="2">
         <v>1953</v>
       </c>
@@ -2209,8 +2254,9 @@
         <v>15.096</v>
       </c>
       <c r="AS18" s="10"/>
+      <c r="AU18" s="10"/>
     </row>
-    <row r="19" spans="2:45">
+    <row r="19" spans="2:47">
       <c r="B19" s="2">
         <v>1953.25</v>
       </c>
@@ -2276,8 +2322,9 @@
         <v>15.125</v>
       </c>
       <c r="AS19" s="10"/>
+      <c r="AU19" s="10"/>
     </row>
-    <row r="20" spans="2:45">
+    <row r="20" spans="2:47">
       <c r="B20" s="2">
         <v>1953.5</v>
       </c>
@@ -2343,8 +2390,9 @@
         <v>15.188000000000001</v>
       </c>
       <c r="AS20" s="10"/>
+      <c r="AU20" s="10"/>
     </row>
-    <row r="21" spans="2:45">
+    <row r="21" spans="2:47">
       <c r="B21" s="2">
         <v>1953.75</v>
       </c>
@@ -2410,8 +2458,9 @@
         <v>15.218999999999999</v>
       </c>
       <c r="AS21" s="10"/>
+      <c r="AU21" s="10"/>
     </row>
-    <row r="22" spans="2:45">
+    <row r="22" spans="2:47">
       <c r="B22" s="2">
         <v>1954</v>
       </c>
@@ -2477,8 +2526,9 @@
         <v>15.266</v>
       </c>
       <c r="AS22" s="10"/>
+      <c r="AU22" s="10"/>
     </row>
-    <row r="23" spans="2:45">
+    <row r="23" spans="2:47">
       <c r="B23" s="2">
         <v>1954.25</v>
       </c>
@@ -2544,8 +2594,9 @@
         <v>15.281000000000001</v>
       </c>
       <c r="AS23" s="10"/>
+      <c r="AU23" s="10"/>
     </row>
-    <row r="24" spans="2:45">
+    <row r="24" spans="2:47">
       <c r="B24" s="2">
         <v>1954.5</v>
       </c>
@@ -2614,8 +2665,11 @@
         <v>15.3</v>
       </c>
       <c r="AS24" s="10"/>
+      <c r="AU24" s="10">
+        <v>1.06</v>
+      </c>
     </row>
-    <row r="25" spans="2:45">
+    <row r="25" spans="2:47">
       <c r="B25" s="2">
         <v>1954.75</v>
       </c>
@@ -2684,8 +2738,11 @@
         <v>15.343</v>
       </c>
       <c r="AS25" s="10"/>
+      <c r="AU25" s="10">
+        <v>1.28</v>
+      </c>
     </row>
-    <row r="26" spans="2:45">
+    <row r="26" spans="2:47">
       <c r="B26" s="2">
         <v>1955</v>
       </c>
@@ -2754,8 +2811,11 @@
         <v>15.417</v>
       </c>
       <c r="AS26" s="10"/>
+      <c r="AU26" s="10">
+        <v>1.35</v>
+      </c>
     </row>
-    <row r="27" spans="2:45">
+    <row r="27" spans="2:47">
       <c r="B27" s="2">
         <v>1955.25</v>
       </c>
@@ -2824,8 +2884,11 @@
         <v>15.481</v>
       </c>
       <c r="AS27" s="10"/>
+      <c r="AU27" s="10">
+        <v>1.64</v>
+      </c>
     </row>
-    <row r="28" spans="2:45">
+    <row r="28" spans="2:47">
       <c r="B28" s="2">
         <v>1955.5</v>
       </c>
@@ -2894,8 +2957,11 @@
         <v>15.59</v>
       </c>
       <c r="AS28" s="10"/>
+      <c r="AU28" s="10">
+        <v>2.1800000000000002</v>
+      </c>
     </row>
-    <row r="29" spans="2:45">
+    <row r="29" spans="2:47">
       <c r="B29" s="2">
         <v>1955.75</v>
       </c>
@@ -2964,8 +3030,11 @@
         <v>15.743</v>
       </c>
       <c r="AS29" s="10"/>
+      <c r="AU29" s="10">
+        <v>2.48</v>
+      </c>
     </row>
-    <row r="30" spans="2:45">
+    <row r="30" spans="2:47">
       <c r="B30" s="2">
         <v>1956</v>
       </c>
@@ -3034,8 +3103,11 @@
         <v>15.901999999999999</v>
       </c>
       <c r="AS30" s="10"/>
+      <c r="AU30" s="10">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="31" spans="2:45">
+    <row r="31" spans="2:47">
       <c r="B31" s="2">
         <v>1956.25</v>
       </c>
@@ -3104,8 +3176,11 @@
         <v>15.997</v>
       </c>
       <c r="AS31" s="10"/>
+      <c r="AU31" s="10">
+        <v>2.71</v>
+      </c>
     </row>
-    <row r="32" spans="2:45">
+    <row r="32" spans="2:47">
       <c r="B32" s="2">
         <v>1956.5</v>
       </c>
@@ -3174,8 +3249,11 @@
         <v>16.196999999999999</v>
       </c>
       <c r="AS32" s="10"/>
+      <c r="AU32" s="10">
+        <v>2.95</v>
+      </c>
     </row>
-    <row r="33" spans="2:45">
+    <row r="33" spans="2:47">
       <c r="B33" s="2">
         <v>1956.75</v>
       </c>
@@ -3244,8 +3322,11 @@
         <v>16.263999999999999</v>
       </c>
       <c r="AS33" s="10"/>
+      <c r="AU33" s="10">
+        <v>2.94</v>
+      </c>
     </row>
-    <row r="34" spans="2:45">
+    <row r="34" spans="2:47">
       <c r="B34" s="2">
         <v>1957</v>
       </c>
@@ -3314,8 +3395,11 @@
         <v>16.484999999999999</v>
       </c>
       <c r="AS34" s="10"/>
+      <c r="AU34" s="10">
+        <v>2.96</v>
+      </c>
     </row>
-    <row r="35" spans="2:45">
+    <row r="35" spans="2:47">
       <c r="B35" s="2">
         <v>1957.25</v>
       </c>
@@ -3384,8 +3468,11 @@
         <v>16.600999999999999</v>
       </c>
       <c r="AS35" s="10"/>
+      <c r="AU35" s="10">
+        <v>3</v>
+      </c>
     </row>
-    <row r="36" spans="2:45">
+    <row r="36" spans="2:47">
       <c r="B36" s="2">
         <v>1957.5</v>
       </c>
@@ -3454,8 +3541,11 @@
         <v>16.701000000000001</v>
       </c>
       <c r="AS36" s="10"/>
+      <c r="AU36" s="10">
+        <v>3.47</v>
+      </c>
     </row>
-    <row r="37" spans="2:45">
+    <row r="37" spans="2:47">
       <c r="B37" s="2">
         <v>1957.75</v>
       </c>
@@ -3524,8 +3614,11 @@
         <v>16.710999999999999</v>
       </c>
       <c r="AS37" s="10"/>
+      <c r="AU37" s="10">
+        <v>2.98</v>
+      </c>
     </row>
-    <row r="38" spans="2:45">
+    <row r="38" spans="2:47">
       <c r="B38" s="2">
         <v>1958</v>
       </c>
@@ -3594,8 +3687,11 @@
         <v>16.891999999999999</v>
       </c>
       <c r="AS38" s="10"/>
+      <c r="AU38" s="10">
+        <v>1.2</v>
+      </c>
     </row>
-    <row r="39" spans="2:45">
+    <row r="39" spans="2:47">
       <c r="B39" s="2">
         <v>1958.25</v>
       </c>
@@ -3664,8 +3760,11 @@
         <v>16.940000000000001</v>
       </c>
       <c r="AS39" s="10"/>
+      <c r="AU39" s="10">
+        <v>0.93</v>
+      </c>
     </row>
-    <row r="40" spans="2:45">
+    <row r="40" spans="2:47">
       <c r="B40" s="2">
         <v>1958.5</v>
       </c>
@@ -3734,8 +3833,11 @@
         <v>17.042999999999999</v>
       </c>
       <c r="AS40" s="10"/>
+      <c r="AU40" s="10">
+        <v>1.76</v>
+      </c>
     </row>
-    <row r="41" spans="2:45">
+    <row r="41" spans="2:47">
       <c r="B41" s="2">
         <v>1958.75</v>
       </c>
@@ -3804,8 +3906,11 @@
         <v>17.123000000000001</v>
       </c>
       <c r="AS41" s="10"/>
+      <c r="AU41" s="10">
+        <v>2.42</v>
+      </c>
     </row>
-    <row r="42" spans="2:45">
+    <row r="42" spans="2:47">
       <c r="B42" s="2">
         <v>1959</v>
       </c>
@@ -3874,8 +3979,11 @@
         <v>17.169</v>
       </c>
       <c r="AS42" s="10"/>
+      <c r="AU42" s="10">
+        <v>2.8</v>
+      </c>
     </row>
-    <row r="43" spans="2:45">
+    <row r="43" spans="2:47">
       <c r="B43" s="2">
         <v>1959.25</v>
       </c>
@@ -3944,8 +4052,11 @@
         <v>17.193999999999999</v>
       </c>
       <c r="AS43" s="10"/>
+      <c r="AU43" s="10">
+        <v>3.39</v>
+      </c>
     </row>
-    <row r="44" spans="2:45">
+    <row r="44" spans="2:47">
       <c r="B44" s="2">
         <v>1959.5</v>
       </c>
@@ -4014,8 +4125,11 @@
         <v>17.257999999999999</v>
       </c>
       <c r="AS44" s="10"/>
+      <c r="AU44" s="10">
+        <v>3.76</v>
+      </c>
     </row>
-    <row r="45" spans="2:45">
+    <row r="45" spans="2:47">
       <c r="B45" s="2">
         <v>1959.75</v>
       </c>
@@ -4084,8 +4198,11 @@
         <v>17.326000000000001</v>
       </c>
       <c r="AS45" s="10"/>
+      <c r="AU45" s="10">
+        <v>3.99</v>
+      </c>
     </row>
-    <row r="46" spans="2:45">
+    <row r="46" spans="2:47">
       <c r="B46" s="2">
         <v>1960</v>
       </c>
@@ -4157,8 +4274,11 @@
         <v>17.396999999999998</v>
       </c>
       <c r="AS46" s="10"/>
+      <c r="AU46" s="10">
+        <v>3.84</v>
+      </c>
     </row>
-    <row r="47" spans="2:45">
+    <row r="47" spans="2:47">
       <c r="B47" s="2">
         <v>1960.25</v>
       </c>
@@ -4230,8 +4350,11 @@
         <v>17.443000000000001</v>
       </c>
       <c r="AS47" s="10"/>
+      <c r="AU47" s="10">
+        <v>3.32</v>
+      </c>
     </row>
-    <row r="48" spans="2:45">
+    <row r="48" spans="2:47">
       <c r="B48" s="2">
         <v>1960.5</v>
       </c>
@@ -4303,8 +4426,11 @@
         <v>17.506</v>
       </c>
       <c r="AS48" s="10"/>
+      <c r="AU48" s="10">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="49" spans="2:45">
+    <row r="49" spans="2:47">
       <c r="B49" s="2">
         <v>1960.75</v>
       </c>
@@ -4376,8 +4502,11 @@
         <v>17.559999999999999</v>
       </c>
       <c r="AS49" s="10"/>
+      <c r="AU49" s="10">
+        <v>1.98</v>
+      </c>
     </row>
-    <row r="50" spans="2:45">
+    <row r="50" spans="2:47">
       <c r="B50" s="2">
         <v>1961</v>
       </c>
@@ -4449,8 +4578,11 @@
         <v>17.597999999999999</v>
       </c>
       <c r="AS50" s="10"/>
+      <c r="AU50" s="10">
+        <v>2.02</v>
+      </c>
     </row>
-    <row r="51" spans="2:45">
+    <row r="51" spans="2:47">
       <c r="B51" s="2">
         <v>1961.25</v>
       </c>
@@ -4522,8 +4654,11 @@
         <v>17.640999999999998</v>
       </c>
       <c r="AS51" s="10"/>
+      <c r="AU51" s="10">
+        <v>1.73</v>
+      </c>
     </row>
-    <row r="52" spans="2:45">
+    <row r="52" spans="2:47">
       <c r="B52" s="2">
         <v>1961.5</v>
       </c>
@@ -4595,8 +4730,11 @@
         <v>17.687000000000001</v>
       </c>
       <c r="AS52" s="10"/>
+      <c r="AU52" s="10">
+        <v>1.88</v>
+      </c>
     </row>
-    <row r="53" spans="2:45">
+    <row r="53" spans="2:47">
       <c r="B53" s="2">
         <v>1961.75</v>
       </c>
@@ -4668,8 +4806,11 @@
         <v>17.745000000000001</v>
       </c>
       <c r="AS53" s="10"/>
+      <c r="AU53" s="10">
+        <v>2.33</v>
+      </c>
     </row>
-    <row r="54" spans="2:45">
+    <row r="54" spans="2:47">
       <c r="B54" s="2">
         <v>1962</v>
       </c>
@@ -4741,8 +4882,11 @@
         <v>17.837</v>
       </c>
       <c r="AS54" s="10"/>
+      <c r="AU54" s="10">
+        <v>2.85</v>
+      </c>
     </row>
-    <row r="55" spans="2:45">
+    <row r="55" spans="2:47">
       <c r="B55" s="2">
         <v>1962.25</v>
       </c>
@@ -4814,8 +4958,11 @@
         <v>17.866</v>
       </c>
       <c r="AS55" s="10"/>
+      <c r="AU55" s="10">
+        <v>2.68</v>
+      </c>
     </row>
-    <row r="56" spans="2:45">
+    <row r="56" spans="2:47">
       <c r="B56" s="2">
         <v>1962.5</v>
       </c>
@@ -4887,8 +5034,11 @@
         <v>17.902999999999999</v>
       </c>
       <c r="AS56" s="10"/>
+      <c r="AU56" s="10">
+        <v>2.9</v>
+      </c>
     </row>
-    <row r="57" spans="2:45">
+    <row r="57" spans="2:47">
       <c r="B57" s="2">
         <v>1962.75</v>
       </c>
@@ -4960,8 +5110,11 @@
         <v>17.937999999999999</v>
       </c>
       <c r="AS57" s="10"/>
+      <c r="AU57" s="10">
+        <v>2.93</v>
+      </c>
     </row>
-    <row r="58" spans="2:45">
+    <row r="58" spans="2:47">
       <c r="B58" s="2">
         <v>1963</v>
       </c>
@@ -5033,8 +5186,11 @@
         <v>18.016999999999999</v>
       </c>
       <c r="AS58" s="10"/>
+      <c r="AU58" s="10">
+        <v>2.98</v>
+      </c>
     </row>
-    <row r="59" spans="2:45">
+    <row r="59" spans="2:47">
       <c r="B59" s="2">
         <v>1963.25</v>
       </c>
@@ -5106,8 +5262,11 @@
         <v>18.047000000000001</v>
       </c>
       <c r="AS59" s="10"/>
+      <c r="AU59" s="10">
+        <v>2.99</v>
+      </c>
     </row>
-    <row r="60" spans="2:45">
+    <row r="60" spans="2:47">
       <c r="B60" s="2">
         <v>1963.5</v>
       </c>
@@ -5179,8 +5338,11 @@
         <v>18.068999999999999</v>
       </c>
       <c r="AS60" s="10"/>
+      <c r="AU60" s="10">
+        <v>3.48</v>
+      </c>
     </row>
-    <row r="61" spans="2:45">
+    <row r="61" spans="2:47">
       <c r="B61" s="2">
         <v>1963.75</v>
       </c>
@@ -5252,8 +5414,11 @@
         <v>18.216000000000001</v>
       </c>
       <c r="AS61" s="10"/>
+      <c r="AU61" s="10">
+        <v>3.38</v>
+      </c>
     </row>
-    <row r="62" spans="2:45">
+    <row r="62" spans="2:47">
       <c r="B62" s="2">
         <v>1964</v>
       </c>
@@ -5325,8 +5490,11 @@
         <v>18.274000000000001</v>
       </c>
       <c r="AS62" s="10"/>
+      <c r="AU62" s="10">
+        <v>3.43</v>
+      </c>
     </row>
-    <row r="63" spans="2:45">
+    <row r="63" spans="2:47">
       <c r="B63" s="2">
         <v>1964.25</v>
       </c>
@@ -5398,8 +5566,11 @@
         <v>18.318000000000001</v>
       </c>
       <c r="AS63" s="10"/>
+      <c r="AU63" s="10">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="64" spans="2:45">
+    <row r="64" spans="2:47">
       <c r="B64" s="2">
         <v>1964.5</v>
       </c>
@@ -5471,8 +5642,11 @@
         <v>18.391999999999999</v>
       </c>
       <c r="AS64" s="10"/>
+      <c r="AU64" s="10">
+        <v>3.45</v>
+      </c>
     </row>
-    <row r="65" spans="2:45">
+    <row r="65" spans="2:47">
       <c r="B65" s="2">
         <v>1964.75</v>
       </c>
@@ -5544,8 +5718,11 @@
         <v>18.475999999999999</v>
       </c>
       <c r="AS65" s="10"/>
+      <c r="AU65" s="10">
+        <v>3.85</v>
+      </c>
     </row>
-    <row r="66" spans="2:45">
+    <row r="66" spans="2:47">
       <c r="B66" s="2">
         <v>1965</v>
       </c>
@@ -5617,8 +5794,11 @@
         <v>18.568999999999999</v>
       </c>
       <c r="AS66" s="10"/>
+      <c r="AU66" s="10">
+        <v>4.04</v>
+      </c>
     </row>
-    <row r="67" spans="2:45">
+    <row r="67" spans="2:47">
       <c r="B67" s="2">
         <v>1965.25</v>
       </c>
@@ -5690,8 +5870,11 @@
         <v>18.652000000000001</v>
       </c>
       <c r="AS67" s="10"/>
+      <c r="AU67" s="10">
+        <v>4.04</v>
+      </c>
     </row>
-    <row r="68" spans="2:45">
+    <row r="68" spans="2:47">
       <c r="B68" s="2">
         <v>1965.5</v>
       </c>
@@ -5763,8 +5946,11 @@
         <v>18.725999999999999</v>
       </c>
       <c r="AS68" s="10"/>
+      <c r="AU68" s="10">
+        <v>4.01</v>
+      </c>
     </row>
-    <row r="69" spans="2:45">
+    <row r="69" spans="2:47">
       <c r="B69" s="2">
         <v>1965.75</v>
       </c>
@@ -5836,8 +6022,11 @@
         <v>18.853000000000002</v>
       </c>
       <c r="AS69" s="10"/>
+      <c r="AU69" s="10">
+        <v>4.32</v>
+      </c>
     </row>
-    <row r="70" spans="2:45">
+    <row r="70" spans="2:47">
       <c r="B70" s="2">
         <v>1966</v>
       </c>
@@ -5909,8 +6098,11 @@
         <v>18.975000000000001</v>
       </c>
       <c r="AS70" s="10"/>
+      <c r="AU70" s="10">
+        <v>4.6500000000000004</v>
+      </c>
     </row>
-    <row r="71" spans="2:45">
+    <row r="71" spans="2:47">
       <c r="B71" s="2">
         <v>1966.25</v>
       </c>
@@ -5982,8 +6174,11 @@
         <v>19.131</v>
       </c>
       <c r="AS71" s="10"/>
+      <c r="AU71" s="10">
+        <v>5.17</v>
+      </c>
     </row>
-    <row r="72" spans="2:45">
+    <row r="72" spans="2:47">
       <c r="B72" s="2">
         <v>1966.5</v>
       </c>
@@ -6055,8 +6250,11 @@
         <v>19.317</v>
       </c>
       <c r="AS72" s="10"/>
+      <c r="AU72" s="10">
+        <v>5.4</v>
+      </c>
     </row>
-    <row r="73" spans="2:45">
+    <row r="73" spans="2:47">
       <c r="B73" s="2">
         <v>1966.75</v>
       </c>
@@ -6128,8 +6326,11 @@
         <v>19.481000000000002</v>
       </c>
       <c r="AS73" s="10"/>
+      <c r="AU73" s="10">
+        <v>5.4</v>
+      </c>
     </row>
-    <row r="74" spans="2:45">
+    <row r="74" spans="2:47">
       <c r="B74" s="2">
         <v>1967</v>
       </c>
@@ -6201,8 +6402,11 @@
         <v>19.562000000000001</v>
       </c>
       <c r="AS74" s="10"/>
+      <c r="AU74" s="10">
+        <v>4.53</v>
+      </c>
     </row>
-    <row r="75" spans="2:45">
+    <row r="75" spans="2:47">
       <c r="B75" s="2">
         <v>1967.25</v>
       </c>
@@ -6274,8 +6478,11 @@
         <v>19.661000000000001</v>
       </c>
       <c r="AS75" s="10"/>
+      <c r="AU75" s="10">
+        <v>3.98</v>
+      </c>
     </row>
-    <row r="76" spans="2:45">
+    <row r="76" spans="2:47">
       <c r="B76" s="2">
         <v>1967.5</v>
       </c>
@@ -6348,8 +6555,11 @@
         <v>19.849</v>
       </c>
       <c r="AS76" s="10"/>
+      <c r="AU76" s="10">
+        <v>3.99</v>
+      </c>
     </row>
-    <row r="77" spans="2:45">
+    <row r="77" spans="2:47">
       <c r="B77" s="2">
         <v>1967.75</v>
       </c>
@@ -6422,8 +6632,11 @@
         <v>20.067</v>
       </c>
       <c r="AS77" s="10"/>
+      <c r="AU77" s="10">
+        <v>4.51</v>
+      </c>
     </row>
-    <row r="78" spans="2:45">
+    <row r="78" spans="2:47">
       <c r="B78" s="2">
         <v>1968</v>
       </c>
@@ -6496,8 +6709,11 @@
         <v>20.29</v>
       </c>
       <c r="AS78" s="10"/>
+      <c r="AU78" s="10">
+        <v>5.05</v>
+      </c>
     </row>
-    <row r="79" spans="2:45">
+    <row r="79" spans="2:47">
       <c r="B79" s="2">
         <v>1968.25</v>
       </c>
@@ -6570,8 +6786,11 @@
         <v>20.504000000000001</v>
       </c>
       <c r="AS79" s="10"/>
+      <c r="AU79" s="10">
+        <v>6.07</v>
+      </c>
     </row>
-    <row r="80" spans="2:45">
+    <row r="80" spans="2:47">
       <c r="B80" s="2">
         <v>1968.5</v>
       </c>
@@ -6644,8 +6863,11 @@
         <v>20.706</v>
       </c>
       <c r="AS80" s="10"/>
+      <c r="AU80" s="10">
+        <v>5.78</v>
+      </c>
     </row>
-    <row r="81" spans="2:45">
+    <row r="81" spans="2:47">
       <c r="B81" s="2">
         <v>1968.75</v>
       </c>
@@ -6754,8 +6976,11 @@
         <v>20.998999999999999</v>
       </c>
       <c r="AS81" s="10"/>
+      <c r="AU81" s="10">
+        <v>6.02</v>
+      </c>
     </row>
-    <row r="82" spans="2:45">
+    <row r="82" spans="2:47">
       <c r="B82" s="2">
         <v>1969</v>
       </c>
@@ -6868,8 +7093,11 @@
         <v>21.216999999999999</v>
       </c>
       <c r="AS82" s="10"/>
+      <c r="AU82" s="10">
+        <v>6.79</v>
+      </c>
     </row>
-    <row r="83" spans="2:45">
+    <row r="83" spans="2:47">
       <c r="B83" s="2">
         <v>1969.25</v>
       </c>
@@ -6982,8 +7210,11 @@
         <v>21.488</v>
       </c>
       <c r="AS83" s="10"/>
+      <c r="AU83" s="10">
+        <v>8.9</v>
+      </c>
     </row>
-    <row r="84" spans="2:45">
+    <row r="84" spans="2:47">
       <c r="B84" s="2">
         <v>1969.5</v>
       </c>
@@ -7096,8 +7327,11 @@
         <v>21.79</v>
       </c>
       <c r="AS84" s="10"/>
+      <c r="AU84" s="10">
+        <v>9.15</v>
+      </c>
     </row>
-    <row r="85" spans="2:45">
+    <row r="85" spans="2:47">
       <c r="B85" s="2">
         <v>1969.75</v>
       </c>
@@ -7209,8 +7443,11 @@
         <v>22.071000000000002</v>
       </c>
       <c r="AS85" s="10"/>
+      <c r="AU85" s="10">
+        <v>8.9700000000000006</v>
+      </c>
     </row>
-    <row r="86" spans="2:45">
+    <row r="86" spans="2:47">
       <c r="B86" s="2">
         <v>1970</v>
       </c>
@@ -7324,8 +7561,11 @@
         <v>22.382000000000001</v>
       </c>
       <c r="AS86" s="10"/>
+      <c r="AU86" s="10">
+        <v>7.76</v>
+      </c>
     </row>
-    <row r="87" spans="2:45">
+    <row r="87" spans="2:47">
       <c r="B87" s="2">
         <v>1970.25</v>
       </c>
@@ -7437,8 +7677,11 @@
         <v>22.693999999999999</v>
       </c>
       <c r="AS87" s="10"/>
+      <c r="AU87" s="10">
+        <v>7.6</v>
+      </c>
     </row>
-    <row r="88" spans="2:45">
+    <row r="88" spans="2:47">
       <c r="B88" s="2">
         <v>1970.5</v>
       </c>
@@ -7550,8 +7793,11 @@
         <v>22.88</v>
       </c>
       <c r="AS88" s="10"/>
+      <c r="AU88" s="10">
+        <v>6.29</v>
+      </c>
     </row>
-    <row r="89" spans="2:45">
+    <row r="89" spans="2:47">
       <c r="B89" s="2">
         <v>1970.75</v>
       </c>
@@ -7663,8 +7909,11 @@
         <v>23.181999999999999</v>
       </c>
       <c r="AS89" s="10"/>
+      <c r="AU89" s="10">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="90" spans="2:45">
+    <row r="90" spans="2:47">
       <c r="B90" s="2">
         <v>1971</v>
       </c>
@@ -7776,8 +8025,11 @@
         <v>23.536000000000001</v>
       </c>
       <c r="AS90" s="10"/>
+      <c r="AU90" s="10">
+        <v>3.71</v>
+      </c>
     </row>
-    <row r="91" spans="2:45">
+    <row r="91" spans="2:47">
       <c r="B91" s="2">
         <v>1971.25</v>
       </c>
@@ -7889,8 +8141,11 @@
         <v>23.846</v>
       </c>
       <c r="AS91" s="10"/>
+      <c r="AU91" s="10">
+        <v>4.91</v>
+      </c>
     </row>
-    <row r="92" spans="2:45">
+    <row r="92" spans="2:47">
       <c r="B92" s="2">
         <v>1971.5</v>
       </c>
@@ -8002,8 +8257,11 @@
         <v>24.088000000000001</v>
       </c>
       <c r="AS92" s="10"/>
+      <c r="AU92" s="10">
+        <v>5.55</v>
+      </c>
     </row>
-    <row r="93" spans="2:45">
+    <row r="93" spans="2:47">
       <c r="B93" s="2">
         <v>1971.75</v>
       </c>
@@ -8115,8 +8373,11 @@
         <v>24.288</v>
       </c>
       <c r="AS93" s="10"/>
+      <c r="AU93" s="10">
+        <v>4.1399999999999997</v>
+      </c>
     </row>
-    <row r="94" spans="2:45">
+    <row r="94" spans="2:47">
       <c r="B94" s="2">
         <v>1972</v>
       </c>
@@ -8228,8 +8489,11 @@
         <v>24.664000000000001</v>
       </c>
       <c r="AS94" s="10"/>
+      <c r="AU94" s="10">
+        <v>3.83</v>
+      </c>
     </row>
-    <row r="95" spans="2:45">
+    <row r="95" spans="2:47">
       <c r="B95" s="2">
         <v>1972.25</v>
       </c>
@@ -8341,8 +8605,11 @@
         <v>24.815000000000001</v>
       </c>
       <c r="AS95" s="10"/>
+      <c r="AU95" s="10">
+        <v>4.46</v>
+      </c>
     </row>
-    <row r="96" spans="2:45">
+    <row r="96" spans="2:47">
       <c r="B96" s="2">
         <v>1972.5</v>
       </c>
@@ -8454,8 +8721,11 @@
         <v>25.047999999999998</v>
       </c>
       <c r="AS96" s="10"/>
+      <c r="AU96" s="10">
+        <v>4.87</v>
+      </c>
     </row>
-    <row r="97" spans="2:45">
+    <row r="97" spans="2:47">
       <c r="B97" s="2">
         <v>1972.75</v>
       </c>
@@ -8567,8 +8837,11 @@
         <v>25.366</v>
       </c>
       <c r="AS97" s="10"/>
+      <c r="AU97" s="10">
+        <v>5.33</v>
+      </c>
     </row>
-    <row r="98" spans="2:45">
+    <row r="98" spans="2:47">
       <c r="B98" s="2">
         <v>1973</v>
       </c>
@@ -8680,8 +8953,14 @@
         <v>25.661000000000001</v>
       </c>
       <c r="AS98" s="10"/>
+      <c r="AT98" s="3">
+        <v>1.026</v>
+      </c>
+      <c r="AU98" s="10">
+        <v>7.09</v>
+      </c>
     </row>
-    <row r="99" spans="2:45">
+    <row r="99" spans="2:47">
       <c r="B99" s="2">
         <v>1973.25</v>
       </c>
@@ -8793,8 +9072,14 @@
         <v>26.052</v>
       </c>
       <c r="AS99" s="10"/>
+      <c r="AT99" s="3">
+        <v>1.0113000000000001</v>
+      </c>
+      <c r="AU99" s="10">
+        <v>8.49</v>
+      </c>
     </row>
-    <row r="100" spans="2:45">
+    <row r="100" spans="2:47">
       <c r="B100" s="2">
         <v>1973.5</v>
       </c>
@@ -8906,8 +9191,14 @@
         <v>26.548999999999999</v>
       </c>
       <c r="AS100" s="10"/>
+      <c r="AT100" s="3">
+        <v>0.97560000000000002</v>
+      </c>
+      <c r="AU100" s="10">
+        <v>10.78</v>
+      </c>
     </row>
-    <row r="101" spans="2:45">
+    <row r="101" spans="2:47">
       <c r="B101" s="2">
         <v>1973.75</v>
       </c>
@@ -9019,8 +9310,14 @@
         <v>27.077000000000002</v>
       </c>
       <c r="AS101" s="10"/>
+      <c r="AT101" s="3">
+        <v>1.2197</v>
+      </c>
+      <c r="AU101" s="10">
+        <v>9.9499999999999993</v>
+      </c>
     </row>
-    <row r="102" spans="2:45">
+    <row r="102" spans="2:47">
       <c r="B102" s="2">
         <v>1974</v>
       </c>
@@ -9132,8 +9429,14 @@
         <v>27.591999999999999</v>
       </c>
       <c r="AS102" s="10"/>
+      <c r="AT102" s="3">
+        <v>1.1686000000000001</v>
+      </c>
+      <c r="AU102" s="10">
+        <v>9.35</v>
+      </c>
     </row>
-    <row r="103" spans="2:45">
+    <row r="103" spans="2:47">
       <c r="B103" s="2">
         <v>1974.25</v>
       </c>
@@ -9245,8 +9548,14 @@
         <v>28.248000000000001</v>
       </c>
       <c r="AS103" s="10"/>
+      <c r="AT103" s="3">
+        <v>1.6315</v>
+      </c>
+      <c r="AU103" s="10">
+        <v>11.93</v>
+      </c>
     </row>
-    <row r="104" spans="2:45">
+    <row r="104" spans="2:47">
       <c r="B104" s="2">
         <v>1974.5</v>
       </c>
@@ -9360,8 +9669,14 @@
         <v>29.067</v>
       </c>
       <c r="AS104" s="10"/>
+      <c r="AT104" s="3">
+        <v>2.1772</v>
+      </c>
+      <c r="AU104" s="10">
+        <v>11.34</v>
+      </c>
     </row>
-    <row r="105" spans="2:45">
+    <row r="105" spans="2:47">
       <c r="B105" s="2">
         <v>1974.75</v>
       </c>
@@ -9473,8 +9788,14 @@
         <v>29.922999999999998</v>
       </c>
       <c r="AS105" s="10"/>
+      <c r="AT105" s="3">
+        <v>2.1158999999999999</v>
+      </c>
+      <c r="AU105" s="10">
+        <v>8.5299999999999994</v>
+      </c>
     </row>
-    <row r="106" spans="2:45">
+    <row r="106" spans="2:47">
       <c r="B106" s="2">
         <v>1975</v>
       </c>
@@ -9586,8 +9907,14 @@
         <v>30.600999999999999</v>
       </c>
       <c r="AS106" s="10"/>
+      <c r="AT106" s="3">
+        <v>1.5933999999999999</v>
+      </c>
+      <c r="AU106" s="10">
+        <v>5.54</v>
+      </c>
     </row>
-    <row r="107" spans="2:45">
+    <row r="107" spans="2:47">
       <c r="B107" s="2">
         <v>1975.25</v>
       </c>
@@ -9699,8 +10026,14 @@
         <v>31.059000000000001</v>
       </c>
       <c r="AS107" s="10"/>
+      <c r="AT107" s="3">
+        <v>1.4368000000000001</v>
+      </c>
+      <c r="AU107" s="10">
+        <v>5.55</v>
+      </c>
     </row>
-    <row r="108" spans="2:45">
+    <row r="108" spans="2:47">
       <c r="B108" s="2">
         <v>1975.5</v>
       </c>
@@ -9812,8 +10145,14 @@
         <v>31.611999999999998</v>
       </c>
       <c r="AS108" s="10"/>
+      <c r="AT108" s="3">
+        <v>1.3525</v>
+      </c>
+      <c r="AU108" s="10">
+        <v>6.24</v>
+      </c>
     </row>
-    <row r="109" spans="2:45">
+    <row r="109" spans="2:47">
       <c r="B109" s="2">
         <v>1975.75</v>
       </c>
@@ -9925,8 +10264,14 @@
         <v>32.139000000000003</v>
       </c>
       <c r="AS109" s="10"/>
+      <c r="AT109" s="3">
+        <v>1.1652</v>
+      </c>
+      <c r="AU109" s="10">
+        <v>5.2</v>
+      </c>
     </row>
-    <row r="110" spans="2:45">
+    <row r="110" spans="2:47">
       <c r="B110" s="2">
         <v>1976</v>
       </c>
@@ -10038,8 +10383,14 @@
         <v>32.472999999999999</v>
       </c>
       <c r="AS110" s="10"/>
+      <c r="AT110" s="3">
+        <v>1.0137</v>
+      </c>
+      <c r="AU110" s="10">
+        <v>4.84</v>
+      </c>
     </row>
-    <row r="111" spans="2:45">
+    <row r="111" spans="2:47">
       <c r="B111" s="2">
         <v>1976.25</v>
       </c>
@@ -10151,8 +10502,14 @@
         <v>32.802999999999997</v>
       </c>
       <c r="AS111" s="10"/>
+      <c r="AT111" s="3">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="AU111" s="10">
+        <v>5.48</v>
+      </c>
     </row>
-    <row r="112" spans="2:45">
+    <row r="112" spans="2:47">
       <c r="B112" s="2">
         <v>1976.5</v>
       </c>
@@ -10264,8 +10621,14 @@
         <v>33.225999999999999</v>
       </c>
       <c r="AS112" s="10"/>
+      <c r="AT112" s="3">
+        <v>0.89380000000000004</v>
+      </c>
+      <c r="AU112" s="10">
+        <v>5.25</v>
+      </c>
     </row>
-    <row r="113" spans="2:45">
+    <row r="113" spans="2:47">
       <c r="B113" s="2">
         <v>1976.75</v>
       </c>
@@ -10377,8 +10740,14 @@
         <v>33.814999999999998</v>
       </c>
       <c r="AS113" s="10"/>
+      <c r="AT113" s="3">
+        <v>0.95240000000000002</v>
+      </c>
+      <c r="AU113" s="10">
+        <v>4.6500000000000004</v>
+      </c>
     </row>
-    <row r="114" spans="2:45">
+    <row r="114" spans="2:47">
       <c r="B114" s="2">
         <v>1977</v>
       </c>
@@ -10490,8 +10859,14 @@
         <v>34.359000000000002</v>
       </c>
       <c r="AS114" s="10"/>
+      <c r="AT114" s="3">
+        <v>0.90690000000000004</v>
+      </c>
+      <c r="AU114" s="10">
+        <v>4.6900000000000004</v>
+      </c>
     </row>
-    <row r="115" spans="2:45">
+    <row r="115" spans="2:47">
       <c r="B115" s="2">
         <v>1977.25</v>
       </c>
@@ -10603,8 +10978,14 @@
         <v>34.841000000000001</v>
       </c>
       <c r="AS115" s="10"/>
+      <c r="AT115" s="3">
+        <v>0.84830000000000005</v>
+      </c>
+      <c r="AU115" s="10">
+        <v>5.39</v>
+      </c>
     </row>
-    <row r="116" spans="2:45">
+    <row r="116" spans="2:47">
       <c r="B116" s="2">
         <v>1977.5</v>
       </c>
@@ -10716,8 +11097,14 @@
         <v>35.270000000000003</v>
       </c>
       <c r="AS116" s="10"/>
+      <c r="AT116" s="3">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="AU116" s="10">
+        <v>6.14</v>
+      </c>
     </row>
-    <row r="117" spans="2:45">
+    <row r="117" spans="2:47">
       <c r="B117" s="2">
         <v>1977.75</v>
       </c>
@@ -10829,8 +11216,14 @@
         <v>36.036000000000001</v>
       </c>
       <c r="AS117" s="10"/>
+      <c r="AT117" s="3">
+        <v>0.88529999999999998</v>
+      </c>
+      <c r="AU117" s="10">
+        <v>6.56</v>
+      </c>
     </row>
-    <row r="118" spans="2:45">
+    <row r="118" spans="2:47">
       <c r="B118" s="2">
         <v>1978</v>
       </c>
@@ -10942,8 +11335,14 @@
         <v>36.573</v>
       </c>
       <c r="AS118" s="10"/>
+      <c r="AT118" s="3">
+        <v>0.74839999999999995</v>
+      </c>
+      <c r="AU118" s="10">
+        <v>6.79</v>
+      </c>
     </row>
-    <row r="119" spans="2:45">
+    <row r="119" spans="2:47">
       <c r="B119" s="2">
         <v>1978.25</v>
       </c>
@@ -11058,8 +11457,14 @@
         <v>37.241999999999997</v>
       </c>
       <c r="AS119" s="10"/>
+      <c r="AT119" s="3">
+        <v>0.69720000000000004</v>
+      </c>
+      <c r="AU119" s="10">
+        <v>7.6</v>
+      </c>
     </row>
-    <row r="120" spans="2:45">
+    <row r="120" spans="2:47">
       <c r="B120" s="2">
         <v>1978.5</v>
       </c>
@@ -11174,8 +11579,14 @@
         <v>37.865000000000002</v>
       </c>
       <c r="AS120" s="10"/>
+      <c r="AT120" s="3">
+        <v>0.61029999999999995</v>
+      </c>
+      <c r="AU120" s="10">
+        <v>8.4499999999999993</v>
+      </c>
     </row>
-    <row r="121" spans="2:45">
+    <row r="121" spans="2:47">
       <c r="B121" s="2">
         <v>1978.75</v>
       </c>
@@ -11290,8 +11701,14 @@
         <v>38.661000000000001</v>
       </c>
       <c r="AS121" s="10"/>
+      <c r="AT121" s="3">
+        <v>0.63759999999999994</v>
+      </c>
+      <c r="AU121" s="10">
+        <v>10.029999999999999</v>
+      </c>
     </row>
-    <row r="122" spans="2:45">
+    <row r="122" spans="2:47">
       <c r="B122" s="2">
         <v>1979</v>
       </c>
@@ -11406,8 +11823,14 @@
         <v>39.351999999999997</v>
       </c>
       <c r="AS122" s="10"/>
+      <c r="AT122" s="3">
+        <v>0.66539999999999999</v>
+      </c>
+      <c r="AU122" s="10">
+        <v>10.09</v>
+      </c>
     </row>
-    <row r="123" spans="2:45">
+    <row r="123" spans="2:47">
       <c r="B123" s="2">
         <v>1979.25</v>
       </c>
@@ -11522,8 +11945,14 @@
         <v>40.304000000000002</v>
       </c>
       <c r="AS123" s="10"/>
+      <c r="AT123" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="AU123" s="10">
+        <v>10.29</v>
+      </c>
     </row>
-    <row r="124" spans="2:45">
+    <row r="124" spans="2:47">
       <c r="B124" s="2">
         <v>1979.5</v>
       </c>
@@ -11638,8 +12067,14 @@
         <v>41.164999999999999</v>
       </c>
       <c r="AS124" s="10"/>
+      <c r="AT124" s="3">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="AU124" s="10">
+        <v>11.43</v>
+      </c>
     </row>
-    <row r="125" spans="2:45">
+    <row r="125" spans="2:47">
       <c r="B125" s="2">
         <v>1979.75</v>
       </c>
@@ -11754,8 +12189,14 @@
         <v>41.985999999999997</v>
       </c>
       <c r="AS125" s="10"/>
+      <c r="AT125" s="3">
+        <v>0.77180000000000004</v>
+      </c>
+      <c r="AU125" s="10">
+        <v>13.78</v>
+      </c>
     </row>
-    <row r="126" spans="2:45">
+    <row r="126" spans="2:47">
       <c r="B126" s="2">
         <v>1980</v>
       </c>
@@ -11870,8 +12311,14 @@
         <v>42.859000000000002</v>
       </c>
       <c r="AS126" s="10"/>
+      <c r="AT126" s="3">
+        <v>0.92379999999999995</v>
+      </c>
+      <c r="AU126" s="10">
+        <v>17.190000000000001</v>
+      </c>
     </row>
-    <row r="127" spans="2:45">
+    <row r="127" spans="2:47">
       <c r="B127" s="2">
         <v>1980.25</v>
       </c>
@@ -11986,8 +12433,14 @@
         <v>43.8</v>
       </c>
       <c r="AS127" s="10"/>
+      <c r="AT127" s="3">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="AU127" s="10">
+        <v>9.4700000000000006</v>
+      </c>
     </row>
-    <row r="128" spans="2:45">
+    <row r="128" spans="2:47">
       <c r="B128" s="2">
         <v>1980.5</v>
       </c>
@@ -12102,8 +12555,14 @@
         <v>44.808</v>
       </c>
       <c r="AS128" s="10"/>
+      <c r="AT128" s="3">
+        <v>0.8629</v>
+      </c>
+      <c r="AU128" s="10">
+        <v>10.87</v>
+      </c>
     </row>
-    <row r="129" spans="2:45">
+    <row r="129" spans="2:47">
       <c r="B129" s="2">
         <v>1980.75</v>
       </c>
@@ -12218,8 +12677,14 @@
         <v>46.045999999999999</v>
       </c>
       <c r="AS129" s="10"/>
+      <c r="AT129" s="3">
+        <v>0.98980000000000001</v>
+      </c>
+      <c r="AU129" s="10">
+        <v>18.899999999999999</v>
+      </c>
     </row>
-    <row r="130" spans="2:45">
+    <row r="130" spans="2:47">
       <c r="B130" s="2">
         <v>1981</v>
       </c>
@@ -12334,8 +12799,14 @@
         <v>47.195999999999998</v>
       </c>
       <c r="AS130" s="10"/>
+      <c r="AT130" s="3">
+        <v>0.96340000000000003</v>
+      </c>
+      <c r="AU130" s="10">
+        <v>14.7</v>
+      </c>
     </row>
-    <row r="131" spans="2:45">
+    <row r="131" spans="2:47">
       <c r="B131" s="2">
         <v>1981.25</v>
       </c>
@@ -12450,8 +12921,14 @@
         <v>48.081000000000003</v>
       </c>
       <c r="AS131" s="10"/>
+      <c r="AT131" s="3">
+        <v>1.1214999999999999</v>
+      </c>
+      <c r="AU131" s="10">
+        <v>19.100000000000001</v>
+      </c>
     </row>
-    <row r="132" spans="2:45">
+    <row r="132" spans="2:47">
       <c r="B132" s="2">
         <v>1981.5</v>
       </c>
@@ -12582,8 +13059,14 @@
         <v>48.945999999999998</v>
       </c>
       <c r="AS132" s="10"/>
+      <c r="AT132" s="3">
+        <v>1.1418999999999999</v>
+      </c>
+      <c r="AU132" s="10">
+        <v>15.87</v>
+      </c>
     </row>
-    <row r="133" spans="2:45">
+    <row r="133" spans="2:47">
       <c r="B133" s="2">
         <v>1981.75</v>
       </c>
@@ -12714,8 +13197,14 @@
         <v>49.863</v>
       </c>
       <c r="AS133" s="10"/>
+      <c r="AT133" s="3">
+        <v>1.4448000000000001</v>
+      </c>
+      <c r="AU133" s="10">
+        <v>12.37</v>
+      </c>
     </row>
-    <row r="134" spans="2:45">
+    <row r="134" spans="2:47">
       <c r="B134" s="2">
         <v>1982</v>
       </c>
@@ -12846,8 +13335,14 @@
         <v>50.561</v>
       </c>
       <c r="AS134" s="10"/>
+      <c r="AT134" s="3">
+        <v>1.5509999999999999</v>
+      </c>
+      <c r="AU134" s="10">
+        <v>14.68</v>
+      </c>
     </row>
-    <row r="135" spans="2:45">
+    <row r="135" spans="2:47">
       <c r="B135" s="2">
         <v>1982.25</v>
       </c>
@@ -12978,8 +13473,14 @@
         <v>51.17</v>
       </c>
       <c r="AS135" s="10"/>
+      <c r="AT135" s="3">
+        <v>1.5548999999999999</v>
+      </c>
+      <c r="AU135" s="10">
+        <v>14.15</v>
+      </c>
     </row>
-    <row r="136" spans="2:45">
+    <row r="136" spans="2:47">
       <c r="B136" s="2">
         <v>1982.5</v>
       </c>
@@ -13110,8 +13611,14 @@
         <v>51.906999999999996</v>
       </c>
       <c r="AS136" s="10"/>
+      <c r="AT136" s="3">
+        <v>1.6774</v>
+      </c>
+      <c r="AU136" s="10">
+        <v>10.31</v>
+      </c>
     </row>
-    <row r="137" spans="2:45">
+    <row r="137" spans="2:47">
       <c r="B137" s="2">
         <v>1982.75</v>
       </c>
@@ -13242,8 +13749,14 @@
         <v>52.482999999999997</v>
       </c>
       <c r="AS137" s="10"/>
+      <c r="AT137" s="3">
+        <v>1.5542</v>
+      </c>
+      <c r="AU137" s="10">
+        <v>8.9499999999999993</v>
+      </c>
     </row>
-    <row r="138" spans="2:45">
+    <row r="138" spans="2:47">
       <c r="B138" s="2">
         <v>1983</v>
       </c>
@@ -13374,8 +13887,14 @@
         <v>52.906999999999996</v>
       </c>
       <c r="AS138" s="10"/>
+      <c r="AT138" s="3">
+        <v>1.1416999999999999</v>
+      </c>
+      <c r="AU138" s="10">
+        <v>8.77</v>
+      </c>
     </row>
-    <row r="139" spans="2:45">
+    <row r="139" spans="2:47">
       <c r="B139" s="2">
         <v>1983.25</v>
       </c>
@@ -13506,8 +14025,14 @@
         <v>53.265000000000001</v>
       </c>
       <c r="AS139" s="10"/>
+      <c r="AT139" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="AU139" s="10">
+        <v>8.98</v>
+      </c>
     </row>
-    <row r="140" spans="2:45">
+    <row r="140" spans="2:47">
       <c r="B140" s="2">
         <v>1983.5</v>
       </c>
@@ -13638,8 +14163,14 @@
         <v>53.823</v>
       </c>
       <c r="AS140" s="10"/>
+      <c r="AT140" s="3">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="AU140" s="10">
+        <v>9.4499999999999993</v>
+      </c>
     </row>
-    <row r="141" spans="2:45">
+    <row r="141" spans="2:47">
       <c r="B141" s="2">
         <v>1983.75</v>
       </c>
@@ -13770,8 +14301,14 @@
         <v>54.219000000000001</v>
       </c>
       <c r="AS141" s="10"/>
+      <c r="AT141" s="3">
+        <v>0.94359999999999999</v>
+      </c>
+      <c r="AU141" s="10">
+        <v>9.4700000000000006</v>
+      </c>
     </row>
-    <row r="142" spans="2:45">
+    <row r="142" spans="2:47">
       <c r="B142" s="2">
         <v>1984</v>
       </c>
@@ -13902,8 +14439,14 @@
         <v>54.795999999999999</v>
       </c>
       <c r="AS142" s="10"/>
+      <c r="AT142" s="3">
+        <v>0.95289999999999997</v>
+      </c>
+      <c r="AU142" s="10">
+        <v>9.91</v>
+      </c>
     </row>
-    <row r="143" spans="2:45">
+    <row r="143" spans="2:47">
       <c r="B143" s="2">
         <v>1984.25</v>
       </c>
@@ -14034,8 +14577,14 @@
         <v>55.256999999999998</v>
       </c>
       <c r="AS143" s="10"/>
+      <c r="AT143" s="3">
+        <v>0.877</v>
+      </c>
+      <c r="AU143" s="10">
+        <v>11.06</v>
+      </c>
     </row>
-    <row r="144" spans="2:45">
+    <row r="144" spans="2:47">
       <c r="B144" s="2">
         <v>1984.5</v>
       </c>
@@ -14166,8 +14715,14 @@
         <v>55.704999999999998</v>
       </c>
       <c r="AS144" s="10"/>
+      <c r="AT144" s="3">
+        <v>0.95779999999999998</v>
+      </c>
+      <c r="AU144" s="10">
+        <v>11.3</v>
+      </c>
     </row>
-    <row r="145" spans="2:45">
+    <row r="145" spans="2:47">
       <c r="B145" s="2">
         <v>1984.75</v>
       </c>
@@ -14298,8 +14853,14 @@
         <v>56.079000000000001</v>
       </c>
       <c r="AS145" s="10"/>
+      <c r="AT145" s="3">
+        <v>0.99639999999999995</v>
+      </c>
+      <c r="AU145" s="10">
+        <v>8.3800000000000008</v>
+      </c>
     </row>
-    <row r="146" spans="2:45">
+    <row r="146" spans="2:47">
       <c r="B146" s="2">
         <v>1985</v>
       </c>
@@ -14430,8 +14991,14 @@
         <v>56.723999999999997</v>
       </c>
       <c r="AS146" s="10"/>
+      <c r="AT146" s="3">
+        <v>1.0276000000000001</v>
+      </c>
+      <c r="AU146" s="10">
+        <v>8.58</v>
+      </c>
     </row>
-    <row r="147" spans="2:45">
+    <row r="147" spans="2:47">
       <c r="B147" s="2">
         <v>1985.25</v>
       </c>
@@ -14562,8 +15129,14 @@
         <v>57.075000000000003</v>
       </c>
       <c r="AS147" s="10"/>
+      <c r="AT147" s="3">
+        <v>1.1998</v>
+      </c>
+      <c r="AU147" s="10">
+        <v>7.53</v>
+      </c>
     </row>
-    <row r="148" spans="2:45">
+    <row r="148" spans="2:47">
       <c r="B148" s="2">
         <v>1985.5</v>
       </c>
@@ -14694,8 +15267,14 @@
         <v>57.405999999999999</v>
       </c>
       <c r="AS148" s="10"/>
+      <c r="AT148" s="3">
+        <v>1.2437</v>
+      </c>
+      <c r="AU148" s="10">
+        <v>7.92</v>
+      </c>
     </row>
-    <row r="149" spans="2:45">
+    <row r="149" spans="2:47">
       <c r="B149" s="2">
         <v>1985.75</v>
       </c>
@@ -14826,8 +15405,14 @@
         <v>57.738</v>
       </c>
       <c r="AS149" s="10"/>
+      <c r="AT149" s="3">
+        <v>1.4291</v>
+      </c>
+      <c r="AU149" s="10">
+        <v>8.27</v>
+      </c>
     </row>
-    <row r="150" spans="2:45">
+    <row r="150" spans="2:47">
       <c r="B150" s="2">
         <v>1986</v>
       </c>
@@ -14958,8 +15543,14 @@
         <v>58.02</v>
       </c>
       <c r="AS150" s="10"/>
+      <c r="AT150" s="3">
+        <v>1.8412999999999999</v>
+      </c>
+      <c r="AU150" s="10">
+        <v>7.48</v>
+      </c>
     </row>
-    <row r="151" spans="2:45">
+    <row r="151" spans="2:47">
       <c r="B151" s="2">
         <v>1986.25</v>
       </c>
@@ -15090,8 +15681,14 @@
         <v>58.252000000000002</v>
       </c>
       <c r="AS151" s="10"/>
+      <c r="AT151" s="3">
+        <v>1.972</v>
+      </c>
+      <c r="AU151" s="10">
+        <v>6.92</v>
+      </c>
     </row>
-    <row r="152" spans="2:45">
+    <row r="152" spans="2:47">
       <c r="B152" s="2">
         <v>1986.5</v>
       </c>
@@ -15222,8 +15819,14 @@
         <v>58.487000000000002</v>
       </c>
       <c r="AS152" s="10"/>
+      <c r="AT152" s="3">
+        <v>2.0950000000000002</v>
+      </c>
+      <c r="AU152" s="10">
+        <v>5.89</v>
+      </c>
     </row>
-    <row r="153" spans="2:45">
+    <row r="153" spans="2:47">
       <c r="B153" s="2">
         <v>1986.75</v>
       </c>
@@ -15354,8 +15957,14 @@
         <v>58.813000000000002</v>
       </c>
       <c r="AS153" s="10"/>
+      <c r="AT153" s="3">
+        <v>1.9807999999999999</v>
+      </c>
+      <c r="AU153" s="10">
+        <v>6.91</v>
+      </c>
     </row>
-    <row r="154" spans="2:45">
+    <row r="154" spans="2:47">
       <c r="B154" s="2">
         <v>1987</v>
       </c>
@@ -15486,8 +16095,14 @@
         <v>59.24</v>
       </c>
       <c r="AS154" s="10"/>
+      <c r="AT154" s="3">
+        <v>1.8228</v>
+      </c>
+      <c r="AU154" s="10">
+        <v>6.13</v>
+      </c>
     </row>
-    <row r="155" spans="2:45">
+    <row r="155" spans="2:47">
       <c r="B155" s="2">
         <v>1987.25</v>
       </c>
@@ -15618,8 +16233,14 @@
         <v>59.637</v>
       </c>
       <c r="AS155" s="10"/>
+      <c r="AT155" s="3">
+        <v>1.6871</v>
+      </c>
+      <c r="AU155" s="10">
+        <v>6.73</v>
+      </c>
     </row>
-    <row r="156" spans="2:45">
+    <row r="156" spans="2:47">
       <c r="B156" s="2">
         <v>1987.5</v>
       </c>
@@ -15750,8 +16371,14 @@
         <v>60.07</v>
       </c>
       <c r="AS156" s="10"/>
+      <c r="AT156" s="3">
+        <v>1.6107</v>
+      </c>
+      <c r="AU156" s="10">
+        <v>7.22</v>
+      </c>
     </row>
-    <row r="157" spans="2:45">
+    <row r="157" spans="2:47">
       <c r="B157" s="2">
         <v>1987.75</v>
       </c>
@@ -15882,8 +16509,14 @@
         <v>60.567</v>
       </c>
       <c r="AS157" s="10"/>
+      <c r="AT157" s="3">
+        <v>1.5905</v>
+      </c>
+      <c r="AU157" s="10">
+        <v>6.77</v>
+      </c>
     </row>
-    <row r="158" spans="2:45">
+    <row r="158" spans="2:47">
       <c r="B158" s="2">
         <v>1988</v>
       </c>
@@ -16014,8 +16647,14 @@
         <v>61.042999999999999</v>
       </c>
       <c r="AS158" s="10"/>
+      <c r="AT158" s="3">
+        <v>1.593</v>
+      </c>
+      <c r="AU158" s="10">
+        <v>6.58</v>
+      </c>
     </row>
-    <row r="159" spans="2:45">
+    <row r="159" spans="2:47">
       <c r="B159" s="2">
         <v>1988.25</v>
       </c>
@@ -16146,8 +16785,14 @@
         <v>61.633000000000003</v>
       </c>
       <c r="AS159" s="10"/>
+      <c r="AT159" s="3">
+        <v>1.4676</v>
+      </c>
+      <c r="AU159" s="10">
+        <v>7.51</v>
+      </c>
     </row>
-    <row r="160" spans="2:45">
+    <row r="160" spans="2:47">
       <c r="B160" s="2">
         <v>1988.5</v>
       </c>
@@ -16278,8 +16923,14 @@
         <v>62.359000000000002</v>
       </c>
       <c r="AS160" s="10"/>
+      <c r="AT160" s="3">
+        <v>1.4797</v>
+      </c>
+      <c r="AU160" s="10">
+        <v>8.19</v>
+      </c>
     </row>
-    <row r="161" spans="2:45">
+    <row r="161" spans="2:47">
       <c r="B161" s="2">
         <v>1988.75</v>
       </c>
@@ -16410,8 +17061,14 @@
         <v>62.859000000000002</v>
       </c>
       <c r="AS161" s="10"/>
+      <c r="AT161" s="3">
+        <v>1.524</v>
+      </c>
+      <c r="AU161" s="10">
+        <v>8.76</v>
+      </c>
     </row>
-    <row r="162" spans="2:45">
+    <row r="162" spans="2:47">
       <c r="B162" s="2">
         <v>1989</v>
       </c>
@@ -16542,8 +17199,14 @@
         <v>63.55</v>
       </c>
       <c r="AS162" s="10"/>
+      <c r="AT162" s="3">
+        <v>1.5034000000000001</v>
+      </c>
+      <c r="AU162" s="10">
+        <v>9.85</v>
+      </c>
     </row>
-    <row r="163" spans="2:45">
+    <row r="163" spans="2:47">
       <c r="B163" s="2">
         <v>1989.25</v>
       </c>
@@ -16674,8 +17337,14 @@
         <v>64.206999999999994</v>
       </c>
       <c r="AS163" s="10"/>
+      <c r="AT163" s="3">
+        <v>1.7632000000000001</v>
+      </c>
+      <c r="AU163" s="10">
+        <v>9.5299999999999994</v>
+      </c>
     </row>
-    <row r="164" spans="2:45">
+    <row r="164" spans="2:47">
       <c r="B164" s="2">
         <v>1989.5</v>
       </c>
@@ -16806,8 +17475,14 @@
         <v>64.671999999999997</v>
       </c>
       <c r="AS164" s="10"/>
+      <c r="AT164" s="3">
+        <v>1.7269000000000001</v>
+      </c>
+      <c r="AU164" s="10">
+        <v>9.02</v>
+      </c>
     </row>
-    <row r="165" spans="2:45">
+    <row r="165" spans="2:47">
       <c r="B165" s="2">
         <v>1989.75</v>
       </c>
@@ -16938,8 +17613,14 @@
         <v>65.122</v>
       </c>
       <c r="AS165" s="10"/>
+      <c r="AT165" s="3">
+        <v>1.6442000000000001</v>
+      </c>
+      <c r="AU165" s="10">
+        <v>8.4499999999999993</v>
+      </c>
     </row>
-    <row r="166" spans="2:45">
+    <row r="166" spans="2:47">
       <c r="B166" s="2">
         <v>1990</v>
       </c>
@@ -17072,8 +17753,14 @@
       <c r="AS166" s="10">
         <v>22.174603174603174</v>
       </c>
+      <c r="AT166" s="3">
+        <v>1.4482999999999999</v>
+      </c>
+      <c r="AU166" s="10">
+        <v>8.2799999999999994</v>
+      </c>
     </row>
-    <row r="167" spans="2:45">
+    <row r="167" spans="2:47">
       <c r="B167" s="2">
         <v>1990.25</v>
       </c>
@@ -17206,8 +17893,14 @@
       <c r="AS167" s="10">
         <v>18.722063492063491</v>
       </c>
+      <c r="AT167" s="3">
+        <v>1.2152000000000001</v>
+      </c>
+      <c r="AU167" s="10">
+        <v>8.2899999999999991</v>
+      </c>
     </row>
-    <row r="168" spans="2:45">
+    <row r="168" spans="2:47">
       <c r="B168" s="2">
         <v>1990.5</v>
       </c>
@@ -17340,8 +18033,14 @@
       <c r="AS168" s="10">
         <v>25.195555555555554</v>
       </c>
+      <c r="AT168" s="3">
+        <v>1.2535000000000001</v>
+      </c>
+      <c r="AU168" s="10">
+        <v>8.1999999999999993</v>
+      </c>
     </row>
-    <row r="169" spans="2:45">
+    <row r="169" spans="2:47">
       <c r="B169" s="2">
         <v>1990.75</v>
       </c>
@@ -17474,8 +18173,14 @@
       <c r="AS169" s="10">
         <v>26.11328125</v>
       </c>
+      <c r="AT169" s="3">
+        <v>1.6213</v>
+      </c>
+      <c r="AU169" s="10">
+        <v>7.31</v>
+      </c>
     </row>
-    <row r="170" spans="2:45">
+    <row r="170" spans="2:47">
       <c r="B170" s="2">
         <v>1991</v>
       </c>
@@ -17608,8 +18313,14 @@
       <c r="AS170" s="10">
         <v>22.515833333333333</v>
       </c>
+      <c r="AT170" s="3">
+        <v>1.5216000000000001</v>
+      </c>
+      <c r="AU170" s="10">
+        <v>6.12</v>
+      </c>
     </row>
-    <row r="171" spans="2:45">
+    <row r="171" spans="2:47">
       <c r="B171" s="2">
         <v>1991.25</v>
       </c>
@@ -17742,8 +18453,14 @@
       <c r="AS171" s="10">
         <v>17.147031250000001</v>
       </c>
+      <c r="AT171" s="3">
+        <v>1.4752000000000001</v>
+      </c>
+      <c r="AU171" s="10">
+        <v>5.9</v>
+      </c>
     </row>
-    <row r="172" spans="2:45">
+    <row r="172" spans="2:47">
       <c r="B172" s="2">
         <v>1991.5</v>
       </c>
@@ -17876,8 +18593,14 @@
       <c r="AS172" s="10">
         <v>16.634218749999999</v>
       </c>
+      <c r="AT172" s="3">
+        <v>1.4875</v>
+      </c>
+      <c r="AU172" s="10">
+        <v>5.45</v>
+      </c>
     </row>
-    <row r="173" spans="2:45">
+    <row r="173" spans="2:47">
       <c r="B173" s="2">
         <v>1991.75</v>
       </c>
@@ -18010,8 +18733,14 @@
       <c r="AS173" s="10">
         <v>17.455312500000002</v>
       </c>
+      <c r="AT173" s="3">
+        <v>1.5107999999999999</v>
+      </c>
+      <c r="AU173" s="10">
+        <v>4.43</v>
+      </c>
     </row>
-    <row r="174" spans="2:45">
+    <row r="174" spans="2:47">
       <c r="B174" s="2">
         <v>1992</v>
       </c>
@@ -18144,8 +18873,14 @@
       <c r="AS174" s="10">
         <v>17.564285714285713</v>
       </c>
+      <c r="AT174" s="3">
+        <v>1.3742000000000001</v>
+      </c>
+      <c r="AU174" s="10">
+        <v>3.98</v>
+      </c>
     </row>
-    <row r="175" spans="2:45">
+    <row r="175" spans="2:47">
       <c r="B175" s="2">
         <v>1992.25</v>
       </c>
@@ -18278,8 +19013,14 @@
       <c r="AS175" s="10">
         <v>15.616349206349206</v>
       </c>
+      <c r="AT175" s="3">
+        <v>1.3351999999999999</v>
+      </c>
+      <c r="AU175" s="10">
+        <v>3.76</v>
+      </c>
     </row>
-    <row r="176" spans="2:45">
+    <row r="176" spans="2:47">
       <c r="B176" s="2">
         <v>1992.5</v>
       </c>
@@ -18412,8 +19153,14 @@
       <c r="AS176" s="10">
         <v>13.90203125</v>
       </c>
+      <c r="AT176" s="3">
+        <v>1.5062</v>
+      </c>
+      <c r="AU176" s="10">
+        <v>3.22</v>
+      </c>
     </row>
-    <row r="177" spans="2:45">
+    <row r="177" spans="2:47">
       <c r="B177" s="2">
         <v>1992.75</v>
       </c>
@@ -18546,8 +19293,14 @@
       <c r="AS177" s="10">
         <v>14.761093750000001</v>
       </c>
+      <c r="AT177" s="3">
+        <v>1.4388000000000001</v>
+      </c>
+      <c r="AU177" s="10">
+        <v>2.92</v>
+      </c>
     </row>
-    <row r="178" spans="2:45">
+    <row r="178" spans="2:47">
       <c r="B178" s="2">
         <v>1993</v>
       </c>
@@ -18680,8 +19433,14 @@
       <c r="AS178" s="10">
         <v>13.255322580645162</v>
       </c>
+      <c r="AT178" s="3">
+        <v>1.4533</v>
+      </c>
+      <c r="AU178" s="10">
+        <v>3.07</v>
+      </c>
     </row>
-    <row r="179" spans="2:45">
+    <row r="179" spans="2:47">
       <c r="B179" s="2">
         <v>1993.25</v>
       </c>
@@ -18814,8 +19573,14 @@
       <c r="AS179" s="10">
         <v>12.973174603174604</v>
       </c>
+      <c r="AT179" s="3">
+        <v>1.4012</v>
+      </c>
+      <c r="AU179" s="10">
+        <v>3.04</v>
+      </c>
     </row>
-    <row r="180" spans="2:45">
+    <row r="180" spans="2:47">
       <c r="B180" s="2">
         <v>1993.5</v>
       </c>
@@ -18948,8 +19713,14 @@
       <c r="AS180" s="10">
         <v>12.1171875</v>
       </c>
+      <c r="AT180" s="3">
+        <v>1.4315</v>
+      </c>
+      <c r="AU180" s="10">
+        <v>3.09</v>
+      </c>
     </row>
-    <row r="181" spans="2:45">
+    <row r="181" spans="2:47">
       <c r="B181" s="2">
         <v>1993.75</v>
       </c>
@@ -19082,8 +19853,14 @@
       <c r="AS181" s="10">
         <v>12.4215625</v>
       </c>
+      <c r="AT181" s="3">
+        <v>1.3460000000000001</v>
+      </c>
+      <c r="AU181" s="10">
+        <v>2.96</v>
+      </c>
     </row>
-    <row r="182" spans="2:45">
+    <row r="182" spans="2:47">
       <c r="B182" s="2">
         <v>1994</v>
       </c>
@@ -19216,8 +19993,14 @@
       <c r="AS182" s="10">
         <v>13.436190476190475</v>
       </c>
+      <c r="AT182" s="3">
+        <v>1.2428999999999999</v>
+      </c>
+      <c r="AU182" s="10">
+        <v>3.34</v>
+      </c>
     </row>
-    <row r="183" spans="2:45">
+    <row r="183" spans="2:47">
       <c r="B183" s="2">
         <v>1994.25</v>
       </c>
@@ -19350,8 +20133,14 @@
       <c r="AS183" s="10">
         <v>14.51258064516129</v>
       </c>
+      <c r="AT183" s="3">
+        <v>1.2508999999999999</v>
+      </c>
+      <c r="AU183" s="10">
+        <v>4.25</v>
+      </c>
     </row>
-    <row r="184" spans="2:45">
+    <row r="184" spans="2:47">
       <c r="B184" s="2">
         <v>1994.5</v>
       </c>
@@ -19484,8 +20273,14 @@
       <c r="AS184" s="10">
         <v>12.516249999999999</v>
       </c>
+      <c r="AT184" s="3">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="AU184" s="10">
+        <v>4.7300000000000004</v>
+      </c>
     </row>
-    <row r="185" spans="2:45">
+    <row r="185" spans="2:47">
       <c r="B185" s="2">
         <v>1994.75</v>
       </c>
@@ -19618,8 +20413,14 @@
       <c r="AS185" s="10">
         <v>15.268730158730159</v>
       </c>
+      <c r="AT185" s="3">
+        <v>1.2815000000000001</v>
+      </c>
+      <c r="AU185" s="10">
+        <v>5.45</v>
+      </c>
     </row>
-    <row r="186" spans="2:45">
+    <row r="186" spans="2:47">
       <c r="B186" s="2">
         <v>1995</v>
       </c>
@@ -19752,8 +20553,14 @@
       <c r="AS186" s="10">
         <v>11.992380952380952</v>
       </c>
+      <c r="AT186" s="3">
+        <v>1.2770999999999999</v>
+      </c>
+      <c r="AU186" s="10">
+        <v>5.98</v>
+      </c>
     </row>
-    <row r="187" spans="2:45">
+    <row r="187" spans="2:47">
       <c r="B187" s="2">
         <v>1995.25</v>
       </c>
@@ -19886,8 +20693,14 @@
       <c r="AS187" s="10">
         <v>12.190317460317461</v>
       </c>
+      <c r="AT187" s="3">
+        <v>1.3073999999999999</v>
+      </c>
+      <c r="AU187" s="10">
+        <v>6</v>
+      </c>
     </row>
-    <row r="188" spans="2:45">
+    <row r="188" spans="2:47">
       <c r="B188" s="2">
         <v>1995.5</v>
       </c>
@@ -20020,8 +20833,14 @@
       <c r="AS188" s="10">
         <v>12.472698412698414</v>
       </c>
+      <c r="AT188" s="3">
+        <v>1.3132999999999999</v>
+      </c>
+      <c r="AU188" s="10">
+        <v>5.8</v>
+      </c>
     </row>
-    <row r="189" spans="2:45">
+    <row r="189" spans="2:47">
       <c r="B189" s="2">
         <v>1995.75</v>
       </c>
@@ -20154,8 +20973,14 @@
       <c r="AS189" s="10">
         <v>12.899682539682539</v>
       </c>
+      <c r="AT189" s="3">
+        <v>1.4167000000000001</v>
+      </c>
+      <c r="AU189" s="10">
+        <v>5.6</v>
+      </c>
     </row>
-    <row r="190" spans="2:45">
+    <row r="190" spans="2:47">
       <c r="B190" s="2">
         <v>1996</v>
       </c>
@@ -20288,8 +21113,14 @@
       <c r="AS190" s="10">
         <v>15.398253968253968</v>
       </c>
+      <c r="AT190" s="3">
+        <v>1.3314999999999999</v>
+      </c>
+      <c r="AU190" s="10">
+        <v>5.31</v>
+      </c>
     </row>
-    <row r="191" spans="2:45">
+    <row r="191" spans="2:47">
       <c r="B191" s="2">
         <v>1996.25</v>
       </c>
@@ -20422,8 +21253,14 @@
       <c r="AS191" s="10">
         <v>16.368253968253967</v>
       </c>
+      <c r="AT191" s="3">
+        <v>1.2784</v>
+      </c>
+      <c r="AU191" s="10">
+        <v>5.27</v>
+      </c>
     </row>
-    <row r="192" spans="2:45">
+    <row r="192" spans="2:47">
       <c r="B192" s="2">
         <v>1996.5</v>
       </c>
@@ -20556,8 +21393,14 @@
       <c r="AS192" s="10">
         <v>16.778437499999999</v>
       </c>
+      <c r="AT192" s="3">
+        <v>1.2848999999999999</v>
+      </c>
+      <c r="AU192" s="10">
+        <v>5.3</v>
+      </c>
     </row>
-    <row r="193" spans="2:45">
+    <row r="193" spans="2:47">
       <c r="B193" s="2">
         <v>1996.75</v>
       </c>
@@ -20690,8 +21533,14 @@
       <c r="AS193" s="10">
         <v>17.206250000000001</v>
       </c>
+      <c r="AT193" s="3">
+        <v>1.3058000000000001</v>
+      </c>
+      <c r="AU193" s="10">
+        <v>5.29</v>
+      </c>
     </row>
-    <row r="194" spans="2:45">
+    <row r="194" spans="2:47">
       <c r="B194" s="2">
         <v>1997</v>
       </c>
@@ -20824,8 +21673,14 @@
       <c r="AS194" s="10">
         <v>19.916499999999999</v>
       </c>
+      <c r="AT194" s="3">
+        <v>1.2424999999999999</v>
+      </c>
+      <c r="AU194" s="10">
+        <v>5.39</v>
+      </c>
     </row>
-    <row r="195" spans="2:45">
+    <row r="195" spans="2:47">
       <c r="B195" s="2">
         <v>1997.25</v>
       </c>
@@ -20958,8 +21813,14 @@
       <c r="AS195" s="10">
         <v>19.922968749999999</v>
       </c>
+      <c r="AT195" s="3">
+        <v>1.1975</v>
+      </c>
+      <c r="AU195" s="10">
+        <v>5.56</v>
+      </c>
     </row>
-    <row r="196" spans="2:45">
+    <row r="196" spans="2:47">
       <c r="B196" s="2">
         <v>1997.5</v>
       </c>
@@ -21092,8 +21953,14 @@
       <c r="AS196" s="10">
         <v>22.445</v>
       </c>
+      <c r="AT196" s="3">
+        <v>1.2225999999999999</v>
+      </c>
+      <c r="AU196" s="10">
+        <v>5.54</v>
+      </c>
     </row>
-    <row r="197" spans="2:45">
+    <row r="197" spans="2:47">
       <c r="B197" s="2">
         <v>1997.75</v>
       </c>
@@ -21226,8 +22093,14 @@
       <c r="AS197" s="10">
         <v>27.092380952380953</v>
       </c>
+      <c r="AT197" s="3">
+        <v>1.3562000000000001</v>
+      </c>
+      <c r="AU197" s="10">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="198" spans="2:45">
+    <row r="198" spans="2:47">
       <c r="B198" s="2">
         <v>1998</v>
       </c>
@@ -21360,8 +22233,14 @@
       <c r="AS198" s="10">
         <v>21.324590163934428</v>
       </c>
+      <c r="AT198" s="3">
+        <v>1.3443000000000001</v>
+      </c>
+      <c r="AU198" s="10">
+        <v>5.49</v>
+      </c>
     </row>
-    <row r="199" spans="2:45">
+    <row r="199" spans="2:47">
       <c r="B199" s="2">
         <v>1998.25</v>
       </c>
@@ -21494,8 +22373,14 @@
       <c r="AS199" s="10">
         <v>21.534285714285716</v>
       </c>
+      <c r="AT199" s="3">
+        <v>1.3249</v>
+      </c>
+      <c r="AU199" s="10">
+        <v>5.56</v>
+      </c>
     </row>
-    <row r="200" spans="2:45">
+    <row r="200" spans="2:47">
       <c r="B200" s="2">
         <v>1998.5</v>
       </c>
@@ -21628,8 +22513,14 @@
       <c r="AS200" s="10">
         <v>29.751718749999998</v>
       </c>
+      <c r="AT200" s="3">
+        <v>2.0169000000000001</v>
+      </c>
+      <c r="AU200" s="10">
+        <v>5.51</v>
+      </c>
     </row>
-    <row r="201" spans="2:45">
+    <row r="201" spans="2:47">
       <c r="B201" s="2">
         <v>1998.75</v>
       </c>
@@ -21762,8 +22653,14 @@
       <c r="AS201" s="10">
         <v>29.537187500000002</v>
       </c>
+      <c r="AT201" s="3">
+        <v>2.1269</v>
+      </c>
+      <c r="AU201" s="10">
+        <v>4.68</v>
+      </c>
     </row>
-    <row r="202" spans="2:45">
+    <row r="202" spans="2:47">
       <c r="B202" s="2">
         <v>1999</v>
       </c>
@@ -21896,8 +22793,14 @@
       <c r="AS202" s="10">
         <v>27.2527868852459</v>
       </c>
+      <c r="AT202" s="3">
+        <v>1.833</v>
+      </c>
+      <c r="AU202" s="10">
+        <v>4.8099999999999996</v>
+      </c>
     </row>
-    <row r="203" spans="2:45">
+    <row r="203" spans="2:47">
       <c r="B203" s="2">
         <v>1999.25</v>
       </c>
@@ -22030,8 +22933,14 @@
       <c r="AS203" s="10">
         <v>24.395555555555557</v>
       </c>
+      <c r="AT203" s="3">
+        <v>1.7621</v>
+      </c>
+      <c r="AU203" s="10">
+        <v>4.76</v>
+      </c>
     </row>
-    <row r="204" spans="2:45">
+    <row r="204" spans="2:47">
       <c r="B204" s="2">
         <v>1999.5</v>
       </c>
@@ -22164,8 +23073,14 @@
       <c r="AS204" s="10">
         <v>23.320625</v>
       </c>
+      <c r="AT204" s="3">
+        <v>2.0268999999999999</v>
+      </c>
+      <c r="AU204" s="10">
+        <v>5.22</v>
+      </c>
     </row>
-    <row r="205" spans="2:45">
+    <row r="205" spans="2:47">
       <c r="B205" s="2">
         <v>1999.75</v>
       </c>
@@ -22298,8 +23213,14 @@
       <c r="AS205" s="10">
         <v>22.658281250000002</v>
       </c>
+      <c r="AT205" s="3">
+        <v>2.0446</v>
+      </c>
+      <c r="AU205" s="10">
+        <v>5.3</v>
+      </c>
     </row>
-    <row r="206" spans="2:45">
+    <row r="206" spans="2:47">
       <c r="B206" s="2">
         <v>2000</v>
       </c>
@@ -22432,8 +23353,14 @@
       <c r="AS206" s="10">
         <v>23.15031746031746</v>
       </c>
+      <c r="AT206" s="3">
+        <v>2.3315999999999999</v>
+      </c>
+      <c r="AU206" s="10">
+        <v>5.85</v>
+      </c>
     </row>
-    <row r="207" spans="2:45">
+    <row r="207" spans="2:47">
       <c r="B207" s="2">
         <v>2000.25</v>
       </c>
@@ -22566,8 +23493,14 @@
       <c r="AS207" s="10">
         <v>24.923968253968255</v>
       </c>
+      <c r="AT207" s="3">
+        <v>2.835</v>
+      </c>
+      <c r="AU207" s="10">
+        <v>6.53</v>
+      </c>
     </row>
-    <row r="208" spans="2:45">
+    <row r="208" spans="2:47">
       <c r="B208" s="2">
         <v>2000.5</v>
       </c>
@@ -22700,8 +23633,14 @@
       <c r="AS208" s="10">
         <v>19.169047619047618</v>
       </c>
+      <c r="AT208" s="3">
+        <v>3.2391999999999999</v>
+      </c>
+      <c r="AU208" s="10">
+        <v>6.52</v>
+      </c>
     </row>
-    <row r="209" spans="2:45">
+    <row r="209" spans="2:47">
       <c r="B209" s="2">
         <v>2000.75</v>
       </c>
@@ -22834,8 +23773,14 @@
       <c r="AS209" s="10">
         <v>26.016666666666666</v>
       </c>
+      <c r="AT209" s="3">
+        <v>3.6334</v>
+      </c>
+      <c r="AU209" s="10">
+        <v>6.4</v>
+      </c>
     </row>
-    <row r="210" spans="2:45">
+    <row r="210" spans="2:47">
       <c r="B210" s="2">
         <v>2001</v>
       </c>
@@ -22968,8 +23913,14 @@
       <c r="AS210" s="10">
         <v>25.726451612903226</v>
       </c>
+      <c r="AT210" s="3">
+        <v>3.2886000000000002</v>
+      </c>
+      <c r="AU210" s="10">
+        <v>5.31</v>
+      </c>
     </row>
-    <row r="211" spans="2:45">
+    <row r="211" spans="2:47">
       <c r="B211" s="2">
         <v>2001.25</v>
       </c>
@@ -23102,8 +24053,14 @@
       <c r="AS211" s="10">
         <v>23.923809523809524</v>
       </c>
+      <c r="AT211" s="3">
+        <v>3.1236000000000002</v>
+      </c>
+      <c r="AU211" s="10">
+        <v>3.97</v>
+      </c>
     </row>
-    <row r="212" spans="2:45">
+    <row r="212" spans="2:47">
       <c r="B212" s="2">
         <v>2001.5</v>
       </c>
@@ -23236,8 +24193,14 @@
       <c r="AS212" s="10">
         <v>25.380338983050848</v>
       </c>
+      <c r="AT212" s="3">
+        <v>3.3347000000000002</v>
+      </c>
+      <c r="AU212" s="10">
+        <v>3.07</v>
+      </c>
     </row>
-    <row r="213" spans="2:45">
+    <row r="213" spans="2:47">
       <c r="B213" s="2">
         <v>2001.75</v>
       </c>
@@ -23370,8 +24333,14 @@
       <c r="AS213" s="10">
         <v>27.91</v>
       </c>
+      <c r="AT213" s="3">
+        <v>3.0945</v>
+      </c>
+      <c r="AU213" s="10">
+        <v>1.82</v>
+      </c>
     </row>
-    <row r="214" spans="2:45">
+    <row r="214" spans="2:47">
       <c r="B214" s="2">
         <v>2002</v>
       </c>
@@ -23504,8 +24473,14 @@
       <c r="AS214" s="10">
         <v>21.360833333333332</v>
       </c>
+      <c r="AT214" s="3">
+        <v>2.7568000000000001</v>
+      </c>
+      <c r="AU214" s="10">
+        <v>1.73</v>
+      </c>
     </row>
-    <row r="215" spans="2:45">
+    <row r="215" spans="2:47">
       <c r="B215" s="2">
         <v>2002.25</v>
       </c>
@@ -23638,8 +24613,14 @@
       <c r="AS215" s="10">
         <v>21.643125000000001</v>
       </c>
+      <c r="AT215" s="3">
+        <v>3.1526999999999998</v>
+      </c>
+      <c r="AU215" s="10">
+        <v>1.75</v>
+      </c>
     </row>
-    <row r="216" spans="2:45">
+    <row r="216" spans="2:47">
       <c r="B216" s="2">
         <v>2002.5</v>
       </c>
@@ -23772,8 +24753,14 @@
       <c r="AS216" s="10">
         <v>35.068437500000002</v>
       </c>
+      <c r="AT216" s="3">
+        <v>4.1440999999999999</v>
+      </c>
+      <c r="AU216" s="10">
+        <v>1.75</v>
+      </c>
     </row>
-    <row r="217" spans="2:45">
+    <row r="217" spans="2:47">
       <c r="B217" s="2">
         <v>2002.75</v>
       </c>
@@ -23906,8 +24893,14 @@
       <c r="AS217" s="10">
         <v>30.72671875</v>
       </c>
+      <c r="AT217" s="3">
+        <v>3.87</v>
+      </c>
+      <c r="AU217" s="10">
+        <v>1.24</v>
+      </c>
     </row>
-    <row r="218" spans="2:45">
+    <row r="218" spans="2:47">
       <c r="B218" s="2">
         <v>2003</v>
       </c>
@@ -24040,8 +25033,14 @@
       <c r="AS218" s="10">
         <v>30.022622950819674</v>
       </c>
+      <c r="AT218" s="3">
+        <v>3.2366999999999999</v>
+      </c>
+      <c r="AU218" s="10">
+        <v>1.25</v>
+      </c>
     </row>
-    <row r="219" spans="2:45">
+    <row r="219" spans="2:47">
       <c r="B219" s="2">
         <v>2003.25</v>
       </c>
@@ -24174,8 +25173,14 @@
       <c r="AS219" s="10">
         <v>21.53126984126984</v>
       </c>
+      <c r="AT219" s="3">
+        <v>2.6349999999999998</v>
+      </c>
+      <c r="AU219" s="10">
+        <v>1.22</v>
+      </c>
     </row>
-    <row r="220" spans="2:45">
+    <row r="220" spans="2:47">
       <c r="B220" s="2">
         <v>2003.5</v>
       </c>
@@ -24308,8 +25313,14 @@
       <c r="AS220" s="10">
         <v>19.32015625</v>
       </c>
+      <c r="AT220" s="3">
+        <v>2.359</v>
+      </c>
+      <c r="AU220" s="10">
+        <v>1.01</v>
+      </c>
     </row>
-    <row r="221" spans="2:45">
+    <row r="221" spans="2:47">
       <c r="B221" s="2">
         <v>2003.75</v>
       </c>
@@ -24442,8 +25453,14 @@
       <c r="AS221" s="10">
         <v>17.427187499999999</v>
       </c>
+      <c r="AT221" s="3">
+        <v>1.982</v>
+      </c>
+      <c r="AU221" s="10">
+        <v>0.98</v>
+      </c>
     </row>
-    <row r="222" spans="2:45">
+    <row r="222" spans="2:47">
       <c r="B222" s="2">
         <v>2004</v>
       </c>
@@ -24576,8 +25593,14 @@
       <c r="AS222" s="10">
         <v>16.658064516129031</v>
       </c>
+      <c r="AT222" s="3">
+        <v>1.8884000000000001</v>
+      </c>
+      <c r="AU222" s="10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="223" spans="2:45">
+    <row r="223" spans="2:47">
       <c r="B223" s="2">
         <v>2004.25</v>
       </c>
@@ -24710,8 +25733,14 @@
       <c r="AS223" s="10">
         <v>16.230161290322581</v>
       </c>
+      <c r="AT223" s="3">
+        <v>1.8445</v>
+      </c>
+      <c r="AU223" s="10">
+        <v>1.03</v>
+      </c>
     </row>
-    <row r="224" spans="2:45">
+    <row r="224" spans="2:47">
       <c r="B224" s="2">
         <v>2004.5</v>
       </c>
@@ -24844,8 +25873,14 @@
       <c r="AS224" s="10">
         <v>15.442187499999999</v>
       </c>
+      <c r="AT224" s="3">
+        <v>1.8208</v>
+      </c>
+      <c r="AU224" s="10">
+        <v>1.61</v>
+      </c>
     </row>
-    <row r="225" spans="2:45">
+    <row r="225" spans="2:47">
       <c r="B225" s="2">
         <v>2004.75</v>
       </c>
@@ -24978,8 +26013,14 @@
       <c r="AS225" s="10">
         <v>13.651249999999999</v>
       </c>
+      <c r="AT225" s="3">
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="AU225" s="10">
+        <v>2.16</v>
+      </c>
     </row>
-    <row r="226" spans="2:45">
+    <row r="226" spans="2:47">
       <c r="B226" s="2">
         <v>2005</v>
       </c>
@@ -25112,8 +26153,14 @@
       <c r="AS226" s="10">
         <v>12.78704918032787</v>
       </c>
+      <c r="AT226" s="3">
+        <v>1.8519000000000001</v>
+      </c>
+      <c r="AU226" s="10">
+        <v>2.63</v>
+      </c>
     </row>
-    <row r="227" spans="2:45">
+    <row r="227" spans="2:47">
       <c r="B227" s="2">
         <v>2005.25</v>
       </c>
@@ -25246,8 +26293,14 @@
       <c r="AS227" s="10">
         <v>13.407343750000001</v>
       </c>
+      <c r="AT227" s="3">
+        <v>1.9699</v>
+      </c>
+      <c r="AU227" s="10">
+        <v>3.04</v>
+      </c>
     </row>
-    <row r="228" spans="2:45">
+    <row r="228" spans="2:47">
       <c r="B228" s="2">
         <v>2005.5</v>
       </c>
@@ -25380,8 +26433,14 @@
       <c r="AS228" s="10">
         <v>12.250781249999999</v>
       </c>
+      <c r="AT228" s="3">
+        <v>1.7806999999999999</v>
+      </c>
+      <c r="AU228" s="10">
+        <v>3.62</v>
+      </c>
     </row>
-    <row r="229" spans="2:45">
+    <row r="229" spans="2:47">
       <c r="B229" s="2">
         <v>2005.75</v>
       </c>
@@ -25514,8 +26573,14 @@
       <c r="AS229" s="10">
         <v>12.781746031746032</v>
       </c>
+      <c r="AT229" s="3">
+        <v>1.8502000000000001</v>
+      </c>
+      <c r="AU229" s="10">
+        <v>4.16</v>
+      </c>
     </row>
-    <row r="230" spans="2:45">
+    <row r="230" spans="2:47">
       <c r="B230" s="2">
         <v>2006</v>
       </c>
@@ -25648,8 +26713,14 @@
       <c r="AS230" s="10">
         <v>12.04241935483871</v>
       </c>
+      <c r="AT230" s="3">
+        <v>1.6903999999999999</v>
+      </c>
+      <c r="AU230" s="10">
+        <v>4.59</v>
+      </c>
     </row>
-    <row r="231" spans="2:45">
+    <row r="231" spans="2:47">
       <c r="B231" s="2">
         <v>2006.25</v>
       </c>
@@ -25780,8 +26851,14 @@
       <c r="AS231" s="10">
         <v>14.528730158730159</v>
       </c>
+      <c r="AT231" s="3">
+        <v>1.6846000000000001</v>
+      </c>
+      <c r="AU231" s="10">
+        <v>4.99</v>
+      </c>
     </row>
-    <row r="232" spans="2:45">
+    <row r="232" spans="2:47">
       <c r="B232" s="2">
         <v>2006.5</v>
       </c>
@@ -25912,8 +26989,14 @@
       <c r="AS232" s="10">
         <v>13.607936507936508</v>
       </c>
+      <c r="AT232" s="3">
+        <v>1.772</v>
+      </c>
+      <c r="AU232" s="10">
+        <v>5.25</v>
+      </c>
     </row>
-    <row r="233" spans="2:45">
+    <row r="233" spans="2:47">
       <c r="B233" s="2">
         <v>2006.75</v>
       </c>
@@ -26044,8 +27127,14 @@
       <c r="AS233" s="10">
         <v>11.034920634920635</v>
       </c>
+      <c r="AT233" s="3">
+        <v>1.6173999999999999</v>
+      </c>
+      <c r="AU233" s="10">
+        <v>5.24</v>
+      </c>
     </row>
-    <row r="234" spans="2:45">
+    <row r="234" spans="2:47">
       <c r="B234" s="2">
         <v>2007</v>
       </c>
@@ -26161,8 +27250,14 @@
       <c r="AS234" s="10">
         <v>12.563606557377049</v>
       </c>
+      <c r="AT234" s="3">
+        <v>1.5329999999999999</v>
+      </c>
+      <c r="AU234" s="10">
+        <v>5.26</v>
+      </c>
     </row>
-    <row r="235" spans="2:45">
+    <row r="235" spans="2:47">
       <c r="B235" s="2">
         <v>2007.25</v>
       </c>
@@ -26278,8 +27373,14 @@
       <c r="AS235" s="10">
         <v>13.731904761904762</v>
       </c>
+      <c r="AT235" s="3">
+        <v>1.6978</v>
+      </c>
+      <c r="AU235" s="10">
+        <v>5.25</v>
+      </c>
     </row>
-    <row r="236" spans="2:45">
+    <row r="236" spans="2:47">
       <c r="B236" s="2">
         <v>2007.5</v>
       </c>
@@ -26395,8 +27496,14 @@
       <c r="AS236" s="10">
         <v>21.58920634920635</v>
       </c>
+      <c r="AT236" s="3">
+        <v>2.2343999999999999</v>
+      </c>
+      <c r="AU236" s="10">
+        <v>4.9400000000000004</v>
+      </c>
     </row>
-    <row r="237" spans="2:45">
+    <row r="237" spans="2:47">
       <c r="B237" s="2">
         <v>2007.75</v>
       </c>
@@ -26512,8 +27619,14 @@
       <c r="AS237" s="10">
         <v>22.029843750000001</v>
       </c>
+      <c r="AT237" s="3">
+        <v>2.7972999999999999</v>
+      </c>
+      <c r="AU237" s="10">
+        <v>4.24</v>
+      </c>
     </row>
-    <row r="238" spans="2:45">
+    <row r="238" spans="2:47">
       <c r="B238" s="2">
         <v>2008</v>
       </c>
@@ -26629,8 +27742,14 @@
       <c r="AS238" s="10">
         <v>26.12016393442623</v>
       </c>
+      <c r="AT238" s="3">
+        <v>3.5019999999999998</v>
+      </c>
+      <c r="AU238" s="10">
+        <v>2.61</v>
+      </c>
     </row>
-    <row r="239" spans="2:45">
+    <row r="239" spans="2:47">
       <c r="B239" s="2">
         <v>2008.25</v>
       </c>
@@ -26746,8 +27865,14 @@
       <c r="AS239" s="10">
         <v>20.672968749999999</v>
       </c>
+      <c r="AT239" s="3">
+        <v>3.4013</v>
+      </c>
+      <c r="AU239" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="240" spans="2:45">
+    <row r="240" spans="2:47">
       <c r="B240" s="2">
         <v>2008.5</v>
       </c>
@@ -26863,8 +27988,14 @@
       <c r="AS240" s="10">
         <v>25.073281250000001</v>
       </c>
+      <c r="AT240" s="3">
+        <v>4.8465999999999996</v>
+      </c>
+      <c r="AU240" s="10">
+        <v>1.81</v>
+      </c>
     </row>
-    <row r="241" spans="2:45">
+    <row r="241" spans="2:47">
       <c r="B241" s="2">
         <v>2008.75</v>
       </c>
@@ -26980,8 +28111,14 @@
       <c r="AS241" s="10">
         <v>58.595937499999998</v>
       </c>
+      <c r="AT241" s="3">
+        <v>7.2518000000000002</v>
+      </c>
+      <c r="AU241" s="10">
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="242" spans="2:45">
+    <row r="242" spans="2:47">
       <c r="B242" s="2">
         <v>2009</v>
       </c>
@@ -27097,8 +28234,14 @@
       <c r="AS242" s="10">
         <v>45</v>
       </c>
+      <c r="AT242" s="3">
+        <v>6.0926</v>
+      </c>
+      <c r="AU242" s="10">
+        <v>0.18</v>
+      </c>
     </row>
-    <row r="243" spans="2:45">
+    <row r="243" spans="2:47">
       <c r="B243" s="2">
         <v>2009.25</v>
       </c>
@@ -27214,8 +28357,14 @@
       <c r="AS243" s="10">
         <v>33.015714285714289</v>
       </c>
+      <c r="AT243" s="3">
+        <v>4.5029000000000003</v>
+      </c>
+      <c r="AU243" s="10">
+        <v>0.21</v>
+      </c>
     </row>
-    <row r="244" spans="2:45">
+    <row r="244" spans="2:47">
       <c r="B244" s="2">
         <v>2009.5</v>
       </c>
@@ -27331,8 +28480,14 @@
       <c r="AS244" s="10">
         <v>25.486249999999998</v>
       </c>
+      <c r="AT244" s="3">
+        <v>3.1901999999999999</v>
+      </c>
+      <c r="AU244" s="10">
+        <v>0.15</v>
+      </c>
     </row>
-    <row r="245" spans="2:45">
+    <row r="245" spans="2:47">
       <c r="B245" s="2">
         <v>2009.75</v>
       </c>
@@ -27448,8 +28603,14 @@
       <c r="AS245" s="10">
         <v>23.07015625</v>
       </c>
+      <c r="AT245" s="3">
+        <v>2.6547999999999998</v>
+      </c>
+      <c r="AU245" s="10">
+        <v>0.12</v>
+      </c>
     </row>
-    <row r="246" spans="2:45">
+    <row r="246" spans="2:47">
       <c r="B246" s="2">
         <v>2010</v>
       </c>
@@ -27563,8 +28724,14 @@
       <c r="AS246" s="10">
         <v>20.14967213114754</v>
       </c>
+      <c r="AT246" s="3">
+        <v>2.3338000000000001</v>
+      </c>
+      <c r="AU246" s="10">
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="247" spans="2:45">
+    <row r="247" spans="2:47">
       <c r="B247" s="2">
         <v>2010.25</v>
       </c>
@@ -27678,8 +28845,14 @@
       <c r="AS247" s="10">
         <v>26.39142857142857</v>
       </c>
+      <c r="AT247" s="3">
+        <v>2.5171999999999999</v>
+      </c>
+      <c r="AU247" s="10">
+        <v>0.18</v>
+      </c>
     </row>
-    <row r="248" spans="2:45">
+    <row r="248" spans="2:47">
       <c r="B248" s="2">
         <v>2010.5</v>
       </c>
@@ -27793,8 +28966,14 @@
       <c r="AS248" s="10">
         <v>24.283593750000001</v>
       </c>
+      <c r="AT248" s="3">
+        <v>2.5743</v>
+      </c>
+      <c r="AU248" s="10">
+        <v>0.19</v>
+      </c>
     </row>
-    <row r="249" spans="2:45">
+    <row r="249" spans="2:47">
       <c r="B249" s="2">
         <v>2010.75</v>
       </c>
@@ -27908,8 +29087,14 @@
       <c r="AS249" s="10">
         <v>19.318437500000002</v>
       </c>
+      <c r="AT249" s="3">
+        <v>2.3157999999999999</v>
+      </c>
+      <c r="AU249" s="10">
+        <v>0.18</v>
+      </c>
     </row>
-    <row r="250" spans="2:45">
+    <row r="250" spans="2:47">
       <c r="B250" s="2">
         <v>2011</v>
       </c>
@@ -28023,8 +29208,14 @@
       <c r="AS250" s="10">
         <v>18.614838709677418</v>
       </c>
+      <c r="AT250" s="3">
+        <v>2.0299</v>
+      </c>
+      <c r="AU250" s="10">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
-    <row r="251" spans="2:45">
+    <row r="251" spans="2:47">
       <c r="B251" s="2">
         <v>2011.25</v>
       </c>
@@ -28138,8 +29329,14 @@
       <c r="AS251" s="10">
         <v>17.482380952380954</v>
       </c>
+      <c r="AT251" s="3">
+        <v>2.1107</v>
+      </c>
+      <c r="AU251" s="10">
+        <v>0.09</v>
+      </c>
     </row>
-    <row r="252" spans="2:45">
+    <row r="252" spans="2:47">
       <c r="B252" s="2">
         <v>2011.5</v>
       </c>
@@ -28253,8 +29450,14 @@
       <c r="AS252" s="10">
         <v>30.583593749999999</v>
       </c>
+      <c r="AT252" s="3">
+        <v>2.7482000000000002</v>
+      </c>
+      <c r="AU252" s="10">
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="253" spans="2:45">
+    <row r="253" spans="2:47">
       <c r="B253" s="2">
         <v>2011.75</v>
       </c>
@@ -28368,8 +29571,14 @@
       <c r="AS253" s="10">
         <v>29.939523809523809</v>
       </c>
+      <c r="AT253" s="3">
+        <v>2.8654000000000002</v>
+      </c>
+      <c r="AU253" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
-    <row r="254" spans="2:45">
+    <row r="254" spans="2:47">
       <c r="B254" s="2">
         <v>2012</v>
       </c>
@@ -28483,8 +29692,14 @@
       <c r="AS254" s="10">
         <v>18.204032258064515</v>
       </c>
+      <c r="AT254" s="3">
+        <v>2.5446</v>
+      </c>
+      <c r="AU254" s="10">
+        <v>0.13</v>
+      </c>
     </row>
-    <row r="255" spans="2:45">
+    <row r="255" spans="2:47">
       <c r="B255" s="2">
         <v>2012.25</v>
       </c>
@@ -28598,8 +29813,14 @@
       <c r="AS255" s="10">
         <v>20.035714285714285</v>
       </c>
+      <c r="AT255" s="3">
+        <v>2.6608999999999998</v>
+      </c>
+      <c r="AU255" s="10">
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="256" spans="2:45">
+    <row r="256" spans="2:47">
       <c r="B256" s="2">
         <v>2012.5</v>
       </c>
@@ -28713,8 +29934,14 @@
       <c r="AS256" s="10">
         <v>16.192698412698412</v>
       </c>
+      <c r="AT256" s="3">
+        <v>2.4359999999999999</v>
+      </c>
+      <c r="AU256" s="10">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
-    <row r="257" spans="2:45">
+    <row r="257" spans="2:47">
       <c r="B257" s="2">
         <v>2012.75</v>
       </c>
@@ -28828,8 +30055,14 @@
       <c r="AS257" s="10">
         <v>16.752903225806453</v>
       </c>
+      <c r="AT257" s="3">
+        <v>2.2204999999999999</v>
+      </c>
+      <c r="AU257" s="10">
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="258" spans="2:45">
+    <row r="258" spans="2:47">
       <c r="B258" s="2">
         <v>2013</v>
       </c>
@@ -28943,8 +30176,14 @@
       <c r="AS258" s="10">
         <v>13.526999999999999</v>
       </c>
+      <c r="AT258" s="3">
+        <v>2.1053999999999999</v>
+      </c>
+      <c r="AU258" s="10">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
-    <row r="259" spans="2:45">
+    <row r="259" spans="2:47">
       <c r="B259" s="2">
         <v>2013.25</v>
       </c>
@@ -29058,8 +30297,14 @@
       <c r="AS259" s="10">
         <v>14.837031250000001</v>
       </c>
+      <c r="AT259" s="3">
+        <v>2.0493000000000001</v>
+      </c>
+      <c r="AU259" s="10">
+        <v>0.09</v>
+      </c>
     </row>
-    <row r="260" spans="2:45">
+    <row r="260" spans="2:47">
       <c r="B260" s="2">
         <v>2013.5</v>
       </c>
@@ -29173,8 +30418,14 @@
       <c r="AS260" s="10">
         <v>14.2796875</v>
       </c>
+      <c r="AT260" s="3">
+        <v>2.0004</v>
+      </c>
+      <c r="AU260" s="10">
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="261" spans="2:45">
+    <row r="261" spans="2:47">
       <c r="B261" s="2">
         <v>2013.75</v>
       </c>
@@ -29288,8 +30539,14 @@
       <c r="AS261" s="10">
         <v>14.2328125</v>
       </c>
+      <c r="AT261" s="3">
+        <v>1.8586</v>
+      </c>
+      <c r="AU261" s="10">
+        <v>0.09</v>
+      </c>
     </row>
-    <row r="262" spans="2:45">
+    <row r="262" spans="2:47">
       <c r="B262" s="2">
         <v>2014</v>
       </c>
@@ -29403,8 +30660,14 @@
       <c r="AS262" s="10">
         <v>14.828852459016394</v>
       </c>
+      <c r="AT262" s="3">
+        <v>1.6918</v>
+      </c>
+      <c r="AU262" s="10">
+        <v>0.08</v>
+      </c>
     </row>
-    <row r="263" spans="2:45">
+    <row r="263" spans="2:47">
       <c r="B263" s="2">
         <v>2014.25</v>
       </c>
@@ -29518,8 +30781,14 @@
       <c r="AS263" s="10">
         <v>12.738253968253968</v>
       </c>
+      <c r="AT263" s="3">
+        <v>1.5889</v>
+      </c>
+      <c r="AU263" s="10">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="264" spans="2:45">
+    <row r="264" spans="2:47">
       <c r="B264" s="2">
         <v>2014.5</v>
       </c>
@@ -29633,8 +30902,14 @@
       <c r="AS264" s="10">
         <v>13.07265625</v>
       </c>
+      <c r="AT264" s="3">
+        <v>1.6941999999999999</v>
+      </c>
+      <c r="AU264" s="10">
+        <v>0.09</v>
+      </c>
     </row>
-    <row r="265" spans="2:45">
+    <row r="265" spans="2:47">
       <c r="B265" s="2">
         <v>2014.75</v>
       </c>
@@ -29748,8 +31023,14 @@
       <c r="AS265" s="10">
         <v>16.072343750000002</v>
       </c>
+      <c r="AT265" s="3">
+        <v>1.9925999999999999</v>
+      </c>
+      <c r="AU265" s="10">
+        <v>0.12</v>
+      </c>
     </row>
-    <row r="266" spans="2:45">
+    <row r="266" spans="2:47">
       <c r="B266" s="2">
         <v>2015</v>
       </c>
@@ -29863,8 +31144,14 @@
       <c r="AS266" s="10">
         <v>16.564754098360655</v>
       </c>
+      <c r="AT266" s="3">
+        <v>2.0068999999999999</v>
+      </c>
+      <c r="AU266" s="10">
+        <v>0.11</v>
+      </c>
     </row>
-    <row r="267" spans="2:45">
+    <row r="267" spans="2:47">
       <c r="B267" s="2">
         <v>2015.25</v>
       </c>
@@ -29978,8 +31265,14 @@
       <c r="AS267" s="10">
         <v>13.740158730158731</v>
       </c>
+      <c r="AT267" s="3">
+        <v>2.0863999999999998</v>
+      </c>
+      <c r="AU267" s="10">
+        <v>0.13</v>
+      </c>
     </row>
-    <row r="268" spans="2:45">
+    <row r="268" spans="2:47">
       <c r="B268" s="2">
         <v>2015.5</v>
       </c>
@@ -30093,8 +31386,14 @@
       <c r="AS268" s="10">
         <v>19.307343750000001</v>
       </c>
+      <c r="AT268" s="3">
+        <v>2.3969999999999998</v>
+      </c>
+      <c r="AU268" s="10">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
-    <row r="269" spans="2:45">
+    <row r="269" spans="2:47">
       <c r="B269" s="2">
         <v>2015.75</v>
       </c>
@@ -30208,8 +31507,14 @@
       <c r="AS269" s="10">
         <v>17.033281250000002</v>
       </c>
+      <c r="AT269" s="3">
+        <v>2.6116000000000001</v>
+      </c>
+      <c r="AU269" s="10">
+        <v>0.24</v>
+      </c>
     </row>
-    <row r="270" spans="2:45">
+    <row r="270" spans="2:47">
       <c r="B270" s="2">
         <v>2016</v>
       </c>
@@ -30323,8 +31628,14 @@
       <c r="AS270" s="10">
         <v>20.486229508196722</v>
       </c>
+      <c r="AT270" s="3">
+        <v>2.6930000000000001</v>
+      </c>
+      <c r="AU270" s="10">
+        <v>0.36</v>
+      </c>
     </row>
-    <row r="271" spans="2:45">
+    <row r="271" spans="2:47">
       <c r="B271" s="2">
         <v>2016.25</v>
       </c>
@@ -30438,8 +31749,14 @@
       <c r="AS271" s="10">
         <v>15.6759375</v>
       </c>
+      <c r="AT271" s="3">
+        <v>2.0855000000000001</v>
+      </c>
+      <c r="AU271" s="10">
+        <v>0.38</v>
+      </c>
     </row>
-    <row r="272" spans="2:45">
+    <row r="272" spans="2:47">
       <c r="B272" s="2">
         <v>2016.5</v>
       </c>
@@ -30553,8 +31870,11 @@
       <c r="AS272" s="10">
         <v>13.23390625</v>
       </c>
+      <c r="AU272" s="10">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="273" spans="2:45">
+    <row r="273" spans="2:47">
       <c r="B273" s="2">
         <v>2016.75</v>
       </c>
@@ -30668,8 +31988,11 @@
       <c r="AS273" s="10">
         <v>14.097936507936508</v>
       </c>
+      <c r="AU273" s="10">
+        <v>0.54</v>
+      </c>
     </row>
-    <row r="274" spans="2:45">
+    <row r="274" spans="2:47">
       <c r="B274" s="2">
         <v>2017</v>
       </c>
@@ -30783,8 +32106,11 @@
       <c r="AS274" s="10">
         <v>11.691935483870967</v>
       </c>
+      <c r="AU274" s="10">
+        <v>0.79</v>
+      </c>
     </row>
-    <row r="275" spans="2:45">
+    <row r="275" spans="2:47">
       <c r="B275" s="2">
         <v>2017.25</v>
       </c>
@@ -30898,8 +32224,11 @@
       <c r="AS275" s="10">
         <v>11.426349206349206</v>
       </c>
+      <c r="AU275" s="10">
+        <v>1.04</v>
+      </c>
     </row>
-    <row r="276" spans="2:45">
+    <row r="276" spans="2:47">
       <c r="B276" s="2">
         <v>2017.5</v>
       </c>
@@ -30998,8 +32327,11 @@
       <c r="AS276" s="10">
         <v>10.944285714285714</v>
       </c>
+      <c r="AU276" s="10">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
-    <row r="277" spans="2:45">
+    <row r="277" spans="2:47">
       <c r="B277" s="2">
         <v>2017.75</v>
       </c>
@@ -31064,8 +32396,9 @@
       <c r="AS277" s="10">
         <v>10.307936507936509</v>
       </c>
+      <c r="AU277" s="10"/>
     </row>
-    <row r="278" spans="2:45">
+    <row r="278" spans="2:47">
       <c r="B278" s="2">
         <v>2018</v>
       </c>
@@ -31130,8 +32463,9 @@
       <c r="AS278" s="10">
         <v>17.354754098360655</v>
       </c>
+      <c r="AU278" s="10"/>
     </row>
-    <row r="279" spans="2:45">
+    <row r="279" spans="2:47">
       <c r="B279" s="2">
         <v>2018.25</v>
       </c>
@@ -31196,8 +32530,9 @@
       <c r="AS279" s="10">
         <v>15.3375</v>
       </c>
+      <c r="AU279" s="10"/>
     </row>
-    <row r="280" spans="2:45">
+    <row r="280" spans="2:47">
       <c r="J280" s="4"/>
       <c r="K280" s="11"/>
       <c r="N280" s="4"/>
@@ -31216,8 +32551,9 @@
       <c r="AA280" s="2"/>
       <c r="AR280" s="9"/>
       <c r="AS280" s="10"/>
+      <c r="AU280" s="10"/>
     </row>
-    <row r="281" spans="2:45">
+    <row r="281" spans="2:47">
       <c r="J281" s="4"/>
       <c r="K281" s="11"/>
       <c r="N281" s="4"/>
@@ -31236,8 +32572,9 @@
       <c r="AA281" s="2"/>
       <c r="AR281" s="9"/>
       <c r="AS281" s="10"/>
+      <c r="AU281" s="10"/>
     </row>
-    <row r="282" spans="2:45">
+    <row r="282" spans="2:47">
       <c r="J282" s="4"/>
       <c r="K282" s="11"/>
       <c r="N282" s="4"/>
@@ -31255,232 +32592,272 @@
       <c r="Z282" s="4"/>
       <c r="AA282" s="2"/>
       <c r="AR282" s="9"/>
+      <c r="AU282" s="10"/>
     </row>
-    <row r="283" spans="2:45">
+    <row r="283" spans="2:47">
       <c r="J283" s="4"/>
       <c r="K283" s="11"/>
       <c r="AA283" s="2"/>
       <c r="AR283" s="9"/>
+      <c r="AU283" s="10"/>
     </row>
-    <row r="284" spans="2:45">
+    <row r="284" spans="2:47">
       <c r="J284" s="4"/>
       <c r="K284" s="11"/>
       <c r="AA284" s="2"/>
       <c r="AR284" s="9"/>
+      <c r="AU284" s="10"/>
     </row>
-    <row r="285" spans="2:45">
+    <row r="285" spans="2:47">
       <c r="J285" s="4"/>
       <c r="K285" s="11"/>
       <c r="AA285" s="2"/>
       <c r="AR285" s="9"/>
+      <c r="AU285" s="10"/>
     </row>
-    <row r="286" spans="2:45">
+    <row r="286" spans="2:47">
       <c r="J286" s="4"/>
       <c r="K286" s="11"/>
       <c r="AA286" s="2"/>
       <c r="AR286" s="9"/>
+      <c r="AU286" s="10"/>
     </row>
-    <row r="287" spans="2:45">
+    <row r="287" spans="2:47">
       <c r="J287" s="4"/>
       <c r="K287" s="11"/>
       <c r="AA287" s="2"/>
       <c r="AR287" s="9"/>
+      <c r="AU287" s="10"/>
     </row>
-    <row r="288" spans="2:45">
+    <row r="288" spans="2:47">
       <c r="J288" s="4"/>
       <c r="K288" s="11"/>
       <c r="AA288" s="2"/>
       <c r="AR288" s="9"/>
+      <c r="AU288" s="10"/>
     </row>
-    <row r="289" spans="10:44">
+    <row r="289" spans="10:47">
       <c r="J289" s="4"/>
       <c r="K289" s="11"/>
       <c r="AA289" s="2"/>
       <c r="AR289" s="9"/>
+      <c r="AU289" s="10"/>
     </row>
-    <row r="290" spans="10:44">
+    <row r="290" spans="10:47">
       <c r="J290" s="4"/>
       <c r="K290" s="11"/>
       <c r="AA290" s="2"/>
       <c r="AR290" s="9"/>
+      <c r="AU290" s="10"/>
     </row>
-    <row r="291" spans="10:44">
+    <row r="291" spans="10:47">
       <c r="J291" s="4"/>
       <c r="K291" s="11"/>
       <c r="AA291" s="2"/>
       <c r="AR291" s="9"/>
+      <c r="AU291" s="10"/>
     </row>
-    <row r="292" spans="10:44">
+    <row r="292" spans="10:47">
       <c r="J292" s="4"/>
       <c r="K292" s="11"/>
       <c r="AA292" s="2"/>
       <c r="AR292" s="9"/>
+      <c r="AU292" s="10"/>
     </row>
-    <row r="293" spans="10:44">
+    <row r="293" spans="10:47">
       <c r="J293" s="4"/>
       <c r="K293" s="11"/>
       <c r="AA293" s="2"/>
       <c r="AR293" s="9"/>
+      <c r="AU293" s="10"/>
     </row>
-    <row r="294" spans="10:44">
+    <row r="294" spans="10:47">
       <c r="J294" s="4"/>
       <c r="K294" s="11"/>
       <c r="AA294" s="2"/>
       <c r="AR294" s="9"/>
+      <c r="AU294" s="10"/>
     </row>
-    <row r="295" spans="10:44">
+    <row r="295" spans="10:47">
       <c r="J295" s="4"/>
       <c r="K295" s="11"/>
       <c r="AA295" s="2"/>
       <c r="AR295" s="9"/>
+      <c r="AU295" s="10"/>
     </row>
-    <row r="296" spans="10:44">
+    <row r="296" spans="10:47">
       <c r="J296" s="4"/>
       <c r="K296" s="11"/>
       <c r="AA296" s="2"/>
       <c r="AR296" s="9"/>
+      <c r="AU296" s="10"/>
     </row>
-    <row r="297" spans="10:44">
+    <row r="297" spans="10:47">
       <c r="J297" s="4"/>
       <c r="K297" s="11"/>
       <c r="AA297" s="2"/>
       <c r="AR297" s="9"/>
+      <c r="AU297" s="10"/>
     </row>
-    <row r="298" spans="10:44">
+    <row r="298" spans="10:47">
       <c r="K298" s="11"/>
       <c r="AA298" s="2"/>
       <c r="AR298" s="9"/>
+      <c r="AU298" s="10"/>
     </row>
-    <row r="299" spans="10:44">
+    <row r="299" spans="10:47">
       <c r="K299" s="11"/>
       <c r="L299" s="5" t="s">
         <v>49</v>
       </c>
       <c r="AA299" s="2"/>
       <c r="AR299" s="9"/>
+      <c r="AU299" s="10"/>
     </row>
-    <row r="300" spans="10:44">
+    <row r="300" spans="10:47">
       <c r="K300" s="11"/>
       <c r="AA300" s="2"/>
       <c r="AR300" s="9"/>
+      <c r="AU300" s="10"/>
     </row>
-    <row r="301" spans="10:44">
+    <row r="301" spans="10:47">
       <c r="K301" s="11"/>
       <c r="AA301" s="2"/>
       <c r="AR301" s="9"/>
+      <c r="AU301" s="10"/>
     </row>
-    <row r="302" spans="10:44">
+    <row r="302" spans="10:47">
       <c r="K302" s="11"/>
       <c r="AA302" s="2"/>
       <c r="AR302" s="9"/>
+      <c r="AU302" s="10"/>
     </row>
-    <row r="303" spans="10:44">
+    <row r="303" spans="10:47">
       <c r="K303" s="11"/>
       <c r="AA303" s="2"/>
       <c r="AR303" s="9"/>
+      <c r="AU303" s="10"/>
     </row>
-    <row r="304" spans="10:44">
+    <row r="304" spans="10:47">
       <c r="K304" s="11"/>
       <c r="AA304" s="2"/>
       <c r="AR304" s="9"/>
+      <c r="AU304" s="10"/>
     </row>
-    <row r="305" spans="11:44">
+    <row r="305" spans="11:47">
       <c r="K305" s="11"/>
       <c r="AA305" s="2"/>
       <c r="AR305" s="9"/>
+      <c r="AU305" s="10"/>
     </row>
-    <row r="306" spans="11:44">
+    <row r="306" spans="11:47">
       <c r="K306" s="11"/>
       <c r="AA306" s="2"/>
       <c r="AR306" s="9"/>
+      <c r="AU306" s="10"/>
     </row>
-    <row r="307" spans="11:44">
+    <row r="307" spans="11:47">
       <c r="K307" s="11"/>
       <c r="AA307" s="2"/>
       <c r="AR307" s="9"/>
+      <c r="AU307" s="10"/>
     </row>
-    <row r="308" spans="11:44">
+    <row r="308" spans="11:47">
       <c r="K308" s="11"/>
       <c r="AA308" s="2"/>
       <c r="AR308" s="9"/>
+      <c r="AU308" s="10"/>
     </row>
-    <row r="309" spans="11:44">
+    <row r="309" spans="11:47">
       <c r="K309" s="11"/>
       <c r="AA309" s="2"/>
       <c r="AR309" s="9"/>
+      <c r="AU309" s="10"/>
     </row>
-    <row r="310" spans="11:44">
+    <row r="310" spans="11:47">
       <c r="K310" s="11"/>
       <c r="AA310" s="2"/>
       <c r="AR310" s="9"/>
+      <c r="AU310" s="10"/>
     </row>
-    <row r="311" spans="11:44">
+    <row r="311" spans="11:47">
       <c r="K311" s="11"/>
       <c r="AA311" s="2"/>
       <c r="AR311" s="9"/>
+      <c r="AU311" s="10"/>
     </row>
-    <row r="312" spans="11:44">
+    <row r="312" spans="11:47">
       <c r="K312" s="11"/>
       <c r="AA312" s="2"/>
       <c r="AR312" s="9"/>
+      <c r="AU312" s="10"/>
     </row>
-    <row r="313" spans="11:44">
+    <row r="313" spans="11:47">
       <c r="K313" s="11"/>
       <c r="AA313" s="2"/>
       <c r="AR313" s="9"/>
+      <c r="AU313" s="10"/>
     </row>
-    <row r="314" spans="11:44">
+    <row r="314" spans="11:47">
       <c r="K314" s="11"/>
       <c r="AA314" s="2"/>
       <c r="AR314" s="9"/>
+      <c r="AU314" s="10"/>
     </row>
-    <row r="315" spans="11:44">
+    <row r="315" spans="11:47">
       <c r="K315" s="11"/>
       <c r="AA315" s="2"/>
       <c r="AR315" s="9"/>
+      <c r="AU315" s="10"/>
     </row>
-    <row r="316" spans="11:44">
+    <row r="316" spans="11:47">
       <c r="K316" s="11"/>
       <c r="AA316" s="2"/>
       <c r="AR316" s="9"/>
+      <c r="AU316" s="10"/>
     </row>
-    <row r="317" spans="11:44">
+    <row r="317" spans="11:47">
       <c r="K317" s="11"/>
       <c r="AA317" s="2"/>
       <c r="AR317" s="9"/>
+      <c r="AU317" s="10"/>
     </row>
-    <row r="318" spans="11:44">
+    <row r="318" spans="11:47">
       <c r="AA318" s="2"/>
       <c r="AR318" s="9"/>
+      <c r="AU318" s="10"/>
     </row>
-    <row r="319" spans="11:44">
+    <row r="319" spans="11:47">
       <c r="AA319" s="2"/>
       <c r="AR319" s="9"/>
+      <c r="AU319" s="10"/>
     </row>
-    <row r="320" spans="11:44">
+    <row r="320" spans="11:47">
       <c r="AA320" s="2"/>
       <c r="AR320" s="9"/>
+      <c r="AU320" s="10"/>
     </row>
-    <row r="321" spans="27:44">
+    <row r="321" spans="27:47">
       <c r="AA321" s="2"/>
       <c r="AR321" s="9"/>
+      <c r="AU321" s="10"/>
     </row>
-    <row r="322" spans="27:44">
+    <row r="322" spans="27:47">
       <c r="AA322" s="2"/>
     </row>
-    <row r="323" spans="27:44">
+    <row r="323" spans="27:47">
       <c r="AA323" s="2"/>
     </row>
-    <row r="324" spans="27:44">
+    <row r="324" spans="27:47">
       <c r="AA324" s="2"/>
     </row>
-    <row r="325" spans="27:44">
+    <row r="325" spans="27:47">
       <c r="AA325" s="2"/>
     </row>
-    <row r="326" spans="27:44">
+    <row r="326" spans="27:47">
       <c r="AA326" s="2"/>
     </row>
-    <row r="327" spans="27:44">
+    <row r="327" spans="27:47">
       <c r="AA327" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bootstrap cumulate first and select later
</commit_message>
<xml_diff>
--- a/Data/main_file.xlsx
+++ b/Data/main_file.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vitocormun 1/Desktop/Literature/Noise_Over_Cycles/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Brianti\Documents\GitHub\Noise_Over_Cycles\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6B9D1E13-66C5-A949-8FD3-38A400FB77EF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990B68FF-EE05-473D-ACB7-DC9B18B05EDF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="25598" windowHeight="15458" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -652,16 +652,16 @@
   <dimension ref="A1:AT327"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AK6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AA6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AK2" sqref="AK2"/>
+      <selection pane="bottomRight" activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="22" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.46484375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.46484375" style="2" customWidth="1"/>
     <col min="3" max="3" width="22" style="3" customWidth="1"/>
     <col min="4" max="5" width="22" style="2"/>
     <col min="6" max="6" width="22" style="3"/>
@@ -926,52 +926,52 @@
         <v>3</v>
       </c>
       <c r="AE2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AH2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AI2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AJ2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AK2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AL2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AM2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AN2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AO2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AP2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AQ2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AR2" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AS2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AT2" s="16">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:46" s="16" customFormat="1">

</xml_diff>

<commit_message>
recovering Barsky Sims 2011
</commit_message>
<xml_diff>
--- a/Data/main_file.xlsx
+++ b/Data/main_file.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>MUNI1Y</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>BloomFinDistress</t>
+  </si>
+  <si>
+    <t>BarskySims_News</t>
   </si>
 </sst>
 </file>
@@ -886,13 +889,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI629"/>
+  <dimension ref="A1:BJ629"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="BA240" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="BB16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BG6" sqref="BG6:BG273"/>
+      <selection pane="bottomRight" activeCell="BK267" sqref="BK267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="15.75"/>
@@ -933,7 +936,7 @@
     <col min="62" max="16384" width="22" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="7" customFormat="1">
+    <row r="1" spans="1:62" s="7" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1117,8 +1120,11 @@
       <c r="BI1" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="BJ1" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="2" spans="1:61" s="7" customFormat="1">
+    <row r="2" spans="1:62" s="7" customFormat="1">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1302,8 +1308,11 @@
       <c r="BI2" s="1">
         <v>3</v>
       </c>
+      <c r="BJ2" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:61" s="7" customFormat="1">
+    <row r="3" spans="1:62" s="7" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1487,8 +1496,11 @@
       <c r="BI3" s="1">
         <v>1</v>
       </c>
+      <c r="BJ3" s="7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:61" s="7" customFormat="1">
+    <row r="4" spans="1:62" s="7" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1672,8 +1684,11 @@
       <c r="BI4" s="1">
         <v>60</v>
       </c>
+      <c r="BJ4" s="7">
+        <v>61</v>
+      </c>
     </row>
-    <row r="5" spans="1:61" s="7" customFormat="1">
+    <row r="5" spans="1:62" s="7" customFormat="1">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -1857,8 +1872,11 @@
       <c r="BI5" s="1">
         <v>60</v>
       </c>
+      <c r="BJ5" s="7">
+        <v>61</v>
+      </c>
     </row>
-    <row r="6" spans="1:61" s="5" customFormat="1">
+    <row r="6" spans="1:62" s="5" customFormat="1">
       <c r="B6" s="5">
         <v>1950</v>
       </c>
@@ -1952,7 +1970,7 @@
         <v>-25.047000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:61" s="5" customFormat="1">
+    <row r="7" spans="1:62" s="5" customFormat="1">
       <c r="B7" s="5">
         <v>1950.25</v>
       </c>
@@ -2046,7 +2064,7 @@
         <v>-25.356999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:61" s="5" customFormat="1">
+    <row r="8" spans="1:62" s="5" customFormat="1">
       <c r="B8" s="5">
         <v>1950.5</v>
       </c>
@@ -2140,7 +2158,7 @@
         <v>-25.962</v>
       </c>
     </row>
-    <row r="9" spans="1:61" s="5" customFormat="1">
+    <row r="9" spans="1:62" s="5" customFormat="1">
       <c r="B9" s="5">
         <v>1950.75</v>
       </c>
@@ -2234,7 +2252,7 @@
         <v>-26.004000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:61" s="5" customFormat="1">
+    <row r="10" spans="1:62" s="5" customFormat="1">
       <c r="B10" s="5">
         <v>1951</v>
       </c>
@@ -2328,7 +2346,7 @@
         <v>-26.062999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:61" s="5" customFormat="1">
+    <row r="11" spans="1:62" s="5" customFormat="1">
       <c r="B11" s="5">
         <v>1951.25</v>
       </c>
@@ -2422,7 +2440,7 @@
         <v>-25.963999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:61" s="5" customFormat="1">
+    <row r="12" spans="1:62" s="5" customFormat="1">
       <c r="B12" s="5">
         <v>1951.5</v>
       </c>
@@ -2516,7 +2534,7 @@
         <v>-26.617999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:61" s="5" customFormat="1">
+    <row r="13" spans="1:62" s="5" customFormat="1">
       <c r="B13" s="5">
         <v>1951.75</v>
       </c>
@@ -2610,7 +2628,7 @@
         <v>-26.686</v>
       </c>
     </row>
-    <row r="14" spans="1:61" s="5" customFormat="1">
+    <row r="14" spans="1:62" s="5" customFormat="1">
       <c r="B14" s="5">
         <v>1952</v>
       </c>
@@ -2707,7 +2725,7 @@
         <v>156522.33333333334</v>
       </c>
     </row>
-    <row r="15" spans="1:61" s="5" customFormat="1">
+    <row r="15" spans="1:62" s="5" customFormat="1">
       <c r="B15" s="5">
         <v>1952.25</v>
       </c>
@@ -2804,7 +2822,7 @@
         <v>157142</v>
       </c>
     </row>
-    <row r="16" spans="1:61" s="5" customFormat="1">
+    <row r="16" spans="1:62" s="5" customFormat="1">
       <c r="B16" s="5">
         <v>1952.5</v>
       </c>
@@ -6296,7 +6314,7 @@
         <v>180951.33333333334</v>
       </c>
     </row>
-    <row r="49" spans="2:61" s="5" customFormat="1">
+    <row r="49" spans="2:62" s="5" customFormat="1">
       <c r="B49" s="5">
         <v>1960.75</v>
       </c>
@@ -6408,7 +6426,7 @@
         <v>181788.66666666666</v>
       </c>
     </row>
-    <row r="50" spans="2:61" s="5" customFormat="1">
+    <row r="50" spans="2:62" s="5" customFormat="1">
       <c r="B50" s="5">
         <v>1961</v>
       </c>
@@ -6519,8 +6537,11 @@
       <c r="BI50" s="5">
         <v>182516.33333333334</v>
       </c>
+      <c r="BJ50" s="5">
+        <v>1.8066305846179943E-2</v>
+      </c>
     </row>
-    <row r="51" spans="2:61" s="5" customFormat="1">
+    <row r="51" spans="2:62" s="5" customFormat="1">
       <c r="B51" s="5">
         <v>1961.25</v>
       </c>
@@ -6631,8 +6652,11 @@
       <c r="BI51" s="5">
         <v>183220.33333333334</v>
       </c>
+      <c r="BJ51" s="5">
+        <v>0.77760697138650436</v>
+      </c>
     </row>
-    <row r="52" spans="2:61" s="5" customFormat="1">
+    <row r="52" spans="2:62" s="5" customFormat="1">
       <c r="B52" s="5">
         <v>1961.5</v>
       </c>
@@ -6743,8 +6767,11 @@
       <c r="BI52" s="5">
         <v>183964</v>
       </c>
+      <c r="BJ52" s="5">
+        <v>-2.6865341405642139E-2</v>
+      </c>
     </row>
-    <row r="53" spans="2:61" s="5" customFormat="1">
+    <row r="53" spans="2:62" s="5" customFormat="1">
       <c r="B53" s="5">
         <v>1961.75</v>
       </c>
@@ -6855,8 +6882,11 @@
       <c r="BI53" s="5">
         <v>184774.33333333334</v>
       </c>
+      <c r="BJ53" s="5">
+        <v>-1.0455617282093341</v>
+      </c>
     </row>
-    <row r="54" spans="2:61" s="5" customFormat="1">
+    <row r="54" spans="2:62" s="5" customFormat="1">
       <c r="B54" s="5">
         <v>1962</v>
       </c>
@@ -6967,8 +6997,11 @@
       <c r="BI54" s="5">
         <v>185448</v>
       </c>
+      <c r="BJ54" s="5">
+        <v>-1.6013540445227588</v>
+      </c>
     </row>
-    <row r="55" spans="2:61" s="5" customFormat="1">
+    <row r="55" spans="2:62" s="5" customFormat="1">
       <c r="B55" s="5">
         <v>1962.25</v>
       </c>
@@ -7079,8 +7112,11 @@
       <c r="BI55" s="5">
         <v>186091.66666666666</v>
       </c>
+      <c r="BJ55" s="5">
+        <v>-0.88075573341854252</v>
+      </c>
     </row>
-    <row r="56" spans="2:61" s="5" customFormat="1">
+    <row r="56" spans="2:62" s="5" customFormat="1">
       <c r="B56" s="5">
         <v>1962.5</v>
       </c>
@@ -7191,8 +7227,11 @@
       <c r="BI56" s="5">
         <v>186795.33333333334</v>
       </c>
+      <c r="BJ56" s="5">
+        <v>6.553053860594274E-2</v>
+      </c>
     </row>
-    <row r="57" spans="2:61" s="5" customFormat="1">
+    <row r="57" spans="2:62" s="5" customFormat="1">
       <c r="B57" s="5">
         <v>1962.75</v>
       </c>
@@ -7303,8 +7342,11 @@
       <c r="BI57" s="5">
         <v>187564.33333333334</v>
       </c>
+      <c r="BJ57" s="5">
+        <v>1.735585487183273</v>
+      </c>
     </row>
-    <row r="58" spans="2:61" s="5" customFormat="1">
+    <row r="58" spans="2:62" s="5" customFormat="1">
       <c r="B58" s="5">
         <v>1963</v>
       </c>
@@ -7415,8 +7457,11 @@
       <c r="BI58" s="5">
         <v>188204.33333333334</v>
       </c>
+      <c r="BJ58" s="5">
+        <v>0.18478526037869225</v>
+      </c>
     </row>
-    <row r="59" spans="2:61" s="5" customFormat="1">
+    <row r="59" spans="2:62" s="5" customFormat="1">
       <c r="B59" s="5">
         <v>1963.25</v>
       </c>
@@ -7527,8 +7572,11 @@
       <c r="BI59" s="5">
         <v>188796</v>
       </c>
+      <c r="BJ59" s="5">
+        <v>-0.19787610598384714</v>
+      </c>
     </row>
-    <row r="60" spans="2:61" s="5" customFormat="1">
+    <row r="60" spans="2:62" s="5" customFormat="1">
       <c r="B60" s="5">
         <v>1963.5</v>
       </c>
@@ -7639,8 +7687,11 @@
       <c r="BI60" s="5">
         <v>189499.66666666666</v>
       </c>
+      <c r="BJ60" s="5">
+        <v>-2.6147161336458153</v>
+      </c>
     </row>
-    <row r="61" spans="2:61" s="5" customFormat="1">
+    <row r="61" spans="2:62" s="5" customFormat="1">
       <c r="B61" s="5">
         <v>1963.75</v>
       </c>
@@ -7751,8 +7802,11 @@
       <c r="BI61" s="5">
         <v>190255</v>
       </c>
+      <c r="BJ61" s="5">
+        <v>0.93629151504747465</v>
+      </c>
     </row>
-    <row r="62" spans="2:61" s="5" customFormat="1">
+    <row r="62" spans="2:62" s="5" customFormat="1">
       <c r="B62" s="5">
         <v>1964</v>
       </c>
@@ -7863,8 +7917,11 @@
       <c r="BI62" s="5">
         <v>190857.66666666666</v>
       </c>
+      <c r="BJ62" s="5">
+        <v>0.23788109749820491</v>
+      </c>
     </row>
-    <row r="63" spans="2:61" s="5" customFormat="1">
+    <row r="63" spans="2:62" s="5" customFormat="1">
       <c r="B63" s="5">
         <v>1964.25</v>
       </c>
@@ -7975,8 +8032,11 @@
       <c r="BI63" s="5">
         <v>191452.66666666666</v>
       </c>
+      <c r="BJ63" s="5">
+        <v>1.6194867597563276</v>
+      </c>
     </row>
-    <row r="64" spans="2:61" s="5" customFormat="1">
+    <row r="64" spans="2:62" s="5" customFormat="1">
       <c r="B64" s="5">
         <v>1964.5</v>
       </c>
@@ -8087,8 +8147,11 @@
       <c r="BI64" s="5">
         <v>192132</v>
       </c>
+      <c r="BJ64" s="5">
+        <v>0.24319784316205897</v>
+      </c>
     </row>
-    <row r="65" spans="2:61" s="5" customFormat="1">
+    <row r="65" spans="2:62" s="5" customFormat="1">
       <c r="B65" s="5">
         <v>1964.75</v>
       </c>
@@ -8199,8 +8262,11 @@
       <c r="BI65" s="5">
         <v>192839</v>
       </c>
+      <c r="BJ65" s="5">
+        <v>-0.59536345440670824</v>
+      </c>
     </row>
-    <row r="66" spans="2:61" s="5" customFormat="1">
+    <row r="66" spans="2:62" s="5" customFormat="1">
       <c r="B66" s="5">
         <v>1965</v>
       </c>
@@ -8311,8 +8377,11 @@
       <c r="BI66" s="5">
         <v>193385.33333333334</v>
       </c>
+      <c r="BJ66" s="5">
+        <v>1.6564223845860053</v>
+      </c>
     </row>
-    <row r="67" spans="2:61" s="5" customFormat="1">
+    <row r="67" spans="2:62" s="5" customFormat="1">
       <c r="B67" s="5">
         <v>1965.25</v>
       </c>
@@ -8423,8 +8492,11 @@
       <c r="BI67" s="5">
         <v>193894.66666666666</v>
       </c>
+      <c r="BJ67" s="5">
+        <v>-1.147103166407208</v>
+      </c>
     </row>
-    <row r="68" spans="2:61" s="5" customFormat="1">
+    <row r="68" spans="2:62" s="5" customFormat="1">
       <c r="B68" s="5">
         <v>1965.5</v>
       </c>
@@ -8535,8 +8607,11 @@
       <c r="BI68" s="5">
         <v>194530.66666666666</v>
       </c>
+      <c r="BJ68" s="5">
+        <v>0.82298591058892301</v>
+      </c>
     </row>
-    <row r="69" spans="2:61" s="5" customFormat="1">
+    <row r="69" spans="2:62" s="5" customFormat="1">
       <c r="B69" s="5">
         <v>1965.75</v>
       </c>
@@ -8647,8 +8722,11 @@
       <c r="BI69" s="5">
         <v>195188</v>
       </c>
+      <c r="BJ69" s="5">
+        <v>-0.77700243293762505</v>
+      </c>
     </row>
-    <row r="70" spans="2:61" s="5" customFormat="1">
+    <row r="70" spans="2:62" s="5" customFormat="1">
       <c r="B70" s="5">
         <v>1966</v>
       </c>
@@ -8759,8 +8837,11 @@
       <c r="BI70" s="5">
         <v>195686</v>
       </c>
+      <c r="BJ70" s="5">
+        <v>-1.2161278691325919</v>
+      </c>
     </row>
-    <row r="71" spans="2:61" s="5" customFormat="1">
+    <row r="71" spans="2:62" s="5" customFormat="1">
       <c r="B71" s="5">
         <v>1966.25</v>
       </c>
@@ -8872,8 +8953,11 @@
       <c r="BI71" s="5">
         <v>196183</v>
       </c>
+      <c r="BJ71" s="5">
+        <v>-0.32531901533246499</v>
+      </c>
     </row>
-    <row r="72" spans="2:61" s="5" customFormat="1">
+    <row r="72" spans="2:62" s="5" customFormat="1">
       <c r="B72" s="5">
         <v>1966.5</v>
       </c>
@@ -8985,8 +9069,11 @@
       <c r="BI72" s="5">
         <v>196768.66666666666</v>
       </c>
+      <c r="BJ72" s="5">
+        <v>-0.36759516176909873</v>
+      </c>
     </row>
-    <row r="73" spans="2:61" s="5" customFormat="1">
+    <row r="73" spans="2:62" s="5" customFormat="1">
       <c r="B73" s="5">
         <v>1966.75</v>
       </c>
@@ -9098,8 +9185,11 @@
       <c r="BI73" s="5">
         <v>197392.33333333334</v>
       </c>
+      <c r="BJ73" s="5">
+        <v>0.16082403484004959</v>
+      </c>
     </row>
-    <row r="74" spans="2:61" s="5" customFormat="1">
+    <row r="74" spans="2:62" s="5" customFormat="1">
       <c r="B74" s="5">
         <v>1967</v>
       </c>
@@ -9215,8 +9305,11 @@
       <c r="BI74" s="5">
         <v>197888.33333333334</v>
       </c>
+      <c r="BJ74" s="5">
+        <v>-1.0257593834492538</v>
+      </c>
     </row>
-    <row r="75" spans="2:61" s="5" customFormat="1">
+    <row r="75" spans="2:62" s="5" customFormat="1">
       <c r="B75" s="5">
         <v>1967.25</v>
       </c>
@@ -9332,8 +9425,11 @@
       <c r="BI75" s="5">
         <v>198368.66666666666</v>
       </c>
+      <c r="BJ75" s="5">
+        <v>0.59546976933815354</v>
+      </c>
     </row>
-    <row r="76" spans="2:61" s="5" customFormat="1">
+    <row r="76" spans="2:62" s="5" customFormat="1">
       <c r="B76" s="5">
         <v>1967.5</v>
       </c>
@@ -9450,8 +9546,11 @@
       <c r="BI76" s="5">
         <v>198912</v>
       </c>
+      <c r="BJ76" s="5">
+        <v>-0.44670610787686815</v>
+      </c>
     </row>
-    <row r="77" spans="2:61" s="5" customFormat="1">
+    <row r="77" spans="2:62" s="5" customFormat="1">
       <c r="B77" s="5">
         <v>1967.75</v>
       </c>
@@ -9568,8 +9667,11 @@
       <c r="BI77" s="5">
         <v>199488.66666666666</v>
       </c>
+      <c r="BJ77" s="5">
+        <v>0.79740285920288234</v>
+      </c>
     </row>
-    <row r="78" spans="2:61" s="5" customFormat="1">
+    <row r="78" spans="2:62" s="5" customFormat="1">
       <c r="B78" s="5">
         <v>1968</v>
       </c>
@@ -9686,8 +9788,11 @@
       <c r="BI78" s="5">
         <v>199928</v>
       </c>
+      <c r="BJ78" s="5">
+        <v>0.2797039149725265</v>
+      </c>
     </row>
-    <row r="79" spans="2:61" s="5" customFormat="1">
+    <row r="79" spans="2:62" s="5" customFormat="1">
       <c r="B79" s="5">
         <v>1968.25</v>
       </c>
@@ -9804,8 +9909,11 @@
       <c r="BI79" s="5">
         <v>200368.33333333334</v>
       </c>
+      <c r="BJ79" s="5">
+        <v>0.86951984071792821</v>
+      </c>
     </row>
-    <row r="80" spans="2:61" s="5" customFormat="1">
+    <row r="80" spans="2:62" s="5" customFormat="1">
       <c r="B80" s="5">
         <v>1968.5</v>
       </c>
@@ -9922,8 +10030,11 @@
       <c r="BI80" s="5">
         <v>200899.66666666666</v>
       </c>
+      <c r="BJ80" s="5">
+        <v>-0.58280150236253359</v>
+      </c>
     </row>
-    <row r="81" spans="2:61" s="5" customFormat="1">
+    <row r="81" spans="2:62" s="5" customFormat="1">
       <c r="B81" s="5">
         <v>1968.75</v>
       </c>
@@ -10076,8 +10187,11 @@
       <c r="BI81" s="5">
         <v>201459</v>
       </c>
+      <c r="BJ81" s="5">
+        <v>0.18596221165346902</v>
+      </c>
     </row>
-    <row r="82" spans="2:61" s="5" customFormat="1">
+    <row r="82" spans="2:62" s="5" customFormat="1">
       <c r="B82" s="5">
         <v>1969</v>
       </c>
@@ -10234,8 +10348,11 @@
       <c r="BI82" s="5">
         <v>201888</v>
       </c>
+      <c r="BJ82" s="5">
+        <v>-1.2371995856409392</v>
+      </c>
     </row>
-    <row r="83" spans="2:61" s="5" customFormat="1">
+    <row r="83" spans="2:62" s="5" customFormat="1">
       <c r="B83" s="5">
         <v>1969.25</v>
       </c>
@@ -10392,8 +10509,11 @@
       <c r="BI83" s="5">
         <v>202333</v>
       </c>
+      <c r="BJ83" s="5">
+        <v>0.10344993447461717</v>
+      </c>
     </row>
-    <row r="84" spans="2:61" s="5" customFormat="1">
+    <row r="84" spans="2:62" s="5" customFormat="1">
       <c r="B84" s="5">
         <v>1969.5</v>
       </c>
@@ -10550,8 +10670,11 @@
       <c r="BI84" s="5">
         <v>202881.33333333334</v>
       </c>
+      <c r="BJ84" s="5">
+        <v>0.49571730193259356</v>
+      </c>
     </row>
-    <row r="85" spans="2:61" s="5" customFormat="1">
+    <row r="85" spans="2:62" s="5" customFormat="1">
       <c r="B85" s="5">
         <v>1969.75</v>
       </c>
@@ -10707,8 +10830,11 @@
       <c r="BI85" s="5">
         <v>203492.33333333334</v>
       </c>
+      <c r="BJ85" s="5">
+        <v>0.94655490629996875</v>
+      </c>
     </row>
-    <row r="86" spans="2:61" s="5" customFormat="1">
+    <row r="86" spans="2:62" s="5" customFormat="1">
       <c r="B86" s="5">
         <v>1970</v>
       </c>
@@ -10866,8 +10992,11 @@
       <c r="BI86" s="5">
         <v>204004.33333333334</v>
       </c>
+      <c r="BJ86" s="5">
+        <v>0.15456380802888742</v>
+      </c>
     </row>
-    <row r="87" spans="2:61" s="5" customFormat="1">
+    <row r="87" spans="2:62" s="5" customFormat="1">
       <c r="B87" s="5">
         <v>1970.25</v>
       </c>
@@ -11023,8 +11152,11 @@
       <c r="BI87" s="5">
         <v>204612.66666666666</v>
       </c>
+      <c r="BJ87" s="5">
+        <v>0.78992700281644268</v>
+      </c>
     </row>
-    <row r="88" spans="2:61" s="5" customFormat="1">
+    <row r="88" spans="2:62" s="5" customFormat="1">
       <c r="B88" s="5">
         <v>1970.5</v>
       </c>
@@ -11180,8 +11312,11 @@
       <c r="BI88" s="5">
         <v>205295.66666666666</v>
       </c>
+      <c r="BJ88" s="5">
+        <v>0.57853730217822985</v>
+      </c>
     </row>
-    <row r="89" spans="2:61" s="5" customFormat="1">
+    <row r="89" spans="2:62" s="5" customFormat="1">
       <c r="B89" s="5">
         <v>1970.75</v>
       </c>
@@ -11337,8 +11472,11 @@
       <c r="BI89" s="5">
         <v>206016.66666666666</v>
       </c>
+      <c r="BJ89" s="5">
+        <v>0.72162875444462515</v>
+      </c>
     </row>
-    <row r="90" spans="2:61" s="5" customFormat="1">
+    <row r="90" spans="2:62" s="5" customFormat="1">
       <c r="B90" s="5">
         <v>1971</v>
       </c>
@@ -11494,8 +11632,11 @@
       <c r="BI90" s="5">
         <v>206663</v>
       </c>
+      <c r="BJ90" s="5">
+        <v>0.39213466947051479</v>
+      </c>
     </row>
-    <row r="91" spans="2:61" s="5" customFormat="1">
+    <row r="91" spans="2:62" s="5" customFormat="1">
       <c r="B91" s="5">
         <v>1971.25</v>
       </c>
@@ -11651,8 +11792,11 @@
       <c r="BI91" s="5">
         <v>207262.33333333334</v>
       </c>
+      <c r="BJ91" s="5">
+        <v>0.84653495441183813</v>
+      </c>
     </row>
-    <row r="92" spans="2:61" s="5" customFormat="1">
+    <row r="92" spans="2:62" s="5" customFormat="1">
       <c r="B92" s="5">
         <v>1971.5</v>
       </c>
@@ -11808,8 +11952,11 @@
       <c r="BI92" s="5">
         <v>207885.33333333334</v>
       </c>
+      <c r="BJ92" s="5">
+        <v>0.13694182386202802</v>
+      </c>
     </row>
-    <row r="93" spans="2:61" s="5" customFormat="1">
+    <row r="93" spans="2:62" s="5" customFormat="1">
       <c r="B93" s="5">
         <v>1971.75</v>
       </c>
@@ -11965,8 +12112,11 @@
       <c r="BI93" s="5">
         <v>208546.66666666666</v>
       </c>
+      <c r="BJ93" s="5">
+        <v>-0.17597323375223428</v>
+      </c>
     </row>
-    <row r="94" spans="2:61" s="5" customFormat="1">
+    <row r="94" spans="2:62" s="5" customFormat="1">
       <c r="B94" s="5">
         <v>1972</v>
       </c>
@@ -12122,8 +12272,11 @@
       <c r="BI94" s="5">
         <v>209063.33333333334</v>
       </c>
+      <c r="BJ94" s="5">
+        <v>-0.13648611966246665</v>
+      </c>
     </row>
-    <row r="95" spans="2:61" s="5" customFormat="1">
+    <row r="95" spans="2:62" s="5" customFormat="1">
       <c r="B95" s="5">
         <v>1972.25</v>
       </c>
@@ -12279,8 +12432,11 @@
       <c r="BI95" s="5">
         <v>209552</v>
       </c>
+      <c r="BJ95" s="5">
+        <v>-1.1956689730359069</v>
+      </c>
     </row>
-    <row r="96" spans="2:61" s="5" customFormat="1">
+    <row r="96" spans="2:62" s="5" customFormat="1">
       <c r="B96" s="5">
         <v>1972.5</v>
       </c>
@@ -12436,8 +12592,11 @@
       <c r="BI96" s="5">
         <v>210083</v>
       </c>
+      <c r="BJ96" s="5">
+        <v>1.9677645520177809</v>
+      </c>
     </row>
-    <row r="97" spans="2:61" s="5" customFormat="1">
+    <row r="97" spans="2:62" s="5" customFormat="1">
       <c r="B97" s="5">
         <v>1972.75</v>
       </c>
@@ -12593,8 +12752,11 @@
       <c r="BI97" s="5">
         <v>210652</v>
       </c>
+      <c r="BJ97" s="5">
+        <v>0.55439697192577553</v>
+      </c>
     </row>
-    <row r="98" spans="2:61" s="5" customFormat="1">
+    <row r="98" spans="2:62" s="5" customFormat="1">
       <c r="B98" s="5">
         <v>1973</v>
       </c>
@@ -12753,8 +12915,11 @@
       <c r="BI98" s="5">
         <v>211119.66666666666</v>
       </c>
+      <c r="BJ98" s="5">
+        <v>-2.9581193780114954</v>
+      </c>
     </row>
-    <row r="99" spans="2:61" s="5" customFormat="1">
+    <row r="99" spans="2:62" s="5" customFormat="1">
       <c r="B99" s="5">
         <v>1973.25</v>
       </c>
@@ -12913,8 +13078,11 @@
       <c r="BI99" s="5">
         <v>211581</v>
       </c>
+      <c r="BJ99" s="5">
+        <v>-1.3149625422057518</v>
+      </c>
     </row>
-    <row r="100" spans="2:61" s="5" customFormat="1">
+    <row r="100" spans="2:62" s="5" customFormat="1">
       <c r="B100" s="5">
         <v>1973.5</v>
       </c>
@@ -13073,8 +13241,11 @@
       <c r="BI100" s="5">
         <v>212096.66666666666</v>
       </c>
+      <c r="BJ100" s="5">
+        <v>1.2069000586331566</v>
+      </c>
     </row>
-    <row r="101" spans="2:61" s="5" customFormat="1">
+    <row r="101" spans="2:62" s="5" customFormat="1">
       <c r="B101" s="5">
         <v>1973.75</v>
       </c>
@@ -13233,8 +13404,11 @@
       <c r="BI101" s="5">
         <v>212631.33333333334</v>
       </c>
+      <c r="BJ101" s="5">
+        <v>-2.3229412531303026</v>
+      </c>
     </row>
-    <row r="102" spans="2:61" s="5" customFormat="1">
+    <row r="102" spans="2:62" s="5" customFormat="1">
       <c r="B102" s="5">
         <v>1974</v>
       </c>
@@ -13393,8 +13567,11 @@
       <c r="BI102" s="5">
         <v>213072.33333333334</v>
       </c>
+      <c r="BJ102" s="5">
+        <v>-1.2750514571005933</v>
+      </c>
     </row>
-    <row r="103" spans="2:61" s="5" customFormat="1">
+    <row r="103" spans="2:62" s="5" customFormat="1">
       <c r="B103" s="5">
         <v>1974.25</v>
       </c>
@@ -13553,8 +13730,11 @@
       <c r="BI103" s="5">
         <v>213520</v>
       </c>
+      <c r="BJ103" s="5">
+        <v>0.76752528898868166</v>
+      </c>
     </row>
-    <row r="104" spans="2:61" s="5" customFormat="1">
+    <row r="104" spans="2:62" s="5" customFormat="1">
       <c r="B104" s="5">
         <v>1974.5</v>
       </c>
@@ -13715,8 +13895,11 @@
       <c r="BI104" s="5">
         <v>214047.33333333334</v>
       </c>
+      <c r="BJ104" s="5">
+        <v>1.4088521195154355</v>
+      </c>
     </row>
-    <row r="105" spans="2:61" s="5" customFormat="1">
+    <row r="105" spans="2:62" s="5" customFormat="1">
       <c r="B105" s="5">
         <v>1974.75</v>
       </c>
@@ -13875,8 +14058,11 @@
       <c r="BI105" s="5">
         <v>214619.33333333334</v>
       </c>
+      <c r="BJ105" s="5">
+        <v>-0.2402299117350889</v>
+      </c>
     </row>
-    <row r="106" spans="2:61" s="5" customFormat="1">
+    <row r="106" spans="2:62" s="5" customFormat="1">
       <c r="B106" s="5">
         <v>1975</v>
       </c>
@@ -14035,8 +14221,11 @@
       <c r="BI106" s="5">
         <v>215064.66666666666</v>
       </c>
+      <c r="BJ106" s="5">
+        <v>0.54795137402078431</v>
+      </c>
     </row>
-    <row r="107" spans="2:61" s="5" customFormat="1">
+    <row r="107" spans="2:62" s="5" customFormat="1">
       <c r="B107" s="5">
         <v>1975.25</v>
       </c>
@@ -14195,8 +14384,11 @@
       <c r="BI107" s="5">
         <v>215548</v>
       </c>
+      <c r="BJ107" s="5">
+        <v>1.2077310323012673</v>
+      </c>
     </row>
-    <row r="108" spans="2:61" s="5" customFormat="1">
+    <row r="108" spans="2:62" s="5" customFormat="1">
       <c r="B108" s="5">
         <v>1975.5</v>
       </c>
@@ -14355,8 +14547,11 @@
       <c r="BI108" s="5">
         <v>216187</v>
       </c>
+      <c r="BJ108" s="5">
+        <v>-0.74670711676322377</v>
+      </c>
     </row>
-    <row r="109" spans="2:61" s="5" customFormat="1">
+    <row r="109" spans="2:62" s="5" customFormat="1">
       <c r="B109" s="5">
         <v>1975.75</v>
       </c>
@@ -14515,8 +14710,11 @@
       <c r="BI109" s="5">
         <v>216763</v>
       </c>
+      <c r="BJ109" s="5">
+        <v>3.1710000206158773E-4</v>
+      </c>
     </row>
-    <row r="110" spans="2:61" s="5" customFormat="1">
+    <row r="110" spans="2:62" s="5" customFormat="1">
       <c r="B110" s="5">
         <v>1976</v>
       </c>
@@ -14675,8 +14873,11 @@
       <c r="BI110" s="5">
         <v>217241.66666666666</v>
       </c>
+      <c r="BJ110" s="5">
+        <v>-1.38538633821923E-2</v>
+      </c>
     </row>
-    <row r="111" spans="2:61" s="5" customFormat="1">
+    <row r="111" spans="2:62" s="5" customFormat="1">
       <c r="B111" s="5">
         <v>1976.25</v>
       </c>
@@ -14835,8 +15036,11 @@
       <c r="BI111" s="5">
         <v>217691.33333333334</v>
       </c>
+      <c r="BJ111" s="5">
+        <v>0.62375192706789517</v>
+      </c>
     </row>
-    <row r="112" spans="2:61" s="5" customFormat="1">
+    <row r="112" spans="2:62" s="5" customFormat="1">
       <c r="B112" s="5">
         <v>1976.5</v>
       </c>
@@ -14995,8 +15199,11 @@
       <c r="BI112" s="5">
         <v>218236</v>
       </c>
+      <c r="BJ112" s="5">
+        <v>0.32131581717887803</v>
+      </c>
     </row>
-    <row r="113" spans="2:61" s="5" customFormat="1">
+    <row r="113" spans="2:62" s="5" customFormat="1">
       <c r="B113" s="5">
         <v>1976.75</v>
       </c>
@@ -15155,8 +15362,11 @@
       <c r="BI113" s="5">
         <v>218828</v>
       </c>
+      <c r="BJ113" s="5">
+        <v>0.67094192522375729</v>
+      </c>
     </row>
-    <row r="114" spans="2:61" s="5" customFormat="1">
+    <row r="114" spans="2:62" s="5" customFormat="1">
       <c r="B114" s="5">
         <v>1977</v>
       </c>
@@ -15315,8 +15525,11 @@
       <c r="BI114" s="5">
         <v>219342.33333333334</v>
       </c>
+      <c r="BJ114" s="5">
+        <v>9.3953106362731104E-2</v>
+      </c>
     </row>
-    <row r="115" spans="2:61" s="5" customFormat="1">
+    <row r="115" spans="2:62" s="5" customFormat="1">
       <c r="B115" s="5">
         <v>1977.25</v>
       </c>
@@ -15475,8 +15688,11 @@
       <c r="BI115" s="5">
         <v>219863</v>
       </c>
+      <c r="BJ115" s="5">
+        <v>-1.2618600802020823</v>
+      </c>
     </row>
-    <row r="116" spans="2:61" s="5" customFormat="1">
+    <row r="116" spans="2:62" s="5" customFormat="1">
       <c r="B116" s="5">
         <v>1977.5</v>
       </c>
@@ -15635,8 +15851,11 @@
       <c r="BI116" s="5">
         <v>220461.66666666666</v>
       </c>
+      <c r="BJ116" s="5">
+        <v>-1.5336741611098712</v>
+      </c>
     </row>
-    <row r="117" spans="2:61" s="5" customFormat="1">
+    <row r="117" spans="2:62" s="5" customFormat="1">
       <c r="B117" s="5">
         <v>1977.75</v>
       </c>
@@ -15795,8 +16014,11 @@
       <c r="BI117" s="5">
         <v>221105.33333333334</v>
       </c>
+      <c r="BJ117" s="5">
+        <v>1.4605479879109931</v>
+      </c>
     </row>
-    <row r="118" spans="2:61" s="5" customFormat="1">
+    <row r="118" spans="2:62" s="5" customFormat="1">
       <c r="B118" s="5">
         <v>1978</v>
       </c>
@@ -15955,8 +16177,11 @@
       <c r="BI118" s="5">
         <v>221632.66666666666</v>
       </c>
+      <c r="BJ118" s="5">
+        <v>1.8898476297325426</v>
+      </c>
     </row>
-    <row r="119" spans="2:61" s="5" customFormat="1">
+    <row r="119" spans="2:62" s="5" customFormat="1">
       <c r="B119" s="5">
         <v>1978.25</v>
       </c>
@@ -16118,8 +16343,11 @@
       <c r="BI119" s="5">
         <v>222182</v>
       </c>
+      <c r="BJ119" s="5">
+        <v>-2.8303062930852656</v>
+      </c>
     </row>
-    <row r="120" spans="2:61" s="5" customFormat="1">
+    <row r="120" spans="2:62" s="5" customFormat="1">
       <c r="B120" s="5">
         <v>1978.5</v>
       </c>
@@ -16281,8 +16509,11 @@
       <c r="BI120" s="5">
         <v>222814.33333333334</v>
       </c>
+      <c r="BJ120" s="5">
+        <v>-1.2376194449220692</v>
+      </c>
     </row>
-    <row r="121" spans="2:61" s="5" customFormat="1">
+    <row r="121" spans="2:62" s="5" customFormat="1">
       <c r="B121" s="5">
         <v>1978.75</v>
       </c>
@@ -16444,8 +16675,11 @@
       <c r="BI121" s="5">
         <v>223472.66666666666</v>
       </c>
+      <c r="BJ121" s="5">
+        <v>-0.15835149616905947</v>
+      </c>
     </row>
-    <row r="122" spans="2:61" s="5" customFormat="1">
+    <row r="122" spans="2:62" s="5" customFormat="1">
       <c r="B122" s="5">
         <v>1979</v>
       </c>
@@ -16607,8 +16841,11 @@
       <c r="BI122" s="5">
         <v>224051</v>
       </c>
+      <c r="BJ122" s="5">
+        <v>1.6716834715960625</v>
+      </c>
     </row>
-    <row r="123" spans="2:61" s="5" customFormat="1">
+    <row r="123" spans="2:62" s="5" customFormat="1">
       <c r="B123" s="5">
         <v>1979.25</v>
       </c>
@@ -16770,8 +17007,11 @@
       <c r="BI123" s="5">
         <v>224637.66666666666</v>
       </c>
+      <c r="BJ123" s="5">
+        <v>1.436167679159893</v>
+      </c>
     </row>
-    <row r="124" spans="2:61" s="5" customFormat="1">
+    <row r="124" spans="2:62" s="5" customFormat="1">
       <c r="B124" s="5">
         <v>1979.5</v>
       </c>
@@ -16933,8 +17173,11 @@
       <c r="BI124" s="5">
         <v>225299</v>
       </c>
+      <c r="BJ124" s="5">
+        <v>0.41340291301625365</v>
+      </c>
     </row>
-    <row r="125" spans="2:61" s="5" customFormat="1">
+    <row r="125" spans="2:62" s="5" customFormat="1">
       <c r="B125" s="5">
         <v>1979.75</v>
       </c>
@@ -17096,8 +17339,11 @@
       <c r="BI125" s="5">
         <v>226023.66666666666</v>
       </c>
+      <c r="BJ125" s="5">
+        <v>-0.75652630102839646</v>
+      </c>
     </row>
-    <row r="126" spans="2:61" s="5" customFormat="1">
+    <row r="126" spans="2:62" s="5" customFormat="1">
       <c r="B126" s="5">
         <v>1980</v>
       </c>
@@ -17259,8 +17505,11 @@
       <c r="BI126" s="5">
         <v>226652</v>
       </c>
+      <c r="BJ126" s="5">
+        <v>-1.901864320385654</v>
+      </c>
     </row>
-    <row r="127" spans="2:61" s="5" customFormat="1">
+    <row r="127" spans="2:62" s="5" customFormat="1">
       <c r="B127" s="5">
         <v>1980.25</v>
       </c>
@@ -17422,8 +17671,11 @@
       <c r="BI127" s="5">
         <v>227278</v>
       </c>
+      <c r="BJ127" s="5">
+        <v>-0.96954038975492862</v>
+      </c>
     </row>
-    <row r="128" spans="2:61" s="5" customFormat="1">
+    <row r="128" spans="2:62" s="5" customFormat="1">
       <c r="B128" s="5">
         <v>1980.5</v>
       </c>
@@ -17585,8 +17837,11 @@
       <c r="BI128" s="5">
         <v>227955</v>
       </c>
+      <c r="BJ128" s="5">
+        <v>1.5543834265239762</v>
+      </c>
     </row>
-    <row r="129" spans="2:61" s="5" customFormat="1">
+    <row r="129" spans="2:62" s="5" customFormat="1">
       <c r="B129" s="5">
         <v>1980.75</v>
       </c>
@@ -17748,8 +18003,11 @@
       <c r="BI129" s="5">
         <v>228602.66666666666</v>
       </c>
+      <c r="BJ129" s="5">
+        <v>1.5529028859415792</v>
+      </c>
     </row>
-    <row r="130" spans="2:61" s="5" customFormat="1">
+    <row r="130" spans="2:62" s="5" customFormat="1">
       <c r="B130" s="5">
         <v>1981</v>
       </c>
@@ -17911,8 +18169,11 @@
       <c r="BI130" s="5">
         <v>229077.33333333334</v>
       </c>
+      <c r="BJ130" s="5">
+        <v>-1.0640685798151637</v>
+      </c>
     </row>
-    <row r="131" spans="2:61" s="5" customFormat="1">
+    <row r="131" spans="2:62" s="5" customFormat="1">
       <c r="B131" s="5">
         <v>1981.25</v>
       </c>
@@ -18074,8 +18335,11 @@
       <c r="BI131" s="5">
         <v>229579.66666666666</v>
       </c>
+      <c r="BJ131" s="5">
+        <v>0.4015570536489883</v>
+      </c>
     </row>
-    <row r="132" spans="2:61" s="5" customFormat="1">
+    <row r="132" spans="2:62" s="5" customFormat="1">
       <c r="B132" s="5">
         <v>1981.5</v>
       </c>
@@ -18253,8 +18517,11 @@
       <c r="BI132" s="5">
         <v>230188.33333333334</v>
       </c>
+      <c r="BJ132" s="5">
+        <v>-1.4170220468477082</v>
+      </c>
     </row>
-    <row r="133" spans="2:61" s="5" customFormat="1">
+    <row r="133" spans="2:62" s="5" customFormat="1">
       <c r="B133" s="5">
         <v>1981.75</v>
       </c>
@@ -18432,8 +18699,11 @@
       <c r="BI133" s="5">
         <v>230817.33333333334</v>
       </c>
+      <c r="BJ133" s="5">
+        <v>-0.11831062477680188</v>
+      </c>
     </row>
-    <row r="134" spans="2:61" s="5" customFormat="1">
+    <row r="134" spans="2:62" s="5" customFormat="1">
       <c r="B134" s="5">
         <v>1982</v>
       </c>
@@ -18611,8 +18881,11 @@
       <c r="BI134" s="5">
         <v>231313.33333333334</v>
       </c>
+      <c r="BJ134" s="5">
+        <v>1.0384858942959863</v>
+      </c>
     </row>
-    <row r="135" spans="2:61" s="5" customFormat="1">
+    <row r="135" spans="2:62" s="5" customFormat="1">
       <c r="B135" s="5">
         <v>1982.25</v>
       </c>
@@ -18790,8 +19063,11 @@
       <c r="BI135" s="5">
         <v>231815.33333333334</v>
       </c>
+      <c r="BJ135" s="5">
+        <v>-1.1034179579887</v>
+      </c>
     </row>
-    <row r="136" spans="2:61" s="5" customFormat="1">
+    <row r="136" spans="2:62" s="5" customFormat="1">
       <c r="B136" s="5">
         <v>1982.5</v>
       </c>
@@ -18969,8 +19245,11 @@
       <c r="BI136" s="5">
         <v>232393</v>
       </c>
+      <c r="BJ136" s="5">
+        <v>2.4238716148289337</v>
+      </c>
     </row>
-    <row r="137" spans="2:61" s="5" customFormat="1">
+    <row r="137" spans="2:62" s="5" customFormat="1">
       <c r="B137" s="5">
         <v>1982.75</v>
       </c>
@@ -19148,8 +19427,11 @@
       <c r="BI137" s="5">
         <v>232989.66666666666</v>
       </c>
+      <c r="BJ137" s="5">
+        <v>0.567904873232145</v>
+      </c>
     </row>
-    <row r="138" spans="2:61" s="5" customFormat="1">
+    <row r="138" spans="2:62" s="5" customFormat="1">
       <c r="B138" s="5">
         <v>1983</v>
       </c>
@@ -19327,8 +19609,11 @@
       <c r="BI138" s="5">
         <v>233469.33333333334</v>
       </c>
+      <c r="BJ138" s="5">
+        <v>-1.1944733442745086</v>
+      </c>
     </row>
-    <row r="139" spans="2:61" s="5" customFormat="1">
+    <row r="139" spans="2:62" s="5" customFormat="1">
       <c r="B139" s="5">
         <v>1983.25</v>
       </c>
@@ -19506,8 +19791,11 @@
       <c r="BI139" s="5">
         <v>233940.33333333334</v>
       </c>
+      <c r="BJ139" s="5">
+        <v>1.1915027561518516</v>
+      </c>
     </row>
-    <row r="140" spans="2:61" s="5" customFormat="1">
+    <row r="140" spans="2:62" s="5" customFormat="1">
       <c r="B140" s="5">
         <v>1983.5</v>
       </c>
@@ -19685,8 +19973,11 @@
       <c r="BI140" s="5">
         <v>234503</v>
       </c>
+      <c r="BJ140" s="5">
+        <v>-0.21117945629191109</v>
+      </c>
     </row>
-    <row r="141" spans="2:61" s="5" customFormat="1">
+    <row r="141" spans="2:62" s="5" customFormat="1">
       <c r="B141" s="5">
         <v>1983.75</v>
       </c>
@@ -19864,8 +20155,11 @@
       <c r="BI141" s="5">
         <v>235073.33333333334</v>
       </c>
+      <c r="BJ141" s="5">
+        <v>0.91367000367353568</v>
+      </c>
     </row>
-    <row r="142" spans="2:61" s="5" customFormat="1">
+    <row r="142" spans="2:62" s="5" customFormat="1">
       <c r="B142" s="5">
         <v>1984</v>
       </c>
@@ -20043,8 +20337,11 @@
       <c r="BI142" s="5">
         <v>235529</v>
       </c>
+      <c r="BJ142" s="5">
+        <v>-0.28351565872687429</v>
+      </c>
     </row>
-    <row r="143" spans="2:61" s="5" customFormat="1">
+    <row r="143" spans="2:62" s="5" customFormat="1">
       <c r="B143" s="5">
         <v>1984.25</v>
       </c>
@@ -20222,8 +20519,11 @@
       <c r="BI143" s="5">
         <v>235997.33333333334</v>
       </c>
+      <c r="BJ143" s="5">
+        <v>-0.32890105947430143</v>
+      </c>
     </row>
-    <row r="144" spans="2:61" s="5" customFormat="1">
+    <row r="144" spans="2:62" s="5" customFormat="1">
       <c r="B144" s="5">
         <v>1984.5</v>
       </c>
@@ -20401,8 +20701,11 @@
       <c r="BI144" s="5">
         <v>236552.33333333334</v>
       </c>
+      <c r="BJ144" s="5">
+        <v>-0.21892478745542024</v>
+      </c>
     </row>
-    <row r="145" spans="2:61" s="5" customFormat="1">
+    <row r="145" spans="2:62" s="5" customFormat="1">
       <c r="B145" s="5">
         <v>1984.75</v>
       </c>
@@ -20580,8 +20883,11 @@
       <c r="BI145" s="5">
         <v>237150.33333333334</v>
       </c>
+      <c r="BJ145" s="5">
+        <v>0.91920152522747278</v>
+      </c>
     </row>
-    <row r="146" spans="2:61" s="5" customFormat="1">
+    <row r="146" spans="2:62" s="5" customFormat="1">
       <c r="B146" s="5">
         <v>1985</v>
       </c>
@@ -20759,8 +21065,11 @@
       <c r="BI146" s="5">
         <v>237600.66666666666</v>
       </c>
+      <c r="BJ146" s="5">
+        <v>0.34172478323639566</v>
+      </c>
     </row>
-    <row r="147" spans="2:61" s="5" customFormat="1">
+    <row r="147" spans="2:62" s="5" customFormat="1">
       <c r="B147" s="5">
         <v>1985.25</v>
       </c>
@@ -20938,8 +21247,11 @@
       <c r="BI147" s="5">
         <v>238081.33333333334</v>
       </c>
+      <c r="BJ147" s="5">
+        <v>0.16542903196494202</v>
+      </c>
     </row>
-    <row r="148" spans="2:61" s="5" customFormat="1">
+    <row r="148" spans="2:62" s="5" customFormat="1">
       <c r="B148" s="5">
         <v>1985.5</v>
       </c>
@@ -21117,8 +21429,11 @@
       <c r="BI148" s="5">
         <v>238681</v>
       </c>
+      <c r="BJ148" s="5">
+        <v>-0.40062104799300202</v>
+      </c>
     </row>
-    <row r="149" spans="2:61" s="5" customFormat="1">
+    <row r="149" spans="2:62" s="5" customFormat="1">
       <c r="B149" s="5">
         <v>1985.75</v>
       </c>
@@ -21296,8 +21611,11 @@
       <c r="BI149" s="5">
         <v>239299</v>
       </c>
+      <c r="BJ149" s="5">
+        <v>0.74926423047502855</v>
+      </c>
     </row>
-    <row r="150" spans="2:61" s="5" customFormat="1">
+    <row r="150" spans="2:62" s="5" customFormat="1">
       <c r="B150" s="5">
         <v>1986</v>
       </c>
@@ -21477,8 +21795,11 @@
       <c r="BI150" s="5">
         <v>239784.66666666666</v>
       </c>
+      <c r="BJ150" s="5">
+        <v>0.12053170727172968</v>
+      </c>
     </row>
-    <row r="151" spans="2:61" s="5" customFormat="1">
+    <row r="151" spans="2:62" s="5" customFormat="1">
       <c r="B151" s="5">
         <v>1986.25</v>
       </c>
@@ -21658,8 +21979,11 @@
       <c r="BI151" s="5">
         <v>240274.66666666666</v>
       </c>
+      <c r="BJ151" s="5">
+        <v>0.81373264995085748</v>
+      </c>
     </row>
-    <row r="152" spans="2:61" s="5" customFormat="1">
+    <row r="152" spans="2:62" s="5" customFormat="1">
       <c r="B152" s="5">
         <v>1986.5</v>
       </c>
@@ -21839,8 +22163,11 @@
       <c r="BI152" s="5">
         <v>240857.66666666666</v>
       </c>
+      <c r="BJ152" s="5">
+        <v>-0.30721244070305004</v>
+      </c>
     </row>
-    <row r="153" spans="2:61" s="5" customFormat="1">
+    <row r="153" spans="2:62" s="5" customFormat="1">
       <c r="B153" s="5">
         <v>1986.75</v>
       </c>
@@ -22020,8 +22347,11 @@
       <c r="BI153" s="5">
         <v>241453.66666666666</v>
       </c>
+      <c r="BJ153" s="5">
+        <v>-1.1656474689589211</v>
+      </c>
     </row>
-    <row r="154" spans="2:61" s="5" customFormat="1">
+    <row r="154" spans="2:62" s="5" customFormat="1">
       <c r="B154" s="5">
         <v>1987</v>
       </c>
@@ -22201,8 +22531,11 @@
       <c r="BI154" s="5">
         <v>241931</v>
       </c>
+      <c r="BJ154" s="5">
+        <v>1.7687032395636987E-3</v>
+      </c>
     </row>
-    <row r="155" spans="2:61" s="5" customFormat="1">
+    <row r="155" spans="2:62" s="5" customFormat="1">
       <c r="B155" s="5">
         <v>1987.25</v>
       </c>
@@ -22382,8 +22715,11 @@
       <c r="BI155" s="5">
         <v>242427.66666666666</v>
       </c>
+      <c r="BJ155" s="5">
+        <v>0.3514757937034847</v>
+      </c>
     </row>
-    <row r="156" spans="2:61" s="5" customFormat="1">
+    <row r="156" spans="2:62" s="5" customFormat="1">
       <c r="B156" s="5">
         <v>1987.5</v>
       </c>
@@ -22563,8 +22899,11 @@
       <c r="BI156" s="5">
         <v>243013</v>
       </c>
+      <c r="BJ156" s="5">
+        <v>0.28423303141966538</v>
+      </c>
     </row>
-    <row r="157" spans="2:61" s="5" customFormat="1">
+    <row r="157" spans="2:62" s="5" customFormat="1">
       <c r="B157" s="5">
         <v>1987.75</v>
       </c>
@@ -22744,8 +23083,11 @@
       <c r="BI157" s="5">
         <v>243631.33333333334</v>
       </c>
+      <c r="BJ157" s="5">
+        <v>-3.2709786979047335</v>
+      </c>
     </row>
-    <row r="158" spans="2:61" s="5" customFormat="1">
+    <row r="158" spans="2:62" s="5" customFormat="1">
       <c r="B158" s="5">
         <v>1988</v>
       </c>
@@ -22925,8 +23267,11 @@
       <c r="BI158" s="5">
         <v>244130.33333333334</v>
       </c>
+      <c r="BJ158" s="5">
+        <v>2.2618152952896837</v>
+      </c>
     </row>
-    <row r="159" spans="2:61" s="5" customFormat="1">
+    <row r="159" spans="2:62" s="5" customFormat="1">
       <c r="B159" s="5">
         <v>1988.25</v>
       </c>
@@ -23106,8 +23451,11 @@
       <c r="BI159" s="5">
         <v>244620.33333333334</v>
       </c>
+      <c r="BJ159" s="5">
+        <v>-1.2485259384360714</v>
+      </c>
     </row>
-    <row r="160" spans="2:61" s="5" customFormat="1">
+    <row r="160" spans="2:62" s="5" customFormat="1">
       <c r="B160" s="5">
         <v>1988.5</v>
       </c>
@@ -23287,8 +23635,11 @@
       <c r="BI160" s="5">
         <v>245241.66666666666</v>
       </c>
+      <c r="BJ160" s="5">
+        <v>0.85447427158424205</v>
+      </c>
     </row>
-    <row r="161" spans="2:61" s="5" customFormat="1">
+    <row r="161" spans="2:62" s="5" customFormat="1">
       <c r="B161" s="5">
         <v>1988.75</v>
       </c>
@@ -23468,8 +23819,11 @@
       <c r="BI161" s="5">
         <v>245877.66666666666</v>
       </c>
+      <c r="BJ161" s="5">
+        <v>-0.42037296780382333</v>
+      </c>
     </row>
-    <row r="162" spans="2:61" s="5" customFormat="1">
+    <row r="162" spans="2:62" s="5" customFormat="1">
       <c r="B162" s="5">
         <v>1989</v>
       </c>
@@ -23649,8 +24003,11 @@
       <c r="BI162" s="5">
         <v>246377.33333333334</v>
       </c>
+      <c r="BJ162" s="5">
+        <v>-0.69178422773163806</v>
+      </c>
     </row>
-    <row r="163" spans="2:61" s="5" customFormat="1">
+    <row r="163" spans="2:62" s="5" customFormat="1">
       <c r="B163" s="5">
         <v>1989.25</v>
       </c>
@@ -23830,8 +24187,11 @@
       <c r="BI163" s="5">
         <v>246913.66666666666</v>
       </c>
+      <c r="BJ163" s="5">
+        <v>-1.0199095706878334</v>
+      </c>
     </row>
-    <row r="164" spans="2:61" s="5" customFormat="1">
+    <row r="164" spans="2:62" s="5" customFormat="1">
       <c r="B164" s="5">
         <v>1989.5</v>
       </c>
@@ -24011,8 +24371,11 @@
       <c r="BI164" s="5">
         <v>247577</v>
       </c>
+      <c r="BJ164" s="5">
+        <v>0.24183771237822532</v>
+      </c>
     </row>
-    <row r="165" spans="2:61" s="5" customFormat="1">
+    <row r="165" spans="2:62" s="5" customFormat="1">
       <c r="B165" s="5">
         <v>1989.75</v>
       </c>
@@ -24192,8 +24555,11 @@
       <c r="BI165" s="5">
         <v>248275.66666666666</v>
       </c>
+      <c r="BJ165" s="5">
+        <v>0.34787890661935611</v>
+      </c>
     </row>
-    <row r="166" spans="2:61" s="5" customFormat="1">
+    <row r="166" spans="2:62" s="5" customFormat="1">
       <c r="B166" s="5">
         <v>1990</v>
       </c>
@@ -24375,8 +24741,11 @@
       <c r="BI166" s="5">
         <v>248832.66666666666</v>
       </c>
+      <c r="BJ166" s="5">
+        <v>-1.3496184956234738</v>
+      </c>
     </row>
-    <row r="167" spans="2:61" s="5" customFormat="1">
+    <row r="167" spans="2:62" s="5" customFormat="1">
       <c r="B167" s="5">
         <v>1990.25</v>
       </c>
@@ -24558,8 +24927,11 @@
       <c r="BI167" s="5">
         <v>249573.33333333334</v>
       </c>
+      <c r="BJ167" s="5">
+        <v>0.19603304285078071</v>
+      </c>
     </row>
-    <row r="168" spans="2:61" s="5" customFormat="1">
+    <row r="168" spans="2:62" s="5" customFormat="1">
       <c r="B168" s="5">
         <v>1990.5</v>
       </c>
@@ -24741,8 +25113,11 @@
       <c r="BI168" s="5">
         <v>250440.66666666666</v>
       </c>
+      <c r="BJ168" s="5">
+        <v>-1.8263070468672131</v>
+      </c>
     </row>
-    <row r="169" spans="2:61" s="5" customFormat="1">
+    <row r="169" spans="2:62" s="5" customFormat="1">
       <c r="B169" s="5">
         <v>1990.75</v>
       </c>
@@ -24924,8 +25299,11 @@
       <c r="BI169" s="5">
         <v>251343</v>
       </c>
+      <c r="BJ169" s="5">
+        <v>-1.5241561972788626</v>
+      </c>
     </row>
-    <row r="170" spans="2:61" s="5" customFormat="1">
+    <row r="170" spans="2:62" s="5" customFormat="1">
       <c r="B170" s="5">
         <v>1991</v>
       </c>
@@ -25107,8 +25485,11 @@
       <c r="BI170" s="5">
         <v>252132</v>
       </c>
+      <c r="BJ170" s="5">
+        <v>1.2335047258616973</v>
+      </c>
     </row>
-    <row r="171" spans="2:61" s="5" customFormat="1">
+    <row r="171" spans="2:62" s="5" customFormat="1">
       <c r="B171" s="5">
         <v>1991.25</v>
       </c>
@@ -25290,8 +25671,11 @@
       <c r="BI171" s="5">
         <v>252921</v>
       </c>
+      <c r="BJ171" s="5">
+        <v>-0.72472465086146665</v>
+      </c>
     </row>
-    <row r="172" spans="2:61" s="5" customFormat="1">
+    <row r="172" spans="2:62" s="5" customFormat="1">
       <c r="B172" s="5">
         <v>1991.5</v>
       </c>
@@ -25473,8 +25857,11 @@
       <c r="BI172" s="5">
         <v>253808.66666666666</v>
       </c>
+      <c r="BJ172" s="5">
+        <v>-0.44930879559356895</v>
+      </c>
     </row>
-    <row r="173" spans="2:61" s="5" customFormat="1">
+    <row r="173" spans="2:62" s="5" customFormat="1">
       <c r="B173" s="5">
         <v>1991.75</v>
       </c>
@@ -25656,8 +26043,11 @@
       <c r="BI173" s="5">
         <v>254705.66666666666</v>
       </c>
+      <c r="BJ173" s="5">
+        <v>3.6424497268885692E-2</v>
+      </c>
     </row>
-    <row r="174" spans="2:61" s="5" customFormat="1">
+    <row r="174" spans="2:62" s="5" customFormat="1">
       <c r="B174" s="5">
         <v>1992</v>
       </c>
@@ -25839,8 +26229,11 @@
       <c r="BI174" s="5">
         <v>255455</v>
       </c>
+      <c r="BJ174" s="5">
+        <v>-0.73845899788021918</v>
+      </c>
     </row>
-    <row r="175" spans="2:61" s="5" customFormat="1">
+    <row r="175" spans="2:62" s="5" customFormat="1">
       <c r="B175" s="5">
         <v>1992.25</v>
       </c>
@@ -26022,8 +26415,11 @@
       <c r="BI175" s="5">
         <v>256288.66666666666</v>
       </c>
+      <c r="BJ175" s="5">
+        <v>-0.73368194416615484</v>
+      </c>
     </row>
-    <row r="176" spans="2:61" s="5" customFormat="1">
+    <row r="176" spans="2:62" s="5" customFormat="1">
       <c r="B176" s="5">
         <v>1992.5</v>
       </c>
@@ -26205,8 +26601,11 @@
       <c r="BI176" s="5">
         <v>257224.66666666666</v>
       </c>
+      <c r="BJ176" s="5">
+        <v>-0.74316377383236376</v>
+      </c>
     </row>
-    <row r="177" spans="2:61" s="5" customFormat="1">
+    <row r="177" spans="2:62" s="5" customFormat="1">
       <c r="B177" s="5">
         <v>1992.75</v>
       </c>
@@ -26388,8 +26787,11 @@
       <c r="BI177" s="5">
         <v>258140.33333333334</v>
       </c>
+      <c r="BJ177" s="5">
+        <v>0.18190710425034598</v>
+      </c>
     </row>
-    <row r="178" spans="2:61" s="5" customFormat="1">
+    <row r="178" spans="2:62" s="5" customFormat="1">
       <c r="B178" s="5">
         <v>1993</v>
       </c>
@@ -26571,8 +26973,11 @@
       <c r="BI178" s="5">
         <v>258916.66666666666</v>
       </c>
+      <c r="BJ178" s="5">
+        <v>7.6639182021132526E-2</v>
+      </c>
     </row>
-    <row r="179" spans="2:61" s="5" customFormat="1">
+    <row r="179" spans="2:62" s="5" customFormat="1">
       <c r="B179" s="5">
         <v>1993.25</v>
       </c>
@@ -26754,8 +27159,11 @@
       <c r="BI179" s="5">
         <v>259685.66666666666</v>
       </c>
+      <c r="BJ179" s="5">
+        <v>0.92620666114400774</v>
+      </c>
     </row>
-    <row r="180" spans="2:61" s="5" customFormat="1">
+    <row r="180" spans="2:62" s="5" customFormat="1">
       <c r="B180" s="5">
         <v>1993.5</v>
       </c>
@@ -26937,8 +27345,11 @@
       <c r="BI180" s="5">
         <v>260562.66666666666</v>
       </c>
+      <c r="BJ180" s="5">
+        <v>0.312354556604094</v>
+      </c>
     </row>
-    <row r="181" spans="2:61" s="5" customFormat="1">
+    <row r="181" spans="2:62" s="5" customFormat="1">
       <c r="B181" s="5">
         <v>1993.75</v>
       </c>
@@ -27120,8 +27531,11 @@
       <c r="BI181" s="5">
         <v>261420.66666666666</v>
       </c>
+      <c r="BJ181" s="5">
+        <v>-0.36971918642198226</v>
+      </c>
     </row>
-    <row r="182" spans="2:61" s="5" customFormat="1">
+    <row r="182" spans="2:62" s="5" customFormat="1">
       <c r="B182" s="5">
         <v>1994</v>
       </c>
@@ -27303,8 +27717,11 @@
       <c r="BI182" s="5">
         <v>262131.33333333334</v>
       </c>
+      <c r="BJ182" s="5">
+        <v>0.92236320330114063</v>
+      </c>
     </row>
-    <row r="183" spans="2:61" s="5" customFormat="1">
+    <row r="183" spans="2:62" s="5" customFormat="1">
       <c r="B183" s="5">
         <v>1994.25</v>
       </c>
@@ -27486,8 +27903,11 @@
       <c r="BI183" s="5">
         <v>262886.66666666669</v>
       </c>
+      <c r="BJ183" s="5">
+        <v>-0.93247871883086475</v>
+      </c>
     </row>
-    <row r="184" spans="2:61" s="5" customFormat="1">
+    <row r="184" spans="2:62" s="5" customFormat="1">
       <c r="B184" s="5">
         <v>1994.5</v>
       </c>
@@ -27669,8 +28089,11 @@
       <c r="BI184" s="5">
         <v>263725.66666666669</v>
       </c>
+      <c r="BJ184" s="5">
+        <v>0.48459398910188323</v>
+      </c>
     </row>
-    <row r="185" spans="2:61" s="5" customFormat="1">
+    <row r="185" spans="2:62" s="5" customFormat="1">
       <c r="B185" s="5">
         <v>1994.75</v>
       </c>
@@ -27852,8 +28275,11 @@
       <c r="BI185" s="5">
         <v>264554.66666666669</v>
       </c>
+      <c r="BJ185" s="5">
+        <v>0.14063224387775503</v>
+      </c>
     </row>
-    <row r="186" spans="2:61" s="5" customFormat="1">
+    <row r="186" spans="2:62" s="5" customFormat="1">
       <c r="B186" s="5">
         <v>1995</v>
       </c>
@@ -28035,8 +28461,11 @@
       <c r="BI186" s="5">
         <v>265269.66666666669</v>
       </c>
+      <c r="BJ186" s="5">
+        <v>0.31161719291288414</v>
+      </c>
     </row>
-    <row r="187" spans="2:61" s="5" customFormat="1">
+    <row r="187" spans="2:62" s="5" customFormat="1">
       <c r="B187" s="5">
         <v>1995.25</v>
       </c>
@@ -28218,8 +28647,11 @@
       <c r="BI187" s="5">
         <v>266007.66666666669</v>
       </c>
+      <c r="BJ187" s="5">
+        <v>0.96273189313448082</v>
+      </c>
     </row>
-    <row r="188" spans="2:61" s="5" customFormat="1">
+    <row r="188" spans="2:62" s="5" customFormat="1">
       <c r="B188" s="5">
         <v>1995.5</v>
       </c>
@@ -28401,8 +28833,11 @@
       <c r="BI188" s="5">
         <v>266850.66666666669</v>
       </c>
+      <c r="BJ188" s="5">
+        <v>-0.8578301452664403</v>
+      </c>
     </row>
-    <row r="189" spans="2:61" s="5" customFormat="1">
+    <row r="189" spans="2:62" s="5" customFormat="1">
       <c r="B189" s="5">
         <v>1995.75</v>
       </c>
@@ -28584,8 +29019,11 @@
       <c r="BI189" s="5">
         <v>267704.66666666669</v>
       </c>
+      <c r="BJ189" s="5">
+        <v>0.84886772276594713</v>
+      </c>
     </row>
-    <row r="190" spans="2:61" s="5" customFormat="1">
+    <row r="190" spans="2:62" s="5" customFormat="1">
       <c r="B190" s="5">
         <v>1996</v>
       </c>
@@ -28767,8 +29205,11 @@
       <c r="BI190" s="5">
         <v>268370</v>
       </c>
+      <c r="BJ190" s="5">
+        <v>1.4359382113885837</v>
+      </c>
     </row>
-    <row r="191" spans="2:61" s="5" customFormat="1">
+    <row r="191" spans="2:62" s="5" customFormat="1">
       <c r="B191" s="5">
         <v>1996.25</v>
       </c>
@@ -28950,8 +29391,11 @@
       <c r="BI191" s="5">
         <v>269115.66666666669</v>
       </c>
+      <c r="BJ191" s="5">
+        <v>-0.95174536009696586</v>
+      </c>
     </row>
-    <row r="192" spans="2:61" s="5" customFormat="1">
+    <row r="192" spans="2:62" s="5" customFormat="1">
       <c r="B192" s="5">
         <v>1996.5</v>
       </c>
@@ -29133,8 +29577,11 @@
       <c r="BI192" s="5">
         <v>269975.66666666669</v>
       </c>
+      <c r="BJ192" s="5">
+        <v>3.1927144438610361E-2</v>
+      </c>
     </row>
-    <row r="193" spans="2:61" s="5" customFormat="1">
+    <row r="193" spans="2:62" s="5" customFormat="1">
       <c r="B193" s="5">
         <v>1996.75</v>
       </c>
@@ -29316,8 +29763,11 @@
       <c r="BI193" s="5">
         <v>270861.33333333331</v>
       </c>
+      <c r="BJ193" s="5">
+        <v>-0.16990347005782611</v>
+      </c>
     </row>
-    <row r="194" spans="2:61" s="5" customFormat="1">
+    <row r="194" spans="2:62" s="5" customFormat="1">
       <c r="B194" s="5">
         <v>1997</v>
       </c>
@@ -29499,8 +29949,11 @@
       <c r="BI194" s="5">
         <v>271588.66666666669</v>
       </c>
+      <c r="BJ194" s="5">
+        <v>0.28745033486153937</v>
+      </c>
     </row>
-    <row r="195" spans="2:61" s="5" customFormat="1">
+    <row r="195" spans="2:62" s="5" customFormat="1">
       <c r="B195" s="5">
         <v>1997.25</v>
       </c>
@@ -29682,8 +30135,11 @@
       <c r="BI195" s="5">
         <v>272349</v>
       </c>
+      <c r="BJ195" s="5">
+        <v>-0.28044375169786961</v>
+      </c>
     </row>
-    <row r="196" spans="2:61" s="5" customFormat="1">
+    <row r="196" spans="2:62" s="5" customFormat="1">
       <c r="B196" s="5">
         <v>1997.5</v>
       </c>
@@ -29865,8 +30321,11 @@
       <c r="BI196" s="5">
         <v>273234</v>
       </c>
+      <c r="BJ196" s="5">
+        <v>1.2403852513674416</v>
+      </c>
     </row>
-    <row r="197" spans="2:61" s="5" customFormat="1">
+    <row r="197" spans="2:62" s="5" customFormat="1">
       <c r="B197" s="5">
         <v>1997.75</v>
       </c>
@@ -30048,8 +30507,11 @@
       <c r="BI197" s="5">
         <v>274116.66666666669</v>
       </c>
+      <c r="BJ197" s="5">
+        <v>-0.21648807811035534</v>
+      </c>
     </row>
-    <row r="198" spans="2:61" s="5" customFormat="1">
+    <row r="198" spans="2:62" s="5" customFormat="1">
       <c r="B198" s="5">
         <v>1998</v>
       </c>
@@ -30231,8 +30693,11 @@
       <c r="BI198" s="5">
         <v>274837</v>
       </c>
+      <c r="BJ198" s="5">
+        <v>1.4836851603724148</v>
+      </c>
     </row>
-    <row r="199" spans="2:61" s="5" customFormat="1">
+    <row r="199" spans="2:62" s="5" customFormat="1">
       <c r="B199" s="5">
         <v>1998.25</v>
       </c>
@@ -30414,8 +30879,11 @@
       <c r="BI199" s="5">
         <v>275568</v>
       </c>
+      <c r="BJ199" s="5">
+        <v>0.94287385898046483</v>
+      </c>
     </row>
-    <row r="200" spans="2:61" s="5" customFormat="1">
+    <row r="200" spans="2:62" s="5" customFormat="1">
       <c r="B200" s="5">
         <v>1998.5</v>
       </c>
@@ -30597,8 +31065,11 @@
       <c r="BI200" s="5">
         <v>276415.66666666669</v>
       </c>
+      <c r="BJ200" s="5">
+        <v>-0.14252559952605592</v>
+      </c>
     </row>
-    <row r="201" spans="2:61" s="5" customFormat="1">
+    <row r="201" spans="2:62" s="5" customFormat="1">
       <c r="B201" s="5">
         <v>1998.75</v>
       </c>
@@ -30780,8 +31251,11 @@
       <c r="BI201" s="5">
         <v>277268.66666666669</v>
       </c>
+      <c r="BJ201" s="5">
+        <v>0.61426536727205328</v>
+      </c>
     </row>
-    <row r="202" spans="2:61" s="5" customFormat="1">
+    <row r="202" spans="2:62" s="5" customFormat="1">
       <c r="B202" s="5">
         <v>1999</v>
       </c>
@@ -30963,8 +31437,11 @@
       <c r="BI202" s="5">
         <v>277993.33333333331</v>
       </c>
+      <c r="BJ202" s="5">
+        <v>0.84309013957548273</v>
+      </c>
     </row>
-    <row r="203" spans="2:61" s="5" customFormat="1">
+    <row r="203" spans="2:62" s="5" customFormat="1">
       <c r="B203" s="5">
         <v>1999.25</v>
       </c>
@@ -31146,8 +31623,11 @@
       <c r="BI203" s="5">
         <v>278723</v>
       </c>
+      <c r="BJ203" s="5">
+        <v>0.90577948670457487</v>
+      </c>
     </row>
-    <row r="204" spans="2:61" s="5" customFormat="1">
+    <row r="204" spans="2:62" s="5" customFormat="1">
       <c r="B204" s="5">
         <v>1999.5</v>
       </c>
@@ -31329,8 +31809,11 @@
       <c r="BI204" s="5">
         <v>279600</v>
       </c>
+      <c r="BJ204" s="5">
+        <v>-0.72854383058207239</v>
+      </c>
     </row>
-    <row r="205" spans="2:61" s="5" customFormat="1">
+    <row r="205" spans="2:62" s="5" customFormat="1">
       <c r="B205" s="5">
         <v>1999.75</v>
       </c>
@@ -31512,8 +31995,11 @@
       <c r="BI205" s="5">
         <v>280463.33333333331</v>
       </c>
+      <c r="BJ205" s="5">
+        <v>0.16084504094770527</v>
+      </c>
     </row>
-    <row r="206" spans="2:61" s="5" customFormat="1">
+    <row r="206" spans="2:62" s="5" customFormat="1">
       <c r="B206" s="5">
         <v>2000</v>
       </c>
@@ -31695,8 +32181,11 @@
       <c r="BI206" s="5">
         <v>281191.66666666669</v>
       </c>
+      <c r="BJ206" s="5">
+        <v>1.0460116071022079</v>
+      </c>
     </row>
-    <row r="207" spans="2:61" s="5" customFormat="1">
+    <row r="207" spans="2:62" s="5" customFormat="1">
       <c r="B207" s="5">
         <v>2000.25</v>
       </c>
@@ -31878,8 +32367,11 @@
       <c r="BI207" s="5">
         <v>281885.33333333331</v>
       </c>
+      <c r="BJ207" s="5">
+        <v>-0.33163609638803099</v>
+      </c>
     </row>
-    <row r="208" spans="2:61" s="5" customFormat="1">
+    <row r="208" spans="2:62" s="5" customFormat="1">
       <c r="B208" s="5">
         <v>2000.5</v>
       </c>
@@ -32061,8 +32553,11 @@
       <c r="BI208" s="5">
         <v>282656.66666666669</v>
       </c>
+      <c r="BJ208" s="5">
+        <v>1.2559313919169601</v>
+      </c>
     </row>
-    <row r="209" spans="2:61" s="5" customFormat="1">
+    <row r="209" spans="2:62" s="5" customFormat="1">
       <c r="B209" s="5">
         <v>2000.75</v>
       </c>
@@ -32244,8 +32739,11 @@
       <c r="BI209" s="5">
         <v>283450</v>
       </c>
+      <c r="BJ209" s="5">
+        <v>-0.41579112645012323</v>
+      </c>
     </row>
-    <row r="210" spans="2:61" s="5" customFormat="1">
+    <row r="210" spans="2:62" s="5" customFormat="1">
       <c r="B210" s="5">
         <v>2001</v>
       </c>
@@ -32427,8 +32925,11 @@
       <c r="BI210" s="5">
         <v>284135.66666666669</v>
       </c>
+      <c r="BJ210" s="5">
+        <v>-1.1384550240317992</v>
+      </c>
     </row>
-    <row r="211" spans="2:61" s="5" customFormat="1">
+    <row r="211" spans="2:62" s="5" customFormat="1">
       <c r="B211" s="5">
         <v>2001.25</v>
       </c>
@@ -32610,8 +33111,11 @@
       <c r="BI211" s="5">
         <v>284817.66666666669</v>
       </c>
+      <c r="BJ211" s="5">
+        <v>-0.32266807682579757</v>
+      </c>
     </row>
-    <row r="212" spans="2:61" s="5" customFormat="1">
+    <row r="212" spans="2:62" s="5" customFormat="1">
       <c r="B212" s="5">
         <v>2001.5</v>
       </c>
@@ -32793,8 +33297,11 @@
       <c r="BI212" s="5">
         <v>285574</v>
       </c>
+      <c r="BJ212" s="5">
+        <v>1.3392736784193853</v>
+      </c>
     </row>
-    <row r="213" spans="2:61" s="5" customFormat="1">
+    <row r="213" spans="2:62" s="5" customFormat="1">
       <c r="B213" s="5">
         <v>2001.75</v>
       </c>
@@ -32976,8 +33483,11 @@
       <c r="BI213" s="5">
         <v>286336.33333333331</v>
       </c>
+      <c r="BJ213" s="5">
+        <v>0.71798715729442608</v>
+      </c>
     </row>
-    <row r="214" spans="2:61" s="5" customFormat="1">
+    <row r="214" spans="2:62" s="5" customFormat="1">
       <c r="B214" s="5">
         <v>2002</v>
       </c>
@@ -33159,8 +33669,11 @@
       <c r="BI214" s="5">
         <v>286990.66666666669</v>
       </c>
+      <c r="BJ214" s="5">
+        <v>-1.5422091995498892</v>
+      </c>
     </row>
-    <row r="215" spans="2:61" s="5" customFormat="1">
+    <row r="215" spans="2:62" s="5" customFormat="1">
       <c r="B215" s="5">
         <v>2002.25</v>
       </c>
@@ -33342,8 +33855,11 @@
       <c r="BI215" s="5">
         <v>287628</v>
       </c>
+      <c r="BJ215" s="5">
+        <v>-1.5789544591951095</v>
+      </c>
     </row>
-    <row r="216" spans="2:61" s="5" customFormat="1">
+    <row r="216" spans="2:62" s="5" customFormat="1">
       <c r="B216" s="5">
         <v>2002.5</v>
       </c>
@@ -33525,8 +34041,11 @@
       <c r="BI216" s="5">
         <v>288361</v>
       </c>
+      <c r="BJ216" s="5">
+        <v>-0.80047023112522808</v>
+      </c>
     </row>
-    <row r="217" spans="2:61" s="5" customFormat="1">
+    <row r="217" spans="2:62" s="5" customFormat="1">
       <c r="B217" s="5">
         <v>2002.75</v>
       </c>
@@ -33708,8 +34227,11 @@
       <c r="BI217" s="5">
         <v>289096.33333333331</v>
       </c>
+      <c r="BJ217" s="5">
+        <v>1.8528330602082972</v>
+      </c>
     </row>
-    <row r="218" spans="2:61" s="5" customFormat="1">
+    <row r="218" spans="2:62" s="5" customFormat="1">
       <c r="B218" s="5">
         <v>2003</v>
       </c>
@@ -33891,8 +34413,11 @@
       <c r="BI218" s="5">
         <v>289714.33333333331</v>
       </c>
+      <c r="BJ218" s="5">
+        <v>-0.54315443142572672</v>
+      </c>
     </row>
-    <row r="219" spans="2:61" s="5" customFormat="1">
+    <row r="219" spans="2:62" s="5" customFormat="1">
       <c r="B219" s="5">
         <v>2003.25</v>
       </c>
@@ -34074,8 +34599,11 @@
       <c r="BI219" s="5">
         <v>290351.66666666669</v>
       </c>
+      <c r="BJ219" s="5">
+        <v>2.1719733827314802</v>
+      </c>
     </row>
-    <row r="220" spans="2:61" s="5" customFormat="1">
+    <row r="220" spans="2:62" s="5" customFormat="1">
       <c r="B220" s="5">
         <v>2003.5</v>
       </c>
@@ -34257,8 +34785,11 @@
       <c r="BI220" s="5">
         <v>291071</v>
       </c>
+      <c r="BJ220" s="5">
+        <v>0.19727166714554464</v>
+      </c>
     </row>
-    <row r="221" spans="2:61" s="5" customFormat="1">
+    <row r="221" spans="2:62" s="5" customFormat="1">
       <c r="B221" s="5">
         <v>2003.75</v>
       </c>
@@ -34440,8 +34971,11 @@
       <c r="BI221" s="5">
         <v>291796.33333333331</v>
       </c>
+      <c r="BJ221" s="5">
+        <v>-0.57888530690222861</v>
+      </c>
     </row>
-    <row r="222" spans="2:61" s="5" customFormat="1">
+    <row r="222" spans="2:62" s="5" customFormat="1">
       <c r="B222" s="5">
         <v>2004</v>
       </c>
@@ -34623,8 +35157,11 @@
       <c r="BI222" s="5">
         <v>292373.66666666669</v>
       </c>
+      <c r="BJ222" s="5">
+        <v>0.31948986608639685</v>
+      </c>
     </row>
-    <row r="223" spans="2:61" s="5" customFormat="1">
+    <row r="223" spans="2:62" s="5" customFormat="1">
       <c r="B223" s="5">
         <v>2004.25</v>
       </c>
@@ -34806,8 +35343,11 @@
       <c r="BI223" s="5">
         <v>292999.66666666669</v>
       </c>
+      <c r="BJ223" s="5">
+        <v>0.93107052430315451</v>
+      </c>
     </row>
-    <row r="224" spans="2:61" s="5" customFormat="1">
+    <row r="224" spans="2:62" s="5" customFormat="1">
       <c r="B224" s="5">
         <v>2004.5</v>
       </c>
@@ -34989,8 +35529,11 @@
       <c r="BI224" s="5">
         <v>293717.66666666669</v>
       </c>
+      <c r="BJ224" s="5">
+        <v>0.81255432441198483</v>
+      </c>
     </row>
-    <row r="225" spans="2:61" s="5" customFormat="1">
+    <row r="225" spans="2:62" s="5" customFormat="1">
       <c r="B225" s="5">
         <v>2004.75</v>
       </c>
@@ -35172,8 +35715,11 @@
       <c r="BI225" s="5">
         <v>294463.33333333331</v>
       </c>
+      <c r="BJ225" s="5">
+        <v>0.24521538666287182</v>
+      </c>
     </row>
-    <row r="226" spans="2:61" s="5" customFormat="1">
+    <row r="226" spans="2:62" s="5" customFormat="1">
       <c r="B226" s="5">
         <v>2005</v>
       </c>
@@ -35355,8 +35901,11 @@
       <c r="BI226" s="5">
         <v>295102</v>
       </c>
+      <c r="BJ226" s="5">
+        <v>-0.8364855876510966</v>
+      </c>
     </row>
-    <row r="227" spans="2:61" s="5" customFormat="1">
+    <row r="227" spans="2:62" s="5" customFormat="1">
       <c r="B227" s="5">
         <v>2005.25</v>
       </c>
@@ -35538,8 +36087,11 @@
       <c r="BI227" s="5">
         <v>295710</v>
       </c>
+      <c r="BJ227" s="5">
+        <v>1.2805168030399474</v>
+      </c>
     </row>
-    <row r="228" spans="2:61" s="5" customFormat="1">
+    <row r="228" spans="2:62" s="5" customFormat="1">
       <c r="B228" s="5">
         <v>2005.5</v>
       </c>
@@ -35721,8 +36273,11 @@
       <c r="BI228" s="5">
         <v>296444.33333333331</v>
       </c>
+      <c r="BJ228" s="5">
+        <v>-0.28211898651404216</v>
+      </c>
     </row>
-    <row r="229" spans="2:61" s="5" customFormat="1">
+    <row r="229" spans="2:62" s="5" customFormat="1">
       <c r="B229" s="5">
         <v>2005.75</v>
       </c>
@@ -35904,8 +36459,11 @@
       <c r="BI229" s="5">
         <v>297203.33333333331</v>
       </c>
+      <c r="BJ229" s="5">
+        <v>0.17093970210224091</v>
+      </c>
     </row>
-    <row r="230" spans="2:61" s="5" customFormat="1">
+    <row r="230" spans="2:62" s="5" customFormat="1">
       <c r="B230" s="5">
         <v>2006</v>
       </c>
@@ -36087,8 +36645,11 @@
       <c r="BI230" s="5">
         <v>297853.66666666669</v>
       </c>
+      <c r="BJ230" s="5">
+        <v>-0.43612719934649813</v>
+      </c>
     </row>
-    <row r="231" spans="2:61" s="5" customFormat="1">
+    <row r="231" spans="2:62" s="5" customFormat="1">
       <c r="B231" s="5">
         <v>2006.25</v>
       </c>
@@ -36267,8 +36828,11 @@
       <c r="BI231" s="5">
         <v>298505.33333333331</v>
       </c>
+      <c r="BJ231" s="5">
+        <v>-0.1232373998568112</v>
+      </c>
     </row>
-    <row r="232" spans="2:61" s="5" customFormat="1">
+    <row r="232" spans="2:62" s="5" customFormat="1">
       <c r="B232" s="5">
         <v>2006.5</v>
       </c>
@@ -36447,8 +37011,11 @@
       <c r="BI232" s="5">
         <v>299271</v>
       </c>
+      <c r="BJ232" s="5">
+        <v>1.1383148295083174</v>
+      </c>
     </row>
-    <row r="233" spans="2:61" s="5" customFormat="1">
+    <row r="233" spans="2:62" s="5" customFormat="1">
       <c r="B233" s="5">
         <v>2006.75</v>
       </c>
@@ -36627,8 +37194,11 @@
       <c r="BI233" s="5">
         <v>300089.66666666669</v>
       </c>
+      <c r="BJ233" s="5">
+        <v>-0.52466810848248713</v>
+      </c>
     </row>
-    <row r="234" spans="2:61" s="5" customFormat="1">
+    <row r="234" spans="2:62" s="5" customFormat="1">
       <c r="B234" s="5">
         <v>2007</v>
       </c>
@@ -36792,8 +37362,11 @@
       <c r="BI234" s="5">
         <v>300799</v>
       </c>
+      <c r="BJ234" s="5">
+        <v>-4.8163545428100918E-2</v>
+      </c>
     </row>
-    <row r="235" spans="2:61" s="5" customFormat="1">
+    <row r="235" spans="2:62" s="5" customFormat="1">
       <c r="B235" s="5">
         <v>2007.25</v>
       </c>
@@ -36957,8 +37530,11 @@
       <c r="BI235" s="5">
         <v>301492</v>
       </c>
+      <c r="BJ235" s="5">
+        <v>-0.30908344185091363</v>
+      </c>
     </row>
-    <row r="236" spans="2:61" s="5" customFormat="1">
+    <row r="236" spans="2:62" s="5" customFormat="1">
       <c r="B236" s="5">
         <v>2007.5</v>
       </c>
@@ -37122,8 +37698,11 @@
       <c r="BI236" s="5">
         <v>302272.33333333331</v>
       </c>
+      <c r="BJ236" s="5">
+        <v>-0.41663774514533153</v>
+      </c>
     </row>
-    <row r="237" spans="2:61" s="5" customFormat="1">
+    <row r="237" spans="2:62" s="5" customFormat="1">
       <c r="B237" s="5">
         <v>2007.75</v>
       </c>
@@ -37287,8 +37866,11 @@
       <c r="BI237" s="5">
         <v>303049.33333333331</v>
       </c>
+      <c r="BJ237" s="5">
+        <v>-2.2360110590831246</v>
+      </c>
     </row>
-    <row r="238" spans="2:61" s="5" customFormat="1">
+    <row r="238" spans="2:62" s="5" customFormat="1">
       <c r="B238" s="5">
         <v>2008</v>
       </c>
@@ -37452,8 +38034,11 @@
       <c r="BI238" s="5">
         <v>303708</v>
       </c>
+      <c r="BJ238" s="5">
+        <v>-1.5925408085839163</v>
+      </c>
     </row>
-    <row r="239" spans="2:61" s="5" customFormat="1">
+    <row r="239" spans="2:62" s="5" customFormat="1">
       <c r="B239" s="5">
         <v>2008.25</v>
       </c>
@@ -37617,8 +38202,11 @@
       <c r="BI239" s="5">
         <v>304332</v>
       </c>
+      <c r="BJ239" s="5">
+        <v>-1.385779374207684</v>
+      </c>
     </row>
-    <row r="240" spans="2:61" s="5" customFormat="1">
+    <row r="240" spans="2:62" s="5" customFormat="1">
       <c r="B240" s="5">
         <v>2008.5</v>
       </c>
@@ -37782,8 +38370,11 @@
       <c r="BI240" s="5">
         <v>305050.66666666669</v>
       </c>
+      <c r="BJ240" s="5">
+        <v>-2.2000806019784833</v>
+      </c>
     </row>
-    <row r="241" spans="2:61" s="5" customFormat="1">
+    <row r="241" spans="2:62" s="5" customFormat="1">
       <c r="B241" s="5">
         <v>2008.75</v>
       </c>
@@ -37947,8 +38538,11 @@
       <c r="BI241" s="5">
         <v>305781.33333333331</v>
       </c>
+      <c r="BJ241" s="5">
+        <v>-0.92854785697595432</v>
+      </c>
     </row>
-    <row r="242" spans="2:61" s="5" customFormat="1">
+    <row r="242" spans="2:62" s="5" customFormat="1">
       <c r="B242" s="5">
         <v>2009</v>
       </c>
@@ -38112,8 +38706,11 @@
       <c r="BI242" s="5">
         <v>306399.33333333331</v>
       </c>
+      <c r="BJ242" s="5">
+        <v>-1.3548250081833153</v>
+      </c>
     </row>
-    <row r="243" spans="2:61" s="5" customFormat="1">
+    <row r="243" spans="2:62" s="5" customFormat="1">
       <c r="B243" s="5">
         <v>2009.25</v>
       </c>
@@ -38277,8 +38874,11 @@
       <c r="BI243" s="5">
         <v>306992.33333333331</v>
       </c>
+      <c r="BJ243" s="5">
+        <v>-0.63560991684100432</v>
+      </c>
     </row>
-    <row r="244" spans="2:61" s="5" customFormat="1">
+    <row r="244" spans="2:62" s="5" customFormat="1">
       <c r="B244" s="5">
         <v>2009.5</v>
       </c>
@@ -38442,8 +39042,11 @@
       <c r="BI244" s="5">
         <v>307690</v>
       </c>
+      <c r="BJ244" s="5">
+        <v>0.50969311128592709</v>
+      </c>
     </row>
-    <row r="245" spans="2:61" s="5" customFormat="1">
+    <row r="245" spans="2:62" s="5" customFormat="1">
       <c r="B245" s="5">
         <v>2009.75</v>
       </c>
@@ -38607,8 +39210,11 @@
       <c r="BI245" s="5">
         <v>308413.33333333331</v>
       </c>
+      <c r="BJ245" s="5">
+        <v>-0.60406586003873675</v>
+      </c>
     </row>
-    <row r="246" spans="2:61" s="5" customFormat="1">
+    <row r="246" spans="2:62" s="5" customFormat="1">
       <c r="B246" s="5">
         <v>2010</v>
       </c>
@@ -38770,8 +39376,11 @@
       <c r="BI246" s="5">
         <v>309024</v>
       </c>
+      <c r="BJ246" s="5">
+        <v>0.78904451047844559</v>
+      </c>
     </row>
-    <row r="247" spans="2:61" s="5" customFormat="1">
+    <row r="247" spans="2:62" s="5" customFormat="1">
       <c r="B247" s="5">
         <v>2010.25</v>
       </c>
@@ -38933,8 +39542,11 @@
       <c r="BI247" s="5">
         <v>309373.66666666669</v>
       </c>
+      <c r="BJ247" s="5">
+        <v>-3.0824010865585227E-2</v>
+      </c>
     </row>
-    <row r="248" spans="2:61" s="5" customFormat="1">
+    <row r="248" spans="2:62" s="5" customFormat="1">
       <c r="B248" s="5">
         <v>2010.5</v>
       </c>
@@ -39096,8 +39708,11 @@
       <c r="BI248" s="5">
         <v>309976.33333333331</v>
       </c>
+      <c r="BJ248" s="5">
+        <v>0.97538850393538057</v>
+      </c>
     </row>
-    <row r="249" spans="2:61" s="5" customFormat="1">
+    <row r="249" spans="2:62" s="5" customFormat="1">
       <c r="B249" s="5">
         <v>2010.75</v>
       </c>
@@ -39259,8 +39874,11 @@
       <c r="BI249" s="5">
         <v>310622</v>
       </c>
+      <c r="BJ249" s="5">
+        <v>3.7279266098707187E-2</v>
+      </c>
     </row>
-    <row r="250" spans="2:61" s="5" customFormat="1">
+    <row r="250" spans="2:62" s="5" customFormat="1">
       <c r="B250" s="5">
         <v>2011</v>
       </c>
@@ -39422,8 +40040,11 @@
       <c r="BI250" s="5">
         <v>311155.66666666669</v>
       </c>
+      <c r="BJ250" s="5">
+        <v>-8.4124336774218988E-2</v>
+      </c>
     </row>
-    <row r="251" spans="2:61" s="5" customFormat="1">
+    <row r="251" spans="2:62" s="5" customFormat="1">
       <c r="B251" s="5">
         <v>2011.25</v>
       </c>
@@ -39585,8 +40206,11 @@
       <c r="BI251" s="5">
         <v>311667.33333333331</v>
       </c>
+      <c r="BJ251" s="5">
+        <v>-1.0353901971414661</v>
+      </c>
     </row>
-    <row r="252" spans="2:61" s="5" customFormat="1">
+    <row r="252" spans="2:62" s="5" customFormat="1">
       <c r="B252" s="5">
         <v>2011.5</v>
       </c>
@@ -39748,8 +40372,11 @@
       <c r="BI252" s="5">
         <v>312279.33333333331</v>
       </c>
+      <c r="BJ252" s="5">
+        <v>-3.8909081821970892E-3</v>
+      </c>
     </row>
-    <row r="253" spans="2:61" s="5" customFormat="1">
+    <row r="253" spans="2:62" s="5" customFormat="1">
       <c r="B253" s="5">
         <v>2011.75</v>
       </c>
@@ -39911,8 +40538,11 @@
       <c r="BI253" s="5">
         <v>312910.33333333331</v>
       </c>
+      <c r="BJ253" s="5">
+        <v>0.36269951165478465</v>
+      </c>
     </row>
-    <row r="254" spans="2:61" s="5" customFormat="1">
+    <row r="254" spans="2:62" s="5" customFormat="1">
       <c r="B254" s="5">
         <v>2012</v>
       </c>
@@ -40074,8 +40704,11 @@
       <c r="BI254" s="5">
         <v>313436.66666666669</v>
       </c>
+      <c r="BJ254" s="5">
+        <v>0.63772860475439652</v>
+      </c>
     </row>
-    <row r="255" spans="2:61" s="5" customFormat="1">
+    <row r="255" spans="2:62" s="5" customFormat="1">
       <c r="B255" s="5">
         <v>2012.25</v>
       </c>
@@ -40237,8 +40870,11 @@
       <c r="BI255" s="5">
         <v>313948</v>
       </c>
+      <c r="BJ255" s="5">
+        <v>-1.946757759348738</v>
+      </c>
     </row>
-    <row r="256" spans="2:61" s="5" customFormat="1">
+    <row r="256" spans="2:62" s="5" customFormat="1">
       <c r="B256" s="5">
         <v>2012.5</v>
       </c>
@@ -40400,8 +41036,11 @@
       <c r="BI256" s="5">
         <v>314550.33333333331</v>
       </c>
+      <c r="BJ256" s="5">
+        <v>0.35338216846130355</v>
+      </c>
     </row>
-    <row r="257" spans="2:61" s="5" customFormat="1">
+    <row r="257" spans="2:62" s="5" customFormat="1">
       <c r="B257" s="5">
         <v>2012.75</v>
       </c>
@@ -40563,8 +41202,11 @@
       <c r="BI257" s="5">
         <v>315185</v>
       </c>
+      <c r="BJ257" s="5">
+        <v>0.47394483934834525</v>
+      </c>
     </row>
-    <row r="258" spans="2:61" s="5" customFormat="1">
+    <row r="258" spans="2:62" s="5" customFormat="1">
       <c r="B258" s="5">
         <v>2013</v>
       </c>
@@ -40726,8 +41368,11 @@
       <c r="BI258" s="5">
         <v>315677</v>
       </c>
+      <c r="BJ258" s="5">
+        <v>0.17351122553958465</v>
+      </c>
     </row>
-    <row r="259" spans="2:61" s="5" customFormat="1">
+    <row r="259" spans="2:62" s="5" customFormat="1">
       <c r="B259" s="5">
         <v>2013.25</v>
       </c>
@@ -40889,8 +41534,11 @@
       <c r="BI259" s="5">
         <v>316158</v>
       </c>
+      <c r="BJ259" s="5">
+        <v>1.0337190873751706E-2</v>
+      </c>
     </row>
-    <row r="260" spans="2:61" s="5" customFormat="1">
+    <row r="260" spans="2:62" s="5" customFormat="1">
       <c r="B260" s="5">
         <v>2013.5</v>
       </c>
@@ -41052,8 +41700,11 @@
       <c r="BI260" s="5">
         <v>316763.66666666669</v>
       </c>
+      <c r="BJ260" s="5">
+        <v>0.50037042911282181</v>
+      </c>
     </row>
-    <row r="261" spans="2:61" s="5" customFormat="1">
+    <row r="261" spans="2:62" s="5" customFormat="1">
       <c r="B261" s="5">
         <v>2013.75</v>
       </c>
@@ -41215,8 +41866,11 @@
       <c r="BI261" s="5">
         <v>317417.33333333331</v>
       </c>
+      <c r="BJ261" s="5">
+        <v>-0.55513502836771011</v>
+      </c>
     </row>
-    <row r="262" spans="2:61" s="5" customFormat="1">
+    <row r="262" spans="2:62" s="5" customFormat="1">
       <c r="B262" s="5">
         <v>2014</v>
       </c>
@@ -41378,8 +42032,11 @@
       <c r="BI262" s="5">
         <v>317966.33333333331</v>
       </c>
+      <c r="BJ262" s="5">
+        <v>0.96761063151986237</v>
+      </c>
     </row>
-    <row r="263" spans="2:61" s="5" customFormat="1">
+    <row r="263" spans="2:62" s="5" customFormat="1">
       <c r="B263" s="5">
         <v>2014.25</v>
       </c>
@@ -41541,8 +42198,11 @@
       <c r="BI263" s="5">
         <v>318500.33333333331</v>
       </c>
+      <c r="BJ263" s="5">
+        <v>1.2103592077627205</v>
+      </c>
     </row>
-    <row r="264" spans="2:61" s="5" customFormat="1">
+    <row r="264" spans="2:62" s="5" customFormat="1">
       <c r="B264" s="5">
         <v>2014.5</v>
       </c>
@@ -41704,8 +42364,11 @@
       <c r="BI264" s="5">
         <v>319135</v>
       </c>
+      <c r="BJ264" s="5">
+        <v>-0.39850508577793659</v>
+      </c>
     </row>
-    <row r="265" spans="2:61" s="5" customFormat="1">
+    <row r="265" spans="2:62" s="5" customFormat="1">
       <c r="B265" s="5">
         <v>2014.75</v>
       </c>
@@ -41867,8 +42530,11 @@
       <c r="BI265" s="5">
         <v>319811.33333333331</v>
       </c>
+      <c r="BJ265" s="5">
+        <v>0.11250005587509349</v>
+      </c>
     </row>
-    <row r="266" spans="2:61" s="5" customFormat="1">
+    <row r="266" spans="2:62" s="5" customFormat="1">
       <c r="B266" s="5">
         <v>2015</v>
       </c>
@@ -42030,8 +42696,11 @@
       <c r="BI266" s="5">
         <v>320349.66666666669</v>
       </c>
+      <c r="BJ266" s="5">
+        <v>0.11388620008488515</v>
+      </c>
     </row>
-    <row r="267" spans="2:61" s="5" customFormat="1">
+    <row r="267" spans="2:62" s="5" customFormat="1">
       <c r="B267" s="5">
         <v>2015.25</v>
       </c>
@@ -42193,8 +42862,11 @@
       <c r="BI267" s="5">
         <v>320873.66666666669</v>
       </c>
+      <c r="BJ267" s="5">
+        <v>0.19791755307625811</v>
+      </c>
     </row>
-    <row r="268" spans="2:61" s="5" customFormat="1">
+    <row r="268" spans="2:62" s="5" customFormat="1">
       <c r="B268" s="5">
         <v>2015.5</v>
       </c>
@@ -42356,8 +43028,11 @@
       <c r="BI268" s="5">
         <v>321505</v>
       </c>
+      <c r="BJ268" s="5">
+        <v>-4.0990677086138419E-2</v>
+      </c>
     </row>
-    <row r="269" spans="2:61" s="5" customFormat="1">
+    <row r="269" spans="2:62" s="5" customFormat="1">
       <c r="B269" s="5">
         <v>2015.75</v>
       </c>
@@ -42519,8 +43194,11 @@
       <c r="BI269" s="5">
         <v>322168.66666666669</v>
       </c>
+      <c r="BJ269" s="5">
+        <v>9.9458361439364595E-3</v>
+      </c>
     </row>
-    <row r="270" spans="2:61" s="5" customFormat="1">
+    <row r="270" spans="2:62" s="5" customFormat="1">
       <c r="B270" s="5">
         <v>2016</v>
       </c>
@@ -42682,8 +43360,11 @@
       <c r="BI270" s="5">
         <v>322712.66666666669</v>
       </c>
+      <c r="BJ270" s="5">
+        <v>-0.327572783436476</v>
+      </c>
     </row>
-    <row r="271" spans="2:61" s="5" customFormat="1">
+    <row r="271" spans="2:62" s="5" customFormat="1">
       <c r="B271" s="5">
         <v>2016.25</v>
       </c>
@@ -42845,8 +43526,11 @@
       <c r="BI271" s="5">
         <v>323228.66666666669</v>
       </c>
+      <c r="BJ271" s="5">
+        <v>1.027472306460014</v>
+      </c>
     </row>
-    <row r="272" spans="2:61" s="5" customFormat="1">
+    <row r="272" spans="2:62" s="5" customFormat="1">
       <c r="B272" s="5">
         <v>2016.5</v>
       </c>
@@ -43005,8 +43689,11 @@
       <c r="BI272" s="5">
         <v>323849.33333333331</v>
       </c>
+      <c r="BJ272" s="5">
+        <v>4.9199649393765199E-2</v>
+      </c>
     </row>
-    <row r="273" spans="2:61" s="5" customFormat="1">
+    <row r="273" spans="2:62" s="5" customFormat="1">
       <c r="B273" s="5">
         <v>2016.75</v>
       </c>
@@ -43165,8 +43852,11 @@
       <c r="BI273" s="5">
         <v>324496.33333333331</v>
       </c>
+      <c r="BJ273" s="5">
+        <v>1.2445327234387613</v>
+      </c>
     </row>
-    <row r="274" spans="2:61" s="5" customFormat="1">
+    <row r="274" spans="2:62" s="5" customFormat="1">
       <c r="B274" s="5">
         <v>2017</v>
       </c>
@@ -43323,8 +44013,11 @@
       <c r="BI274" s="5">
         <v>325028.33333333331</v>
       </c>
+      <c r="BJ274" s="5">
+        <v>0.40149107434930342</v>
+      </c>
     </row>
-    <row r="275" spans="2:61" s="5" customFormat="1">
+    <row r="275" spans="2:62" s="5" customFormat="1">
       <c r="B275" s="5">
         <v>2017.25</v>
       </c>
@@ -43482,7 +44175,7 @@
         <v>325543.33333333331</v>
       </c>
     </row>
-    <row r="276" spans="2:61" s="5" customFormat="1">
+    <row r="276" spans="2:62" s="5" customFormat="1">
       <c r="B276" s="5">
         <v>2017.5</v>
       </c>
@@ -43625,7 +44318,7 @@
         <v>326163.33333333331</v>
       </c>
     </row>
-    <row r="277" spans="2:61" s="5" customFormat="1">
+    <row r="277" spans="2:62" s="5" customFormat="1">
       <c r="B277" s="5">
         <v>2017.75</v>
       </c>
@@ -43730,7 +44423,7 @@
         <v>326810.33333333331</v>
       </c>
     </row>
-    <row r="278" spans="2:61" s="5" customFormat="1">
+    <row r="278" spans="2:62" s="5" customFormat="1">
       <c r="B278" s="5">
         <v>2018</v>
       </c>
@@ -43835,7 +44528,7 @@
         <v>327342.66666666669</v>
       </c>
     </row>
-    <row r="279" spans="2:61" s="5" customFormat="1">
+    <row r="279" spans="2:62" s="5" customFormat="1">
       <c r="B279" s="5">
         <v>2018.25</v>
       </c>
@@ -43930,7 +44623,7 @@
         <v>327857.66666666669</v>
       </c>
     </row>
-    <row r="280" spans="2:61" s="5" customFormat="1">
+    <row r="280" spans="2:62" s="5" customFormat="1">
       <c r="J280" s="4"/>
       <c r="K280" s="4"/>
       <c r="N280" s="4"/>
@@ -43962,7 +44655,7 @@
         <v>328477.33333333331</v>
       </c>
     </row>
-    <row r="281" spans="2:61" s="5" customFormat="1">
+    <row r="281" spans="2:62" s="5" customFormat="1">
       <c r="J281" s="4"/>
       <c r="K281" s="4"/>
       <c r="N281" s="4"/>
@@ -43993,7 +44686,7 @@
         <v>329124.33333333331</v>
       </c>
     </row>
-    <row r="282" spans="2:61" s="5" customFormat="1">
+    <row r="282" spans="2:62" s="5" customFormat="1">
       <c r="J282" s="4"/>
       <c r="K282" s="4"/>
       <c r="N282" s="4"/>
@@ -44013,42 +44706,42 @@
       <c r="BF282" s="8"/>
       <c r="BG282" s="8"/>
     </row>
-    <row r="283" spans="2:61" s="5" customFormat="1">
+    <row r="283" spans="2:62" s="5" customFormat="1">
       <c r="J283" s="4"/>
       <c r="K283" s="4"/>
       <c r="AY283" s="8"/>
       <c r="BF283" s="8"/>
       <c r="BG283" s="8"/>
     </row>
-    <row r="284" spans="2:61" s="5" customFormat="1">
+    <row r="284" spans="2:62" s="5" customFormat="1">
       <c r="J284" s="4"/>
       <c r="K284" s="4"/>
       <c r="AY284" s="8"/>
       <c r="BF284" s="8"/>
       <c r="BG284" s="8"/>
     </row>
-    <row r="285" spans="2:61" s="5" customFormat="1">
+    <row r="285" spans="2:62" s="5" customFormat="1">
       <c r="J285" s="4"/>
       <c r="K285" s="4"/>
       <c r="AY285" s="8"/>
       <c r="BF285" s="8"/>
       <c r="BG285" s="8"/>
     </row>
-    <row r="286" spans="2:61" s="5" customFormat="1">
+    <row r="286" spans="2:62" s="5" customFormat="1">
       <c r="J286" s="4"/>
       <c r="K286" s="4"/>
       <c r="AY286" s="8"/>
       <c r="BF286" s="8"/>
       <c r="BG286" s="8"/>
     </row>
-    <row r="287" spans="2:61" s="5" customFormat="1">
+    <row r="287" spans="2:62" s="5" customFormat="1">
       <c r="J287" s="4"/>
       <c r="K287" s="4"/>
       <c r="AY287" s="8"/>
       <c r="BF287" s="8"/>
       <c r="BG287" s="8"/>
     </row>
-    <row r="288" spans="2:61" s="5" customFormat="1">
+    <row r="288" spans="2:62" s="5" customFormat="1">
       <c r="J288" s="4"/>
       <c r="K288" s="4"/>
       <c r="AY288" s="8"/>

</xml_diff>

<commit_message>
adding a paper and checking busines confidence
</commit_message>
<xml_diff>
--- a/Data/main_file.xlsx
+++ b/Data/main_file.xlsx
@@ -284,12 +284,61 @@
         </r>
       </text>
     </comment>
+    <comment ref="CK1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marco Brianti:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Business Tendency Surveys for Manufacturing: Confidence Indicators: Composite Indicators: European Commission and National Indicators for the United States, Net Percent, Quarterly, Seasonally Adjusted
+Code FRED: BSCICP02USQ460S</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CL1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marco Brianti:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Consumer Confidence of Michigan Index - Table 1</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
   <si>
     <t>MUNI1Y</t>
   </si>
@@ -572,6 +621,12 @@
   <si>
     <t>RDurableCons</t>
   </si>
+  <si>
+    <t>MichIndexConfidence</t>
+  </si>
+  <si>
+    <t>BusinessConfidenceEC</t>
+  </si>
 </sst>
 </file>
 
@@ -581,7 +636,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +715,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1042,13 +1110,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ629"/>
+  <dimension ref="A1:CL629"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AS231" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="CE265" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AW236" sqref="AW236"/>
+      <selection pane="bottomRight" activeCell="CM280" sqref="CM280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22" defaultRowHeight="15.75"/>
@@ -1101,7 +1169,7 @@
     <col min="79" max="16384" width="22" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" s="7" customFormat="1">
+    <row r="1" spans="1:90" s="7" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1366,8 +1434,14 @@
       <c r="CJ1" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="CK1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="CL1" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="2" spans="1:88" s="7" customFormat="1">
+    <row r="2" spans="1:90" s="7" customFormat="1">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1632,8 +1706,14 @@
       <c r="CJ2" s="7">
         <v>2</v>
       </c>
+      <c r="CK2" s="7">
+        <v>2</v>
+      </c>
+      <c r="CL2" s="7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:88" s="7" customFormat="1">
+    <row r="3" spans="1:90" s="7" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1898,8 +1978,14 @@
       <c r="CJ3" s="7">
         <v>1</v>
       </c>
+      <c r="CK3" s="7">
+        <v>1</v>
+      </c>
+      <c r="CL3" s="7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:88" s="7" customFormat="1">
+    <row r="4" spans="1:90" s="7" customFormat="1">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -2164,8 +2250,14 @@
       <c r="CJ4" s="1">
         <v>87</v>
       </c>
+      <c r="CK4" s="7">
+        <v>88</v>
+      </c>
+      <c r="CL4" s="7">
+        <v>89</v>
+      </c>
     </row>
-    <row r="5" spans="1:88" s="7" customFormat="1">
+    <row r="5" spans="1:90" s="7" customFormat="1">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -2430,8 +2522,14 @@
       <c r="CJ5" s="1">
         <v>87</v>
       </c>
+      <c r="CK5" s="7">
+        <v>88</v>
+      </c>
+      <c r="CL5" s="7">
+        <v>89</v>
+      </c>
     </row>
-    <row r="6" spans="1:88" s="5" customFormat="1">
+    <row r="6" spans="1:90" s="5" customFormat="1">
       <c r="B6" s="5">
         <v>1950</v>
       </c>
@@ -2529,7 +2627,7 @@
         <v>-25.047000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:88" s="5" customFormat="1">
+    <row r="7" spans="1:90" s="5" customFormat="1">
       <c r="B7" s="5">
         <v>1950.25</v>
       </c>
@@ -2627,7 +2725,7 @@
         <v>-25.356999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:88" s="5" customFormat="1">
+    <row r="8" spans="1:90" s="5" customFormat="1">
       <c r="B8" s="5">
         <v>1950.5</v>
       </c>
@@ -2725,7 +2823,7 @@
         <v>-25.962</v>
       </c>
     </row>
-    <row r="9" spans="1:88" s="5" customFormat="1">
+    <row r="9" spans="1:90" s="5" customFormat="1">
       <c r="B9" s="5">
         <v>1950.75</v>
       </c>
@@ -2823,7 +2921,7 @@
         <v>-26.004000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:88" s="5" customFormat="1">
+    <row r="10" spans="1:90" s="5" customFormat="1">
       <c r="B10" s="5">
         <v>1951</v>
       </c>
@@ -2921,7 +3019,7 @@
         <v>-26.062999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:88" s="5" customFormat="1">
+    <row r="11" spans="1:90" s="5" customFormat="1">
       <c r="B11" s="5">
         <v>1951.25</v>
       </c>
@@ -3019,7 +3117,7 @@
         <v>-25.963999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:88" s="5" customFormat="1">
+    <row r="12" spans="1:90" s="5" customFormat="1">
       <c r="B12" s="5">
         <v>1951.5</v>
       </c>
@@ -3117,7 +3215,7 @@
         <v>-26.617999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:88" s="5" customFormat="1">
+    <row r="13" spans="1:90" s="5" customFormat="1">
       <c r="B13" s="5">
         <v>1951.75</v>
       </c>
@@ -3215,7 +3313,7 @@
         <v>-26.686</v>
       </c>
     </row>
-    <row r="14" spans="1:88" s="5" customFormat="1">
+    <row r="14" spans="1:90" s="5" customFormat="1">
       <c r="B14" s="5">
         <v>1952</v>
       </c>
@@ -3316,7 +3414,7 @@
         <v>156522.33333333334</v>
       </c>
     </row>
-    <row r="15" spans="1:88" s="5" customFormat="1">
+    <row r="15" spans="1:90" s="5" customFormat="1">
       <c r="B15" s="5">
         <v>1952.25</v>
       </c>
@@ -3417,7 +3515,7 @@
         <v>157142</v>
       </c>
     </row>
-    <row r="16" spans="1:88" s="5" customFormat="1">
+    <row r="16" spans="1:90" s="5" customFormat="1">
       <c r="B16" s="5">
         <v>1952.5</v>
       </c>
@@ -3518,7 +3616,7 @@
         <v>157801.33333333334</v>
       </c>
     </row>
-    <row r="17" spans="2:78" s="5" customFormat="1">
+    <row r="17" spans="2:90" s="5" customFormat="1">
       <c r="B17" s="5">
         <v>1952.75</v>
       </c>
@@ -3619,7 +3717,7 @@
         <v>158504.66666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:78" s="5" customFormat="1">
+    <row r="18" spans="2:90" s="5" customFormat="1">
       <c r="B18" s="5">
         <v>1953</v>
       </c>
@@ -3723,7 +3821,7 @@
         <v>159164</v>
       </c>
     </row>
-    <row r="19" spans="2:78" s="5" customFormat="1">
+    <row r="19" spans="2:90" s="5" customFormat="1">
       <c r="B19" s="5">
         <v>1953.25</v>
       </c>
@@ -3827,7 +3925,7 @@
         <v>159752.33333333334</v>
       </c>
     </row>
-    <row r="20" spans="2:78" s="5" customFormat="1">
+    <row r="20" spans="2:90" s="5" customFormat="1">
       <c r="B20" s="5">
         <v>1953.5</v>
       </c>
@@ -3931,7 +4029,7 @@
         <v>160450.33333333334</v>
       </c>
     </row>
-    <row r="21" spans="2:78" s="5" customFormat="1">
+    <row r="21" spans="2:90" s="5" customFormat="1">
       <c r="B21" s="5">
         <v>1953.75</v>
       </c>
@@ -4035,7 +4133,7 @@
         <v>161218</v>
       </c>
     </row>
-    <row r="22" spans="2:78" s="5" customFormat="1">
+    <row r="22" spans="2:90" s="5" customFormat="1">
       <c r="B22" s="5">
         <v>1954</v>
       </c>
@@ -4139,7 +4237,7 @@
         <v>161908.66666666666</v>
       </c>
     </row>
-    <row r="23" spans="2:78" s="5" customFormat="1">
+    <row r="23" spans="2:90" s="5" customFormat="1">
       <c r="B23" s="5">
         <v>1954.25</v>
       </c>
@@ -4242,8 +4340,9 @@
       <c r="BZ23" s="5">
         <v>162568</v>
       </c>
+      <c r="CL23" s="4"/>
     </row>
-    <row r="24" spans="2:78" s="5" customFormat="1">
+    <row r="24" spans="2:90" s="5" customFormat="1">
       <c r="B24" s="5">
         <v>1954.5</v>
       </c>
@@ -4349,8 +4448,9 @@
       <c r="BZ24" s="5">
         <v>163295.33333333334</v>
       </c>
+      <c r="CL24" s="4"/>
     </row>
-    <row r="25" spans="2:78" s="5" customFormat="1">
+    <row r="25" spans="2:90" s="5" customFormat="1">
       <c r="B25" s="5">
         <v>1954.75</v>
       </c>
@@ -4456,8 +4556,9 @@
       <c r="BZ25" s="5">
         <v>164101</v>
       </c>
+      <c r="CL25" s="4"/>
     </row>
-    <row r="26" spans="2:78" s="5" customFormat="1">
+    <row r="26" spans="2:90" s="5" customFormat="1">
       <c r="B26" s="5">
         <v>1955</v>
       </c>
@@ -4563,8 +4664,9 @@
       <c r="BZ26" s="5">
         <v>164805</v>
       </c>
+      <c r="CL26" s="4"/>
     </row>
-    <row r="27" spans="2:78" s="5" customFormat="1">
+    <row r="27" spans="2:90" s="5" customFormat="1">
       <c r="B27" s="5">
         <v>1955.25</v>
       </c>
@@ -4670,8 +4772,9 @@
       <c r="BZ27" s="5">
         <v>165469.66666666666</v>
       </c>
+      <c r="CL27" s="4"/>
     </row>
-    <row r="28" spans="2:78" s="5" customFormat="1">
+    <row r="28" spans="2:90" s="5" customFormat="1">
       <c r="B28" s="5">
         <v>1955.5</v>
       </c>
@@ -4777,8 +4880,9 @@
       <c r="BZ28" s="5">
         <v>166198.66666666666</v>
       </c>
+      <c r="CL28" s="4"/>
     </row>
-    <row r="29" spans="2:78" s="5" customFormat="1">
+    <row r="29" spans="2:90" s="5" customFormat="1">
       <c r="B29" s="5">
         <v>1955.75</v>
       </c>
@@ -4884,8 +4988,9 @@
       <c r="BZ29" s="5">
         <v>167016</v>
       </c>
+      <c r="CL29" s="4"/>
     </row>
-    <row r="30" spans="2:78" s="5" customFormat="1">
+    <row r="30" spans="2:90" s="5" customFormat="1">
       <c r="B30" s="5">
         <v>1956</v>
       </c>
@@ -4997,8 +5102,9 @@
       <c r="BZ30" s="5">
         <v>167745.33333333334</v>
       </c>
+      <c r="CL30" s="4"/>
     </row>
-    <row r="31" spans="2:78" s="5" customFormat="1">
+    <row r="31" spans="2:90" s="5" customFormat="1">
       <c r="B31" s="5">
         <v>1956.25</v>
       </c>
@@ -5110,8 +5216,9 @@
       <c r="BZ31" s="5">
         <v>168438.66666666666</v>
       </c>
+      <c r="CL31" s="4"/>
     </row>
-    <row r="32" spans="2:78" s="5" customFormat="1">
+    <row r="32" spans="2:90" s="5" customFormat="1">
       <c r="B32" s="5">
         <v>1956.5</v>
       </c>
@@ -5223,8 +5330,9 @@
       <c r="BZ32" s="5">
         <v>169194</v>
       </c>
+      <c r="CL32" s="4"/>
     </row>
-    <row r="33" spans="2:88" s="5" customFormat="1">
+    <row r="33" spans="2:90" s="5" customFormat="1">
       <c r="B33" s="5">
         <v>1956.75</v>
       </c>
@@ -5336,8 +5444,9 @@
       <c r="BZ33" s="5">
         <v>170052.66666666666</v>
       </c>
+      <c r="CL33" s="4"/>
     </row>
-    <row r="34" spans="2:88" s="5" customFormat="1">
+    <row r="34" spans="2:90" s="5" customFormat="1">
       <c r="B34" s="5">
         <v>1957</v>
       </c>
@@ -5450,7 +5559,7 @@
         <v>170802</v>
       </c>
     </row>
-    <row r="35" spans="2:88" s="5" customFormat="1">
+    <row r="35" spans="2:90" s="5" customFormat="1">
       <c r="B35" s="5">
         <v>1957.25</v>
       </c>
@@ -5563,7 +5672,7 @@
         <v>171504.33333333334</v>
       </c>
     </row>
-    <row r="36" spans="2:88" s="5" customFormat="1">
+    <row r="36" spans="2:90" s="5" customFormat="1">
       <c r="B36" s="5">
         <v>1957.5</v>
       </c>
@@ -5676,7 +5785,7 @@
         <v>172259.66666666666</v>
       </c>
     </row>
-    <row r="37" spans="2:88" s="5" customFormat="1">
+    <row r="37" spans="2:90" s="5" customFormat="1">
       <c r="B37" s="5">
         <v>1957.75</v>
       </c>
@@ -5789,7 +5898,7 @@
         <v>173061.33333333334</v>
       </c>
     </row>
-    <row r="38" spans="2:88" s="5" customFormat="1">
+    <row r="38" spans="2:90" s="5" customFormat="1">
       <c r="B38" s="5">
         <v>1958</v>
       </c>
@@ -5902,7 +6011,7 @@
         <v>173741.33333333334</v>
       </c>
     </row>
-    <row r="39" spans="2:88" s="5" customFormat="1">
+    <row r="39" spans="2:90" s="5" customFormat="1">
       <c r="B39" s="5">
         <v>1958.25</v>
       </c>
@@ -6015,7 +6124,7 @@
         <v>174404</v>
       </c>
     </row>
-    <row r="40" spans="2:88" s="5" customFormat="1">
+    <row r="40" spans="2:90" s="5" customFormat="1">
       <c r="B40" s="5">
         <v>1958.5</v>
       </c>
@@ -6128,7 +6237,7 @@
         <v>175146</v>
       </c>
     </row>
-    <row r="41" spans="2:88" s="5" customFormat="1">
+    <row r="41" spans="2:90" s="5" customFormat="1">
       <c r="B41" s="5">
         <v>1958.75</v>
       </c>
@@ -6241,7 +6350,7 @@
         <v>175956.66666666666</v>
       </c>
     </row>
-    <row r="42" spans="2:88" s="5" customFormat="1">
+    <row r="42" spans="2:90" s="5" customFormat="1">
       <c r="B42" s="5">
         <v>1959</v>
       </c>
@@ -6360,7 +6469,7 @@
         <v>176679</v>
       </c>
     </row>
-    <row r="43" spans="2:88" s="5" customFormat="1">
+    <row r="43" spans="2:90" s="5" customFormat="1">
       <c r="B43" s="5">
         <v>1959.25</v>
       </c>
@@ -6479,7 +6588,7 @@
         <v>177367.33333333334</v>
       </c>
     </row>
-    <row r="44" spans="2:88" s="5" customFormat="1">
+    <row r="44" spans="2:90" s="5" customFormat="1">
       <c r="B44" s="5">
         <v>1959.5</v>
       </c>
@@ -6598,7 +6707,7 @@
         <v>178102.33333333334</v>
       </c>
     </row>
-    <row r="45" spans="2:88" s="5" customFormat="1">
+    <row r="45" spans="2:90" s="5" customFormat="1">
       <c r="B45" s="5">
         <v>1959.75</v>
       </c>
@@ -6717,7 +6826,7 @@
         <v>178910.33333333334</v>
       </c>
     </row>
-    <row r="46" spans="2:88" s="5" customFormat="1">
+    <row r="46" spans="2:90" s="5" customFormat="1">
       <c r="B46" s="5">
         <v>1960</v>
       </c>
@@ -6867,8 +6976,14 @@
       <c r="CJ46" s="5">
         <v>7.8638197749387898E-4</v>
       </c>
+      <c r="CK46" s="5">
+        <v>7.7333333333333298</v>
+      </c>
+      <c r="CL46" s="5">
+        <v>100</v>
+      </c>
     </row>
-    <row r="47" spans="2:88" s="5" customFormat="1">
+    <row r="47" spans="2:90" s="5" customFormat="1">
       <c r="B47" s="5">
         <v>1960.25</v>
       </c>
@@ -7018,8 +7133,14 @@
       <c r="CJ47" s="5">
         <v>-3.6071713538996297E-2</v>
       </c>
+      <c r="CK47" s="5">
+        <v>-11.8</v>
+      </c>
+      <c r="CL47" s="5">
+        <v>93.3</v>
+      </c>
     </row>
-    <row r="48" spans="2:88" s="5" customFormat="1">
+    <row r="48" spans="2:90" s="5" customFormat="1">
       <c r="B48" s="5">
         <v>1960.5</v>
       </c>
@@ -7169,8 +7290,14 @@
       <c r="CJ48" s="5">
         <v>-7.9959583259723299E-3</v>
       </c>
+      <c r="CK48" s="5">
+        <v>-8.86666666666666</v>
+      </c>
+      <c r="CL48" s="5">
+        <v>97.2</v>
+      </c>
     </row>
-    <row r="49" spans="2:88" s="5" customFormat="1">
+    <row r="49" spans="2:90" s="5" customFormat="1">
       <c r="B49" s="5">
         <v>1960.75</v>
       </c>
@@ -7320,8 +7447,14 @@
       <c r="CJ49" s="5">
         <v>-1.7704313463465401E-2</v>
       </c>
+      <c r="CK49" s="5">
+        <v>-10.266666666666699</v>
+      </c>
+      <c r="CL49" s="5">
+        <v>90.1</v>
+      </c>
     </row>
-    <row r="50" spans="2:88" s="5" customFormat="1">
+    <row r="50" spans="2:90" s="5" customFormat="1">
       <c r="B50" s="5">
         <v>1961</v>
       </c>
@@ -7474,8 +7607,14 @@
       <c r="CJ50" s="5">
         <v>-9.9481713269569602E-3</v>
       </c>
+      <c r="CK50" s="5">
+        <v>-8.93333333333333</v>
+      </c>
+      <c r="CL50" s="5">
+        <v>91.6</v>
+      </c>
     </row>
-    <row r="51" spans="2:88" s="5" customFormat="1">
+    <row r="51" spans="2:90" s="5" customFormat="1">
       <c r="B51" s="5">
         <v>1961.25</v>
       </c>
@@ -7628,8 +7767,14 @@
       <c r="CJ51" s="5">
         <v>-5.98190082653066E-3</v>
       </c>
+      <c r="CK51" s="5">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="CL51" s="5">
+        <v>92.5</v>
+      </c>
     </row>
-    <row r="52" spans="2:88" s="5" customFormat="1">
+    <row r="52" spans="2:90" s="5" customFormat="1">
       <c r="B52" s="5">
         <v>1961.5</v>
       </c>
@@ -7782,8 +7927,14 @@
       <c r="CJ52" s="5">
         <v>3.3559755912520501E-3</v>
       </c>
+      <c r="CK52" s="5">
+        <v>21.266666666666701</v>
+      </c>
+      <c r="CL52" s="5">
+        <v>99.2</v>
+      </c>
     </row>
-    <row r="53" spans="2:88" s="5" customFormat="1">
+    <row r="53" spans="2:90" s="5" customFormat="1">
       <c r="B53" s="5">
         <v>1961.75</v>
       </c>
@@ -7936,8 +8087,14 @@
       <c r="CJ53" s="5">
         <v>-1.2412114789528601E-2</v>
       </c>
+      <c r="CK53" s="5">
+        <v>23.6</v>
+      </c>
+      <c r="CL53" s="5">
+        <v>93</v>
+      </c>
     </row>
-    <row r="54" spans="2:88" s="5" customFormat="1">
+    <row r="54" spans="2:90" s="5" customFormat="1">
       <c r="B54" s="5">
         <v>1962</v>
       </c>
@@ -8090,8 +8247,14 @@
       <c r="CJ54" s="5">
         <v>8.5387391027952203E-3</v>
       </c>
+      <c r="CK54" s="5">
+        <v>21.733333333333299</v>
+      </c>
+      <c r="CL54" s="5">
+        <v>99.9</v>
+      </c>
     </row>
-    <row r="55" spans="2:88" s="5" customFormat="1">
+    <row r="55" spans="2:90" s="5" customFormat="1">
       <c r="B55" s="5">
         <v>1962.25</v>
       </c>
@@ -8244,8 +8407,14 @@
       <c r="CJ55" s="5">
         <v>-1.3735966321321001E-3</v>
       </c>
+      <c r="CK55" s="5">
+        <v>5.4</v>
+      </c>
+      <c r="CL55" s="5">
+        <v>95.4</v>
+      </c>
     </row>
-    <row r="56" spans="2:88" s="5" customFormat="1">
+    <row r="56" spans="2:90" s="5" customFormat="1">
       <c r="B56" s="5">
         <v>1962.5</v>
       </c>
@@ -8398,8 +8567,14 @@
       <c r="CJ56" s="5">
         <v>-1.06963446697858E-2</v>
       </c>
+      <c r="CK56" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="CL56" s="5">
+        <v>91.6</v>
+      </c>
     </row>
-    <row r="57" spans="2:88" s="5" customFormat="1">
+    <row r="57" spans="2:90" s="5" customFormat="1">
       <c r="B57" s="5">
         <v>1962.75</v>
       </c>
@@ -8552,8 +8727,14 @@
       <c r="CJ57" s="5">
         <v>2.4205736713034899E-3</v>
       </c>
+      <c r="CK57" s="5">
+        <v>8.1333333333333293</v>
+      </c>
+      <c r="CL57" s="5">
+        <v>95</v>
+      </c>
     </row>
-    <row r="58" spans="2:88" s="5" customFormat="1">
+    <row r="58" spans="2:90" s="5" customFormat="1">
       <c r="B58" s="5">
         <v>1963</v>
       </c>
@@ -8706,8 +8887,14 @@
       <c r="CJ58" s="5">
         <v>-1.79358959855043E-2</v>
       </c>
+      <c r="CK58" s="5">
+        <v>10</v>
+      </c>
+      <c r="CL58" s="5">
+        <v>98.4</v>
+      </c>
     </row>
-    <row r="59" spans="2:88" s="5" customFormat="1">
+    <row r="59" spans="2:90" s="5" customFormat="1">
       <c r="B59" s="5">
         <v>1963.25</v>
       </c>
@@ -8860,8 +9047,14 @@
       <c r="CJ59" s="5">
         <v>-5.1817488316995997E-3</v>
       </c>
+      <c r="CK59" s="5">
+        <v>17.066666666666698</v>
+      </c>
+      <c r="CL59" s="5">
+        <v>91.7</v>
+      </c>
     </row>
-    <row r="60" spans="2:88" s="5" customFormat="1">
+    <row r="60" spans="2:90" s="5" customFormat="1">
       <c r="B60" s="5">
         <v>1963.5</v>
       </c>
@@ -9014,8 +9207,14 @@
       <c r="CJ60" s="5">
         <v>1.13912814349227E-2</v>
       </c>
+      <c r="CK60" s="5">
+        <v>11.6666666666667</v>
+      </c>
+      <c r="CL60" s="5">
+        <v>96.4</v>
+      </c>
     </row>
-    <row r="61" spans="2:88" s="5" customFormat="1">
+    <row r="61" spans="2:90" s="5" customFormat="1">
       <c r="B61" s="5">
         <v>1963.75</v>
       </c>
@@ -9168,8 +9367,14 @@
       <c r="CJ61" s="5">
         <v>2.9906963725886701E-3</v>
       </c>
+      <c r="CK61" s="5">
+        <v>12.8</v>
+      </c>
+      <c r="CL61" s="5">
+        <v>94.4</v>
+      </c>
     </row>
-    <row r="62" spans="2:88" s="5" customFormat="1">
+    <row r="62" spans="2:90" s="5" customFormat="1">
       <c r="B62" s="5">
         <v>1964</v>
       </c>
@@ -9322,8 +9527,14 @@
       <c r="CJ62" s="5">
         <v>7.8780881380367297E-3</v>
       </c>
+      <c r="CK62" s="5">
+        <v>16.8</v>
+      </c>
+      <c r="CL62" s="5">
+        <v>99.5</v>
+      </c>
     </row>
-    <row r="63" spans="2:88" s="5" customFormat="1">
+    <row r="63" spans="2:90" s="5" customFormat="1">
       <c r="B63" s="5">
         <v>1964.25</v>
       </c>
@@ -9476,8 +9687,14 @@
       <c r="CJ63" s="5">
         <v>-2.1175911641922E-3</v>
       </c>
+      <c r="CK63" s="5">
+        <v>18.6666666666667</v>
+      </c>
+      <c r="CL63" s="5">
+        <v>98.5</v>
+      </c>
     </row>
-    <row r="64" spans="2:88" s="5" customFormat="1">
+    <row r="64" spans="2:90" s="5" customFormat="1">
       <c r="B64" s="5">
         <v>1964.5</v>
       </c>
@@ -9630,8 +9847,14 @@
       <c r="CJ64" s="5">
         <v>5.2007396643525298E-3</v>
       </c>
+      <c r="CK64" s="5">
+        <v>26.3333333333333</v>
+      </c>
+      <c r="CL64" s="5">
+        <v>100.6</v>
+      </c>
     </row>
-    <row r="65" spans="2:88" s="5" customFormat="1">
+    <row r="65" spans="2:90" s="5" customFormat="1">
       <c r="B65" s="5">
         <v>1964.75</v>
       </c>
@@ -9784,8 +10007,14 @@
       <c r="CJ65" s="5">
         <v>-2.72822583929868E-2</v>
       </c>
+      <c r="CK65" s="5">
+        <v>23.266666666666701</v>
+      </c>
+      <c r="CL65" s="5">
+        <v>99.9</v>
+      </c>
     </row>
-    <row r="66" spans="2:88" s="5" customFormat="1">
+    <row r="66" spans="2:90" s="5" customFormat="1">
       <c r="B66" s="5">
         <v>1965</v>
       </c>
@@ -9938,8 +10167,14 @@
       <c r="CJ66" s="5">
         <v>6.43639232266917E-3</v>
       </c>
+      <c r="CK66" s="5">
+        <v>25.3333333333333</v>
+      </c>
+      <c r="CL66" s="5">
+        <v>102</v>
+      </c>
     </row>
-    <row r="67" spans="2:88" s="5" customFormat="1">
+    <row r="67" spans="2:90" s="5" customFormat="1">
       <c r="B67" s="5">
         <v>1965.25</v>
       </c>
@@ -10092,8 +10327,14 @@
       <c r="CJ67" s="14">
         <v>9.8121750592130894E-5</v>
       </c>
+      <c r="CK67" s="5">
+        <v>21.3333333333333</v>
+      </c>
+      <c r="CL67" s="5">
+        <v>105.4</v>
+      </c>
     </row>
-    <row r="68" spans="2:88" s="5" customFormat="1">
+    <row r="68" spans="2:90" s="5" customFormat="1">
       <c r="B68" s="5">
         <v>1965.5</v>
       </c>
@@ -10246,8 +10487,14 @@
       <c r="CJ68" s="5">
         <v>3.1387146898428801E-2</v>
       </c>
+      <c r="CK68" s="5">
+        <v>18.133333333333301</v>
+      </c>
+      <c r="CL68" s="5">
+        <v>103.4</v>
+      </c>
     </row>
-    <row r="69" spans="2:88" s="5" customFormat="1">
+    <row r="69" spans="2:90" s="5" customFormat="1">
       <c r="B69" s="5">
         <v>1965.75</v>
       </c>
@@ -10400,8 +10647,14 @@
       <c r="CJ69" s="5">
         <v>1.8626568343602198E-2</v>
       </c>
+      <c r="CK69" s="5">
+        <v>20.533333333333299</v>
+      </c>
+      <c r="CL69" s="5">
+        <v>102.9</v>
+      </c>
     </row>
-    <row r="70" spans="2:88" s="5" customFormat="1">
+    <row r="70" spans="2:90" s="5" customFormat="1">
       <c r="B70" s="5">
         <v>1966</v>
       </c>
@@ -10554,8 +10807,14 @@
       <c r="CJ70" s="5">
         <v>1.9711456206016598E-2</v>
       </c>
+      <c r="CK70" s="5">
+        <v>31.3333333333333</v>
+      </c>
+      <c r="CL70" s="5">
+        <v>100</v>
+      </c>
     </row>
-    <row r="71" spans="2:88" s="5" customFormat="1">
+    <row r="71" spans="2:90" s="5" customFormat="1">
       <c r="B71" s="5">
         <v>1966.25</v>
       </c>
@@ -10711,8 +10970,14 @@
       <c r="CJ71" s="5">
         <v>-6.2435263480286702E-3</v>
       </c>
+      <c r="CK71" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="CL71" s="5">
+        <v>95.7</v>
+      </c>
     </row>
-    <row r="72" spans="2:88" s="5" customFormat="1">
+    <row r="72" spans="2:90" s="5" customFormat="1">
       <c r="B72" s="5">
         <v>1966.5</v>
       </c>
@@ -10868,8 +11133,14 @@
       <c r="CJ72" s="5">
         <v>2.0016180917610798E-3</v>
       </c>
+      <c r="CK72" s="5">
+        <v>18.3333333333333</v>
+      </c>
+      <c r="CL72" s="5">
+        <v>91.2</v>
+      </c>
     </row>
-    <row r="73" spans="2:88" s="5" customFormat="1">
+    <row r="73" spans="2:90" s="5" customFormat="1">
       <c r="B73" s="5">
         <v>1966.75</v>
       </c>
@@ -11025,8 +11296,14 @@
       <c r="CJ73" s="5">
         <v>6.0446484271542804E-3</v>
       </c>
+      <c r="CK73" s="5">
+        <v>8.8666666666666707</v>
+      </c>
+      <c r="CL73" s="5">
+        <v>88.3</v>
+      </c>
     </row>
-    <row r="74" spans="2:88" s="5" customFormat="1">
+    <row r="74" spans="2:90" s="5" customFormat="1">
       <c r="B74" s="5">
         <v>1967</v>
       </c>
@@ -11186,8 +11463,14 @@
       <c r="CJ74" s="5">
         <v>2.8983439275141399E-2</v>
       </c>
+      <c r="CK74" s="5">
+        <v>-5.3333333333333304</v>
+      </c>
+      <c r="CL74" s="5">
+        <v>94.1</v>
+      </c>
     </row>
-    <row r="75" spans="2:88" s="5" customFormat="1">
+    <row r="75" spans="2:90" s="5" customFormat="1">
       <c r="B75" s="5">
         <v>1967.25</v>
       </c>
@@ -11347,8 +11630,14 @@
       <c r="CJ75" s="5">
         <v>-1.00378523797748E-2</v>
       </c>
+      <c r="CK75" s="5">
+        <v>-10.6</v>
+      </c>
+      <c r="CL75" s="5">
+        <v>95.9</v>
+      </c>
     </row>
-    <row r="76" spans="2:88" s="5" customFormat="1">
+    <row r="76" spans="2:90" s="5" customFormat="1">
       <c r="B76" s="5">
         <v>1967.5</v>
       </c>
@@ -11511,8 +11800,14 @@
       <c r="CJ76" s="5">
         <v>1.8683298396634501E-3</v>
       </c>
+      <c r="CK76" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="CL76" s="5">
+        <v>97</v>
+      </c>
     </row>
-    <row r="77" spans="2:88" s="5" customFormat="1">
+    <row r="77" spans="2:90" s="5" customFormat="1">
       <c r="B77" s="5">
         <v>1967.75</v>
       </c>
@@ -11675,8 +11970,14 @@
       <c r="CJ77" s="5">
         <v>-1.6396904118731501E-2</v>
       </c>
+      <c r="CK77" s="5">
+        <v>9.2666666666666693</v>
+      </c>
+      <c r="CL77" s="5">
+        <v>92.9</v>
+      </c>
     </row>
-    <row r="78" spans="2:88" s="5" customFormat="1">
+    <row r="78" spans="2:90" s="5" customFormat="1">
       <c r="B78" s="5">
         <v>1968</v>
       </c>
@@ -11839,8 +12140,14 @@
       <c r="CJ78" s="5">
         <v>3.1113101665193502E-2</v>
       </c>
+      <c r="CK78" s="5">
+        <v>10.266666666666699</v>
+      </c>
+      <c r="CL78" s="5">
+        <v>97.2</v>
+      </c>
     </row>
-    <row r="79" spans="2:88" s="5" customFormat="1">
+    <row r="79" spans="2:90" s="5" customFormat="1">
       <c r="B79" s="5">
         <v>1968.25</v>
       </c>
@@ -12003,8 +12310,14 @@
       <c r="CJ79" s="5">
         <v>1.57428156922799E-2</v>
       </c>
+      <c r="CK79" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="CL79" s="5">
+        <v>92.4</v>
+      </c>
     </row>
-    <row r="80" spans="2:88" s="5" customFormat="1">
+    <row r="80" spans="2:90" s="5" customFormat="1">
       <c r="B80" s="5">
         <v>1968.5</v>
       </c>
@@ -12167,8 +12480,14 @@
       <c r="CJ80" s="5">
         <v>-3.6361841455941702E-3</v>
       </c>
+      <c r="CK80" s="5">
+        <v>5.7333333333333298</v>
+      </c>
+      <c r="CL80" s="5">
+        <v>92.4</v>
+      </c>
     </row>
-    <row r="81" spans="2:88" s="5" customFormat="1">
+    <row r="81" spans="2:90" s="5" customFormat="1">
       <c r="B81" s="5">
         <v>1968.75</v>
       </c>
@@ -12387,8 +12706,14 @@
       <c r="CJ81" s="5">
         <v>2.5938710953296198E-3</v>
       </c>
+      <c r="CK81" s="5">
+        <v>13.3333333333333</v>
+      </c>
+      <c r="CL81" s="5">
+        <v>91.7</v>
+      </c>
     </row>
-    <row r="82" spans="2:88" s="5" customFormat="1">
+    <row r="82" spans="2:90" s="5" customFormat="1">
       <c r="B82" s="5">
         <v>1969</v>
       </c>
@@ -12611,8 +12936,14 @@
       <c r="CJ82" s="5">
         <v>-1.29453921026654E-2</v>
       </c>
+      <c r="CK82" s="5">
+        <v>12.6666666666667</v>
+      </c>
+      <c r="CL82" s="5">
+        <v>98.2</v>
+      </c>
     </row>
-    <row r="83" spans="2:88" s="5" customFormat="1">
+    <row r="83" spans="2:90" s="5" customFormat="1">
       <c r="B83" s="5">
         <v>1969.25</v>
       </c>
@@ -12835,8 +13166,14 @@
       <c r="CJ83" s="5">
         <v>-3.5813990293846899E-3</v>
       </c>
+      <c r="CK83" s="5">
+        <v>11.6</v>
+      </c>
+      <c r="CL83" s="5">
+        <v>91.5</v>
+      </c>
     </row>
-    <row r="84" spans="2:88" s="5" customFormat="1">
+    <row r="84" spans="2:90" s="5" customFormat="1">
       <c r="B84" s="5">
         <v>1969.5</v>
       </c>
@@ -13059,8 +13396,14 @@
       <c r="CJ84" s="5">
         <v>1.3459612687061499E-3</v>
       </c>
+      <c r="CK84" s="5">
+        <v>8</v>
+      </c>
+      <c r="CL84" s="5">
+        <v>86.4</v>
+      </c>
     </row>
-    <row r="85" spans="2:88" s="5" customFormat="1">
+    <row r="85" spans="2:90" s="5" customFormat="1">
       <c r="B85" s="5">
         <v>1969.75</v>
       </c>
@@ -13282,8 +13625,14 @@
       <c r="CJ85" s="5">
         <v>-9.7952743462173496E-3</v>
       </c>
+      <c r="CK85" s="5">
+        <v>6.5333333333333297</v>
+      </c>
+      <c r="CL85" s="5">
+        <v>79.7</v>
+      </c>
     </row>
-    <row r="86" spans="2:88" s="5" customFormat="1">
+    <row r="86" spans="2:90" s="5" customFormat="1">
       <c r="B86" s="5">
         <v>1970</v>
       </c>
@@ -13507,8 +13856,14 @@
       <c r="CJ86" s="5">
         <v>-7.9234874482972794E-3</v>
       </c>
+      <c r="CK86" s="5">
+        <v>-4.6666666666666696</v>
+      </c>
+      <c r="CL86" s="5">
+        <v>78.099999999999994</v>
+      </c>
     </row>
-    <row r="87" spans="2:88" s="5" customFormat="1">
+    <row r="87" spans="2:90" s="5" customFormat="1">
       <c r="B87" s="5">
         <v>1970.25</v>
       </c>
@@ -13730,8 +14085,14 @@
       <c r="CJ87" s="5">
         <v>6.7811858923314903E-3</v>
       </c>
+      <c r="CK87" s="5">
+        <v>-4.4666666666666703</v>
+      </c>
+      <c r="CL87" s="5">
+        <v>75.400000000000006</v>
+      </c>
     </row>
-    <row r="88" spans="2:88" s="5" customFormat="1">
+    <row r="88" spans="2:90" s="5" customFormat="1">
       <c r="B88" s="5">
         <v>1970.5</v>
       </c>
@@ -13953,8 +14314,14 @@
       <c r="CJ88" s="5">
         <v>2.4595647576654101E-2</v>
       </c>
+      <c r="CK88" s="5">
+        <v>-6.06666666666667</v>
+      </c>
+      <c r="CL88" s="5">
+        <v>77.599999999999994</v>
+      </c>
     </row>
-    <row r="89" spans="2:88" s="5" customFormat="1">
+    <row r="89" spans="2:90" s="5" customFormat="1">
       <c r="B89" s="5">
         <v>1970.75</v>
       </c>
@@ -14176,8 +14543,14 @@
       <c r="CJ89" s="5">
         <v>-2.8253454283296599E-2</v>
       </c>
+      <c r="CK89" s="5">
+        <v>-15</v>
+      </c>
+      <c r="CL89" s="5">
+        <v>72.400000000000006</v>
+      </c>
     </row>
-    <row r="90" spans="2:88" s="5" customFormat="1">
+    <row r="90" spans="2:90" s="5" customFormat="1">
       <c r="B90" s="5">
         <v>1971</v>
       </c>
@@ -14399,8 +14772,14 @@
       <c r="CJ90" s="5">
         <v>4.37380951812332E-2</v>
       </c>
+      <c r="CK90" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="CL90" s="5">
+        <v>78.099999999999994</v>
+      </c>
     </row>
-    <row r="91" spans="2:88" s="5" customFormat="1">
+    <row r="91" spans="2:90" s="5" customFormat="1">
       <c r="B91" s="5">
         <v>1971.25</v>
       </c>
@@ -14622,8 +15001,14 @@
       <c r="CJ91" s="5">
         <v>1.0777853295959801E-2</v>
       </c>
+      <c r="CK91" s="5">
+        <v>8.3333333333333393</v>
+      </c>
+      <c r="CL91" s="5">
+        <v>80.2</v>
+      </c>
     </row>
-    <row r="92" spans="2:88" s="5" customFormat="1">
+    <row r="92" spans="2:90" s="5" customFormat="1">
       <c r="B92" s="5">
         <v>1971.5</v>
       </c>
@@ -14845,8 +15230,14 @@
       <c r="CJ92" s="5">
         <v>-8.1895526156409593E-3</v>
       </c>
+      <c r="CK92" s="5">
+        <v>8.7333333333333307</v>
+      </c>
+      <c r="CL92" s="5">
+        <v>82.1</v>
+      </c>
     </row>
-    <row r="93" spans="2:88" s="5" customFormat="1">
+    <row r="93" spans="2:90" s="5" customFormat="1">
       <c r="B93" s="5">
         <v>1971.75</v>
       </c>
@@ -15068,8 +15459,14 @@
       <c r="CJ93" s="5">
         <v>-2.1672918217825798E-2</v>
       </c>
+      <c r="CK93" s="5">
+        <v>9.93333333333333</v>
+      </c>
+      <c r="CL93" s="5">
+        <v>82</v>
+      </c>
     </row>
-    <row r="94" spans="2:88" s="5" customFormat="1">
+    <row r="94" spans="2:90" s="5" customFormat="1">
       <c r="B94" s="5">
         <v>1972</v>
       </c>
@@ -15291,8 +15688,14 @@
       <c r="CJ94" s="5">
         <v>1.15188195651216E-2</v>
       </c>
+      <c r="CK94" s="5">
+        <v>20</v>
+      </c>
+      <c r="CL94" s="5">
+        <v>92.8</v>
+      </c>
     </row>
-    <row r="95" spans="2:88" s="5" customFormat="1">
+    <row r="95" spans="2:90" s="5" customFormat="1">
       <c r="B95" s="5">
         <v>1972.25</v>
       </c>
@@ -15514,8 +15917,14 @@
       <c r="CJ95" s="5">
         <v>1.9823175681064401E-2</v>
       </c>
+      <c r="CK95" s="5">
+        <v>19.533333333333299</v>
+      </c>
+      <c r="CL95" s="5">
+        <v>88.6</v>
+      </c>
     </row>
-    <row r="96" spans="2:88" s="5" customFormat="1">
+    <row r="96" spans="2:90" s="5" customFormat="1">
       <c r="B96" s="5">
         <v>1972.5</v>
       </c>
@@ -15737,8 +16146,14 @@
       <c r="CJ96" s="5">
         <v>-8.1720271197613099E-4</v>
       </c>
+      <c r="CK96" s="5">
+        <v>24.6</v>
+      </c>
+      <c r="CL96" s="5">
+        <v>95.2</v>
+      </c>
     </row>
-    <row r="97" spans="2:88" s="5" customFormat="1">
+    <row r="97" spans="2:90" s="5" customFormat="1">
       <c r="B97" s="5">
         <v>1972.75</v>
       </c>
@@ -15960,8 +16375,14 @@
       <c r="CJ97" s="5">
         <v>3.2907362123183098E-2</v>
       </c>
+      <c r="CK97" s="5">
+        <v>38.266666666666701</v>
+      </c>
+      <c r="CL97" s="5">
+        <v>90.7</v>
+      </c>
     </row>
-    <row r="98" spans="2:88" s="5" customFormat="1">
+    <row r="98" spans="2:90" s="5" customFormat="1">
       <c r="B98" s="5">
         <v>1973</v>
       </c>
@@ -16186,8 +16607,14 @@
       <c r="CJ98" s="5">
         <v>2.4625794911433099E-2</v>
       </c>
+      <c r="CK98" s="5">
+        <v>40.866666666666703</v>
+      </c>
+      <c r="CL98" s="5">
+        <v>81.900000000000006</v>
+      </c>
     </row>
-    <row r="99" spans="2:88" s="5" customFormat="1">
+    <row r="99" spans="2:90" s="5" customFormat="1">
       <c r="B99" s="5">
         <v>1973.25</v>
       </c>
@@ -16412,8 +16839,14 @@
       <c r="CJ99" s="5">
         <v>1.8131958757523398E-2</v>
       </c>
+      <c r="CK99" s="5">
+        <v>31.6666666666667</v>
+      </c>
+      <c r="CL99" s="5">
+        <v>77</v>
+      </c>
     </row>
-    <row r="100" spans="2:88" s="5" customFormat="1">
+    <row r="100" spans="2:90" s="5" customFormat="1">
       <c r="B100" s="5">
         <v>1973.5</v>
       </c>
@@ -16638,8 +17071,14 @@
       <c r="CJ100" s="5">
         <v>-1.4233891781791999E-2</v>
       </c>
+      <c r="CK100" s="5">
+        <v>22.6666666666667</v>
+      </c>
+      <c r="CL100" s="5">
+        <v>72</v>
+      </c>
     </row>
-    <row r="101" spans="2:88" s="5" customFormat="1">
+    <row r="101" spans="2:90" s="5" customFormat="1">
       <c r="B101" s="5">
         <v>1973.75</v>
       </c>
@@ -16864,8 +17303,14 @@
       <c r="CJ101" s="5">
         <v>9.5798763049893005E-3</v>
       </c>
+      <c r="CK101" s="5">
+        <v>31.933333333333302</v>
+      </c>
+      <c r="CL101" s="5">
+        <v>76.5</v>
+      </c>
     </row>
-    <row r="102" spans="2:88" s="5" customFormat="1">
+    <row r="102" spans="2:90" s="5" customFormat="1">
       <c r="B102" s="5">
         <v>1974</v>
       </c>
@@ -17090,8 +17535,14 @@
       <c r="CJ102" s="5">
         <v>-6.0257762836848905E-4</v>
       </c>
+      <c r="CK102" s="5">
+        <v>21.6666666666667</v>
+      </c>
+      <c r="CL102" s="5">
+        <v>61.8</v>
+      </c>
     </row>
-    <row r="103" spans="2:88" s="5" customFormat="1">
+    <row r="103" spans="2:90" s="5" customFormat="1">
       <c r="B103" s="5">
         <v>1974.25</v>
       </c>
@@ -17316,8 +17767,14 @@
       <c r="CJ103" s="5">
         <v>-5.7993778054585905E-4</v>
       </c>
+      <c r="CK103" s="5">
+        <v>13.533333333333299</v>
+      </c>
+      <c r="CL103" s="5">
+        <v>72.099999999999994</v>
+      </c>
     </row>
-    <row r="104" spans="2:88" s="5" customFormat="1">
+    <row r="104" spans="2:90" s="5" customFormat="1">
       <c r="B104" s="5">
         <v>1974.5</v>
       </c>
@@ -17544,8 +18001,14 @@
       <c r="CJ104" s="5">
         <v>-3.6289752336907898E-3</v>
       </c>
+      <c r="CK104" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="CL104" s="5">
+        <v>64.400000000000006</v>
+      </c>
     </row>
-    <row r="105" spans="2:88" s="5" customFormat="1">
+    <row r="105" spans="2:90" s="5" customFormat="1">
       <c r="B105" s="5">
         <v>1974.75</v>
       </c>
@@ -17770,8 +18233,14 @@
       <c r="CJ105" s="5">
         <v>4.7282335271450503E-2</v>
       </c>
+      <c r="CK105" s="5">
+        <v>-25.6666666666667</v>
+      </c>
+      <c r="CL105" s="5">
+        <v>59.5</v>
+      </c>
     </row>
-    <row r="106" spans="2:88" s="5" customFormat="1">
+    <row r="106" spans="2:90" s="5" customFormat="1">
       <c r="B106" s="5">
         <v>1975</v>
       </c>
@@ -17996,8 +18465,14 @@
       <c r="CJ106" s="5">
         <v>2.2531887259838498E-2</v>
       </c>
+      <c r="CK106" s="5">
+        <v>-35.533333333333303</v>
+      </c>
+      <c r="CL106" s="5">
+        <v>57.6</v>
+      </c>
     </row>
-    <row r="107" spans="2:88" s="5" customFormat="1">
+    <row r="107" spans="2:90" s="5" customFormat="1">
       <c r="B107" s="5">
         <v>1975.25</v>
       </c>
@@ -18222,8 +18697,14 @@
       <c r="CJ107" s="5">
         <v>2.9909429797396501E-2</v>
       </c>
+      <c r="CK107" s="5">
+        <v>-17.466666666666701</v>
+      </c>
+      <c r="CL107" s="5">
+        <v>72.8</v>
+      </c>
     </row>
-    <row r="108" spans="2:88" s="5" customFormat="1">
+    <row r="108" spans="2:90" s="5" customFormat="1">
       <c r="B108" s="5">
         <v>1975.5</v>
       </c>
@@ -18448,8 +18929,14 @@
       <c r="CJ108" s="5">
         <v>-3.6090548093797199E-2</v>
       </c>
+      <c r="CK108" s="5">
+        <v>2</v>
+      </c>
+      <c r="CL108" s="5">
+        <v>75.7</v>
+      </c>
     </row>
-    <row r="109" spans="2:88" s="5" customFormat="1">
+    <row r="109" spans="2:90" s="5" customFormat="1">
       <c r="B109" s="5">
         <v>1975.75</v>
       </c>
@@ -18674,8 +19161,14 @@
       <c r="CJ109" s="5">
         <v>-1.9788649487133898E-3</v>
       </c>
+      <c r="CK109" s="5">
+        <v>9.93333333333333</v>
+      </c>
+      <c r="CL109" s="5">
+        <v>75.599999999999994</v>
+      </c>
     </row>
-    <row r="110" spans="2:88" s="5" customFormat="1">
+    <row r="110" spans="2:90" s="5" customFormat="1">
       <c r="B110" s="5">
         <v>1976</v>
       </c>
@@ -18900,8 +19393,14 @@
       <c r="CJ110" s="5">
         <v>1.9518752694796899E-3</v>
       </c>
+      <c r="CK110" s="5">
+        <v>19.133333333333301</v>
+      </c>
+      <c r="CL110" s="5">
+        <v>84.6</v>
+      </c>
     </row>
-    <row r="111" spans="2:88" s="5" customFormat="1">
+    <row r="111" spans="2:90" s="5" customFormat="1">
       <c r="B111" s="5">
         <v>1976.25</v>
       </c>
@@ -19126,8 +19625,14 @@
       <c r="CJ111" s="5">
         <v>-6.3756800711962198E-3</v>
       </c>
+      <c r="CK111" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="CL111" s="5">
+        <v>83.3</v>
+      </c>
     </row>
-    <row r="112" spans="2:88" s="5" customFormat="1">
+    <row r="112" spans="2:90" s="5" customFormat="1">
       <c r="B112" s="5">
         <v>1976.5</v>
       </c>
@@ -19352,8 +19857,14 @@
       <c r="CJ112" s="5">
         <v>-1.81158524796558E-3</v>
       </c>
+      <c r="CK112" s="5">
+        <v>9.3333333333333393</v>
+      </c>
+      <c r="CL112" s="5">
+        <v>89.7</v>
+      </c>
     </row>
-    <row r="113" spans="2:88" s="5" customFormat="1">
+    <row r="113" spans="2:90" s="5" customFormat="1">
       <c r="B113" s="5">
         <v>1976.75</v>
       </c>
@@ -19578,8 +20089,14 @@
       <c r="CJ113" s="5">
         <v>-4.5985727080735802E-3</v>
       </c>
+      <c r="CK113" s="5">
+        <v>7.8666666666666698</v>
+      </c>
+      <c r="CL113" s="5">
+        <v>87</v>
+      </c>
     </row>
-    <row r="114" spans="2:88" s="5" customFormat="1">
+    <row r="114" spans="2:90" s="5" customFormat="1">
       <c r="B114" s="5">
         <v>1977</v>
       </c>
@@ -19804,8 +20321,14 @@
       <c r="CJ114" s="5">
         <v>8.2945134922311899E-4</v>
       </c>
+      <c r="CK114" s="5">
+        <v>12.133333333333301</v>
+      </c>
+      <c r="CL114" s="5">
+        <v>87.1</v>
+      </c>
     </row>
-    <row r="115" spans="2:88" s="5" customFormat="1">
+    <row r="115" spans="2:90" s="5" customFormat="1">
       <c r="B115" s="5">
         <v>1977.25</v>
       </c>
@@ -20030,8 +20553,14 @@
       <c r="CJ115" s="5">
         <v>1.6821080539751902E-2</v>
       </c>
+      <c r="CK115" s="5">
+        <v>15.6</v>
+      </c>
+      <c r="CL115" s="5">
+        <v>90.2</v>
+      </c>
     </row>
-    <row r="116" spans="2:88" s="5" customFormat="1">
+    <row r="116" spans="2:90" s="5" customFormat="1">
       <c r="B116" s="5">
         <v>1977.5</v>
       </c>
@@ -20256,8 +20785,14 @@
       <c r="CJ116" s="5">
         <v>2.7201678158590498E-2</v>
       </c>
+      <c r="CK116" s="5">
+        <v>11</v>
+      </c>
+      <c r="CL116" s="5">
+        <v>89</v>
+      </c>
     </row>
-    <row r="117" spans="2:88" s="5" customFormat="1">
+    <row r="117" spans="2:90" s="5" customFormat="1">
       <c r="B117" s="5">
         <v>1977.75</v>
       </c>
@@ -20482,8 +21017,14 @@
       <c r="CJ117" s="5">
         <v>-7.52802378952761E-3</v>
       </c>
+      <c r="CK117" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="CL117" s="5">
+        <v>84.4</v>
+      </c>
     </row>
-    <row r="118" spans="2:88" s="5" customFormat="1">
+    <row r="118" spans="2:90" s="5" customFormat="1">
       <c r="B118" s="5">
         <v>1978</v>
       </c>
@@ -20708,8 +21249,14 @@
       <c r="CJ118" s="5">
         <v>8.5885759992089597E-3</v>
       </c>
+      <c r="CK118" s="5">
+        <v>12.2</v>
+      </c>
+      <c r="CL118" s="5">
+        <v>82.6</v>
+      </c>
     </row>
-    <row r="119" spans="2:88" s="5" customFormat="1">
+    <row r="119" spans="2:90" s="5" customFormat="1">
       <c r="B119" s="5">
         <v>1978.25</v>
       </c>
@@ -20937,8 +21484,14 @@
       <c r="CJ119" s="5">
         <v>3.5340999926325299E-2</v>
       </c>
+      <c r="CK119" s="5">
+        <v>18.933333333333302</v>
+      </c>
+      <c r="CL119" s="5">
+        <v>81.8</v>
+      </c>
     </row>
-    <row r="120" spans="2:88" s="5" customFormat="1">
+    <row r="120" spans="2:90" s="5" customFormat="1">
       <c r="B120" s="5">
         <v>1978.5</v>
       </c>
@@ -21166,8 +21719,14 @@
       <c r="CJ120" s="5">
         <v>1.50415230455264E-2</v>
       </c>
+      <c r="CK120" s="5">
+        <v>22</v>
+      </c>
+      <c r="CL120" s="5">
+        <v>80</v>
+      </c>
     </row>
-    <row r="121" spans="2:88" s="5" customFormat="1">
+    <row r="121" spans="2:90" s="5" customFormat="1">
       <c r="B121" s="5">
         <v>1978.75</v>
       </c>
@@ -21395,8 +21954,14 @@
       <c r="CJ121" s="5">
         <v>1.2238576233187101E-2</v>
       </c>
+      <c r="CK121" s="5">
+        <v>20.533333333333299</v>
+      </c>
+      <c r="CL121" s="5">
+        <v>73.8</v>
+      </c>
     </row>
-    <row r="122" spans="2:88" s="5" customFormat="1">
+    <row r="122" spans="2:90" s="5" customFormat="1">
       <c r="B122" s="5">
         <v>1979</v>
       </c>
@@ -21624,8 +22189,14 @@
       <c r="CJ122" s="5">
         <v>2.49356852063406E-3</v>
       </c>
+      <c r="CK122" s="5">
+        <v>16.266666666666701</v>
+      </c>
+      <c r="CL122" s="5">
+        <v>71.900000000000006</v>
+      </c>
     </row>
-    <row r="123" spans="2:88" s="5" customFormat="1">
+    <row r="123" spans="2:90" s="5" customFormat="1">
       <c r="B123" s="5">
         <v>1979.25</v>
       </c>
@@ -21853,8 +22424,14 @@
       <c r="CJ123" s="5">
         <v>1.6408142304312302E-2</v>
       </c>
+      <c r="CK123" s="5">
+        <v>8.8666666666666707</v>
+      </c>
+      <c r="CL123" s="5">
+        <v>66.7</v>
+      </c>
     </row>
-    <row r="124" spans="2:88" s="5" customFormat="1">
+    <row r="124" spans="2:90" s="5" customFormat="1">
       <c r="B124" s="5">
         <v>1979.5</v>
       </c>
@@ -22082,8 +22659,14 @@
       <c r="CJ124" s="5">
         <v>1.5135395401414601E-2</v>
       </c>
+      <c r="CK124" s="5">
+        <v>0.266666666666667</v>
+      </c>
+      <c r="CL124" s="5">
+        <v>63.7</v>
+      </c>
     </row>
-    <row r="125" spans="2:88" s="5" customFormat="1">
+    <row r="125" spans="2:90" s="5" customFormat="1">
       <c r="B125" s="5">
         <v>1979.75</v>
       </c>
@@ -22311,8 +22894,14 @@
       <c r="CJ125" s="5">
         <v>-1.77335731795797E-3</v>
       </c>
+      <c r="CK125" s="5">
+        <v>-5.4666666666666703</v>
+      </c>
+      <c r="CL125" s="5">
+        <v>62.3</v>
+      </c>
     </row>
-    <row r="126" spans="2:88" s="5" customFormat="1">
+    <row r="126" spans="2:90" s="5" customFormat="1">
       <c r="B126" s="5">
         <v>1980</v>
       </c>
@@ -22540,8 +23129,14 @@
       <c r="CJ126" s="5">
         <v>7.5180462808402604E-3</v>
       </c>
+      <c r="CK126" s="5">
+        <v>-6.6666666666666696</v>
+      </c>
+      <c r="CL126" s="5">
+        <v>63.9</v>
+      </c>
     </row>
-    <row r="127" spans="2:88" s="5" customFormat="1">
+    <row r="127" spans="2:90" s="5" customFormat="1">
       <c r="B127" s="5">
         <v>1980.25</v>
       </c>
@@ -22769,8 +23364,14 @@
       <c r="CJ127" s="5">
         <v>-5.9538889677259498E-3</v>
       </c>
+      <c r="CK127" s="5">
+        <v>-35.266666666666701</v>
+      </c>
+      <c r="CL127" s="5">
+        <v>54.4</v>
+      </c>
     </row>
-    <row r="128" spans="2:88" s="5" customFormat="1">
+    <row r="128" spans="2:90" s="5" customFormat="1">
       <c r="B128" s="5">
         <v>1980.5</v>
       </c>
@@ -22998,8 +23599,14 @@
       <c r="CJ128" s="5">
         <v>2.30220674676514E-3</v>
       </c>
+      <c r="CK128" s="5">
+        <v>-12.9333333333333</v>
+      </c>
+      <c r="CL128" s="5">
+        <v>67.8</v>
+      </c>
     </row>
-    <row r="129" spans="2:88" s="5" customFormat="1">
+    <row r="129" spans="2:90" s="5" customFormat="1">
       <c r="B129" s="5">
         <v>1980.75</v>
       </c>
@@ -23227,8 +23834,14 @@
       <c r="CJ129" s="5">
         <v>1.2135402400851199E-2</v>
       </c>
+      <c r="CK129" s="5">
+        <v>11.133333333333301</v>
+      </c>
+      <c r="CL129" s="5">
+        <v>72</v>
+      </c>
     </row>
-    <row r="130" spans="2:88" s="5" customFormat="1">
+    <row r="130" spans="2:90" s="5" customFormat="1">
       <c r="B130" s="5">
         <v>1981</v>
       </c>
@@ -23456,8 +24069,14 @@
       <c r="CJ130" s="5">
         <v>7.81521448152123E-3</v>
       </c>
+      <c r="CK130" s="5">
+        <v>-1.6</v>
+      </c>
+      <c r="CL130" s="5">
+        <v>68.3</v>
+      </c>
     </row>
-    <row r="131" spans="2:88" s="5" customFormat="1">
+    <row r="131" spans="2:90" s="5" customFormat="1">
       <c r="B131" s="5">
         <v>1981.25</v>
       </c>
@@ -23685,8 +24304,14 @@
       <c r="CJ131" s="5">
         <v>-2.6719124530656099E-2</v>
       </c>
+      <c r="CK131" s="5">
+        <v>3.8666666666666698</v>
+      </c>
+      <c r="CL131" s="5">
+        <v>73.900000000000006</v>
+      </c>
     </row>
-    <row r="132" spans="2:88" s="5" customFormat="1">
+    <row r="132" spans="2:90" s="5" customFormat="1">
       <c r="B132" s="5">
         <v>1981.5</v>
       </c>
@@ -23942,8 +24567,14 @@
       <c r="CJ132" s="5">
         <v>1.4149532435050001E-2</v>
       </c>
+      <c r="CK132" s="5">
+        <v>-8.3333333333333393</v>
+      </c>
+      <c r="CL132" s="5">
+        <v>74.8</v>
+      </c>
     </row>
-    <row r="133" spans="2:88" s="5" customFormat="1">
+    <row r="133" spans="2:90" s="5" customFormat="1">
       <c r="B133" s="5">
         <v>1981.75</v>
       </c>
@@ -24199,8 +24830,14 @@
       <c r="CJ133" s="5">
         <v>-1.05526819598614E-2</v>
       </c>
+      <c r="CK133" s="5">
+        <v>-24.066666666666698</v>
+      </c>
+      <c r="CL133" s="5">
+        <v>65.7</v>
+      </c>
     </row>
-    <row r="134" spans="2:88" s="5" customFormat="1">
+    <row r="134" spans="2:90" s="5" customFormat="1">
       <c r="B134" s="5">
         <v>1982</v>
       </c>
@@ -24456,8 +25093,14 @@
       <c r="CJ134" s="5">
         <v>-2.9584826689864702E-2</v>
       </c>
+      <c r="CK134" s="5">
+        <v>-24.466666666666701</v>
+      </c>
+      <c r="CL134" s="5">
+        <v>66.599999999999994</v>
+      </c>
     </row>
-    <row r="135" spans="2:88" s="5" customFormat="1">
+    <row r="135" spans="2:90" s="5" customFormat="1">
       <c r="B135" s="5">
         <v>1982.25</v>
       </c>
@@ -24713,8 +25356,14 @@
       <c r="CJ135" s="5">
         <v>-8.9879104661265193E-3</v>
       </c>
+      <c r="CK135" s="5">
+        <v>-25.6</v>
+      </c>
+      <c r="CL135" s="5">
+        <v>66.2</v>
+      </c>
     </row>
-    <row r="136" spans="2:88" s="5" customFormat="1">
+    <row r="136" spans="2:90" s="5" customFormat="1">
       <c r="B136" s="5">
         <v>1982.5</v>
       </c>
@@ -24970,8 +25619,14 @@
       <c r="CJ136" s="5">
         <v>-1.4677434409829699E-2</v>
       </c>
+      <c r="CK136" s="5">
+        <v>-23</v>
+      </c>
+      <c r="CL136" s="5">
+        <v>66.7</v>
+      </c>
     </row>
-    <row r="137" spans="2:88" s="5" customFormat="1">
+    <row r="137" spans="2:90" s="5" customFormat="1">
       <c r="B137" s="5">
         <v>1982.75</v>
       </c>
@@ -25227,8 +25882,14 @@
       <c r="CJ137" s="5">
         <v>3.5736775186874402E-3</v>
       </c>
+      <c r="CK137" s="5">
+        <v>-19.066666666666698</v>
+      </c>
+      <c r="CL137" s="5">
+        <v>72.5</v>
+      </c>
     </row>
-    <row r="138" spans="2:88" s="5" customFormat="1">
+    <row r="138" spans="2:90" s="5" customFormat="1">
       <c r="B138" s="5">
         <v>1983</v>
       </c>
@@ -25484,8 +26145,14 @@
       <c r="CJ138" s="5">
         <v>9.6087197400545592E-3</v>
       </c>
+      <c r="CK138" s="5">
+        <v>2.8666666666666698</v>
+      </c>
+      <c r="CL138" s="5">
+        <v>75</v>
+      </c>
     </row>
-    <row r="139" spans="2:88" s="5" customFormat="1">
+    <row r="139" spans="2:90" s="5" customFormat="1">
       <c r="B139" s="5">
         <v>1983.25</v>
       </c>
@@ -25741,8 +26408,14 @@
       <c r="CJ139" s="5">
         <v>-1.45846345968117E-2</v>
       </c>
+      <c r="CK139" s="5">
+        <v>11.866666666666699</v>
+      </c>
+      <c r="CL139" s="5">
+        <v>91.5</v>
+      </c>
     </row>
-    <row r="140" spans="2:88" s="5" customFormat="1">
+    <row r="140" spans="2:90" s="5" customFormat="1">
       <c r="B140" s="5">
         <v>1983.5</v>
       </c>
@@ -25998,8 +26671,14 @@
       <c r="CJ140" s="5">
         <v>-2.2666119795900198E-2</v>
       </c>
+      <c r="CK140" s="5">
+        <v>26.133333333333301</v>
+      </c>
+      <c r="CL140" s="5">
+        <v>91.2</v>
+      </c>
     </row>
-    <row r="141" spans="2:88" s="5" customFormat="1">
+    <row r="141" spans="2:90" s="5" customFormat="1">
       <c r="B141" s="5">
         <v>1983.75</v>
       </c>
@@ -26255,8 +26934,14 @@
       <c r="CJ141" s="5">
         <v>2.3585127497542401E-3</v>
       </c>
+      <c r="CK141" s="5">
+        <v>33.533333333333303</v>
+      </c>
+      <c r="CL141" s="5">
+        <v>91.6</v>
+      </c>
     </row>
-    <row r="142" spans="2:88" s="5" customFormat="1">
+    <row r="142" spans="2:90" s="5" customFormat="1">
       <c r="B142" s="5">
         <v>1984</v>
       </c>
@@ -26512,8 +27197,14 @@
       <c r="CJ142" s="5">
         <v>-8.4012163750365196E-4</v>
       </c>
+      <c r="CK142" s="5">
+        <v>20.466666666666701</v>
+      </c>
+      <c r="CL142" s="5">
+        <v>99.5</v>
+      </c>
     </row>
-    <row r="143" spans="2:88" s="5" customFormat="1">
+    <row r="143" spans="2:90" s="5" customFormat="1">
       <c r="B143" s="5">
         <v>1984.25</v>
       </c>
@@ -26769,8 +27460,14 @@
       <c r="CJ143" s="5">
         <v>5.07562691168458E-3</v>
       </c>
+      <c r="CK143" s="5">
+        <v>18.466666666666701</v>
+      </c>
+      <c r="CL143" s="5">
+        <v>96.6</v>
+      </c>
     </row>
-    <row r="144" spans="2:88" s="5" customFormat="1">
+    <row r="144" spans="2:90" s="5" customFormat="1">
       <c r="B144" s="5">
         <v>1984.5</v>
       </c>
@@ -27026,8 +27723,14 @@
       <c r="CJ144" s="5">
         <v>4.8297766572274496E-3</v>
       </c>
+      <c r="CK144" s="5">
+        <v>6.06666666666667</v>
+      </c>
+      <c r="CL144" s="5">
+        <v>98.9</v>
+      </c>
     </row>
-    <row r="145" spans="2:88" s="5" customFormat="1">
+    <row r="145" spans="2:90" s="5" customFormat="1">
       <c r="B145" s="5">
         <v>1984.75</v>
       </c>
@@ -27283,8 +27986,14 @@
       <c r="CJ145" s="5">
         <v>-8.2257885185561593E-3</v>
       </c>
+      <c r="CK145" s="5">
+        <v>1.13333333333333</v>
+      </c>
+      <c r="CL145" s="5">
+        <v>95</v>
+      </c>
     </row>
-    <row r="146" spans="2:88" s="5" customFormat="1">
+    <row r="146" spans="2:90" s="5" customFormat="1">
       <c r="B146" s="5">
         <v>1985</v>
       </c>
@@ -27540,8 +28249,14 @@
       <c r="CJ146" s="5">
         <v>-6.8648617411885904E-3</v>
       </c>
+      <c r="CK146" s="5">
+        <v>-1.3333333333333299</v>
+      </c>
+      <c r="CL146" s="5">
+        <v>94.5</v>
+      </c>
     </row>
-    <row r="147" spans="2:88" s="5" customFormat="1">
+    <row r="147" spans="2:90" s="5" customFormat="1">
       <c r="B147" s="5">
         <v>1985.25</v>
       </c>
@@ -27797,8 +28512,14 @@
       <c r="CJ147" s="5">
         <v>1.31735103044334E-2</v>
       </c>
+      <c r="CK147" s="5">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="CL147" s="5">
+        <v>94.3</v>
+      </c>
     </row>
-    <row r="148" spans="2:88" s="5" customFormat="1">
+    <row r="148" spans="2:90" s="5" customFormat="1">
       <c r="B148" s="5">
         <v>1985.5</v>
       </c>
@@ -28054,8 +28775,14 @@
       <c r="CJ148" s="5">
         <v>-2.6564199442022699E-3</v>
       </c>
+      <c r="CK148" s="5">
+        <v>-3</v>
+      </c>
+      <c r="CL148" s="5">
+        <v>92.8</v>
+      </c>
     </row>
-    <row r="149" spans="2:88" s="5" customFormat="1">
+    <row r="149" spans="2:90" s="5" customFormat="1">
       <c r="B149" s="5">
         <v>1985.75</v>
       </c>
@@ -28311,8 +29038,14 @@
       <c r="CJ149" s="5">
         <v>-5.7451357677765899E-3</v>
       </c>
+      <c r="CK149" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="CL149" s="5">
+        <v>91</v>
+      </c>
     </row>
-    <row r="150" spans="2:88" s="5" customFormat="1">
+    <row r="150" spans="2:90" s="5" customFormat="1">
       <c r="B150" s="5">
         <v>1986</v>
       </c>
@@ -28570,8 +29303,14 @@
       <c r="CJ150" s="5">
         <v>8.4905755528145305E-3</v>
       </c>
+      <c r="CK150" s="5">
+        <v>2.1333333333333302</v>
+      </c>
+      <c r="CL150" s="5">
+        <v>95.5</v>
+      </c>
     </row>
-    <row r="151" spans="2:88" s="5" customFormat="1">
+    <row r="151" spans="2:90" s="5" customFormat="1">
       <c r="B151" s="5">
         <v>1986.25</v>
       </c>
@@ -28829,8 +29568,14 @@
       <c r="CJ151" s="5">
         <v>1.65081754043548E-3</v>
       </c>
+      <c r="CK151" s="5">
+        <v>2.4</v>
+      </c>
+      <c r="CL151" s="5">
+        <v>96.8</v>
+      </c>
     </row>
-    <row r="152" spans="2:88" s="5" customFormat="1">
+    <row r="152" spans="2:90" s="5" customFormat="1">
       <c r="B152" s="5">
         <v>1986.5</v>
       </c>
@@ -29088,8 +29833,14 @@
       <c r="CJ152" s="5">
         <v>5.7215867995677998E-3</v>
       </c>
+      <c r="CK152" s="5">
+        <v>2</v>
+      </c>
+      <c r="CL152" s="5">
+        <v>94.9</v>
+      </c>
     </row>
-    <row r="153" spans="2:88" s="5" customFormat="1">
+    <row r="153" spans="2:90" s="5" customFormat="1">
       <c r="B153" s="5">
         <v>1986.75</v>
       </c>
@@ -29347,8 +30098,14 @@
       <c r="CJ153" s="5">
         <v>-1.8092106728583301E-2</v>
       </c>
+      <c r="CK153" s="5">
+        <v>1.93333333333333</v>
+      </c>
+      <c r="CL153" s="5">
+        <v>92</v>
+      </c>
     </row>
-    <row r="154" spans="2:88" s="5" customFormat="1">
+    <row r="154" spans="2:90" s="5" customFormat="1">
       <c r="B154" s="5">
         <v>1987</v>
       </c>
@@ -29606,8 +30363,14 @@
       <c r="CJ154" s="5">
         <v>-1.8237261946746301E-2</v>
       </c>
+      <c r="CK154" s="5">
+        <v>8.3333333333333393</v>
+      </c>
+      <c r="CL154" s="5">
+        <v>90.5</v>
+      </c>
     </row>
-    <row r="155" spans="2:88" s="5" customFormat="1">
+    <row r="155" spans="2:90" s="5" customFormat="1">
       <c r="B155" s="5">
         <v>1987.25</v>
       </c>
@@ -29865,8 +30628,14 @@
       <c r="CJ155" s="5">
         <v>-2.5550677344443599E-2</v>
       </c>
+      <c r="CK155" s="5">
+        <v>13.4</v>
+      </c>
+      <c r="CL155" s="5">
+        <v>91.8</v>
+      </c>
     </row>
-    <row r="156" spans="2:88" s="5" customFormat="1">
+    <row r="156" spans="2:90" s="5" customFormat="1">
       <c r="B156" s="5">
         <v>1987.5</v>
       </c>
@@ -30124,8 +30893,14 @@
       <c r="CJ156" s="5">
         <v>-1.1590071737180799E-2</v>
       </c>
+      <c r="CK156" s="5">
+        <v>17.933333333333302</v>
+      </c>
+      <c r="CL156" s="5">
+        <v>93.9</v>
+      </c>
     </row>
-    <row r="157" spans="2:88" s="5" customFormat="1">
+    <row r="157" spans="2:90" s="5" customFormat="1">
       <c r="B157" s="5">
         <v>1987.75</v>
       </c>
@@ -30383,8 +31158,14 @@
       <c r="CJ157" s="5">
         <v>-5.3787751455692196E-3</v>
       </c>
+      <c r="CK157" s="5">
+        <v>20.3333333333333</v>
+      </c>
+      <c r="CL157" s="5">
+        <v>86.4</v>
+      </c>
     </row>
-    <row r="158" spans="2:88" s="5" customFormat="1">
+    <row r="158" spans="2:90" s="5" customFormat="1">
       <c r="B158" s="5">
         <v>1988</v>
       </c>
@@ -30642,8 +31423,14 @@
       <c r="CJ158" s="5">
         <v>-3.3175210014501099E-3</v>
       </c>
+      <c r="CK158" s="5">
+        <v>12.2</v>
+      </c>
+      <c r="CL158" s="5">
+        <v>92.3</v>
+      </c>
     </row>
-    <row r="159" spans="2:88" s="5" customFormat="1">
+    <row r="159" spans="2:90" s="5" customFormat="1">
       <c r="B159" s="5">
         <v>1988.25</v>
       </c>
@@ -30901,8 +31688,14 @@
       <c r="CJ159" s="5">
         <v>1.19821199225164E-3</v>
       </c>
+      <c r="CK159" s="5">
+        <v>13.733333333333301</v>
+      </c>
+      <c r="CL159" s="5">
+        <v>93.5</v>
+      </c>
     </row>
-    <row r="160" spans="2:88" s="5" customFormat="1">
+    <row r="160" spans="2:90" s="5" customFormat="1">
       <c r="B160" s="5">
         <v>1988.5</v>
       </c>
@@ -31160,8 +31953,14 @@
       <c r="CJ160" s="5">
         <v>-1.10150862293894E-2</v>
       </c>
+      <c r="CK160" s="5">
+        <v>12.533333333333299</v>
+      </c>
+      <c r="CL160" s="5">
+        <v>96</v>
+      </c>
     </row>
-    <row r="161" spans="2:88" s="5" customFormat="1">
+    <row r="161" spans="2:90" s="5" customFormat="1">
       <c r="B161" s="5">
         <v>1988.75</v>
       </c>
@@ -31419,8 +32218,14 @@
       <c r="CJ161" s="5">
         <v>-7.46555530368342E-3</v>
       </c>
+      <c r="CK161" s="5">
+        <v>11.4</v>
+      </c>
+      <c r="CL161" s="5">
+        <v>93</v>
+      </c>
     </row>
-    <row r="162" spans="2:88" s="5" customFormat="1">
+    <row r="162" spans="2:90" s="5" customFormat="1">
       <c r="B162" s="5">
         <v>1989</v>
       </c>
@@ -31678,8 +32483,14 @@
       <c r="CJ162" s="5">
         <v>-1.67804888830459E-2</v>
       </c>
+      <c r="CK162" s="5">
+        <v>6.8666666666666698</v>
+      </c>
+      <c r="CL162" s="5">
+        <v>95.9</v>
+      </c>
     </row>
-    <row r="163" spans="2:88" s="5" customFormat="1">
+    <row r="163" spans="2:90" s="5" customFormat="1">
       <c r="B163" s="5">
         <v>1989.25</v>
       </c>
@@ -31937,8 +32748,14 @@
       <c r="CJ163" s="5">
         <v>-1.2785677255188799E-2</v>
       </c>
+      <c r="CK163" s="5">
+        <v>-0.8</v>
+      </c>
+      <c r="CL163" s="5">
+        <v>90.9</v>
+      </c>
     </row>
-    <row r="164" spans="2:88" s="5" customFormat="1">
+    <row r="164" spans="2:90" s="5" customFormat="1">
       <c r="B164" s="5">
         <v>1989.5</v>
       </c>
@@ -32196,8 +33013,14 @@
       <c r="CJ164" s="5">
         <v>4.9558865983340096E-3</v>
       </c>
+      <c r="CK164" s="5">
+        <v>-8.6666666666666607</v>
+      </c>
+      <c r="CL164" s="5">
+        <v>92.5</v>
+      </c>
     </row>
-    <row r="165" spans="2:88" s="5" customFormat="1">
+    <row r="165" spans="2:90" s="5" customFormat="1">
       <c r="B165" s="5">
         <v>1989.75</v>
       </c>
@@ -32455,8 +33278,14 @@
       <c r="CJ165" s="5">
         <v>-1.8860006906958399E-2</v>
       </c>
+      <c r="CK165" s="5">
+        <v>-6</v>
+      </c>
+      <c r="CL165" s="5">
+        <v>91.8</v>
+      </c>
     </row>
-    <row r="166" spans="2:88" s="5" customFormat="1">
+    <row r="166" spans="2:90" s="5" customFormat="1">
       <c r="B166" s="5">
         <v>1990</v>
       </c>
@@ -32716,8 +33545,14 @@
       <c r="CJ166" s="5">
         <v>1.2294204974872E-3</v>
       </c>
+      <c r="CK166" s="5">
+        <v>-2.5333333333333301</v>
+      </c>
+      <c r="CL166" s="5">
+        <v>91.3</v>
+      </c>
     </row>
-    <row r="167" spans="2:88" s="5" customFormat="1">
+    <row r="167" spans="2:90" s="5" customFormat="1">
       <c r="B167" s="5">
         <v>1990.25</v>
       </c>
@@ -32977,8 +33812,14 @@
       <c r="CJ167" s="5">
         <v>-5.3937523866784201E-3</v>
       </c>
+      <c r="CK167" s="5">
+        <v>-0.86666666666666703</v>
+      </c>
+      <c r="CL167" s="5">
+        <v>90.9</v>
+      </c>
     </row>
-    <row r="168" spans="2:88" s="5" customFormat="1">
+    <row r="168" spans="2:90" s="5" customFormat="1">
       <c r="B168" s="5">
         <v>1990.5</v>
       </c>
@@ -33238,8 +34079,14 @@
       <c r="CJ168" s="5">
         <v>-2.2577607330228702E-2</v>
       </c>
+      <c r="CK168" s="5">
+        <v>-8.5333333333333297</v>
+      </c>
+      <c r="CL168" s="5">
+        <v>79.099999999999994</v>
+      </c>
     </row>
-    <row r="169" spans="2:88" s="5" customFormat="1">
+    <row r="169" spans="2:90" s="5" customFormat="1">
       <c r="B169" s="5">
         <v>1990.75</v>
       </c>
@@ -33499,8 +34346,14 @@
       <c r="CJ169" s="5">
         <v>-1.40359920221198E-2</v>
       </c>
+      <c r="CK169" s="5">
+        <v>-16.466666666666701</v>
+      </c>
+      <c r="CL169" s="5">
+        <v>65.2</v>
+      </c>
     </row>
-    <row r="170" spans="2:88" s="5" customFormat="1">
+    <row r="170" spans="2:90" s="5" customFormat="1">
       <c r="B170" s="5">
         <v>1991</v>
       </c>
@@ -33760,8 +34613,14 @@
       <c r="CJ170" s="5">
         <v>-1.5238658219129401E-2</v>
       </c>
+      <c r="CK170" s="5">
+        <v>-20.466666666666701</v>
+      </c>
+      <c r="CL170" s="5">
+        <v>74.8</v>
+      </c>
     </row>
-    <row r="171" spans="2:88" s="5" customFormat="1">
+    <row r="171" spans="2:90" s="5" customFormat="1">
       <c r="B171" s="5">
         <v>1991.25</v>
       </c>
@@ -34021,8 +34880,14 @@
       <c r="CJ171" s="5">
         <v>-1.1771395425436801E-2</v>
       </c>
+      <c r="CK171" s="5">
+        <v>-8.2666666666666604</v>
+      </c>
+      <c r="CL171" s="5">
+        <v>80.8</v>
+      </c>
     </row>
-    <row r="172" spans="2:88" s="5" customFormat="1">
+    <row r="172" spans="2:90" s="5" customFormat="1">
       <c r="B172" s="5">
         <v>1991.5</v>
       </c>
@@ -34282,8 +35147,14 @@
       <c r="CJ172" s="5">
         <v>-2.5306782989914098E-2</v>
       </c>
+      <c r="CK172" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="CL172" s="5">
+        <v>82.6</v>
+      </c>
     </row>
-    <row r="173" spans="2:88" s="5" customFormat="1">
+    <row r="173" spans="2:90" s="5" customFormat="1">
       <c r="B173" s="5">
         <v>1991.75</v>
       </c>
@@ -34543,8 +35414,14 @@
       <c r="CJ173" s="5">
         <v>2.5178148684257599E-3</v>
       </c>
+      <c r="CK173" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="CL173" s="5">
+        <v>71.900000000000006</v>
+      </c>
     </row>
-    <row r="174" spans="2:88" s="5" customFormat="1">
+    <row r="174" spans="2:90" s="5" customFormat="1">
       <c r="B174" s="5">
         <v>1992</v>
       </c>
@@ -34804,8 +35681,14 @@
       <c r="CJ174" s="5">
         <v>1.45926140713451E-2</v>
       </c>
+      <c r="CK174" s="5">
+        <v>3.06666666666667</v>
+      </c>
+      <c r="CL174" s="5">
+        <v>70.7</v>
+      </c>
     </row>
-    <row r="175" spans="2:88" s="5" customFormat="1">
+    <row r="175" spans="2:90" s="5" customFormat="1">
       <c r="B175" s="5">
         <v>1992.25</v>
       </c>
@@ -35065,8 +35948,14 @@
       <c r="CJ175" s="5">
         <v>-1.4265631016266E-2</v>
       </c>
+      <c r="CK175" s="5">
+        <v>7.93333333333333</v>
+      </c>
+      <c r="CL175" s="5">
+        <v>78.900000000000006</v>
+      </c>
     </row>
-    <row r="176" spans="2:88" s="5" customFormat="1">
+    <row r="176" spans="2:90" s="5" customFormat="1">
       <c r="B176" s="5">
         <v>1992.5</v>
       </c>
@@ -35326,8 +36215,14 @@
       <c r="CJ176" s="5">
         <v>-1.08999592590676E-2</v>
       </c>
+      <c r="CK176" s="5">
+        <v>4.6666666666666696</v>
+      </c>
+      <c r="CL176" s="5">
+        <v>76.099999999999994</v>
+      </c>
     </row>
-    <row r="177" spans="2:88" s="5" customFormat="1">
+    <row r="177" spans="2:90" s="5" customFormat="1">
       <c r="B177" s="5">
         <v>1992.75</v>
       </c>
@@ -35587,8 +36482,14 @@
       <c r="CJ177" s="5">
         <v>-1.6441682203925001E-2</v>
       </c>
+      <c r="CK177" s="5">
+        <v>5.4</v>
+      </c>
+      <c r="CL177" s="5">
+        <v>83.3</v>
+      </c>
     </row>
-    <row r="178" spans="2:88" s="5" customFormat="1">
+    <row r="178" spans="2:90" s="5" customFormat="1">
       <c r="B178" s="5">
         <v>1993</v>
       </c>
@@ -35848,8 +36749,14 @@
       <c r="CJ178" s="5">
         <v>-3.7552448015393099E-2</v>
       </c>
+      <c r="CK178" s="5">
+        <v>9.6666666666666607</v>
+      </c>
+      <c r="CL178" s="5">
+        <v>87.3</v>
+      </c>
     </row>
-    <row r="179" spans="2:88" s="5" customFormat="1">
+    <row r="179" spans="2:90" s="5" customFormat="1">
       <c r="B179" s="5">
         <v>1993.25</v>
       </c>
@@ -36109,8 +37016,14 @@
       <c r="CJ179" s="5">
         <v>-1.4259081345137E-2</v>
       </c>
+      <c r="CK179" s="5">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="CL179" s="5">
+        <v>82.5</v>
+      </c>
     </row>
-    <row r="180" spans="2:88" s="5" customFormat="1">
+    <row r="180" spans="2:90" s="5" customFormat="1">
       <c r="B180" s="5">
         <v>1993.5</v>
       </c>
@@ -36370,8 +37283,14 @@
       <c r="CJ180" s="5">
         <v>-1.7923594816752899E-2</v>
       </c>
+      <c r="CK180" s="5">
+        <v>1.13333333333333</v>
+      </c>
+      <c r="CL180" s="5">
+        <v>77.400000000000006</v>
+      </c>
     </row>
-    <row r="181" spans="2:88" s="5" customFormat="1">
+    <row r="181" spans="2:90" s="5" customFormat="1">
       <c r="B181" s="5">
         <v>1993.75</v>
       </c>
@@ -36631,8 +37550,14 @@
       <c r="CJ181" s="5">
         <v>-9.1289055244539192E-3</v>
       </c>
+      <c r="CK181" s="5">
+        <v>8.5333333333333297</v>
+      </c>
+      <c r="CL181" s="5">
+        <v>84.1</v>
+      </c>
     </row>
-    <row r="182" spans="2:88" s="5" customFormat="1">
+    <row r="182" spans="2:90" s="5" customFormat="1">
       <c r="B182" s="5">
         <v>1994</v>
       </c>
@@ -36892,8 +37817,14 @@
       <c r="CJ182" s="5">
         <v>-3.11869668923309E-2</v>
       </c>
+      <c r="CK182" s="5">
+        <v>12.9333333333333</v>
+      </c>
+      <c r="CL182" s="5">
+        <v>93</v>
+      </c>
     </row>
-    <row r="183" spans="2:88" s="5" customFormat="1">
+    <row r="183" spans="2:90" s="5" customFormat="1">
       <c r="B183" s="5">
         <v>1994.25</v>
       </c>
@@ -37153,8 +38084,14 @@
       <c r="CJ183" s="5">
         <v>-1.1337268521784899E-2</v>
       </c>
+      <c r="CK183" s="5">
+        <v>16.266666666666701</v>
+      </c>
+      <c r="CL183" s="5">
+        <v>92.2</v>
+      </c>
     </row>
-    <row r="184" spans="2:88" s="5" customFormat="1">
+    <row r="184" spans="2:90" s="5" customFormat="1">
       <c r="B184" s="5">
         <v>1994.5</v>
       </c>
@@ -37414,8 +38351,14 @@
       <c r="CJ184" s="5">
         <v>-1.9697901619198498E-2</v>
       </c>
+      <c r="CK184" s="5">
+        <v>17</v>
+      </c>
+      <c r="CL184" s="5">
+        <v>90.7</v>
+      </c>
     </row>
-    <row r="185" spans="2:88" s="5" customFormat="1">
+    <row r="185" spans="2:90" s="5" customFormat="1">
       <c r="B185" s="5">
         <v>1994.75</v>
       </c>
@@ -37675,8 +38618,14 @@
       <c r="CJ185" s="5">
         <v>-1.3510620832907799E-2</v>
       </c>
+      <c r="CK185" s="5">
+        <v>16.466666666666701</v>
+      </c>
+      <c r="CL185" s="5">
+        <v>93.1</v>
+      </c>
     </row>
-    <row r="186" spans="2:88" s="5" customFormat="1">
+    <row r="186" spans="2:90" s="5" customFormat="1">
       <c r="B186" s="5">
         <v>1995</v>
       </c>
@@ -37936,8 +38885,14 @@
       <c r="CJ186" s="5">
         <v>-1.1787754668022499E-2</v>
       </c>
+      <c r="CK186" s="5">
+        <v>9.7333333333333307</v>
+      </c>
+      <c r="CL186" s="5">
+        <v>94.3</v>
+      </c>
     </row>
-    <row r="187" spans="2:88" s="5" customFormat="1">
+    <row r="187" spans="2:90" s="5" customFormat="1">
       <c r="B187" s="5">
         <v>1995.25</v>
       </c>
@@ -38197,8 +39152,14 @@
       <c r="CJ187" s="5">
         <v>-7.10985829483306E-3</v>
       </c>
+      <c r="CK187" s="5">
+        <v>-3.93333333333333</v>
+      </c>
+      <c r="CL187" s="5">
+        <v>91.7</v>
+      </c>
     </row>
-    <row r="188" spans="2:88" s="5" customFormat="1">
+    <row r="188" spans="2:90" s="5" customFormat="1">
       <c r="B188" s="5">
         <v>1995.5</v>
       </c>
@@ -38458,8 +39419,14 @@
       <c r="CJ188" s="5">
         <v>-1.4367027923614099E-2</v>
       </c>
+      <c r="CK188" s="5">
+        <v>-2.7333333333333298</v>
+      </c>
+      <c r="CL188" s="5">
+        <v>93.1</v>
+      </c>
     </row>
-    <row r="189" spans="2:88" s="5" customFormat="1">
+    <row r="189" spans="2:90" s="5" customFormat="1">
       <c r="B189" s="5">
         <v>1995.75</v>
       </c>
@@ -38719,8 +39686,14 @@
       <c r="CJ189" s="5">
         <v>-1.3474538462025801E-2</v>
       </c>
+      <c r="CK189" s="5">
+        <v>-7.4666666666666703</v>
+      </c>
+      <c r="CL189" s="5">
+        <v>89.8</v>
+      </c>
     </row>
-    <row r="190" spans="2:88" s="5" customFormat="1">
+    <row r="190" spans="2:90" s="5" customFormat="1">
       <c r="B190" s="5">
         <v>1996</v>
       </c>
@@ -38980,8 +39953,14 @@
       <c r="CJ190" s="5">
         <v>-6.1169994584861897E-3</v>
       </c>
+      <c r="CK190" s="5">
+        <v>-7.8</v>
+      </c>
+      <c r="CL190" s="5">
+        <v>90.5</v>
+      </c>
     </row>
-    <row r="191" spans="2:88" s="5" customFormat="1">
+    <row r="191" spans="2:90" s="5" customFormat="1">
       <c r="B191" s="5">
         <v>1996.25</v>
       </c>
@@ -39241,8 +40220,14 @@
       <c r="CJ191" s="5">
         <v>-1.2040976079404001E-2</v>
       </c>
+      <c r="CK191" s="5">
+        <v>1.3333333333333299</v>
+      </c>
+      <c r="CL191" s="5">
+        <v>91.5</v>
+      </c>
     </row>
-    <row r="192" spans="2:88" s="5" customFormat="1">
+    <row r="192" spans="2:90" s="5" customFormat="1">
       <c r="B192" s="5">
         <v>1996.5</v>
       </c>
@@ -39502,8 +40487,14 @@
       <c r="CJ192" s="5">
         <v>-1.52481406995548E-2</v>
       </c>
+      <c r="CK192" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="CL192" s="5">
+        <v>94.9</v>
+      </c>
     </row>
-    <row r="193" spans="2:88" s="5" customFormat="1">
+    <row r="193" spans="2:90" s="5" customFormat="1">
       <c r="B193" s="5">
         <v>1996.75</v>
       </c>
@@ -39763,8 +40754,14 @@
       <c r="CJ193" s="5">
         <v>-1.3099399403997399E-2</v>
       </c>
+      <c r="CK193" s="5">
+        <v>5.8</v>
+      </c>
+      <c r="CL193" s="5">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="194" spans="2:88" s="5" customFormat="1">
+    <row r="194" spans="2:90" s="5" customFormat="1">
       <c r="B194" s="5">
         <v>1997</v>
       </c>
@@ -40024,8 +41021,14 @@
       <c r="CJ194" s="5">
         <v>-1.6751450455123801E-2</v>
       </c>
+      <c r="CK194" s="5">
+        <v>7.1333333333333302</v>
+      </c>
+      <c r="CL194" s="5">
+        <v>99</v>
+      </c>
     </row>
-    <row r="195" spans="2:88" s="5" customFormat="1">
+    <row r="195" spans="2:90" s="5" customFormat="1">
       <c r="B195" s="5">
         <v>1997.25</v>
       </c>
@@ -40285,8 +41288,14 @@
       <c r="CJ195" s="5">
         <v>6.24306097143965E-3</v>
       </c>
+      <c r="CK195" s="5">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="CL195" s="5">
+        <v>103</v>
+      </c>
     </row>
-    <row r="196" spans="2:88" s="5" customFormat="1">
+    <row r="196" spans="2:90" s="5" customFormat="1">
       <c r="B196" s="5">
         <v>1997.5</v>
       </c>
@@ -40546,8 +41555,14 @@
       <c r="CJ196" s="5">
         <v>-1.39422494855416E-2</v>
       </c>
+      <c r="CK196" s="5">
+        <v>11.9333333333333</v>
+      </c>
+      <c r="CL196" s="5">
+        <v>105.8</v>
+      </c>
     </row>
-    <row r="197" spans="2:88" s="5" customFormat="1">
+    <row r="197" spans="2:90" s="5" customFormat="1">
       <c r="B197" s="5">
         <v>1997.75</v>
       </c>
@@ -40810,8 +41825,14 @@
       <c r="CJ197" s="5">
         <v>-6.4267738385515496E-3</v>
       </c>
+      <c r="CK197" s="5">
+        <v>11.0666666666667</v>
+      </c>
+      <c r="CL197" s="5">
+        <v>105</v>
+      </c>
     </row>
-    <row r="198" spans="2:88" s="5" customFormat="1">
+    <row r="198" spans="2:90" s="5" customFormat="1">
       <c r="B198" s="5">
         <v>1998</v>
       </c>
@@ -41074,8 +42095,14 @@
       <c r="CJ198" s="5">
         <v>6.6784394465075701E-3</v>
       </c>
+      <c r="CK198" s="5">
+        <v>6.4</v>
+      </c>
+      <c r="CL198" s="5">
+        <v>107.8</v>
+      </c>
     </row>
-    <row r="199" spans="2:88" s="5" customFormat="1">
+    <row r="199" spans="2:90" s="5" customFormat="1">
       <c r="B199" s="5">
         <v>1998.25</v>
       </c>
@@ -41338,8 +42365,14 @@
       <c r="CJ199" s="5">
         <v>3.76010396919762E-3</v>
       </c>
+      <c r="CK199" s="5">
+        <v>1.3333333333333299</v>
+      </c>
+      <c r="CL199" s="5">
+        <v>106.9</v>
+      </c>
     </row>
-    <row r="200" spans="2:88" s="5" customFormat="1">
+    <row r="200" spans="2:90" s="5" customFormat="1">
       <c r="B200" s="5">
         <v>1998.5</v>
       </c>
@@ -41602,8 +42635,14 @@
       <c r="CJ200" s="5">
         <v>5.8064143373436896E-3</v>
       </c>
+      <c r="CK200" s="5">
+        <v>-1.86666666666667</v>
+      </c>
+      <c r="CL200" s="5">
+        <v>103.5</v>
+      </c>
     </row>
-    <row r="201" spans="2:88" s="5" customFormat="1">
+    <row r="201" spans="2:90" s="5" customFormat="1">
       <c r="B201" s="5">
         <v>1998.75</v>
       </c>
@@ -41866,8 +42905,14 @@
       <c r="CJ201" s="5">
         <v>1.22483711488984E-2</v>
       </c>
+      <c r="CK201" s="5">
+        <v>-4.2</v>
+      </c>
+      <c r="CL201" s="5">
+        <v>100.2</v>
+      </c>
     </row>
-    <row r="202" spans="2:88" s="5" customFormat="1">
+    <row r="202" spans="2:90" s="5" customFormat="1">
       <c r="B202" s="5">
         <v>1999</v>
       </c>
@@ -42130,8 +43175,14 @@
       <c r="CJ202" s="5">
         <v>-1.46337436998893E-3</v>
       </c>
+      <c r="CK202" s="5">
+        <v>3.1333333333333302</v>
+      </c>
+      <c r="CL202" s="5">
+        <v>105.9</v>
+      </c>
     </row>
-    <row r="203" spans="2:88" s="5" customFormat="1">
+    <row r="203" spans="2:90" s="5" customFormat="1">
       <c r="B203" s="5">
         <v>1999.25</v>
       </c>
@@ -42394,8 +43445,14 @@
       <c r="CJ203" s="5">
         <v>-1.37046893973838E-2</v>
       </c>
+      <c r="CK203" s="5">
+        <v>8.2666666666666604</v>
+      </c>
+      <c r="CL203" s="5">
+        <v>106.2</v>
+      </c>
     </row>
-    <row r="204" spans="2:88" s="5" customFormat="1">
+    <row r="204" spans="2:90" s="5" customFormat="1">
       <c r="B204" s="5">
         <v>1999.5</v>
       </c>
@@ -42658,8 +43715,14 @@
       <c r="CJ204" s="5">
         <v>-2.3373074097014302E-3</v>
       </c>
+      <c r="CK204" s="5">
+        <v>10.266666666666699</v>
+      </c>
+      <c r="CL204" s="5">
+        <v>105.9</v>
+      </c>
     </row>
-    <row r="205" spans="2:88" s="5" customFormat="1">
+    <row r="205" spans="2:90" s="5" customFormat="1">
       <c r="B205" s="5">
         <v>1999.75</v>
       </c>
@@ -42922,8 +43985,14 @@
       <c r="CJ205" s="5">
         <v>1.3187228115563001E-2</v>
       </c>
+      <c r="CK205" s="5">
+        <v>15.4</v>
+      </c>
+      <c r="CL205" s="5">
+        <v>105.2</v>
+      </c>
     </row>
-    <row r="206" spans="2:88" s="5" customFormat="1">
+    <row r="206" spans="2:90" s="5" customFormat="1">
       <c r="B206" s="5">
         <v>2000</v>
       </c>
@@ -43186,8 +44255,14 @@
       <c r="CJ206" s="5">
         <v>-4.0221324137099E-3</v>
       </c>
+      <c r="CK206" s="5">
+        <v>11.6</v>
+      </c>
+      <c r="CL206" s="5">
+        <v>110.1</v>
+      </c>
     </row>
-    <row r="207" spans="2:88" s="5" customFormat="1">
+    <row r="207" spans="2:90" s="5" customFormat="1">
       <c r="B207" s="5">
         <v>2000.25</v>
       </c>
@@ -43450,8 +44525,14 @@
       <c r="CJ207" s="5">
         <v>8.7654216607614497E-3</v>
       </c>
+      <c r="CK207" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="CL207" s="5">
+        <v>108.8</v>
+      </c>
     </row>
-    <row r="208" spans="2:88" s="5" customFormat="1">
+    <row r="208" spans="2:90" s="5" customFormat="1">
       <c r="B208" s="5">
         <v>2000.5</v>
       </c>
@@ -43714,8 +44795,14 @@
       <c r="CJ208" s="5">
         <v>-8.9597872440793898E-4</v>
       </c>
+      <c r="CK208" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="CL208" s="5">
+        <v>107.5</v>
+      </c>
     </row>
-    <row r="209" spans="2:88" s="5" customFormat="1">
+    <row r="209" spans="2:90" s="5" customFormat="1">
       <c r="B209" s="5">
         <v>2000.75</v>
       </c>
@@ -43978,8 +45065,14 @@
       <c r="CJ209" s="5">
         <v>-1.17009395095306E-2</v>
       </c>
+      <c r="CK209" s="5">
+        <v>-5.93333333333333</v>
+      </c>
+      <c r="CL209" s="5">
+        <v>103.9</v>
+      </c>
     </row>
-    <row r="210" spans="2:88" s="5" customFormat="1">
+    <row r="210" spans="2:90" s="5" customFormat="1">
       <c r="B210" s="5">
         <v>2001</v>
       </c>
@@ -44242,8 +45335,14 @@
       <c r="CJ210" s="5">
         <v>1.5863013281614598E-2</v>
       </c>
+      <c r="CK210" s="5">
+        <v>-16.600000000000001</v>
+      </c>
+      <c r="CL210" s="5">
+        <v>92.3</v>
+      </c>
     </row>
-    <row r="211" spans="2:88" s="5" customFormat="1">
+    <row r="211" spans="2:90" s="5" customFormat="1">
       <c r="B211" s="5">
         <v>2001.25</v>
       </c>
@@ -44506,8 +45605,14 @@
       <c r="CJ211" s="5">
         <v>7.9427244941280006E-3</v>
       </c>
+      <c r="CK211" s="5">
+        <v>-14.0666666666667</v>
+      </c>
+      <c r="CL211" s="5">
+        <v>91</v>
+      </c>
     </row>
-    <row r="212" spans="2:88" s="5" customFormat="1">
+    <row r="212" spans="2:90" s="5" customFormat="1">
       <c r="B212" s="5">
         <v>2001.5</v>
       </c>
@@ -44770,8 +45875,14 @@
       <c r="CJ212" s="5">
         <v>2.07578238165739E-2</v>
       </c>
+      <c r="CK212" s="5">
+        <v>-6.2</v>
+      </c>
+      <c r="CL212" s="5">
+        <v>88.5</v>
+      </c>
     </row>
-    <row r="213" spans="2:88" s="5" customFormat="1">
+    <row r="213" spans="2:90" s="5" customFormat="1">
       <c r="B213" s="5">
         <v>2001.75</v>
       </c>
@@ -45034,8 +46145,14 @@
       <c r="CJ213" s="5">
         <v>-1.7677858959726699E-2</v>
       </c>
+      <c r="CK213" s="5">
+        <v>-11.866666666666699</v>
+      </c>
+      <c r="CL213" s="5">
+        <v>85.1</v>
+      </c>
     </row>
-    <row r="214" spans="2:88" s="5" customFormat="1">
+    <row r="214" spans="2:90" s="5" customFormat="1">
       <c r="B214" s="5">
         <v>2002</v>
       </c>
@@ -45298,8 +46415,14 @@
       <c r="CJ214" s="5">
         <v>6.49265828469667E-3</v>
       </c>
+      <c r="CK214" s="5">
+        <v>4.8666666666666698</v>
+      </c>
+      <c r="CL214" s="5">
+        <v>93.1</v>
+      </c>
     </row>
-    <row r="215" spans="2:88" s="5" customFormat="1">
+    <row r="215" spans="2:90" s="5" customFormat="1">
       <c r="B215" s="5">
         <v>2002.25</v>
       </c>
@@ -45562,8 +46685,14 @@
       <c r="CJ215" s="5">
         <v>-2.3106805684169798E-2</v>
       </c>
+      <c r="CK215" s="5">
+        <v>10.266666666666699</v>
+      </c>
+      <c r="CL215" s="5">
+        <v>94.1</v>
+      </c>
     </row>
-    <row r="216" spans="2:88" s="5" customFormat="1">
+    <row r="216" spans="2:90" s="5" customFormat="1">
       <c r="B216" s="5">
         <v>2002.5</v>
       </c>
@@ -45826,8 +46955,14 @@
       <c r="CJ216" s="5">
         <v>-1.12536715707577E-2</v>
       </c>
+      <c r="CK216" s="5">
+        <v>2.2666666666666702</v>
+      </c>
+      <c r="CL216" s="5">
+        <v>87.3</v>
+      </c>
     </row>
-    <row r="217" spans="2:88" s="5" customFormat="1">
+    <row r="217" spans="2:90" s="5" customFormat="1">
       <c r="B217" s="5">
         <v>2002.75</v>
       </c>
@@ -46090,8 +47225,14 @@
       <c r="CJ217" s="5">
         <v>4.4373928928339301E-3</v>
       </c>
+      <c r="CK217" s="5">
+        <v>1.5333333333333301</v>
+      </c>
+      <c r="CL217" s="5">
+        <v>83.8</v>
+      </c>
     </row>
-    <row r="218" spans="2:88" s="5" customFormat="1">
+    <row r="218" spans="2:90" s="5" customFormat="1">
       <c r="B218" s="5">
         <v>2003</v>
       </c>
@@ -46354,8 +47495,14 @@
       <c r="CJ218" s="5">
         <v>-1.8424562917506299E-2</v>
       </c>
+      <c r="CK218" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="CL218" s="5">
+        <v>80</v>
+      </c>
     </row>
-    <row r="219" spans="2:88" s="5" customFormat="1">
+    <row r="219" spans="2:90" s="5" customFormat="1">
       <c r="B219" s="5">
         <v>2003.25</v>
       </c>
@@ -46618,8 +47765,14 @@
       <c r="CJ219" s="5">
         <v>3.2516561263243801E-2</v>
       </c>
+      <c r="CK219" s="5">
+        <v>-2</v>
+      </c>
+      <c r="CL219" s="5">
+        <v>89.3</v>
+      </c>
     </row>
-    <row r="220" spans="2:88" s="5" customFormat="1">
+    <row r="220" spans="2:90" s="5" customFormat="1">
       <c r="B220" s="5">
         <v>2003.5</v>
       </c>
@@ -46882,8 +48035,14 @@
       <c r="CJ220" s="5">
         <v>1.45349088553887E-2</v>
       </c>
+      <c r="CK220" s="5">
+        <v>8.1333333333333293</v>
+      </c>
+      <c r="CL220" s="5">
+        <v>89.3</v>
+      </c>
     </row>
-    <row r="221" spans="2:88" s="5" customFormat="1">
+    <row r="221" spans="2:90" s="5" customFormat="1">
       <c r="B221" s="5">
         <v>2003.75</v>
       </c>
@@ -47146,8 +48305,14 @@
       <c r="CJ221" s="5">
         <v>-7.3532806820449702E-3</v>
       </c>
+      <c r="CK221" s="5">
+        <v>20.6</v>
+      </c>
+      <c r="CL221" s="5">
+        <v>92</v>
+      </c>
     </row>
-    <row r="222" spans="2:88" s="5" customFormat="1">
+    <row r="222" spans="2:90" s="5" customFormat="1">
       <c r="B222" s="5">
         <v>2004</v>
       </c>
@@ -47410,8 +48575,14 @@
       <c r="CJ222" s="5">
         <v>5.4389997636212996E-4</v>
       </c>
+      <c r="CK222" s="5">
+        <v>24.933333333333302</v>
+      </c>
+      <c r="CL222" s="5">
+        <v>98.1</v>
+      </c>
     </row>
-    <row r="223" spans="2:88" s="5" customFormat="1">
+    <row r="223" spans="2:90" s="5" customFormat="1">
       <c r="B223" s="5">
         <v>2004.25</v>
       </c>
@@ -47674,8 +48845,14 @@
       <c r="CJ223" s="5">
         <v>1.19795633745423E-2</v>
       </c>
+      <c r="CK223" s="5">
+        <v>24.933333333333302</v>
+      </c>
+      <c r="CL223" s="5">
+        <v>93.4</v>
+      </c>
     </row>
-    <row r="224" spans="2:88" s="5" customFormat="1">
+    <row r="224" spans="2:90" s="5" customFormat="1">
       <c r="B224" s="5">
         <v>2004.5</v>
       </c>
@@ -47938,8 +49115,14 @@
       <c r="CJ224" s="5">
         <v>6.5881152507438496E-3</v>
       </c>
+      <c r="CK224" s="5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="CL224" s="5">
+        <v>95.6</v>
+      </c>
     </row>
-    <row r="225" spans="2:88" s="5" customFormat="1">
+    <row r="225" spans="2:90" s="5" customFormat="1">
       <c r="B225" s="5">
         <v>2004.75</v>
       </c>
@@ -48202,8 +49385,14 @@
       <c r="CJ225" s="5">
         <v>-1.05470006977894E-2</v>
       </c>
+      <c r="CK225" s="5">
+        <v>14.866666666666699</v>
+      </c>
+      <c r="CL225" s="5">
+        <v>93.9</v>
+      </c>
     </row>
-    <row r="226" spans="2:88" s="5" customFormat="1">
+    <row r="226" spans="2:90" s="5" customFormat="1">
       <c r="B226" s="5">
         <v>2005</v>
       </c>
@@ -48466,8 +49655,14 @@
       <c r="CJ226" s="5">
         <v>3.11273095680971E-4</v>
       </c>
+      <c r="CK226" s="5">
+        <v>11.466666666666701</v>
+      </c>
+      <c r="CL226" s="5">
+        <v>94.1</v>
+      </c>
     </row>
-    <row r="227" spans="2:88" s="5" customFormat="1">
+    <row r="227" spans="2:90" s="5" customFormat="1">
       <c r="B227" s="5">
         <v>2005.25</v>
       </c>
@@ -48730,8 +49925,14 @@
       <c r="CJ227" s="5">
         <v>-1.04508378926534E-2</v>
       </c>
+      <c r="CK227" s="5">
+        <v>6.4</v>
+      </c>
+      <c r="CL227" s="5">
+        <v>90.2</v>
+      </c>
     </row>
-    <row r="228" spans="2:88" s="5" customFormat="1">
+    <row r="228" spans="2:90" s="5" customFormat="1">
       <c r="B228" s="5">
         <v>2005.5</v>
       </c>
@@ -48994,8 +50195,14 @@
       <c r="CJ228" s="5">
         <v>9.7599978032591097E-3</v>
       </c>
+      <c r="CK228" s="5">
+        <v>11.9333333333333</v>
+      </c>
+      <c r="CL228" s="5">
+        <v>87.4</v>
+      </c>
     </row>
-    <row r="229" spans="2:88" s="5" customFormat="1">
+    <row r="229" spans="2:90" s="5" customFormat="1">
       <c r="B229" s="5">
         <v>2005.75</v>
       </c>
@@ -49258,8 +50465,14 @@
       <c r="CJ229" s="5">
         <v>-3.3126701493021199E-3</v>
       </c>
+      <c r="CK229" s="5">
+        <v>14</v>
+      </c>
+      <c r="CL229" s="5">
+        <v>82.4</v>
+      </c>
     </row>
-    <row r="230" spans="2:88" s="5" customFormat="1">
+    <row r="230" spans="2:90" s="5" customFormat="1">
       <c r="B230" s="5">
         <v>2006</v>
       </c>
@@ -49522,8 +50735,14 @@
       <c r="CJ230" s="5">
         <v>3.04723543274069E-2</v>
       </c>
+      <c r="CK230" s="5">
+        <v>9.4</v>
+      </c>
+      <c r="CL230" s="5">
+        <v>88.9</v>
+      </c>
     </row>
-    <row r="231" spans="2:88" s="5" customFormat="1">
+    <row r="231" spans="2:90" s="5" customFormat="1">
       <c r="B231" s="5">
         <v>2006.25</v>
       </c>
@@ -49783,8 +51002,14 @@
       <c r="CJ231" s="5">
         <v>-1.07364250233738E-2</v>
       </c>
+      <c r="CK231" s="5">
+        <v>8.2666666666666604</v>
+      </c>
+      <c r="CL231" s="5">
+        <v>83.8</v>
+      </c>
     </row>
-    <row r="232" spans="2:88" s="5" customFormat="1">
+    <row r="232" spans="2:90" s="5" customFormat="1">
       <c r="B232" s="5">
         <v>2006.5</v>
       </c>
@@ -50044,8 +51269,14 @@
       <c r="CJ232" s="5">
         <v>-8.0862243462785401E-3</v>
       </c>
+      <c r="CK232" s="5">
+        <v>5.8666666666666698</v>
+      </c>
+      <c r="CL232" s="5">
+        <v>84</v>
+      </c>
     </row>
-    <row r="233" spans="2:88" s="5" customFormat="1">
+    <row r="233" spans="2:90" s="5" customFormat="1">
       <c r="B233" s="5">
         <v>2006.75</v>
       </c>
@@ -50305,8 +51536,14 @@
       <c r="CJ233" s="5">
         <v>1.04141196210993E-2</v>
       </c>
+      <c r="CK233" s="5">
+        <v>1.5333333333333301</v>
+      </c>
+      <c r="CL233" s="5">
+        <v>92.5</v>
+      </c>
     </row>
-    <row r="234" spans="2:88" s="5" customFormat="1">
+    <row r="234" spans="2:90" s="5" customFormat="1">
       <c r="B234" s="5">
         <v>2007</v>
       </c>
@@ -50551,8 +51788,14 @@
       <c r="CJ234" s="5">
         <v>4.8808285251708003E-3</v>
       </c>
+      <c r="CK234" s="5">
+        <v>1</v>
+      </c>
+      <c r="CL234" s="5">
+        <v>92.2</v>
+      </c>
     </row>
-    <row r="235" spans="2:88" s="5" customFormat="1">
+    <row r="235" spans="2:90" s="5" customFormat="1">
       <c r="B235" s="5">
         <v>2007.25</v>
       </c>
@@ -50797,8 +52040,14 @@
       <c r="CJ235" s="5">
         <v>2.5347693394994798E-3</v>
       </c>
+      <c r="CK235" s="5">
+        <v>6</v>
+      </c>
+      <c r="CL235" s="5">
+        <v>86.9</v>
+      </c>
     </row>
-    <row r="236" spans="2:88" s="5" customFormat="1">
+    <row r="236" spans="2:90" s="5" customFormat="1">
       <c r="B236" s="5">
         <v>2007.5</v>
       </c>
@@ -51043,8 +52292,14 @@
       <c r="CJ236" s="5">
         <v>1.0392043356263999E-2</v>
       </c>
+      <c r="CK236" s="5">
+        <v>2.6666666666666701</v>
+      </c>
+      <c r="CL236" s="5">
+        <v>85.8</v>
+      </c>
     </row>
-    <row r="237" spans="2:88" s="5" customFormat="1">
+    <row r="237" spans="2:90" s="5" customFormat="1">
       <c r="B237" s="5">
         <v>2007.75</v>
       </c>
@@ -51289,8 +52544,14 @@
       <c r="CJ237" s="5">
         <v>8.4628105308085008E-3</v>
       </c>
+      <c r="CK237" s="5">
+        <v>-0.8</v>
+      </c>
+      <c r="CL237" s="5">
+        <v>77.5</v>
+      </c>
     </row>
-    <row r="238" spans="2:88" s="5" customFormat="1">
+    <row r="238" spans="2:90" s="5" customFormat="1">
       <c r="B238" s="5">
         <v>2008</v>
       </c>
@@ -51535,8 +52796,14 @@
       <c r="CJ238" s="5">
         <v>7.3006611023858402E-3</v>
       </c>
+      <c r="CK238" s="5">
+        <v>-1.6</v>
+      </c>
+      <c r="CL238" s="5">
+        <v>72.900000000000006</v>
+      </c>
     </row>
-    <row r="239" spans="2:88" s="5" customFormat="1">
+    <row r="239" spans="2:90" s="5" customFormat="1">
       <c r="B239" s="5">
         <v>2008.25</v>
       </c>
@@ -51781,8 +53048,14 @@
       <c r="CJ239" s="5">
         <v>3.7088530281313398E-2</v>
       </c>
+      <c r="CK239" s="5">
+        <v>-1.06666666666667</v>
+      </c>
+      <c r="CL239" s="5">
+        <v>59.6</v>
+      </c>
     </row>
-    <row r="240" spans="2:88" s="5" customFormat="1">
+    <row r="240" spans="2:90" s="5" customFormat="1">
       <c r="B240" s="5">
         <v>2008.5</v>
       </c>
@@ -52027,8 +53300,14 @@
       <c r="CJ240" s="5">
         <v>8.4916351160337702E-3</v>
       </c>
+      <c r="CK240" s="5">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="CL240" s="5">
+        <v>64.8</v>
+      </c>
     </row>
-    <row r="241" spans="2:88" s="5" customFormat="1">
+    <row r="241" spans="2:90" s="5" customFormat="1">
       <c r="B241" s="5">
         <v>2008.75</v>
       </c>
@@ -52273,8 +53552,14 @@
       <c r="CJ241" s="5">
         <v>3.2084637248778997E-2</v>
       </c>
+      <c r="CK241" s="5">
+        <v>-28.3333333333333</v>
+      </c>
+      <c r="CL241" s="5">
+        <v>57.7</v>
+      </c>
     </row>
-    <row r="242" spans="2:88" s="5" customFormat="1">
+    <row r="242" spans="2:90" s="5" customFormat="1">
       <c r="B242" s="5">
         <v>2009</v>
       </c>
@@ -52519,8 +53804,14 @@
       <c r="CJ242" s="5">
         <v>-2.1163025076845802E-3</v>
       </c>
+      <c r="CK242" s="5">
+        <v>-28.2</v>
+      </c>
+      <c r="CL242" s="5">
+        <v>58.3</v>
+      </c>
     </row>
-    <row r="243" spans="2:88" s="5" customFormat="1">
+    <row r="243" spans="2:90" s="5" customFormat="1">
       <c r="B243" s="5">
         <v>2009.25</v>
       </c>
@@ -52765,8 +54056,14 @@
       <c r="CJ243" s="5">
         <v>2.3434104297668099E-2</v>
       </c>
+      <c r="CK243" s="5">
+        <v>-14.0666666666667</v>
+      </c>
+      <c r="CL243" s="5">
+        <v>68.2</v>
+      </c>
     </row>
-    <row r="244" spans="2:88" s="5" customFormat="1">
+    <row r="244" spans="2:90" s="5" customFormat="1">
       <c r="B244" s="5">
         <v>2009.5</v>
       </c>
@@ -53011,8 +54308,14 @@
       <c r="CJ244" s="5">
         <v>-4.7274235656577401E-2</v>
       </c>
+      <c r="CK244" s="5">
+        <v>2.8666666666666698</v>
+      </c>
+      <c r="CL244" s="5">
+        <v>68.400000000000006</v>
+      </c>
     </row>
-    <row r="245" spans="2:88" s="5" customFormat="1">
+    <row r="245" spans="2:90" s="5" customFormat="1">
       <c r="B245" s="5">
         <v>2009.75</v>
       </c>
@@ -53257,8 +54560,14 @@
       <c r="CJ245" s="5">
         <v>-1.4296318403493E-2</v>
       </c>
+      <c r="CK245" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="CL245" s="5">
+        <v>70.099999999999994</v>
+      </c>
     </row>
-    <row r="246" spans="2:88" s="5" customFormat="1">
+    <row r="246" spans="2:90" s="5" customFormat="1">
       <c r="B246" s="5">
         <v>2010</v>
       </c>
@@ -53501,8 +54810,14 @@
       <c r="CJ246" s="5">
         <v>-2.71746428289825E-2</v>
       </c>
+      <c r="CK246" s="5">
+        <v>17.266666666666701</v>
+      </c>
+      <c r="CL246" s="5">
+        <v>73.900000000000006</v>
+      </c>
     </row>
-    <row r="247" spans="2:88" s="5" customFormat="1">
+    <row r="247" spans="2:90" s="5" customFormat="1">
       <c r="B247" s="5">
         <v>2010.25</v>
       </c>
@@ -53745,8 +55060,14 @@
       <c r="CJ247" s="5">
         <v>1.15833154386534E-2</v>
       </c>
+      <c r="CK247" s="5">
+        <v>15.133333333333301</v>
+      </c>
+      <c r="CL247" s="5">
+        <v>73.900000000000006</v>
+      </c>
     </row>
-    <row r="248" spans="2:88" s="5" customFormat="1">
+    <row r="248" spans="2:90" s="5" customFormat="1">
       <c r="B248" s="5">
         <v>2010.5</v>
       </c>
@@ -53989,8 +55310,14 @@
       <c r="CJ248" s="5">
         <v>-1.7178467647953001E-3</v>
       </c>
+      <c r="CK248" s="5">
+        <v>10.4</v>
+      </c>
+      <c r="CL248" s="5">
+        <v>68.3</v>
+      </c>
     </row>
-    <row r="249" spans="2:88" s="5" customFormat="1">
+    <row r="249" spans="2:90" s="5" customFormat="1">
       <c r="B249" s="5">
         <v>2010.75</v>
       </c>
@@ -54233,8 +55560,14 @@
       <c r="CJ249" s="5">
         <v>-1.1526989592138201E-3</v>
       </c>
+      <c r="CK249" s="5">
+        <v>15.733333333333301</v>
+      </c>
+      <c r="CL249" s="5">
+        <v>71.2</v>
+      </c>
     </row>
-    <row r="250" spans="2:88" s="5" customFormat="1">
+    <row r="250" spans="2:90" s="5" customFormat="1">
       <c r="B250" s="5">
         <v>2011</v>
       </c>
@@ -54477,8 +55810,14 @@
       <c r="CJ250" s="5">
         <v>-1.39953406233502E-2</v>
       </c>
+      <c r="CK250" s="5">
+        <v>18.933333333333302</v>
+      </c>
+      <c r="CL250" s="5">
+        <v>73.099999999999994</v>
+      </c>
     </row>
-    <row r="251" spans="2:88" s="5" customFormat="1">
+    <row r="251" spans="2:90" s="5" customFormat="1">
       <c r="B251" s="5">
         <v>2011.25</v>
       </c>
@@ -54721,8 +56060,14 @@
       <c r="CJ251" s="5">
         <v>8.6974708402704007E-3</v>
       </c>
+      <c r="CK251" s="5">
+        <v>13</v>
+      </c>
+      <c r="CL251" s="5">
+        <v>71.900000000000006</v>
+      </c>
     </row>
-    <row r="252" spans="2:88" s="5" customFormat="1">
+    <row r="252" spans="2:90" s="5" customFormat="1">
       <c r="B252" s="5">
         <v>2011.5</v>
       </c>
@@ -54965,8 +56310,14 @@
       <c r="CJ252" s="5">
         <v>1.3913719644113301E-2</v>
       </c>
+      <c r="CK252" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="CL252" s="5">
+        <v>59.5</v>
+      </c>
     </row>
-    <row r="253" spans="2:88" s="5" customFormat="1">
+    <row r="253" spans="2:90" s="5" customFormat="1">
       <c r="B253" s="5">
         <v>2011.75</v>
       </c>
@@ -55209,8 +56560,14 @@
       <c r="CJ253" s="5">
         <v>3.4882737376158899E-3</v>
       </c>
+      <c r="CK253" s="5">
+        <v>3.6666666666666701</v>
+      </c>
+      <c r="CL253" s="5">
+        <v>64.7</v>
+      </c>
     </row>
-    <row r="254" spans="2:88" s="5" customFormat="1">
+    <row r="254" spans="2:90" s="5" customFormat="1">
       <c r="B254" s="5">
         <v>2012</v>
       </c>
@@ -55453,8 +56810,14 @@
       <c r="CJ254" s="5">
         <v>2.3936299849649199E-2</v>
       </c>
+      <c r="CK254" s="5">
+        <v>6.8</v>
+      </c>
+      <c r="CL254" s="5">
+        <v>75.5</v>
+      </c>
     </row>
-    <row r="255" spans="2:88" s="5" customFormat="1">
+    <row r="255" spans="2:90" s="5" customFormat="1">
       <c r="B255" s="5">
         <v>2012.25</v>
       </c>
@@ -55697,8 +57060,14 @@
       <c r="CJ255" s="5">
         <v>2.3564825122314101E-3</v>
       </c>
+      <c r="CK255" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="CL255" s="5">
+        <v>76.3</v>
+      </c>
     </row>
-    <row r="256" spans="2:88" s="5" customFormat="1">
+    <row r="256" spans="2:90" s="5" customFormat="1">
       <c r="B256" s="5">
         <v>2012.5</v>
       </c>
@@ -55941,8 +57310,14 @@
       <c r="CJ256" s="5">
         <v>-1.1745773023150499E-3</v>
       </c>
+      <c r="CK256" s="5">
+        <v>1.6666666666666701</v>
+      </c>
+      <c r="CL256" s="5">
+        <v>75</v>
+      </c>
     </row>
-    <row r="257" spans="2:88" s="5" customFormat="1">
+    <row r="257" spans="2:90" s="5" customFormat="1">
       <c r="B257" s="5">
         <v>2012.75</v>
       </c>
@@ -56185,8 +57560,14 @@
       <c r="CJ257" s="5">
         <v>2.1293083098247199E-2</v>
       </c>
+      <c r="CK257" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="CL257" s="5">
+        <v>79.400000000000006</v>
+      </c>
     </row>
-    <row r="258" spans="2:88" s="5" customFormat="1">
+    <row r="258" spans="2:90" s="5" customFormat="1">
       <c r="B258" s="5">
         <v>2013</v>
       </c>
@@ -56429,8 +57810,14 @@
       <c r="CJ258" s="5">
         <v>-4.5014263196975698E-2</v>
       </c>
+      <c r="CK258" s="5">
+        <v>6.6666666666666696</v>
+      </c>
+      <c r="CL258" s="5">
+        <v>76.7</v>
+      </c>
     </row>
-    <row r="259" spans="2:88" s="5" customFormat="1">
+    <row r="259" spans="2:90" s="5" customFormat="1">
       <c r="B259" s="5">
         <v>2013.25</v>
       </c>
@@ -56673,8 +58060,14 @@
       <c r="CJ259" s="5">
         <v>-3.24344269964054E-3</v>
       </c>
+      <c r="CK259" s="5">
+        <v>1.93333333333333</v>
+      </c>
+      <c r="CL259" s="5">
+        <v>81.7</v>
+      </c>
     </row>
-    <row r="260" spans="2:88" s="5" customFormat="1">
+    <row r="260" spans="2:90" s="5" customFormat="1">
       <c r="B260" s="5">
         <v>2013.5</v>
       </c>
@@ -56917,8 +58310,14 @@
       <c r="CJ260" s="5">
         <v>1.15798540862946E-2</v>
       </c>
+      <c r="CK260" s="5">
+        <v>9.86666666666666</v>
+      </c>
+      <c r="CL260" s="5">
+        <v>81.599999999999994</v>
+      </c>
     </row>
-    <row r="261" spans="2:88" s="5" customFormat="1">
+    <row r="261" spans="2:90" s="5" customFormat="1">
       <c r="B261" s="5">
         <v>2013.75</v>
       </c>
@@ -57161,8 +58560,14 @@
       <c r="CJ261" s="5">
         <v>6.8041974631820002E-3</v>
       </c>
+      <c r="CK261" s="5">
+        <v>11.533333333333299</v>
+      </c>
+      <c r="CL261" s="5">
+        <v>76.900000000000006</v>
+      </c>
     </row>
-    <row r="262" spans="2:88" s="5" customFormat="1">
+    <row r="262" spans="2:90" s="5" customFormat="1">
       <c r="B262" s="5">
         <v>2014</v>
       </c>
@@ -57405,8 +58810,14 @@
       <c r="CJ262" s="5">
         <v>7.5393482012172403E-3</v>
       </c>
+      <c r="CK262" s="5">
+        <v>8</v>
+      </c>
+      <c r="CL262" s="5">
+        <v>80.900000000000006</v>
+      </c>
     </row>
-    <row r="263" spans="2:88" s="5" customFormat="1">
+    <row r="263" spans="2:90" s="5" customFormat="1">
       <c r="B263" s="5">
         <v>2014.25</v>
       </c>
@@ -57649,8 +59060,14 @@
       <c r="CJ263" s="5">
         <v>2.3667655996496301E-2</v>
       </c>
+      <c r="CK263" s="5">
+        <v>11</v>
+      </c>
+      <c r="CL263" s="5">
+        <v>82.8</v>
+      </c>
     </row>
-    <row r="264" spans="2:88" s="5" customFormat="1">
+    <row r="264" spans="2:90" s="5" customFormat="1">
       <c r="B264" s="5">
         <v>2014.5</v>
       </c>
@@ -57893,8 +59310,14 @@
       <c r="CJ264" s="5">
         <v>2.6611213320989199E-2</v>
       </c>
+      <c r="CK264" s="5">
+        <v>13</v>
+      </c>
+      <c r="CL264" s="5">
+        <v>83</v>
+      </c>
     </row>
-    <row r="265" spans="2:88" s="5" customFormat="1">
+    <row r="265" spans="2:90" s="5" customFormat="1">
       <c r="B265" s="5">
         <v>2014.75</v>
       </c>
@@ -58137,8 +59560,14 @@
       <c r="CJ265" s="5">
         <v>1.2595507168991099E-2</v>
       </c>
+      <c r="CK265" s="5">
+        <v>13.133333333333301</v>
+      </c>
+      <c r="CL265" s="5">
+        <v>89.8</v>
+      </c>
     </row>
-    <row r="266" spans="2:88" s="5" customFormat="1">
+    <row r="266" spans="2:90" s="5" customFormat="1">
       <c r="B266" s="5">
         <v>2015</v>
       </c>
@@ -58381,8 +59810,14 @@
       <c r="CJ266" s="5">
         <v>2.1122514106683501E-2</v>
       </c>
+      <c r="CK266" s="5">
+        <v>6.3333333333333304</v>
+      </c>
+      <c r="CL266" s="5">
+        <v>95.5</v>
+      </c>
     </row>
-    <row r="267" spans="2:88" s="5" customFormat="1">
+    <row r="267" spans="2:90" s="5" customFormat="1">
       <c r="B267" s="5">
         <v>2015.25</v>
       </c>
@@ -58625,8 +60060,14 @@
       <c r="CJ267" s="5">
         <v>2.0890668801432699E-2</v>
       </c>
+      <c r="CK267" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="CL267" s="5">
+        <v>94.2</v>
+      </c>
     </row>
-    <row r="268" spans="2:88" s="5" customFormat="1">
+    <row r="268" spans="2:90" s="5" customFormat="1">
       <c r="B268" s="5">
         <v>2015.5</v>
       </c>
@@ -58869,8 +60310,14 @@
       <c r="CJ268" s="5">
         <v>7.3587399273475204E-3</v>
       </c>
+      <c r="CK268" s="5">
+        <v>1.93333333333333</v>
+      </c>
+      <c r="CL268" s="5">
+        <v>90.8</v>
+      </c>
     </row>
-    <row r="269" spans="2:88" s="5" customFormat="1">
+    <row r="269" spans="2:90" s="5" customFormat="1">
       <c r="B269" s="5">
         <v>2015.75</v>
       </c>
@@ -59113,8 +60560,14 @@
       <c r="CJ269" s="5">
         <v>9.7422055700901299E-3</v>
       </c>
+      <c r="CK269" s="5">
+        <v>-2.8</v>
+      </c>
+      <c r="CL269" s="5">
+        <v>91.3</v>
+      </c>
     </row>
-    <row r="270" spans="2:88" s="5" customFormat="1">
+    <row r="270" spans="2:90" s="5" customFormat="1">
       <c r="B270" s="5">
         <v>2016</v>
       </c>
@@ -59357,8 +60810,14 @@
       <c r="CJ270" s="5">
         <v>8.7716829805082296E-4</v>
       </c>
+      <c r="CK270" s="5">
+        <v>-0.33333333333333298</v>
+      </c>
+      <c r="CL270" s="5">
+        <v>91.5</v>
+      </c>
     </row>
-    <row r="271" spans="2:88" s="5" customFormat="1">
+    <row r="271" spans="2:90" s="5" customFormat="1">
       <c r="B271" s="5">
         <v>2016.25</v>
       </c>
@@ -59601,8 +61060,14 @@
       <c r="CJ271" s="5">
         <v>8.3717660076668508E-3</v>
       </c>
+      <c r="CK271" s="5">
+        <v>3.5333333333333301</v>
+      </c>
+      <c r="CL271" s="5">
+        <v>92.4</v>
+      </c>
     </row>
-    <row r="272" spans="2:88" s="5" customFormat="1">
+    <row r="272" spans="2:90" s="5" customFormat="1">
       <c r="B272" s="5">
         <v>2016.5</v>
       </c>
@@ -59842,8 +61307,14 @@
       <c r="CJ272" s="5">
         <v>1.38437266541264E-2</v>
       </c>
+      <c r="CK272" s="5">
+        <v>2.3333333333333299</v>
+      </c>
+      <c r="CL272" s="5">
+        <v>90.3</v>
+      </c>
     </row>
-    <row r="273" spans="2:88" s="5" customFormat="1">
+    <row r="273" spans="2:90" s="5" customFormat="1">
       <c r="B273" s="5">
         <v>2016.75</v>
       </c>
@@ -60083,8 +61554,14 @@
       <c r="CJ273" s="5">
         <v>-1.39177968905237E-2</v>
       </c>
+      <c r="CK273" s="5">
+        <v>6.5333333333333297</v>
+      </c>
+      <c r="CL273" s="5">
+        <v>93.2</v>
+      </c>
     </row>
-    <row r="274" spans="2:88" s="5" customFormat="1">
+    <row r="274" spans="2:90" s="5" customFormat="1">
       <c r="B274" s="5">
         <v>2017</v>
       </c>
@@ -60322,8 +61799,14 @@
       <c r="CJ274" s="5">
         <v>1.03870738675536E-2</v>
       </c>
+      <c r="CK274" s="5">
+        <v>13.9333333333333</v>
+      </c>
+      <c r="CL274" s="5">
+        <v>97.2</v>
+      </c>
     </row>
-    <row r="275" spans="2:88" s="5" customFormat="1">
+    <row r="275" spans="2:90" s="5" customFormat="1">
       <c r="B275" s="5">
         <v>2017.25</v>
       </c>
@@ -60558,8 +62041,14 @@
       <c r="CJ275" s="5">
         <v>1.2724508580569799E-3</v>
       </c>
+      <c r="CK275" s="5">
+        <v>11.6666666666667</v>
+      </c>
+      <c r="CL275" s="5">
+        <v>96.4</v>
+      </c>
     </row>
-    <row r="276" spans="2:88" s="5" customFormat="1">
+    <row r="276" spans="2:90" s="5" customFormat="1">
       <c r="B276" s="5">
         <v>2017.5</v>
       </c>
@@ -60755,8 +62244,14 @@
       <c r="BZ276" s="5">
         <v>326163.33333333331</v>
       </c>
+      <c r="CK276" s="5">
+        <v>17.266666666666701</v>
+      </c>
+      <c r="CL276" s="5">
+        <v>95.1</v>
+      </c>
     </row>
-    <row r="277" spans="2:88" s="5" customFormat="1">
+    <row r="277" spans="2:90" s="5" customFormat="1">
       <c r="B277" s="5">
         <v>2017.75</v>
       </c>
@@ -60914,8 +62409,14 @@
       <c r="BZ277" s="5">
         <v>326810.33333333331</v>
       </c>
+      <c r="CK277" s="5">
+        <v>17.733333333333299</v>
+      </c>
+      <c r="CL277" s="5">
+        <v>98.4</v>
+      </c>
     </row>
-    <row r="278" spans="2:88" s="5" customFormat="1">
+    <row r="278" spans="2:90" s="5" customFormat="1">
       <c r="B278" s="5">
         <v>2018</v>
       </c>
@@ -61073,8 +62574,11 @@
       <c r="BZ278" s="5">
         <v>327342.66666666669</v>
       </c>
+      <c r="CK278" s="5">
+        <v>19.466666666666701</v>
+      </c>
     </row>
-    <row r="279" spans="2:88" s="5" customFormat="1">
+    <row r="279" spans="2:90" s="5" customFormat="1">
       <c r="B279" s="5">
         <v>2018.25</v>
       </c>
@@ -61216,8 +62720,11 @@
       <c r="BZ279" s="5">
         <v>327857.66666666669</v>
       </c>
+      <c r="CK279" s="5">
+        <v>17.466666666666701</v>
+      </c>
     </row>
-    <row r="280" spans="2:88" s="5" customFormat="1">
+    <row r="280" spans="2:90" s="5" customFormat="1">
       <c r="J280" s="4"/>
       <c r="K280" s="4"/>
       <c r="N280" s="4"/>
@@ -61267,8 +62774,11 @@
       <c r="BZ280" s="5">
         <v>328477.33333333331</v>
       </c>
+      <c r="CK280" s="5">
+        <v>19.466666666666701</v>
+      </c>
     </row>
-    <row r="281" spans="2:88" s="5" customFormat="1">
+    <row r="281" spans="2:90" s="5" customFormat="1">
       <c r="J281" s="4"/>
       <c r="K281" s="4"/>
       <c r="N281" s="4"/>
@@ -61315,7 +62825,7 @@
         <v>329124.33333333331</v>
       </c>
     </row>
-    <row r="282" spans="2:88" s="5" customFormat="1">
+    <row r="282" spans="2:90" s="5" customFormat="1">
       <c r="J282" s="4"/>
       <c r="K282" s="4"/>
       <c r="P282" s="4"/>
@@ -61343,7 +62853,7 @@
       <c r="BW282" s="8"/>
       <c r="BX282" s="8"/>
     </row>
-    <row r="283" spans="2:88" s="5" customFormat="1">
+    <row r="283" spans="2:90" s="5" customFormat="1">
       <c r="J283" s="4"/>
       <c r="K283" s="4"/>
       <c r="P283" s="4"/>
@@ -61358,7 +62868,7 @@
       <c r="BW283" s="8"/>
       <c r="BX283" s="8"/>
     </row>
-    <row r="284" spans="2:88" s="5" customFormat="1">
+    <row r="284" spans="2:90" s="5" customFormat="1">
       <c r="J284" s="4"/>
       <c r="K284" s="4"/>
       <c r="P284" s="4"/>
@@ -61373,7 +62883,7 @@
       <c r="BW284" s="8"/>
       <c r="BX284" s="8"/>
     </row>
-    <row r="285" spans="2:88" s="5" customFormat="1">
+    <row r="285" spans="2:90" s="5" customFormat="1">
       <c r="J285" s="4"/>
       <c r="K285" s="4"/>
       <c r="P285" s="4"/>
@@ -61388,7 +62898,7 @@
       <c r="BW285" s="8"/>
       <c r="BX285" s="8"/>
     </row>
-    <row r="286" spans="2:88" s="5" customFormat="1">
+    <row r="286" spans="2:90" s="5" customFormat="1">
       <c r="J286" s="4"/>
       <c r="K286" s="4"/>
       <c r="P286" s="4"/>
@@ -61403,7 +62913,7 @@
       <c r="BW286" s="8"/>
       <c r="BX286" s="8"/>
     </row>
-    <row r="287" spans="2:88" s="5" customFormat="1">
+    <row r="287" spans="2:90" s="5" customFormat="1">
       <c r="J287" s="4"/>
       <c r="K287" s="4"/>
       <c r="P287" s="4"/>
@@ -61418,7 +62928,7 @@
       <c r="BW287" s="8"/>
       <c r="BX287" s="8"/>
     </row>
-    <row r="288" spans="2:88" s="5" customFormat="1">
+    <row r="288" spans="2:90" s="5" customFormat="1">
       <c r="J288" s="4"/>
       <c r="K288" s="4"/>
       <c r="P288" s="4"/>

</xml_diff>